<commit_message>
feedstocj and commodities renaming
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://randus-my.sharepoint.com/personal/jrojasa_rand_org/Documents/Documents/GitHub/SJV-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2509" documentId="8_{A1084574-41F8-5F41-86C3-722B91DFE57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C0E5671A-CAAB-4AC1-BAA4-707C8625F646}"/>
+  <xr:revisionPtr revIDLastSave="2515" documentId="8_{A1084574-41F8-5F41-86C3-722B91DFE57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62903949-B00B-4C52-A36A-29AB0BFED731}"/>
   <bookViews>
-    <workbookView xWindow="-7860" yWindow="-16297" windowWidth="28995" windowHeight="15794" tabRatio="622" firstSheet="4" activeTab="11" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="16110" yWindow="-13590" windowWidth="22875" windowHeight="12135" tabRatio="622" firstSheet="10" activeTab="13" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Land" sheetId="14" r:id="rId1"/>
@@ -23,8 +23,8 @@
     <sheet name="Unit Conversion" sheetId="18" r:id="rId8"/>
     <sheet name="Conversion" sheetId="15" r:id="rId9"/>
     <sheet name="Feedstock to Commodity Buildout" sheetId="7" r:id="rId10"/>
-    <sheet name="F2C_ver2" sheetId="20" r:id="rId11"/>
-    <sheet name="Commodity to Use Buildout" sheetId="8" r:id="rId12"/>
+    <sheet name="Commodity to Use Buildout" sheetId="8" r:id="rId11"/>
+    <sheet name="F2C_ver2" sheetId="20" r:id="rId12"/>
     <sheet name="Commodity To Use Matrix" sheetId="6" r:id="rId13"/>
     <sheet name="table from Julia (to be deleted" sheetId="16" r:id="rId14"/>
     <sheet name="Feedstock to Commodity Matrix" sheetId="4" r:id="rId15"/>
@@ -1561,7 +1561,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2981,6 +2981,593 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3F942D-1725-B745-A61F-46451943A74C}">
+  <dimension ref="A1:W8"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.08203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1">
+        <v>2025</v>
+      </c>
+      <c r="D1">
+        <v>2026</v>
+      </c>
+      <c r="E1">
+        <v>2027</v>
+      </c>
+      <c r="F1">
+        <v>2028</v>
+      </c>
+      <c r="G1">
+        <v>2029</v>
+      </c>
+      <c r="H1">
+        <v>2030</v>
+      </c>
+      <c r="I1">
+        <v>2031</v>
+      </c>
+      <c r="J1">
+        <v>2032</v>
+      </c>
+      <c r="K1">
+        <v>2033</v>
+      </c>
+      <c r="L1">
+        <v>2034</v>
+      </c>
+      <c r="M1">
+        <v>2035</v>
+      </c>
+      <c r="N1">
+        <v>2036</v>
+      </c>
+      <c r="O1">
+        <v>2037</v>
+      </c>
+      <c r="P1">
+        <v>2038</v>
+      </c>
+      <c r="Q1">
+        <v>2039</v>
+      </c>
+      <c r="R1">
+        <v>2040</v>
+      </c>
+      <c r="S1">
+        <v>2041</v>
+      </c>
+      <c r="T1">
+        <v>2042</v>
+      </c>
+      <c r="U1">
+        <v>2043</v>
+      </c>
+      <c r="V1">
+        <v>2044</v>
+      </c>
+      <c r="W1">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+      <c r="O2" s="2">
+        <v>1</v>
+      </c>
+      <c r="P2" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>1</v>
+      </c>
+      <c r="R2" s="2">
+        <v>1</v>
+      </c>
+      <c r="S2" s="2">
+        <v>1</v>
+      </c>
+      <c r="T2" s="2">
+        <v>1</v>
+      </c>
+      <c r="U2" s="2">
+        <v>1</v>
+      </c>
+      <c r="V2" s="2">
+        <v>1</v>
+      </c>
+      <c r="W2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
+      </c>
+      <c r="H3" s="2">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2">
+        <v>0</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>0</v>
+      </c>
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>0</v>
+      </c>
+      <c r="R3" s="2">
+        <v>0</v>
+      </c>
+      <c r="S3" s="2">
+        <v>0</v>
+      </c>
+      <c r="T3" s="2">
+        <v>0</v>
+      </c>
+      <c r="U3" s="2">
+        <v>0</v>
+      </c>
+      <c r="V3" s="2">
+        <v>0</v>
+      </c>
+      <c r="W3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>1</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>1</v>
+      </c>
+      <c r="R4" s="2">
+        <v>1</v>
+      </c>
+      <c r="S4" s="2">
+        <v>1</v>
+      </c>
+      <c r="T4" s="2">
+        <v>1</v>
+      </c>
+      <c r="U4" s="2">
+        <v>1</v>
+      </c>
+      <c r="V4" s="2">
+        <v>1</v>
+      </c>
+      <c r="W4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <v>0</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>0</v>
+      </c>
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>0</v>
+      </c>
+      <c r="R5" s="2">
+        <v>0</v>
+      </c>
+      <c r="S5" s="2">
+        <v>0</v>
+      </c>
+      <c r="T5" s="2">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2">
+        <v>0</v>
+      </c>
+      <c r="V5" s="2">
+        <v>0</v>
+      </c>
+      <c r="W5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
+        <v>0</v>
+      </c>
+      <c r="I6" s="2">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>0</v>
+      </c>
+      <c r="R6" s="2">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0</v>
+      </c>
+      <c r="T6" s="2">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2">
+        <v>0</v>
+      </c>
+      <c r="V6" s="2">
+        <v>0</v>
+      </c>
+      <c r="W6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2">
+        <v>1</v>
+      </c>
+      <c r="P7" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>1</v>
+      </c>
+      <c r="R7" s="2">
+        <v>1</v>
+      </c>
+      <c r="S7" s="2">
+        <v>1</v>
+      </c>
+      <c r="T7" s="2">
+        <v>1</v>
+      </c>
+      <c r="U7" s="2">
+        <v>1</v>
+      </c>
+      <c r="V7" s="2">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1</v>
+      </c>
+      <c r="F8" s="2">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+      <c r="L8" s="2">
+        <v>1</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1</v>
+      </c>
+      <c r="N8" s="2">
+        <v>1</v>
+      </c>
+      <c r="O8" s="2">
+        <v>1</v>
+      </c>
+      <c r="P8" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>1</v>
+      </c>
+      <c r="R8" s="2">
+        <v>1</v>
+      </c>
+      <c r="S8" s="2">
+        <v>1</v>
+      </c>
+      <c r="T8" s="2">
+        <v>1</v>
+      </c>
+      <c r="U8" s="2">
+        <v>1</v>
+      </c>
+      <c r="V8" s="2">
+        <v>1</v>
+      </c>
+      <c r="W8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDDA0F3-A3DE-4AB4-98AB-8BE3425A27E0}">
   <dimension ref="A1:G30"/>
   <sheetViews>
@@ -3466,593 +4053,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3F942D-1725-B745-A61F-46451943A74C}">
-  <dimension ref="A1:W8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C1">
-        <v>2025</v>
-      </c>
-      <c r="D1">
-        <v>2026</v>
-      </c>
-      <c r="E1">
-        <v>2027</v>
-      </c>
-      <c r="F1">
-        <v>2028</v>
-      </c>
-      <c r="G1">
-        <v>2029</v>
-      </c>
-      <c r="H1">
-        <v>2030</v>
-      </c>
-      <c r="I1">
-        <v>2031</v>
-      </c>
-      <c r="J1">
-        <v>2032</v>
-      </c>
-      <c r="K1">
-        <v>2033</v>
-      </c>
-      <c r="L1">
-        <v>2034</v>
-      </c>
-      <c r="M1">
-        <v>2035</v>
-      </c>
-      <c r="N1">
-        <v>2036</v>
-      </c>
-      <c r="O1">
-        <v>2037</v>
-      </c>
-      <c r="P1">
-        <v>2038</v>
-      </c>
-      <c r="Q1">
-        <v>2039</v>
-      </c>
-      <c r="R1">
-        <v>2040</v>
-      </c>
-      <c r="S1">
-        <v>2041</v>
-      </c>
-      <c r="T1">
-        <v>2042</v>
-      </c>
-      <c r="U1">
-        <v>2043</v>
-      </c>
-      <c r="V1">
-        <v>2044</v>
-      </c>
-      <c r="W1">
-        <v>2045</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2">
-        <v>1</v>
-      </c>
-      <c r="K2" s="2">
-        <v>1</v>
-      </c>
-      <c r="L2" s="2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2">
-        <v>1</v>
-      </c>
-      <c r="O2" s="2">
-        <v>1</v>
-      </c>
-      <c r="P2" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>1</v>
-      </c>
-      <c r="R2" s="2">
-        <v>1</v>
-      </c>
-      <c r="S2" s="2">
-        <v>1</v>
-      </c>
-      <c r="T2" s="2">
-        <v>1</v>
-      </c>
-      <c r="U2" s="2">
-        <v>1</v>
-      </c>
-      <c r="V2" s="2">
-        <v>1</v>
-      </c>
-      <c r="W2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>64</v>
-      </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-      <c r="G3" s="2">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2">
-        <v>0</v>
-      </c>
-      <c r="I3" s="2">
-        <v>0</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
-      </c>
-      <c r="K3" s="2">
-        <v>0</v>
-      </c>
-      <c r="L3" s="2">
-        <v>0</v>
-      </c>
-      <c r="M3" s="2">
-        <v>0</v>
-      </c>
-      <c r="N3" s="2">
-        <v>0</v>
-      </c>
-      <c r="O3" s="2">
-        <v>0</v>
-      </c>
-      <c r="P3" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="2">
-        <v>0</v>
-      </c>
-      <c r="R3" s="2">
-        <v>0</v>
-      </c>
-      <c r="S3" s="2">
-        <v>0</v>
-      </c>
-      <c r="T3" s="2">
-        <v>0</v>
-      </c>
-      <c r="U3" s="2">
-        <v>0</v>
-      </c>
-      <c r="V3" s="2">
-        <v>0</v>
-      </c>
-      <c r="W3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
-        <v>1</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2">
-        <v>1</v>
-      </c>
-      <c r="K4" s="2">
-        <v>1</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="N4" s="2">
-        <v>1</v>
-      </c>
-      <c r="O4" s="2">
-        <v>1</v>
-      </c>
-      <c r="P4" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>1</v>
-      </c>
-      <c r="R4" s="2">
-        <v>1</v>
-      </c>
-      <c r="S4" s="2">
-        <v>1</v>
-      </c>
-      <c r="T4" s="2">
-        <v>1</v>
-      </c>
-      <c r="U4" s="2">
-        <v>1</v>
-      </c>
-      <c r="V4" s="2">
-        <v>1</v>
-      </c>
-      <c r="W4" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
-        <v>0</v>
-      </c>
-      <c r="N5" s="2">
-        <v>0</v>
-      </c>
-      <c r="O5" s="2">
-        <v>0</v>
-      </c>
-      <c r="P5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>0</v>
-      </c>
-      <c r="R5" s="2">
-        <v>0</v>
-      </c>
-      <c r="S5" s="2">
-        <v>0</v>
-      </c>
-      <c r="T5" s="2">
-        <v>0</v>
-      </c>
-      <c r="U5" s="2">
-        <v>0</v>
-      </c>
-      <c r="V5" s="2">
-        <v>0</v>
-      </c>
-      <c r="W5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
-        <v>0</v>
-      </c>
-      <c r="M6" s="2">
-        <v>0</v>
-      </c>
-      <c r="N6" s="2">
-        <v>0</v>
-      </c>
-      <c r="O6" s="2">
-        <v>0</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>0</v>
-      </c>
-      <c r="R6" s="2">
-        <v>0</v>
-      </c>
-      <c r="S6" s="2">
-        <v>0</v>
-      </c>
-      <c r="T6" s="2">
-        <v>0</v>
-      </c>
-      <c r="U6" s="2">
-        <v>0</v>
-      </c>
-      <c r="V6" s="2">
-        <v>0</v>
-      </c>
-      <c r="W6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7" s="2">
-        <v>1</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2">
-        <v>1</v>
-      </c>
-      <c r="J7" s="2">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2">
-        <v>1</v>
-      </c>
-      <c r="L7" s="2">
-        <v>1</v>
-      </c>
-      <c r="M7" s="2">
-        <v>1</v>
-      </c>
-      <c r="N7" s="2">
-        <v>1</v>
-      </c>
-      <c r="O7" s="2">
-        <v>1</v>
-      </c>
-      <c r="P7" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>1</v>
-      </c>
-      <c r="R7" s="2">
-        <v>1</v>
-      </c>
-      <c r="S7" s="2">
-        <v>1</v>
-      </c>
-      <c r="T7" s="2">
-        <v>1</v>
-      </c>
-      <c r="U7" s="2">
-        <v>1</v>
-      </c>
-      <c r="V7" s="2">
-        <v>1</v>
-      </c>
-      <c r="W7" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="A8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="2">
-        <v>1</v>
-      </c>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1</v>
-      </c>
-      <c r="F8" s="2">
-        <v>1</v>
-      </c>
-      <c r="G8" s="2">
-        <v>1</v>
-      </c>
-      <c r="H8" s="2">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2">
-        <v>1</v>
-      </c>
-      <c r="K8" s="2">
-        <v>1</v>
-      </c>
-      <c r="L8" s="2">
-        <v>1</v>
-      </c>
-      <c r="M8" s="2">
-        <v>1</v>
-      </c>
-      <c r="N8" s="2">
-        <v>1</v>
-      </c>
-      <c r="O8" s="2">
-        <v>1</v>
-      </c>
-      <c r="P8" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>1</v>
-      </c>
-      <c r="R8" s="2">
-        <v>1</v>
-      </c>
-      <c r="S8" s="2">
-        <v>1</v>
-      </c>
-      <c r="T8" s="2">
-        <v>1</v>
-      </c>
-      <c r="U8" s="2">
-        <v>1</v>
-      </c>
-      <c r="V8" s="2">
-        <v>1</v>
-      </c>
-      <c r="W8" s="2">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -4167,8 +4167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF7B0DD-C673-4DCD-83AE-47E17C286F51}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5207,7 +5207,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD9"/>
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5442,7 +5442,7 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
@@ -5903,7 +5903,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B28" t="s">
         <v>19</v>
@@ -6324,7 +6324,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B46" t="s">
         <v>19</v>
@@ -6571,7 +6571,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6666,7 +6666,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
         <v>60</v>
@@ -6745,7 +6745,7 @@
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -7095,7 +7095,7 @@
         <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>63</v>
       </c>
       <c r="C5" t="s">
         <v>76</v>
@@ -7454,7 +7454,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -7663,7 +7663,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>19</v>
@@ -7775,7 +7775,7 @@
         <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C14" t="s">
         <v>82</v>
@@ -7792,7 +7792,7 @@
         <v>44</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C15" t="s">
         <v>82</v>
@@ -8042,7 +8042,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>19</v>
@@ -8682,8 +8682,8 @@
   <dimension ref="A1:AK23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K20" sqref="K20"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9879,7 +9879,7 @@
   <dimension ref="A1:Z37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9973,7 +9973,7 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
filtering out uses without carbon intensity use
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://randus-my.sharepoint.com/personal/jrojasa_rand_org/Documents/Documents/GitHub/SJV-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2515" documentId="8_{A1084574-41F8-5F41-86C3-722B91DFE57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62903949-B00B-4C52-A36A-29AB0BFED731}"/>
+  <xr:revisionPtr revIDLastSave="2518" documentId="8_{A1084574-41F8-5F41-86C3-722B91DFE57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80AD4DE8-8B8F-49D4-862E-77DEE11632C9}"/>
   <bookViews>
-    <workbookView xWindow="16110" yWindow="-13590" windowWidth="22875" windowHeight="12135" tabRatio="622" firstSheet="10" activeTab="13" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="14310" yWindow="-16470" windowWidth="29040" windowHeight="15840" tabRatio="622" firstSheet="3" activeTab="10" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Land" sheetId="14" r:id="rId1"/>
@@ -1561,7 +1561,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2984,8 +2984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3F942D-1725-B745-A61F-46451943A74C}">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -3212,7 +3212,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>294</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -4167,7 +4167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF7B0DD-C673-4DCD-83AE-47E17C286F51}">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -5207,7 +5207,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Update SJV Variable Architecture.xlsx
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://randus-my.sharepoint.com/personal/jrojasa_rand_org/Documents/Documents/GitHub/SJV-/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2518" documentId="8_{A1084574-41F8-5F41-86C3-722B91DFE57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80AD4DE8-8B8F-49D4-862E-77DEE11632C9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2396E1A9-EBA4-427B-9C7E-082F669CF99F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="-16470" windowWidth="29040" windowHeight="15840" tabRatio="622" firstSheet="3" activeTab="10" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView minimized="1" xWindow="-795" yWindow="660" windowWidth="29100" windowHeight="11325" tabRatio="622" firstSheet="2" activeTab="2" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Land" sheetId="14" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="294">
   <si>
     <t>Feedstock</t>
   </si>
@@ -943,9 +943,6 @@
   </si>
   <si>
     <t>MW of electric capacity per 1MCF (64% capacity factor and 50% conversion efficiency)</t>
-  </si>
-  <si>
-    <t>`</t>
   </si>
   <si>
     <t>Ammonia Production</t>
@@ -1564,19 +1561,19 @@
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.25" customWidth="1"/>
     <col min="2" max="2" width="12.75" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="11.25" customWidth="1"/>
     <col min="7" max="7" width="8.25" customWidth="1"/>
-    <col min="8" max="9" width="24.08203125" customWidth="1"/>
+    <col min="8" max="9" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1611,7 +1608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1645,7 +1642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -1682,7 +1679,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -1711,7 +1708,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -1740,7 +1737,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -1769,7 +1766,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1798,7 +1795,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -1832,7 +1829,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -1869,7 +1866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
@@ -1898,7 +1895,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -1930,7 +1927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -1964,7 +1961,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -1993,7 +1990,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -2027,7 +2024,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -2064,7 +2061,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>22</v>
       </c>
@@ -2094,7 +2091,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
@@ -2126,7 +2123,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
@@ -2159,7 +2156,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>22</v>
       </c>
@@ -2202,16 +2199,16 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.08203125" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.125" customWidth="1"/>
+    <col min="2" max="2" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.5" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2291,7 +2288,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2329,7 +2326,7 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2367,7 +2364,7 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2405,7 +2402,7 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2443,7 +2440,7 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2481,7 +2478,7 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2519,7 +2516,7 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -2557,7 +2554,7 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -2595,7 +2592,7 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2633,7 +2630,7 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2671,7 +2668,7 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -2709,7 +2706,7 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>38</v>
       </c>
@@ -2747,7 +2744,7 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -2785,7 +2782,7 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -2823,7 +2820,7 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>162</v>
       </c>
@@ -2861,7 +2858,7 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -2899,7 +2896,7 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -2937,7 +2934,7 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2984,17 +2981,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3F942D-1725-B745-A61F-46451943A74C}">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08203125" customWidth="1"/>
+    <col min="2" max="2" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3065,7 +3062,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3136,7 +3133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3207,12 +3204,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -3278,7 +3275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -3349,7 +3346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -3420,7 +3417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -3491,7 +3488,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
@@ -3575,17 +3572,17 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.75" customWidth="1"/>
     <col min="2" max="2" width="20.75" customWidth="1"/>
-    <col min="3" max="3" width="20.58203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.375" customWidth="1"/>
+    <col min="6" max="6" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
         <v>165</v>
       </c>
@@ -3608,7 +3605,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>11</v>
       </c>
@@ -3629,7 +3626,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>22</v>
       </c>
@@ -3650,7 +3647,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>34</v>
       </c>
@@ -3671,7 +3668,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>35</v>
       </c>
@@ -3692,7 +3689,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>145</v>
       </c>
@@ -3713,7 +3710,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>145</v>
       </c>
@@ -3734,7 +3731,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>38</v>
       </c>
@@ -3755,7 +3752,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>11</v>
       </c>
@@ -3776,7 +3773,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>58</v>
       </c>
@@ -3797,7 +3794,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>145</v>
       </c>
@@ -3818,7 +3815,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>145</v>
       </c>
@@ -3839,7 +3836,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
         <v>38</v>
       </c>
@@ -3860,7 +3857,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
         <v>145</v>
       </c>
@@ -3881,7 +3878,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>145</v>
       </c>
@@ -3902,7 +3899,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
         <v>168</v>
       </c>
@@ -3923,7 +3920,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="15" t="s">
         <v>168</v>
       </c>
@@ -3944,7 +3941,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="15" t="s">
         <v>145</v>
       </c>
@@ -3965,7 +3962,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
         <v>145</v>
       </c>
@@ -3986,7 +3983,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="52" t="s">
         <v>167</v>
       </c>
@@ -3994,7 +3991,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="53" t="s">
         <v>12</v>
       </c>
@@ -4002,7 +3999,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="53" t="s">
         <v>19</v>
       </c>
@@ -4010,7 +4007,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="53" t="s">
         <v>19</v>
       </c>
@@ -4018,7 +4015,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
         <v>38</v>
       </c>
@@ -4026,7 +4023,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="53" t="s">
         <v>38</v>
       </c>
@@ -4034,7 +4031,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="53" t="s">
         <v>38</v>
       </c>
@@ -4042,7 +4039,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="53" t="s">
         <v>71</v>
       </c>
@@ -4064,17 +4061,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.58203125" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4103,7 +4100,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -4114,7 +4111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -4125,7 +4122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -4142,7 +4139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -4150,7 +4147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -4171,17 +4168,17 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.875" customWidth="1"/>
+    <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.58203125" customWidth="1"/>
+    <col min="4" max="4" width="40.875" customWidth="1"/>
+    <col min="5" max="5" width="30.625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -4210,7 +4207,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>58</v>
       </c>
@@ -4237,7 +4234,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>162</v>
       </c>
@@ -4264,7 +4261,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>11</v>
       </c>
@@ -4291,7 +4288,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
@@ -4318,7 +4315,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>22</v>
       </c>
@@ -4345,7 +4342,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>37</v>
       </c>
@@ -4368,7 +4365,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>36</v>
       </c>
@@ -4391,7 +4388,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>187</v>
       </c>
@@ -4416,7 +4413,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>187</v>
       </c>
@@ -4441,7 +4438,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>191</v>
       </c>
@@ -4466,7 +4463,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
         <v>191</v>
       </c>
@@ -4485,7 +4482,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="15"/>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
@@ -4500,7 +4497,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
@@ -4515,7 +4512,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>196</v>
       </c>
@@ -4542,7 +4539,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>179</v>
       </c>
@@ -4565,7 +4562,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>184</v>
       </c>
@@ -4588,7 +4585,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>187</v>
       </c>
@@ -4611,7 +4608,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="21" t="s">
         <v>191</v>
       </c>
@@ -4625,7 +4622,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>192</v>
       </c>
@@ -4639,7 +4636,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>37</v>
       </c>
@@ -4653,7 +4650,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
         <v>36</v>
       </c>
@@ -4667,12 +4664,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="27" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
         <v>0</v>
       </c>
@@ -4689,7 +4686,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
         <v>58</v>
       </c>
@@ -4698,7 +4695,7 @@
       </c>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
         <v>162</v>
       </c>
@@ -4707,7 +4704,7 @@
       </c>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="15" t="s">
         <v>50</v>
       </c>
@@ -4716,7 +4713,7 @@
       </c>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
         <v>11</v>
       </c>
@@ -4727,7 +4724,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
         <v>22</v>
       </c>
@@ -4736,7 +4733,7 @@
       </c>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
         <v>217</v>
       </c>
@@ -4745,7 +4742,7 @@
       </c>
       <c r="C37" s="15"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="15" t="s">
         <v>35</v>
       </c>
@@ -4754,7 +4751,7 @@
       </c>
       <c r="C38" s="15"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
         <v>37</v>
       </c>
@@ -4768,7 +4765,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
         <v>36</v>
       </c>
@@ -4782,7 +4779,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="15" t="s">
         <v>187</v>
       </c>
@@ -4799,7 +4796,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="15" t="s">
         <v>191</v>
       </c>
@@ -4816,12 +4813,12 @@
         <v>221</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="27" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="33" t="s">
         <v>1</v>
       </c>
@@ -4832,7 +4829,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="15" t="s">
         <v>19</v>
       </c>
@@ -4843,7 +4840,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="31" t="s">
         <v>19</v>
       </c>
@@ -4860,7 +4857,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="31" t="s">
         <v>19</v>
       </c>
@@ -4877,7 +4874,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="31" t="s">
         <v>19</v>
       </c>
@@ -4897,7 +4894,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>19</v>
       </c>
@@ -4914,7 +4911,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="28" t="s">
         <v>58</v>
       </c>
@@ -4931,7 +4928,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>58</v>
       </c>
@@ -4942,7 +4939,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="28" t="s">
         <v>58</v>
       </c>
@@ -4959,7 +4956,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="28" t="s">
         <v>12</v>
       </c>
@@ -4976,7 +4973,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>12</v>
       </c>
@@ -4987,12 +4984,12 @@
         <v>234</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="27" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="28" t="s">
         <v>241</v>
       </c>
@@ -5003,7 +5000,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="30" t="s">
         <v>243</v>
       </c>
@@ -5011,7 +5008,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="28" t="s">
         <v>244</v>
       </c>
@@ -5019,12 +5016,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="27" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="28" t="s">
         <v>246</v>
       </c>
@@ -5032,7 +5029,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="28" t="s">
         <v>247</v>
       </c>
@@ -5053,13 +5050,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.58203125" customWidth="1"/>
-    <col min="2" max="5" width="15.58203125" customWidth="1"/>
+    <col min="1" max="1" width="25.625" customWidth="1"/>
+    <col min="2" max="5" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>249</v>
       </c>
@@ -5079,7 +5076,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>250</v>
       </c>
@@ -5090,7 +5087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -5098,7 +5095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -5106,7 +5103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -5120,7 +5117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>148</v>
       </c>
@@ -5134,7 +5131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>251</v>
       </c>
@@ -5148,7 +5145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>252</v>
       </c>
@@ -5159,7 +5156,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>253</v>
       </c>
@@ -5170,7 +5167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>254</v>
       </c>
@@ -5181,7 +5178,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -5189,7 +5186,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -5207,21 +5204,21 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="5" width="26" customWidth="1"/>
-    <col min="6" max="7" width="24.08203125" customWidth="1"/>
+    <col min="6" max="7" width="24.125" customWidth="1"/>
     <col min="8" max="8" width="31.5" customWidth="1"/>
-    <col min="9" max="9" width="36.83203125" customWidth="1"/>
+    <col min="9" max="9" width="36.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5250,7 +5247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -5273,7 +5270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -5302,7 +5299,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -5325,7 +5322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -5348,7 +5345,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -5356,7 +5353,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>293</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>
@@ -5371,7 +5368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
         <v>36</v>
       </c>
@@ -5394,7 +5391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
         <v>37</v>
       </c>
@@ -5417,7 +5414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
         <v>38</v>
       </c>
@@ -5440,7 +5437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -5469,7 +5466,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -5501,7 +5498,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -5533,7 +5530,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
         <v>38</v>
       </c>
@@ -5557,7 +5554,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
         <v>44</v>
       </c>
@@ -5581,7 +5578,7 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
@@ -5607,7 +5604,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -5633,7 +5630,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -5659,7 +5656,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -5688,7 +5685,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -5717,7 +5714,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -5740,7 +5737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>11</v>
       </c>
@@ -5769,7 +5766,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -5792,7 +5789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -5815,7 +5812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>35</v>
       </c>
@@ -5838,7 +5835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
         <v>36</v>
       </c>
@@ -5861,7 +5858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
         <v>37</v>
       </c>
@@ -5881,7 +5878,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
         <v>38</v>
       </c>
@@ -5901,7 +5898,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -5930,7 +5927,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -5951,7 +5948,7 @@
       </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="37" t="s">
         <v>38</v>
       </c>
@@ -5972,7 +5969,7 @@
       </c>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -5993,7 +5990,7 @@
       </c>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="37" t="s">
         <v>44</v>
       </c>
@@ -6020,7 +6017,7 @@
       </c>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -6046,7 +6043,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -6072,7 +6069,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -6098,7 +6095,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -6118,7 +6115,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -6138,7 +6135,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -6161,7 +6158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>11</v>
       </c>
@@ -6190,7 +6187,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -6213,7 +6210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -6236,7 +6233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
@@ -6259,7 +6256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="37" t="s">
         <v>36</v>
       </c>
@@ -6282,7 +6279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="37" t="s">
         <v>37</v>
       </c>
@@ -6302,7 +6299,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="37" t="s">
         <v>38</v>
       </c>
@@ -6322,7 +6319,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>40</v>
       </c>
@@ -6351,7 +6348,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -6372,7 +6369,7 @@
       </c>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="37" t="s">
         <v>38</v>
       </c>
@@ -6393,7 +6390,7 @@
       </c>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>36</v>
       </c>
@@ -6414,7 +6411,7 @@
       </c>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="37" t="s">
         <v>44</v>
       </c>
@@ -6441,7 +6438,7 @@
       </c>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -6467,7 +6464,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -6493,7 +6490,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -6519,7 +6516,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -6539,7 +6536,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -6570,21 +6567,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{950C9CF8-69D9-4059-BEAC-4E8C34B2FEBB}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="173.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="173.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6604,7 +6601,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -6621,7 +6618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -6641,7 +6638,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -6661,7 +6658,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -6678,7 +6675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -6698,12 +6695,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C7" t="s">
         <v>68</v>
@@ -6715,7 +6712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
@@ -6745,20 +6742,20 @@
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.58203125" customWidth="1"/>
-    <col min="2" max="2" width="19.08203125" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="25.75" customWidth="1"/>
-    <col min="6" max="6" width="19.08203125" customWidth="1"/>
+    <col min="6" max="6" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6841,7 +6838,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -6924,7 +6921,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -7007,7 +7004,7 @@
         <v>16.543009238729827</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>38</v>
       </c>
@@ -7090,7 +7087,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -7173,7 +7170,7 @@
         <v>16.543009238729827</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -7256,12 +7253,12 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C7" t="s">
         <v>78</v>
@@ -7360,7 +7357,7 @@
         <v>117.67</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>48</v>
       </c>
@@ -7457,18 +7454,18 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.875" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="8" width="24.08203125" customWidth="1"/>
+    <col min="7" max="8" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7506,7 +7503,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -7523,7 +7520,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -7553,7 +7550,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -7571,7 +7568,7 @@
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -7589,7 +7586,7 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -7607,7 +7604,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>36</v>
       </c>
@@ -7625,7 +7622,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>37</v>
       </c>
@@ -7643,7 +7640,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>38</v>
       </c>
@@ -7661,7 +7658,7 @@
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
@@ -7691,7 +7688,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -7721,7 +7718,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -7752,7 +7749,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>38</v>
       </c>
@@ -7770,7 +7767,7 @@
       </c>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -7787,7 +7784,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -7804,7 +7801,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -7821,7 +7818,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -7838,7 +7835,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -7855,7 +7852,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -7872,7 +7869,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
@@ -7892,7 +7889,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>11</v>
       </c>
@@ -7929,7 +7926,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -7950,7 +7947,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -7968,7 +7965,7 @@
       </c>
       <c r="F23" s="8"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>35</v>
       </c>
@@ -7986,7 +7983,7 @@
       </c>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="13" t="s">
         <v>36</v>
       </c>
@@ -8004,7 +8001,7 @@
       </c>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="13" t="s">
         <v>37</v>
       </c>
@@ -8022,7 +8019,7 @@
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>38</v>
       </c>
@@ -8040,7 +8037,7 @@
       </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -8077,7 +8074,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -8114,7 +8111,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -8145,7 +8142,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>38</v>
       </c>
@@ -8163,7 +8160,7 @@
       </c>
       <c r="F31" s="8"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>45</v>
       </c>
@@ -8183,7 +8180,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>44</v>
       </c>
@@ -8203,7 +8200,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>47</v>
       </c>
@@ -8223,7 +8220,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>50</v>
       </c>
@@ -8243,7 +8240,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -8260,7 +8257,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -8277,35 +8274,35 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
     </row>
@@ -8323,16 +8320,16 @@
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
-    <col min="7" max="8" width="24.08203125" customWidth="1"/>
+    <col min="5" max="5" width="22.875" customWidth="1"/>
+    <col min="7" max="8" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8364,7 +8361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -8384,7 +8381,7 @@
         <v>3.4599999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
         <v>11</v>
       </c>
@@ -8408,7 +8405,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -8428,7 +8425,7 @@
         <v>2.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -8448,7 +8445,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -8468,7 +8465,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -8488,7 +8485,7 @@
         <v>4.0899999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -8508,7 +8505,7 @@
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -8528,7 +8525,7 @@
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -8548,7 +8545,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -8568,7 +8565,7 @@
         <v>5.62E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -8588,7 +8585,7 @@
         <v>5.62E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -8622,15 +8619,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5" customWidth="1"/>
     <col min="4" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -8647,7 +8644,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -8664,7 +8661,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -8683,29 +8680,29 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B26" sqref="B26"/>
+      <selection pane="topRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.75" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="15.25" customWidth="1"/>
-    <col min="6" max="6" width="11.08203125" customWidth="1"/>
+    <col min="6" max="6" width="11.125" customWidth="1"/>
     <col min="7" max="7" width="17.75" customWidth="1"/>
     <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.375" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="43.5" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="19.08203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.375" customWidth="1"/>
+    <col min="13" max="13" width="19.125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="10.5" customWidth="1"/>
     <col min="16" max="16" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8818,7 +8815,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -8911,7 +8908,7 @@
         <v>1216.528453322951</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -8953,7 +8950,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -9046,7 +9043,7 @@
         <v>2101.97739666605</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -9139,7 +9136,7 @@
         <v>1171.0983188067505</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -9232,7 +9229,7 @@
         <v>2214.52431017765</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -9340,7 +9337,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -9370,30 +9367,74 @@
       <c r="J8" s="12"/>
       <c r="K8" s="42"/>
       <c r="L8" s="42"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
-      <c r="AE8" s="5"/>
-      <c r="AF8" s="5"/>
-      <c r="AG8" s="5"/>
-      <c r="AH8" s="5"/>
-      <c r="AI8" s="5"/>
-      <c r="AJ8" s="5"/>
-      <c r="AK8" s="5"/>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="P8" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>6035.0858307307299</v>
+      </c>
+      <c r="R8" s="5">
+        <v>5991.4369513857655</v>
+      </c>
+      <c r="S8" s="5">
+        <v>5947.7880720408011</v>
+      </c>
+      <c r="T8" s="5">
+        <v>5904.1391926958368</v>
+      </c>
+      <c r="U8" s="5">
+        <v>5860.4903133508724</v>
+      </c>
+      <c r="V8" s="5">
+        <v>5816.841434005908</v>
+      </c>
+      <c r="W8" s="5">
+        <v>5773.1925546609436</v>
+      </c>
+      <c r="X8" s="5">
+        <v>5729.5436753159793</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>5685.8947959710149</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>5642.2459166260505</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>5598.5970372810862</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>5554.9481579361218</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>5511.2992785911574</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>5467.650399246193</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>5424.0015199012287</v>
+      </c>
+      <c r="AF8" s="5">
+        <v>5380.3526405562643</v>
+      </c>
+      <c r="AG8" s="5">
+        <v>5336.7037612112999</v>
+      </c>
+      <c r="AH8" s="5">
+        <v>5293.0548818663356</v>
+      </c>
+      <c r="AI8" s="5">
+        <v>5249.4060025213712</v>
+      </c>
+      <c r="AJ8" s="5">
+        <v>5205.7571231764068</v>
+      </c>
+      <c r="AK8" s="5">
+        <v>5162.1082438314425</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -9427,30 +9468,74 @@
         <v>292</v>
       </c>
       <c r="L9" s="42"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="5"/>
-      <c r="AB9" s="5"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="5"/>
-      <c r="AE9" s="5"/>
-      <c r="AF9" s="5"/>
-      <c r="AG9" s="5"/>
-      <c r="AH9" s="5"/>
-      <c r="AI9" s="5"/>
-      <c r="AJ9" s="5"/>
-      <c r="AK9" s="5"/>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="P9" s="41" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>6035.0858307307299</v>
+      </c>
+      <c r="R9" s="5">
+        <v>5991.4369513857655</v>
+      </c>
+      <c r="S9" s="5">
+        <v>5947.7880720408011</v>
+      </c>
+      <c r="T9" s="5">
+        <v>5904.1391926958368</v>
+      </c>
+      <c r="U9" s="5">
+        <v>5860.4903133508724</v>
+      </c>
+      <c r="V9" s="5">
+        <v>5816.841434005908</v>
+      </c>
+      <c r="W9" s="5">
+        <v>5773.1925546609436</v>
+      </c>
+      <c r="X9" s="5">
+        <v>5729.5436753159793</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>5685.8947959710149</v>
+      </c>
+      <c r="Z9" s="5">
+        <v>5642.2459166260505</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>5598.5970372810862</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>5554.9481579361218</v>
+      </c>
+      <c r="AC9" s="5">
+        <v>5511.2992785911574</v>
+      </c>
+      <c r="AD9" s="5">
+        <v>5467.650399246193</v>
+      </c>
+      <c r="AE9" s="5">
+        <v>5424.0015199012287</v>
+      </c>
+      <c r="AF9" s="5">
+        <v>5380.3526405562643</v>
+      </c>
+      <c r="AG9" s="5">
+        <v>5336.7037612112999</v>
+      </c>
+      <c r="AH9" s="5">
+        <v>5293.0548818663356</v>
+      </c>
+      <c r="AI9" s="5">
+        <v>5249.4060025213712</v>
+      </c>
+      <c r="AJ9" s="5">
+        <v>5205.7571231764068</v>
+      </c>
+      <c r="AK9" s="5">
+        <v>5162.1082438314425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -9492,7 +9577,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -9528,7 +9613,7 @@
       <c r="L11" s="45"/>
       <c r="O11" s="38"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -9576,7 +9661,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -9624,7 +9709,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -9663,7 +9748,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -9702,7 +9787,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -9738,7 +9823,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -9774,7 +9859,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -9811,7 +9896,7 @@
       </c>
       <c r="O18" s="55"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -9848,7 +9933,7 @@
       </c>
       <c r="O19" s="55"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L23">
         <v>1000</v>
       </c>
@@ -9882,16 +9967,16 @@
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.58203125" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="30.375" customWidth="1"/>
+    <col min="3" max="3" width="8.375" customWidth="1"/>
+    <col min="4" max="4" width="23.875" customWidth="1"/>
     <col min="5" max="5" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9971,7 +10056,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
@@ -9985,7 +10070,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -9999,7 +10084,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -10079,7 +10164,7 @@
         <v>1216.528453322951</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>22</v>
       </c>
@@ -10159,7 +10244,7 @@
         <v>2101.97739666605</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>145</v>
       </c>
@@ -10239,7 +10324,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>146</v>
       </c>
@@ -10319,7 +10404,7 @@
         <v>1171.0983188067505</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>35</v>
       </c>
@@ -10399,7 +10484,7 @@
         <v>2214.52431017765</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -10413,7 +10498,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>148</v>
       </c>
@@ -10427,7 +10512,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -10441,7 +10526,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -10455,7 +10540,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0.8</v>
       </c>
@@ -10463,7 +10548,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>330.25</v>
       </c>
@@ -10471,7 +10556,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16">
         <f>A15*1.1</f>
         <v>363.27500000000003</v>
@@ -10480,7 +10565,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1250</v>
       </c>
@@ -10488,22 +10573,22 @@
         <v>257</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C18" s="14"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>141</v>
       </c>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f>0.17*A16</f>
         <v>61.756750000000011</v>
@@ -10512,7 +10597,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f>0.19*A16</f>
         <v>69.022250000000014</v>
@@ -10521,12 +10606,12 @@
         <v>259</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1.093</v>
       </c>
@@ -10537,12 +10622,12 @@
         <v>276</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>283</v>
       </c>
@@ -10553,7 +10638,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1000000</v>
       </c>
@@ -10561,7 +10646,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <f>A31*A28</f>
         <v>1093000</v>
@@ -10573,7 +10658,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <f>A32*0.5</f>
         <v>546500</v>
@@ -10591,7 +10676,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="57">
         <f>A33/C34</f>
         <v>151.81303791469193</v>
@@ -10606,7 +10691,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="58">
         <f>A34/8760/C35</f>
         <v>2.7078524171427643E-2</v>
@@ -10621,7 +10706,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="58">
         <v>2.5000000000000001E-2</v>
       </c>

</xml_diff>

<commit_message>
updated code and added feedstocks
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://randus-my.sharepoint.com/personal/jrojasa_rand_org/Documents/Documents/GitHub/SJV-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2518" documentId="8_{A1084574-41F8-5F41-86C3-722B91DFE57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80AD4DE8-8B8F-49D4-862E-77DEE11632C9}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="14_{477DE6F6-3490-4777-94BA-8FDDBCE6B90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5458B0B5-1C76-4642-8F7B-F87A74F6743D}"/>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="-16470" windowWidth="29040" windowHeight="15840" tabRatio="622" firstSheet="3" activeTab="10" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="-14490" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="622" firstSheet="2" activeTab="8" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Land" sheetId="14" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1605" uniqueCount="264">
   <si>
     <t>Feedstock</t>
   </si>
@@ -486,33 +486,12 @@
     <t>EJ per MGal</t>
   </si>
   <si>
-    <t>0.17 tonne fuel per 1 tonne feedstoock</t>
-  </si>
-  <si>
-    <t>0.19 tonne fuel per 1 tonne feedstoock</t>
-  </si>
-  <si>
-    <t>Conversion Factor</t>
-  </si>
-  <si>
-    <t>EJ per metric ton</t>
-  </si>
-  <si>
     <t>Biomass</t>
   </si>
   <si>
-    <t>Li_Battery</t>
-  </si>
-  <si>
-    <t>EJ per mcf production</t>
-  </si>
-  <si>
     <t>Wastewater Gas</t>
   </si>
   <si>
-    <t>EJ per Millions of Gallons</t>
-  </si>
-  <si>
     <t>“Primary” Conversion Technology</t>
   </si>
   <si>
@@ -826,21 +805,6 @@
   </si>
   <si>
     <t>Forest Biomass</t>
-  </si>
-  <si>
-    <t>gallon per US ton</t>
-  </si>
-  <si>
-    <t>kilograms of jet fuel is 1 litre</t>
-  </si>
-  <si>
-    <t>liters is 1 tonne (1,000 kilograms) of jet fuel</t>
-  </si>
-  <si>
-    <t>gallon per metric ton (1 metric ton is 1.1 US ton)</t>
-  </si>
-  <si>
-    <t>gallon per 1 tonne feedstock</t>
   </si>
   <si>
     <t>•	Strategic assessment of sustainable aviation fuel production technologies: Yield improvement and cost reduction opportunities - ScienceDirect
@@ -888,64 +852,7 @@
     <t>165 MJ biomethan to 1kg h2 (120 MJ H2)</t>
   </si>
   <si>
-    <t>Biomethane has an LHV of around 36 MJ/m3</t>
-  </si>
-  <si>
-    <t>MJ/ft3</t>
-  </si>
-  <si>
-    <t>EIA calculator</t>
-  </si>
-  <si>
-    <t>cf biomethane</t>
-  </si>
-  <si>
-    <t>MJ biomethane</t>
-  </si>
-  <si>
-    <t>(1.093 MJ per cft)</t>
-  </si>
-  <si>
-    <t>https://www.iea.org/reports/outlook-for-biogas-and-biomethane-prospects-for-organic-growth/an-introduction-to-biogas-and-biomethane</t>
-  </si>
-  <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>unit</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
-    <t>Capacity Factor (CPUC CSP biogas gen average capacity factor 2024-2035)</t>
-  </si>
-  <si>
-    <t>MW Capacity</t>
-  </si>
-  <si>
-    <t>MJ electricity from biomethane</t>
-  </si>
-  <si>
-    <t>MWh electricity from biomethane</t>
-  </si>
-  <si>
-    <t>(biomethane to electricity)</t>
-  </si>
-  <si>
-    <t>MW per MCF of biomethane</t>
-  </si>
-  <si>
-    <t>50% conversion efficiency (A simple cycle natural gas power plant efficiency rate tends to be the lower, ranging from 33% to 43%. On the other hand, a combined cycle power plant’s efficiency can reach upwards of 60% because it captures and uses the plant’s hot exhaust gases to spin a secondary turbine, which generates more electricity.)</t>
-  </si>
-  <si>
-    <t>https://www.pcienergysolutions.com/2023/04/17/power-plant-efficiency-coal-natural-gas-nuclear-and-more/#:~:text=A%20simple%20cycle%20natural%20gas,turbine%2C%20which%20generates%20more%20electricity.</t>
-  </si>
-  <si>
     <t>MW of electric capacity per 1MCF (64% capacity factor and 50% conversion efficiency)</t>
-  </si>
-  <si>
-    <t>`</t>
   </si>
   <si>
     <t>Ammonia Production</t>
@@ -955,13 +862,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000000000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
-    <numFmt numFmtId="168" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -1150,7 +1056,7 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1167,7 +1073,6 @@
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1240,8 +1145,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1817,7 +1721,7 @@
       <c r="F8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="47">
+      <c r="G8" s="46">
         <f>G11/0.8</f>
         <v>3.4999999999999996</v>
       </c>
@@ -1851,7 +1755,7 @@
       <c r="F9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="47">
+      <c r="G9" s="46">
         <f>G12/0.8</f>
         <v>6.83E-2</v>
       </c>
@@ -1888,7 +1792,7 @@
       <c r="F10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="47">
+      <c r="G10" s="46">
         <v>24</v>
       </c>
       <c r="H10" s="10" t="s">
@@ -1917,7 +1821,7 @@
       <c r="F11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="47">
+      <c r="G11" s="46">
         <v>2.8</v>
       </c>
       <c r="H11" s="10" t="s">
@@ -1949,7 +1853,7 @@
       <c r="F12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="48">
+      <c r="G12" s="47">
         <f>G6*G11/G5</f>
         <v>5.4640000000000001E-2</v>
       </c>
@@ -1983,7 +1887,7 @@
       <c r="F13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="47">
+      <c r="G13" s="46">
         <v>0.8</v>
       </c>
       <c r="H13" s="10" t="s">
@@ -2012,7 +1916,7 @@
       <c r="F14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="47">
+      <c r="G14" s="46">
         <f>G17/0.8</f>
         <v>5.25</v>
       </c>
@@ -2046,7 +1950,7 @@
       <c r="F15" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="47">
+      <c r="G15" s="46">
         <f>G18/0.8</f>
         <v>0.10245</v>
       </c>
@@ -2083,7 +1987,7 @@
       <c r="F16" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G16" s="47">
+      <c r="G16" s="46">
         <v>123</v>
       </c>
       <c r="H16" s="10" t="s">
@@ -2113,7 +2017,7 @@
       <c r="F17" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="47">
+      <c r="G17" s="46">
         <v>4.2</v>
       </c>
       <c r="H17" s="10" t="s">
@@ -2145,7 +2049,7 @@
       <c r="F18" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G18" s="48">
+      <c r="G18" s="47">
         <f>G6*G17/G5</f>
         <v>8.1960000000000005E-2</v>
       </c>
@@ -2178,7 +2082,7 @@
       <c r="F19" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="G19" s="47">
+      <c r="G19" s="46">
         <v>4.2</v>
       </c>
       <c r="H19" s="10" t="s">
@@ -2216,7 +2120,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -2296,7 +2200,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -2334,7 +2238,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -2372,7 +2276,7 @@
         <v>34</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -2410,7 +2314,7 @@
         <v>35</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -2448,7 +2352,7 @@
         <v>36</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -2486,7 +2390,7 @@
         <v>37</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -2524,7 +2428,7 @@
         <v>38</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -2562,7 +2466,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -2600,7 +2504,7 @@
         <v>40</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -2638,7 +2542,7 @@
         <v>37</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -2676,7 +2580,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
@@ -2714,7 +2618,7 @@
         <v>38</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C13" t="s">
         <v>19</v>
@@ -2752,7 +2656,7 @@
         <v>45</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
@@ -2790,7 +2694,7 @@
         <v>44</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C15" t="s">
         <v>38</v>
@@ -2825,10 +2729,10 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>48</v>
@@ -2866,7 +2770,7 @@
         <v>50</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>48</v>
@@ -2904,7 +2808,7 @@
         <v>37</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>48</v>
@@ -2942,7 +2846,7 @@
         <v>36</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>48</v>
@@ -2984,8 +2888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3F942D-1725-B745-A61F-46451943A74C}">
   <dimension ref="A1:W8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -2999,7 +2903,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C1">
         <v>2025</v>
@@ -3212,7 +3116,7 @@
         <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>294</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2">
         <v>1</v>
@@ -3586,20 +3490,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="33" t="s">
-        <v>165</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="C1" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="52" t="s">
-        <v>150</v>
-      </c>
-      <c r="E1" s="52" t="s">
-        <v>167</v>
+      <c r="A1" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>160</v>
       </c>
       <c r="F1" t="s">
         <v>104</v>
@@ -3609,17 +3513,17 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="50"/>
+      <c r="C2" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="53" t="s">
-        <v>151</v>
-      </c>
-      <c r="E2" s="53" t="s">
+      <c r="D2" s="52" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" s="52" t="s">
         <v>12</v>
       </c>
       <c r="F2" t="s">
@@ -3630,17 +3534,17 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="51"/>
-      <c r="C3" s="53" t="s">
+      <c r="B3" s="50"/>
+      <c r="C3" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="53" t="s">
-        <v>152</v>
-      </c>
-      <c r="E3" s="53" t="s">
+      <c r="D3" s="52" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="52" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
@@ -3651,17 +3555,17 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="53" t="s">
+      <c r="B4" s="50"/>
+      <c r="C4" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="53" t="s">
-        <v>153</v>
-      </c>
-      <c r="E4" s="53" t="s">
+      <c r="D4" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="E4" s="52" t="s">
         <v>12</v>
       </c>
       <c r="F4" t="s">
@@ -3672,17 +3576,17 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="51"/>
-      <c r="C5" s="53" t="s">
+      <c r="B5" s="50"/>
+      <c r="C5" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="53" t="s">
-        <v>154</v>
-      </c>
-      <c r="E5" s="53" t="s">
+      <c r="D5" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="E5" s="52" t="s">
         <v>12</v>
       </c>
       <c r="F5" t="s">
@@ -3693,17 +3597,17 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="53" t="s">
+      <c r="A6" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="E6" s="53" t="s">
+      <c r="D6" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="52" t="s">
         <v>12</v>
       </c>
       <c r="F6" t="s">
@@ -3714,17 +3618,17 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="53" t="s">
+      <c r="A7" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="E7" s="53" t="s">
+      <c r="D7" s="52" t="s">
+        <v>148</v>
+      </c>
+      <c r="E7" s="52" t="s">
         <v>12</v>
       </c>
       <c r="F7" t="s">
@@ -3735,17 +3639,17 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="53" t="s">
+      <c r="B8" s="16"/>
+      <c r="C8" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="53" t="s">
-        <v>156</v>
-      </c>
-      <c r="E8" s="53" t="s">
+      <c r="D8" s="52" t="s">
+        <v>149</v>
+      </c>
+      <c r="E8" s="52" t="s">
         <v>12</v>
       </c>
       <c r="F8" t="s">
@@ -3756,17 +3660,17 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="53" t="s">
+      <c r="B9" s="14"/>
+      <c r="C9" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="53" t="s">
-        <v>157</v>
-      </c>
-      <c r="E9" s="53" t="s">
+      <c r="D9" s="52" t="s">
+        <v>150</v>
+      </c>
+      <c r="E9" s="52" t="s">
         <v>19</v>
       </c>
       <c r="F9" t="s">
@@ -3777,17 +3681,17 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="53" t="s">
+      <c r="B10" s="14"/>
+      <c r="C10" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="53" t="s">
-        <v>158</v>
-      </c>
-      <c r="E10" s="53" t="s">
+      <c r="D10" s="52" t="s">
+        <v>151</v>
+      </c>
+      <c r="E10" s="52" t="s">
         <v>19</v>
       </c>
       <c r="F10" t="s">
@@ -3798,17 +3702,17 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="53" t="s">
+      <c r="A11" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="53" t="s">
-        <v>159</v>
-      </c>
-      <c r="E11" s="53" t="s">
+      <c r="D11" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="E11" s="52" t="s">
         <v>19</v>
       </c>
       <c r="F11" t="s">
@@ -3819,17 +3723,17 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="53" t="s">
+      <c r="A12" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="53" t="s">
-        <v>159</v>
-      </c>
-      <c r="E12" s="53" t="s">
+      <c r="D12" s="52" t="s">
+        <v>152</v>
+      </c>
+      <c r="E12" s="52" t="s">
         <v>19</v>
       </c>
       <c r="F12" t="s">
@@ -3840,17 +3744,17 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="53" t="s">
+      <c r="B13" s="14"/>
+      <c r="C13" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="53" t="s">
-        <v>160</v>
-      </c>
-      <c r="E13" s="53" t="s">
+      <c r="D13" s="52" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="52" t="s">
         <v>19</v>
       </c>
       <c r="F13" t="s">
@@ -3861,17 +3765,17 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="53" t="s">
+      <c r="A14" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="53" t="s">
-        <v>161</v>
-      </c>
-      <c r="E14" s="53" t="s">
+      <c r="D14" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="52" t="s">
         <v>38</v>
       </c>
       <c r="F14" t="s">
@@ -3882,17 +3786,17 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="53" t="s">
+      <c r="A15" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="D15" s="53" t="s">
-        <v>161</v>
-      </c>
-      <c r="E15" s="53" t="s">
+      <c r="D15" s="52" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="52" t="s">
         <v>38</v>
       </c>
       <c r="F15" t="s">
@@ -3903,17 +3807,17 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="53" t="s">
-        <v>162</v>
-      </c>
-      <c r="D16" s="53" t="s">
-        <v>163</v>
-      </c>
-      <c r="E16" s="54" t="s">
+      <c r="A16" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="52" t="s">
+        <v>155</v>
+      </c>
+      <c r="D16" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="E16" s="53" t="s">
         <v>48</v>
       </c>
       <c r="F16" t="s">
@@ -3924,17 +3828,17 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="B17" s="15"/>
-      <c r="C17" s="53" t="s">
+      <c r="A17" s="14" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="53" t="s">
-        <v>163</v>
-      </c>
-      <c r="E17" s="54" t="s">
+      <c r="D17" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" s="53" t="s">
         <v>48</v>
       </c>
       <c r="F17" t="s">
@@ -3945,17 +3849,17 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B18" s="15"/>
-      <c r="C18" s="53" t="s">
+      <c r="A18" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="52" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="53" t="s">
-        <v>164</v>
-      </c>
-      <c r="E18" s="54" t="s">
+      <c r="D18" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="E18" s="53" t="s">
         <v>48</v>
       </c>
       <c r="F18" t="s">
@@ -3966,17 +3870,17 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="B19" s="15"/>
-      <c r="C19" s="53" t="s">
+      <c r="A19" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="D19" s="53" t="s">
-        <v>164</v>
-      </c>
-      <c r="E19" s="54" t="s">
+      <c r="D19" s="52" t="s">
+        <v>157</v>
+      </c>
+      <c r="E19" s="53" t="s">
         <v>48</v>
       </c>
       <c r="F19" t="s">
@@ -3987,66 +3891,66 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" s="52" t="s">
-        <v>167</v>
-      </c>
-      <c r="B23" s="33" t="s">
+      <c r="A23" s="51" t="s">
+        <v>160</v>
+      </c>
+      <c r="B23" s="32" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" s="53" t="s">
+      <c r="A24" s="52" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" s="53" t="s">
+      <c r="A25" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A26" s="53" t="s">
+      <c r="A26" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="53" t="s">
+      <c r="A27" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" s="53" t="s">
+      <c r="A28" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" s="53" t="s">
+      <c r="A29" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>70</v>
       </c>
     </row>
@@ -4079,25 +3983,25 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D1" t="s">
         <v>68</v>
       </c>
       <c r="E1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="F1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="G1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="H1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="I1" t="s">
         <v>74</v>
@@ -4152,7 +4056,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -4182,131 +4086,131 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>169</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="15" t="s">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
       </c>
       <c r="J1" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="K1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>178</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="F2" s="15" t="s">
-        <v>179</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>180</v>
+      <c r="C2" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="F2" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>173</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>58</v>
       </c>
       <c r="J2" s="7" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>183</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="F3" s="15" t="s">
-        <v>184</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>180</v>
+      <c r="C3" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="F3" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>173</v>
       </c>
       <c r="I3" s="7" t="s">
         <v>58</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>186</v>
-      </c>
-      <c r="D4" s="16"/>
-      <c r="F4" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="G4" s="15" t="s">
+      <c r="C4" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="F4" s="14" t="s">
         <v>180</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>173</v>
       </c>
       <c r="I4" t="s">
         <v>58</v>
       </c>
       <c r="J4" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="K4" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="D5" s="16"/>
-      <c r="F5" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>180</v>
+      <c r="C5" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="F5" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>173</v>
       </c>
       <c r="I5" s="7" t="s">
         <v>58</v>
@@ -4315,47 +4219,47 @@
         <v>74</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="F6" s="16" t="s">
+        <v>185</v>
+      </c>
+      <c r="G6" s="16" t="s">
         <v>186</v>
-      </c>
-      <c r="D6" s="16"/>
-      <c r="F6" s="17" t="s">
-        <v>192</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>193</v>
       </c>
       <c r="I6" s="7" t="s">
         <v>58</v>
       </c>
       <c r="J6" s="7" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K6" s="7" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16"/>
-      <c r="F7" s="15" t="s">
-        <v>192</v>
-      </c>
-      <c r="G7" s="15" t="s">
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="F7" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>19</v>
       </c>
       <c r="I7" t="s">
@@ -4365,195 +4269,195 @@
         <v>35</v>
       </c>
       <c r="K7" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="16"/>
-      <c r="F8" s="17" t="s">
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="F8" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="17" t="s">
-        <v>193</v>
+      <c r="G8" s="16" t="s">
+        <v>186</v>
       </c>
       <c r="I8" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="J8" t="s">
+        <v>174</v>
+      </c>
+      <c r="K8" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="F9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>186</v>
+      </c>
+      <c r="J9" t="s">
+        <v>178</v>
+      </c>
+      <c r="K9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="F10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>186</v>
+      </c>
+      <c r="I10" t="s">
+        <v>186</v>
+      </c>
+      <c r="J10" t="s">
         <v>181</v>
       </c>
-      <c r="K8" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="16"/>
-      <c r="F9" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="15" t="s">
+      <c r="K10" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="F11" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I9" t="s">
-        <v>193</v>
-      </c>
-      <c r="J9" t="s">
-        <v>185</v>
-      </c>
-      <c r="K9" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="16"/>
-      <c r="F10" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="I10" t="s">
-        <v>193</v>
-      </c>
-      <c r="J10" t="s">
-        <v>188</v>
-      </c>
-      <c r="K10" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="B11" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="F11" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="I11" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="J11" t="s">
         <v>74</v>
       </c>
       <c r="K11" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>195</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
+      <c r="A12" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
       <c r="I12" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="J12" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K12" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
       <c r="I13" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="J13" t="s">
         <v>35</v>
       </c>
       <c r="K13" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
       <c r="I14" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="7" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
+      <c r="A15" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
       <c r="I15" t="s">
         <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="K15" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>200</v>
-      </c>
-      <c r="C16" s="21" t="s">
+      <c r="A16" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D16" s="22" t="s">
-        <v>201</v>
+      <c r="D16" s="21" t="s">
+        <v>194</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>19</v>
@@ -4562,44 +4466,44 @@
         <v>74</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="62" x14ac:dyDescent="0.35">
-      <c r="A17" s="21" t="s">
-        <v>184</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="D17" s="22" t="s">
-        <v>205</v>
+      <c r="A17" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>198</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>19</v>
       </c>
       <c r="J17" s="7" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="62" x14ac:dyDescent="0.35">
-      <c r="A18" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="D18" s="22" t="s">
-        <v>205</v>
+      <c r="A18" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>198</v>
       </c>
       <c r="I18" t="s">
         <v>19</v>
@@ -4608,160 +4512,160 @@
         <v>35</v>
       </c>
       <c r="K18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+      <c r="A19" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="23" t="s">
+        <v>185</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>201</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="26" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>205</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>206</v>
+      </c>
+      <c r="D31" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="62" x14ac:dyDescent="0.35">
-      <c r="A19" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="B19" s="23" t="s">
-        <v>203</v>
-      </c>
-      <c r="C19" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="B20" s="25" t="s">
+      <c r="E31" t="s">
         <v>208</v>
       </c>
-      <c r="C20" s="25" t="s">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" s="14"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="14" t="s">
         <v>209</v>
       </c>
-      <c r="D20" s="26" t="s">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="14" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="24" t="s">
+      <c r="B37" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="C37" s="14"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="C21" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="25" t="s">
-        <v>208</v>
-      </c>
-      <c r="C22" s="25" t="s">
-        <v>209</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="27" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="33" t="s">
-        <v>212</v>
-      </c>
-      <c r="C31" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="D31" t="s">
-        <v>214</v>
-      </c>
-      <c r="E31" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="15"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="15" t="s">
-        <v>162</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C33" s="15"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B34" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C34" s="15"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" s="15" t="s">
+      <c r="B39" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="15" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="15"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="C37" s="15"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>218</v>
-      </c>
-      <c r="C38" s="15"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="27" t="s">
         <v>19</v>
       </c>
       <c r="D39" t="s">
@@ -4769,13 +4673,13 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="28" t="s">
+      <c r="A40" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="27" t="s">
         <v>19</v>
       </c>
       <c r="D40" t="s">
@@ -4783,261 +4687,261 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="15" t="s">
-        <v>187</v>
-      </c>
-      <c r="B41" s="15" t="s">
+      <c r="A41" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="B41" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="D41" t="s">
+        <v>213</v>
+      </c>
+      <c r="E41" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="D42" t="s">
+        <v>213</v>
+      </c>
+      <c r="E42" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="26" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="33" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="31" t="s">
+        <v>218</v>
+      </c>
+      <c r="C48" s="28" t="s">
         <v>219</v>
-      </c>
-      <c r="D41" t="s">
-        <v>220</v>
-      </c>
-      <c r="E41" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="15" t="s">
-        <v>191</v>
-      </c>
-      <c r="B42" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="D42" t="s">
-        <v>220</v>
-      </c>
-      <c r="E42" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="27" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="33" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="C46" s="33" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="C47" s="35" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="32" t="s">
-        <v>225</v>
-      </c>
-      <c r="C48" s="29" t="s">
-        <v>226</v>
       </c>
       <c r="D48" t="s">
         <v>24</v>
       </c>
       <c r="E48" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>166</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="D49" t="s">
+        <v>221</v>
+      </c>
+      <c r="E49" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="D50" t="s">
+        <v>224</v>
+      </c>
+      <c r="E50" t="s">
+        <v>225</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="C51" s="27" t="s">
         <v>227</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="C49" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="D49" t="s">
-        <v>228</v>
-      </c>
-      <c r="E49" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" s="29" t="s">
-        <v>230</v>
-      </c>
-      <c r="D50" t="s">
-        <v>231</v>
-      </c>
-      <c r="E50" t="s">
-        <v>232</v>
-      </c>
-      <c r="F50" s="36" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="C51" s="28" t="s">
-        <v>234</v>
       </c>
       <c r="D51" t="s">
         <v>24</v>
       </c>
       <c r="E51" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="28" t="s">
+      <c r="A52" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B52" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="C52" s="28" t="s">
-        <v>224</v>
+      <c r="B52" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>217</v>
       </c>
       <c r="D52" t="s">
         <v>26</v>
       </c>
       <c r="E52" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="16" t="s">
+      <c r="B53" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="C53" s="35" t="s">
+      <c r="C53" s="34" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="28" t="s">
+      <c r="A54" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="B54" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="C54" s="28" t="s">
+      <c r="B54" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="C54" s="27" t="s">
         <v>58</v>
       </c>
       <c r="D54" t="s">
         <v>26</v>
       </c>
       <c r="E54" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="28" t="s">
+      <c r="A55" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B55" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="C55" s="28" t="s">
-        <v>224</v>
+      <c r="B55" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>217</v>
       </c>
       <c r="D55" t="s">
         <v>24</v>
       </c>
       <c r="E55" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B56" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="C56" s="35" t="s">
+      <c r="B56" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="C56" s="34" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="26" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="27" t="s">
         <v>234</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" s="27" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="28" t="s">
-        <v>241</v>
       </c>
       <c r="D61" t="s">
         <v>24</v>
       </c>
       <c r="E61" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="30" t="s">
-        <v>243</v>
+      <c r="A62" s="29" t="s">
+        <v>236</v>
       </c>
       <c r="D62" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="28" t="s">
-        <v>244</v>
+      <c r="A63" s="27" t="s">
+        <v>237</v>
       </c>
       <c r="D63" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="27" t="s">
-        <v>245</v>
+      <c r="A66" s="26" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="28" t="s">
-        <v>246</v>
+      <c r="A67" s="27" t="s">
+        <v>239</v>
       </c>
       <c r="D67" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="28" t="s">
-        <v>247</v>
+      <c r="A68" s="27" t="s">
+        <v>240</v>
       </c>
       <c r="D68" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -5061,7 +4965,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B1" t="s">
         <v>58</v>
@@ -5076,12 +4980,12 @@
         <v>71</v>
       </c>
       <c r="F1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -5122,7 +5026,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B6" s="2">
         <v>1</v>
@@ -5136,7 +5040,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="B7" s="2">
         <v>1</v>
@@ -5150,7 +5054,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -5161,7 +5065,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -5172,7 +5076,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -5207,7 +5111,7 @@
   <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5292,7 +5196,7 @@
       <c r="F3" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="40">
+      <c r="G3" s="39">
         <v>10.51</v>
       </c>
       <c r="H3" t="s">
@@ -5356,7 +5260,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>293</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
         <v>31</v>
@@ -5372,7 +5276,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="36" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -5395,7 +5299,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -5418,7 +5322,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -5427,7 +5331,7 @@
       <c r="C9" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="50" t="s">
+      <c r="D9" s="49" t="s">
         <v>39</v>
       </c>
       <c r="E9" t="s">
@@ -5436,7 +5340,7 @@
       <c r="F9" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="50">
+      <c r="G9" s="49">
         <v>0</v>
       </c>
     </row>
@@ -5534,7 +5438,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B13" t="s">
@@ -5543,7 +5447,7 @@
       <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="49" t="s">
         <v>39</v>
       </c>
       <c r="E13" t="s">
@@ -5558,7 +5462,7 @@
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="36" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -5839,7 +5743,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="36" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -5862,7 +5766,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A26" s="37" t="s">
+      <c r="A26" s="36" t="s">
         <v>37</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -5882,7 +5786,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -5891,7 +5795,7 @@
       <c r="C27" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="50" t="s">
+      <c r="D27" s="49" t="s">
         <v>39</v>
       </c>
       <c r="E27" t="s">
@@ -5952,7 +5856,7 @@
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B30" t="s">
@@ -5961,7 +5865,7 @@
       <c r="C30" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="50" t="s">
+      <c r="D30" s="49" t="s">
         <v>39</v>
       </c>
       <c r="E30" t="s">
@@ -5994,7 +5898,7 @@
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="36" t="s">
         <v>44</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -6260,7 +6164,7 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A43" s="37" t="s">
+      <c r="A43" s="36" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="1" t="s">
@@ -6283,7 +6187,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="36" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="1" t="s">
@@ -6303,7 +6207,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A45" s="37" t="s">
+      <c r="A45" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -6312,7 +6216,7 @@
       <c r="C45" t="s">
         <v>30</v>
       </c>
-      <c r="D45" s="50" t="s">
+      <c r="D45" s="49" t="s">
         <v>39</v>
       </c>
       <c r="E45" t="s">
@@ -6373,7 +6277,7 @@
       <c r="I47" s="3"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A48" s="37" t="s">
+      <c r="A48" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B48" t="s">
@@ -6382,7 +6286,7 @@
       <c r="C48" t="s">
         <v>30</v>
       </c>
-      <c r="D48" s="50" t="s">
+      <c r="D48" s="49" t="s">
         <v>39</v>
       </c>
       <c r="E48" t="s">
@@ -6415,7 +6319,7 @@
       <c r="I49" s="3"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A50" s="37" t="s">
+      <c r="A50" s="36" t="s">
         <v>44</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -6571,7 +6475,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -6629,7 +6533,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D3" t="s">
         <v>61</v>
@@ -6637,8 +6541,8 @@
       <c r="E3" s="2">
         <v>0.35</v>
       </c>
-      <c r="F3" s="38" t="s">
-        <v>271</v>
+      <c r="F3" s="37" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -6649,7 +6553,7 @@
         <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
       <c r="D4" t="s">
         <v>62</v>
@@ -6657,8 +6561,8 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="F4" s="56" t="s">
-        <v>273</v>
+      <c r="F4" s="55" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -6683,7 +6587,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C6" t="s">
         <v>65</v>
@@ -6694,7 +6598,7 @@
       <c r="E6">
         <v>2.5</v>
       </c>
-      <c r="F6" s="46" t="s">
+      <c r="F6" s="45" t="s">
         <v>67</v>
       </c>
     </row>
@@ -6703,7 +6607,7 @@
         <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
       <c r="C7" t="s">
         <v>68</v>
@@ -6745,7 +6649,7 @@
   <dimension ref="A1:AA8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -7178,7 +7082,7 @@
         <v>19</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C6" t="s">
         <v>77</v>
@@ -7261,7 +7165,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
       <c r="C7" t="s">
         <v>78</v>
@@ -8385,10 +8289,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="49" t="s">
+      <c r="A3" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>19</v>
       </c>
       <c r="C3" t="s">
@@ -8657,7 +8561,7 @@
       <c r="C2" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="37" t="s">
         <v>102</v>
       </c>
       <c r="E2" s="13" t="s">
@@ -8679,11 +8583,12 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA5616B-DF07-465E-AEEB-CCA6D05FE697}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AK23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B26" sqref="B26"/>
+      <pane xSplit="1" topLeftCell="P1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P1" activeCellId="1" sqref="A1:C9 P1:AK9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -8743,10 +8648,10 @@
         <v>112</v>
       </c>
       <c r="M1" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="N1" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="O1" t="s">
         <v>112</v>
@@ -8838,13 +8743,13 @@
       <c r="F2" t="s">
         <v>116</v>
       </c>
-      <c r="G2" s="39">
+      <c r="G2" s="38">
         <v>3.5998225679871703E-9</v>
       </c>
       <c r="H2" t="s">
         <v>117</v>
       </c>
-      <c r="P2" s="41" t="s">
+      <c r="P2" s="40" t="s">
         <v>118</v>
       </c>
       <c r="Q2" s="5">
@@ -8911,7 +8816,7 @@
         <v>1216.528453322951</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -8937,16 +8842,16 @@
       <c r="H3" t="s">
         <v>122</v>
       </c>
-      <c r="I3" s="43">
+      <c r="I3" s="42">
         <v>0.64900000000000002</v>
       </c>
       <c r="J3">
         <v>51.3</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="42" t="s">
         <v>123</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="43" t="s">
         <v>124</v>
       </c>
       <c r="O3" t="s">
@@ -8973,13 +8878,13 @@
       <c r="F4" t="s">
         <v>116</v>
       </c>
-      <c r="G4" s="39">
+      <c r="G4" s="38">
         <v>3.5998225679871703E-9</v>
       </c>
       <c r="H4" t="s">
         <v>117</v>
       </c>
-      <c r="P4" s="41" t="s">
+      <c r="P4" s="40" t="s">
         <v>118</v>
       </c>
       <c r="Q4" s="5">
@@ -9066,13 +8971,13 @@
       <c r="F5" t="s">
         <v>116</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="38">
         <v>3.5998225679871703E-9</v>
       </c>
       <c r="H5" t="s">
         <v>117</v>
       </c>
-      <c r="P5" s="41" t="s">
+      <c r="P5" s="40" t="s">
         <v>118</v>
       </c>
       <c r="Q5" s="5">
@@ -9159,13 +9064,13 @@
       <c r="F6" t="s">
         <v>116</v>
       </c>
-      <c r="G6" s="39">
+      <c r="G6" s="38">
         <v>3.5998225679871703E-9</v>
       </c>
       <c r="H6" t="s">
         <v>117</v>
       </c>
-      <c r="P6" s="41" t="s">
+      <c r="P6" s="40" t="s">
         <v>118</v>
       </c>
       <c r="Q6" s="5">
@@ -9252,18 +9157,18 @@
       <c r="F7" t="s">
         <v>116</v>
       </c>
-      <c r="G7" s="39">
+      <c r="G7" s="38">
         <v>3.5998225679871703E-9</v>
       </c>
       <c r="H7" t="s">
         <v>117</v>
       </c>
-      <c r="I7" s="42">
+      <c r="I7" s="41">
         <v>0.25</v>
       </c>
       <c r="J7" s="12"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="42"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
       <c r="M7">
         <v>19800</v>
       </c>
@@ -9273,7 +9178,7 @@
       <c r="O7" t="s">
         <v>127</v>
       </c>
-      <c r="P7" s="41" t="s">
+      <c r="P7" s="40" t="s">
         <v>118</v>
       </c>
       <c r="Q7" s="5">
@@ -9360,38 +9265,82 @@
       <c r="F8" t="s">
         <v>116</v>
       </c>
-      <c r="G8" s="39">
+      <c r="G8" s="38">
         <v>3.5998225679871703E-9</v>
       </c>
       <c r="H8" t="s">
         <v>117</v>
       </c>
-      <c r="I8" s="42"/>
+      <c r="I8" s="41"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="42"/>
-      <c r="P8" s="41"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
-      <c r="AE8" s="5"/>
-      <c r="AF8" s="5"/>
-      <c r="AG8" s="5"/>
-      <c r="AH8" s="5"/>
-      <c r="AI8" s="5"/>
-      <c r="AJ8" s="5"/>
-      <c r="AK8" s="5"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="P8" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>6035.0858307307299</v>
+      </c>
+      <c r="R8" s="5">
+        <v>5991.4369513857655</v>
+      </c>
+      <c r="S8" s="5">
+        <v>5947.7880720408011</v>
+      </c>
+      <c r="T8" s="5">
+        <v>5904.1391926958368</v>
+      </c>
+      <c r="U8" s="5">
+        <v>5860.4903133508724</v>
+      </c>
+      <c r="V8" s="5">
+        <v>5816.841434005908</v>
+      </c>
+      <c r="W8" s="5">
+        <v>5773.1925546609436</v>
+      </c>
+      <c r="X8" s="5">
+        <v>5729.5436753159793</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>5685.8947959710149</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>5642.2459166260505</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>5598.5970372810862</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>5554.9481579361218</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>5511.2992785911574</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>5467.650399246193</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>5424.0015199012287</v>
+      </c>
+      <c r="AF8" s="5">
+        <v>5380.3526405562643</v>
+      </c>
+      <c r="AG8" s="5">
+        <v>5336.7037612112999</v>
+      </c>
+      <c r="AH8" s="5">
+        <v>5293.0548818663356</v>
+      </c>
+      <c r="AI8" s="5">
+        <v>5249.4060025213712</v>
+      </c>
+      <c r="AJ8" s="5">
+        <v>5205.7571231764068</v>
+      </c>
+      <c r="AK8" s="5">
+        <v>5162.1082438314425</v>
+      </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -9413,44 +9362,88 @@
       <c r="F9" t="s">
         <v>116</v>
       </c>
-      <c r="G9" s="39">
+      <c r="G9" s="38">
         <v>3.5998225679871703E-9</v>
       </c>
       <c r="H9" t="s">
         <v>117</v>
       </c>
-      <c r="I9" s="42"/>
+      <c r="I9" s="41"/>
       <c r="J9" s="12">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="K9" s="42" t="s">
-        <v>292</v>
-      </c>
-      <c r="L9" s="42"/>
-      <c r="P9" s="41"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-      <c r="W9" s="5"/>
-      <c r="X9" s="5"/>
-      <c r="Y9" s="5"/>
-      <c r="Z9" s="5"/>
-      <c r="AA9" s="5"/>
-      <c r="AB9" s="5"/>
-      <c r="AC9" s="5"/>
-      <c r="AD9" s="5"/>
-      <c r="AE9" s="5"/>
-      <c r="AF9" s="5"/>
-      <c r="AG9" s="5"/>
-      <c r="AH9" s="5"/>
-      <c r="AI9" s="5"/>
-      <c r="AJ9" s="5"/>
-      <c r="AK9" s="5"/>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="K9" s="41" t="s">
+        <v>262</v>
+      </c>
+      <c r="L9" s="41"/>
+      <c r="P9" s="40" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>6035.0858307307299</v>
+      </c>
+      <c r="R9" s="5">
+        <v>5991.4369513857655</v>
+      </c>
+      <c r="S9" s="5">
+        <v>5947.7880720408011</v>
+      </c>
+      <c r="T9" s="5">
+        <v>5904.1391926958368</v>
+      </c>
+      <c r="U9" s="5">
+        <v>5860.4903133508724</v>
+      </c>
+      <c r="V9" s="5">
+        <v>5816.841434005908</v>
+      </c>
+      <c r="W9" s="5">
+        <v>5773.1925546609436</v>
+      </c>
+      <c r="X9" s="5">
+        <v>5729.5436753159793</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>5685.8947959710149</v>
+      </c>
+      <c r="Z9" s="5">
+        <v>5642.2459166260505</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>5598.5970372810862</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>5554.9481579361218</v>
+      </c>
+      <c r="AC9" s="5">
+        <v>5511.2992785911574</v>
+      </c>
+      <c r="AD9" s="5">
+        <v>5467.650399246193</v>
+      </c>
+      <c r="AE9" s="5">
+        <v>5424.0015199012287</v>
+      </c>
+      <c r="AF9" s="5">
+        <v>5380.3526405562643</v>
+      </c>
+      <c r="AG9" s="5">
+        <v>5336.7037612112999</v>
+      </c>
+      <c r="AH9" s="5">
+        <v>5293.0548818663356</v>
+      </c>
+      <c r="AI9" s="5">
+        <v>5249.4060025213712</v>
+      </c>
+      <c r="AJ9" s="5">
+        <v>5205.7571231764068</v>
+      </c>
+      <c r="AK9" s="5">
+        <v>5162.1082438314425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -9476,23 +9469,23 @@
       <c r="H10" t="s">
         <v>122</v>
       </c>
-      <c r="I10" s="42">
+      <c r="I10" s="41">
         <v>0.72</v>
       </c>
       <c r="J10">
         <v>0.16700000000000001</v>
       </c>
-      <c r="K10" s="42" t="s">
+      <c r="K10" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="L10" s="45" t="s">
-        <v>267</v>
-      </c>
-      <c r="O10" s="38" t="s">
+      <c r="L10" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="O10" s="37" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -9518,17 +9511,17 @@
       <c r="H11" t="s">
         <v>122</v>
       </c>
-      <c r="I11" s="42"/>
+      <c r="I11" s="41"/>
       <c r="J11" s="12">
         <v>0.16700000000000001</v>
       </c>
-      <c r="K11" s="42" t="s">
+      <c r="K11" s="41" t="s">
         <v>128</v>
       </c>
-      <c r="L11" s="45"/>
-      <c r="O11" s="38"/>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="L11" s="44"/>
+      <c r="O11" s="37"/>
+    </row>
+    <row r="12" spans="1:37" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -9554,16 +9547,16 @@
       <c r="H12" t="s">
         <v>122</v>
       </c>
-      <c r="I12" s="42">
+      <c r="I12" s="41">
         <v>0.44</v>
       </c>
       <c r="J12">
         <v>13</v>
       </c>
-      <c r="K12" s="42" t="s">
+      <c r="K12" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="L12" s="45" t="s">
+      <c r="L12" s="44" t="s">
         <v>129</v>
       </c>
       <c r="M12">
@@ -9576,7 +9569,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -9602,16 +9595,16 @@
       <c r="H13" t="s">
         <v>122</v>
       </c>
-      <c r="I13" s="42">
+      <c r="I13" s="41">
         <v>0.44</v>
       </c>
       <c r="J13">
         <v>13</v>
       </c>
-      <c r="K13" s="42" t="s">
+      <c r="K13" s="41" t="s">
         <v>131</v>
       </c>
-      <c r="L13" s="45" t="s">
+      <c r="L13" s="44" t="s">
         <v>129</v>
       </c>
       <c r="M13">
@@ -9624,7 +9617,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -9653,8 +9646,8 @@
       <c r="J14" s="12">
         <v>50</v>
       </c>
-      <c r="K14" s="42" t="s">
-        <v>270</v>
+      <c r="K14" s="41" t="s">
+        <v>258</v>
       </c>
       <c r="M14">
         <v>19800</v>
@@ -9663,7 +9656,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -9692,7 +9685,7 @@
       <c r="J15" s="12">
         <v>20000</v>
       </c>
-      <c r="K15" s="42" t="s">
+      <c r="K15" s="41" t="s">
         <v>136</v>
       </c>
       <c r="M15">
@@ -9702,7 +9695,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -9731,14 +9724,14 @@
       <c r="J16" s="12">
         <v>1</v>
       </c>
-      <c r="K16" s="42" t="s">
-        <v>262</v>
+      <c r="K16" s="41" t="s">
+        <v>250</v>
       </c>
       <c r="L16" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -9767,14 +9760,14 @@
       <c r="J17" s="12">
         <v>1</v>
       </c>
-      <c r="K17" s="42" t="s">
-        <v>262</v>
+      <c r="K17" s="41" t="s">
+        <v>250</v>
       </c>
       <c r="L17" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -9803,15 +9796,15 @@
       <c r="J18" s="5">
         <v>16181.229773462785</v>
       </c>
-      <c r="K18" s="42" t="s">
-        <v>261</v>
+      <c r="K18" s="41" t="s">
+        <v>249</v>
       </c>
       <c r="L18" t="s">
-        <v>265</v>
-      </c>
-      <c r="O18" s="55"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+        <v>253</v>
+      </c>
+      <c r="O18" s="54"/>
+    </row>
+    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -9840,27 +9833,33 @@
       <c r="J19" s="5">
         <v>14492.753623188406</v>
       </c>
-      <c r="K19" s="42" t="s">
-        <v>261</v>
+      <c r="K19" s="41" t="s">
+        <v>249</v>
       </c>
       <c r="L19" t="s">
-        <v>266</v>
-      </c>
-      <c r="O19" s="55"/>
+        <v>254</v>
+      </c>
+      <c r="O19" s="54"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="L23">
         <v>1000</v>
       </c>
       <c r="M23" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="N23" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK19" xr:uid="{5FA5616B-DF07-465E-AEEB-CCA6D05FE697}"/>
+  <autoFilter ref="A1:AK19" xr:uid="{5FA5616B-DF07-465E-AEEB-CCA6D05FE697}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Electricity"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="O10" r:id="rId1" display="https://netl.doe.gov/projects/files/ComparisonofCommercialStateofArtFossilBasedHydrogenProductionTechnologies_041222.pdf" xr:uid="{E7CB3D97-93CD-4126-9FFC-6A55103A1392}"/>
@@ -9876,10 +9875,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87BF8B-8E54-426F-864A-9E457E959B26}">
-  <dimension ref="A1:Z37"/>
+  <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -9888,10 +9887,10 @@
     <col min="2" max="2" width="30.33203125" customWidth="1"/>
     <col min="3" max="3" width="8.33203125" customWidth="1"/>
     <col min="4" max="4" width="23.83203125" customWidth="1"/>
-    <col min="5" max="5" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="25" width="8.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -9899,741 +9898,621 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" t="s">
         <v>113</v>
       </c>
+      <c r="E1">
+        <v>2025</v>
+      </c>
       <c r="F1">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G1">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="H1">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="I1">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="J1">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="K1">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="L1">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="M1">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="N1">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="O1">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="P1">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="Q1">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="R1">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="S1">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="T1">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="U1">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="V1">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="W1">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="X1">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="Y1">
-        <v>2044</v>
-      </c>
-      <c r="Z1">
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2">
-        <v>1.1999999999999999E-7</v>
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>114</v>
       </c>
       <c r="D2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+      <c r="E2" s="3">
+        <v>2294.03577178978</v>
+      </c>
+      <c r="F2" s="3">
+        <v>2240.1604058664384</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2186.2850399430968</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2132.4096740197551</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2078.5343080964135</v>
+      </c>
+      <c r="J2" s="3">
+        <v>2024.6589421730721</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1970.7835762497307</v>
+      </c>
+      <c r="L2" s="3">
+        <v>1916.9082103263893</v>
+      </c>
+      <c r="M2" s="3">
+        <v>1863.0328444030479</v>
+      </c>
+      <c r="N2" s="3">
+        <v>1809.1574784797065</v>
+      </c>
+      <c r="O2" s="3">
+        <v>1755.2821125563651</v>
+      </c>
+      <c r="P2" s="3">
+        <v>1701.4067466330237</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>1647.5313807096823</v>
+      </c>
+      <c r="R2" s="3">
+        <v>1593.6560147863408</v>
+      </c>
+      <c r="S2" s="3">
+        <v>1539.7806488629994</v>
+      </c>
+      <c r="T2" s="3">
+        <v>1485.905282939658</v>
+      </c>
+      <c r="U2" s="3">
+        <v>1432.0299170163166</v>
+      </c>
+      <c r="V2" s="3">
+        <v>1378.1545510929752</v>
+      </c>
+      <c r="W2" s="3">
+        <v>1324.2791851696338</v>
+      </c>
+      <c r="X2" s="3">
+        <v>1270.4038192462924</v>
+      </c>
+      <c r="Y2" s="3">
+        <v>1216.528453322951</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3">
-        <v>1.1999999999999999E-7</v>
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
       </c>
       <c r="D3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+      <c r="E3" s="3">
+        <v>2502.8086901013899</v>
+      </c>
+      <c r="F3" s="3">
+        <v>2482.7671254296229</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2462.7255607578559</v>
+      </c>
+      <c r="H3" s="3">
+        <v>2442.6839960860889</v>
+      </c>
+      <c r="I3" s="3">
+        <v>2422.6424314143219</v>
+      </c>
+      <c r="J3" s="3">
+        <v>2402.6008667425549</v>
+      </c>
+      <c r="K3" s="3">
+        <v>2382.5593020707879</v>
+      </c>
+      <c r="L3" s="3">
+        <v>2362.5177373990209</v>
+      </c>
+      <c r="M3" s="3">
+        <v>2342.4761727272539</v>
+      </c>
+      <c r="N3" s="3">
+        <v>2322.4346080554869</v>
+      </c>
+      <c r="O3" s="3">
+        <v>2302.3930433837199</v>
+      </c>
+      <c r="P3" s="3">
+        <v>2282.351478711953</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>2262.309914040186</v>
+      </c>
+      <c r="R3" s="3">
+        <v>2242.268349368419</v>
+      </c>
+      <c r="S3" s="3">
+        <v>2222.226784696652</v>
+      </c>
+      <c r="T3" s="3">
+        <v>2202.185220024885</v>
+      </c>
+      <c r="U3" s="3">
+        <v>2182.143655353118</v>
+      </c>
+      <c r="V3" s="3">
+        <v>2162.102090681351</v>
+      </c>
+      <c r="W3" s="3">
+        <v>2142.060526009584</v>
+      </c>
+      <c r="X3" s="3">
+        <v>2122.018961337817</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>2101.97739666605</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="12">
-        <v>3.5998225679871703E-9</v>
+      <c r="C4" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" t="s">
         <v>118</v>
       </c>
-      <c r="F4" s="5">
-        <v>2294.03577178978</v>
-      </c>
-      <c r="G4" s="5">
-        <v>2240.1604058664384</v>
-      </c>
-      <c r="H4" s="5">
-        <v>2186.2850399430968</v>
-      </c>
-      <c r="I4" s="5">
-        <v>2132.4096740197551</v>
-      </c>
-      <c r="J4" s="5">
-        <v>2078.5343080964135</v>
-      </c>
-      <c r="K4" s="5">
-        <v>2024.6589421730721</v>
-      </c>
-      <c r="L4" s="5">
-        <v>1970.7835762497307</v>
-      </c>
-      <c r="M4" s="5">
-        <v>1916.9082103263893</v>
-      </c>
-      <c r="N4" s="5">
-        <v>1863.0328444030479</v>
-      </c>
-      <c r="O4" s="5">
-        <v>1809.1574784797065</v>
-      </c>
-      <c r="P4" s="5">
-        <v>1755.2821125563651</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>1701.4067466330237</v>
-      </c>
-      <c r="R4" s="5">
-        <v>1647.5313807096823</v>
-      </c>
-      <c r="S4" s="5">
-        <v>1593.6560147863408</v>
-      </c>
-      <c r="T4" s="5">
-        <v>1539.7806488629994</v>
-      </c>
-      <c r="U4" s="5">
-        <v>1485.905282939658</v>
-      </c>
-      <c r="V4" s="5">
-        <v>1432.0299170163166</v>
-      </c>
-      <c r="W4" s="5">
-        <v>1378.1545510929752</v>
-      </c>
-      <c r="X4" s="5">
-        <v>1324.2791851696338</v>
-      </c>
-      <c r="Y4" s="5">
-        <v>1270.4038192462924</v>
-      </c>
-      <c r="Z4" s="5">
-        <v>1216.528453322951</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="E4" s="3">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="F4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="G4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="H4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="I4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="J4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="K4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="L4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="M4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="N4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="O4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="P4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="Q4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="R4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="S4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="T4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="U4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="V4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="W4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="X4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="Y4" s="56">
+        <v>1171.0983188067505</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="12">
-        <v>3.5998225679871703E-9</v>
+      <c r="C5" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E5" t="s">
         <v>118</v>
       </c>
-      <c r="F5" s="5">
-        <v>2502.8086901013899</v>
-      </c>
-      <c r="G5" s="5">
-        <v>2482.7671254296229</v>
-      </c>
-      <c r="H5" s="5">
-        <v>2462.7255607578559</v>
-      </c>
-      <c r="I5" s="5">
-        <v>2442.6839960860889</v>
-      </c>
-      <c r="J5" s="5">
-        <v>2422.6424314143219</v>
-      </c>
-      <c r="K5" s="5">
-        <v>2402.6008667425549</v>
-      </c>
-      <c r="L5" s="5">
-        <v>2382.5593020707879</v>
-      </c>
-      <c r="M5" s="5">
-        <v>2362.5177373990209</v>
-      </c>
-      <c r="N5" s="5">
-        <v>2342.4761727272539</v>
-      </c>
-      <c r="O5" s="5">
-        <v>2322.4346080554869</v>
-      </c>
-      <c r="P5" s="5">
-        <v>2302.3930433837199</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>2282.351478711953</v>
-      </c>
-      <c r="R5" s="5">
-        <v>2262.309914040186</v>
-      </c>
-      <c r="S5" s="5">
-        <v>2242.268349368419</v>
-      </c>
-      <c r="T5" s="5">
-        <v>2222.226784696652</v>
-      </c>
-      <c r="U5" s="5">
-        <v>2202.185220024885</v>
-      </c>
-      <c r="V5" s="5">
-        <v>2182.143655353118</v>
-      </c>
-      <c r="W5" s="5">
-        <v>2162.102090681351</v>
-      </c>
-      <c r="X5" s="5">
-        <v>2142.060526009584</v>
-      </c>
-      <c r="Y5" s="5">
-        <v>2122.018961337817</v>
-      </c>
-      <c r="Z5" s="5">
-        <v>2101.97739666605</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="E5" s="3">
+        <v>1670.82114582243</v>
+      </c>
+      <c r="F5" s="56">
+        <v>1698.006304040191</v>
+      </c>
+      <c r="G5" s="56">
+        <v>1725.191462257952</v>
+      </c>
+      <c r="H5" s="56">
+        <v>1752.376620475713</v>
+      </c>
+      <c r="I5" s="56">
+        <v>1779.561778693474</v>
+      </c>
+      <c r="J5" s="56">
+        <v>1806.746936911235</v>
+      </c>
+      <c r="K5" s="56">
+        <v>1833.932095128996</v>
+      </c>
+      <c r="L5" s="56">
+        <v>1861.117253346757</v>
+      </c>
+      <c r="M5" s="56">
+        <v>1888.302411564518</v>
+      </c>
+      <c r="N5" s="56">
+        <v>1915.487569782279</v>
+      </c>
+      <c r="O5" s="56">
+        <v>1942.67272800004</v>
+      </c>
+      <c r="P5" s="56">
+        <v>1969.857886217801</v>
+      </c>
+      <c r="Q5" s="56">
+        <v>1997.043044435562</v>
+      </c>
+      <c r="R5" s="56">
+        <v>2024.228202653323</v>
+      </c>
+      <c r="S5" s="56">
+        <v>2051.413360871084</v>
+      </c>
+      <c r="T5" s="56">
+        <v>2078.598519088845</v>
+      </c>
+      <c r="U5" s="56">
+        <v>2105.783677306606</v>
+      </c>
+      <c r="V5" s="56">
+        <v>2132.968835524367</v>
+      </c>
+      <c r="W5" s="56">
+        <v>2160.153993742128</v>
+      </c>
+      <c r="X5" s="56">
+        <v>2187.339151959889</v>
+      </c>
+      <c r="Y5" s="56">
+        <v>2214.52431017765</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>145</v>
+        <v>36</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="12">
-        <v>3.5998225679871703E-9</v>
+      <c r="C6" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" t="s">
         <v>118</v>
       </c>
-      <c r="F6" s="5">
+      <c r="E6" s="3">
         <v>6035.0858307307299</v>
       </c>
-      <c r="G6" s="5">
+      <c r="F6" s="56">
         <v>5991.4369513857655</v>
       </c>
-      <c r="H6" s="5">
+      <c r="G6" s="56">
         <v>5947.7880720408011</v>
       </c>
-      <c r="I6" s="5">
+      <c r="H6" s="56">
         <v>5904.1391926958368</v>
       </c>
-      <c r="J6" s="5">
+      <c r="I6" s="56">
         <v>5860.4903133508724</v>
       </c>
-      <c r="K6" s="5">
+      <c r="J6" s="56">
         <v>5816.841434005908</v>
       </c>
-      <c r="L6" s="5">
+      <c r="K6" s="56">
         <v>5773.1925546609436</v>
       </c>
-      <c r="M6" s="5">
+      <c r="L6" s="56">
         <v>5729.5436753159793</v>
       </c>
-      <c r="N6" s="5">
+      <c r="M6" s="56">
         <v>5685.8947959710149</v>
       </c>
-      <c r="O6" s="5">
+      <c r="N6" s="56">
         <v>5642.2459166260505</v>
       </c>
-      <c r="P6" s="5">
+      <c r="O6" s="56">
         <v>5598.5970372810862</v>
       </c>
-      <c r="Q6" s="5">
+      <c r="P6" s="56">
         <v>5554.9481579361218</v>
       </c>
-      <c r="R6" s="5">
+      <c r="Q6" s="56">
         <v>5511.2992785911574</v>
       </c>
-      <c r="S6" s="5">
+      <c r="R6" s="56">
         <v>5467.650399246193</v>
       </c>
-      <c r="T6" s="5">
+      <c r="S6" s="56">
         <v>5424.0015199012287</v>
       </c>
-      <c r="U6" s="5">
+      <c r="T6" s="56">
         <v>5380.3526405562643</v>
       </c>
-      <c r="V6" s="5">
+      <c r="U6" s="56">
         <v>5336.7037612112999</v>
       </c>
-      <c r="W6" s="5">
+      <c r="V6" s="56">
         <v>5293.0548818663356</v>
       </c>
-      <c r="X6" s="5">
+      <c r="W6" s="56">
         <v>5249.4060025213712</v>
       </c>
-      <c r="Y6" s="5">
+      <c r="X6" s="56">
         <v>5205.7571231764068</v>
       </c>
-      <c r="Z6" s="5">
+      <c r="Y6" s="56">
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
-        <v>146</v>
+        <v>37</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="12">
-        <v>3.5998225679871703E-9</v>
+      <c r="C7" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E7" t="s">
         <v>118</v>
       </c>
-      <c r="F7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="G7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="H7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="I7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="J7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="K7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="L7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="M7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="N7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="O7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="P7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="R7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="S7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="T7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="U7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="V7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="W7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="X7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="Y7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="Z7" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="E7" s="3">
+        <v>6035.0858307307299</v>
+      </c>
+      <c r="F7" s="56">
+        <v>5991.4369513857655</v>
+      </c>
+      <c r="G7" s="56">
+        <v>5947.7880720408011</v>
+      </c>
+      <c r="H7" s="56">
+        <v>5904.1391926958368</v>
+      </c>
+      <c r="I7" s="56">
+        <v>5860.4903133508724</v>
+      </c>
+      <c r="J7" s="56">
+        <v>5816.841434005908</v>
+      </c>
+      <c r="K7" s="56">
+        <v>5773.1925546609436</v>
+      </c>
+      <c r="L7" s="56">
+        <v>5729.5436753159793</v>
+      </c>
+      <c r="M7" s="56">
+        <v>5685.8947959710149</v>
+      </c>
+      <c r="N7" s="56">
+        <v>5642.2459166260505</v>
+      </c>
+      <c r="O7" s="56">
+        <v>5598.5970372810862</v>
+      </c>
+      <c r="P7" s="56">
+        <v>5554.9481579361218</v>
+      </c>
+      <c r="Q7" s="56">
+        <v>5511.2992785911574</v>
+      </c>
+      <c r="R7" s="56">
+        <v>5467.650399246193</v>
+      </c>
+      <c r="S7" s="56">
+        <v>5424.0015199012287</v>
+      </c>
+      <c r="T7" s="56">
+        <v>5380.3526405562643</v>
+      </c>
+      <c r="U7" s="56">
+        <v>5336.7037612112999</v>
+      </c>
+      <c r="V7" s="56">
+        <v>5293.0548818663356</v>
+      </c>
+      <c r="W7" s="56">
+        <v>5249.4060025213712</v>
+      </c>
+      <c r="X7" s="56">
+        <v>5205.7571231764068</v>
+      </c>
+      <c r="Y7" s="56">
+        <v>5162.1082438314425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="12">
-        <v>3.5998225679871703E-9</v>
+      <c r="C8" s="12" t="s">
+        <v>114</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E8" t="s">
         <v>118</v>
       </c>
-      <c r="F8" s="5">
-        <v>1670.82114582243</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1698.006304040191</v>
-      </c>
-      <c r="H8" s="5">
-        <v>1725.191462257952</v>
-      </c>
-      <c r="I8" s="5">
-        <v>1752.376620475713</v>
-      </c>
-      <c r="J8" s="5">
-        <v>1779.561778693474</v>
-      </c>
-      <c r="K8" s="5">
-        <v>1806.746936911235</v>
-      </c>
-      <c r="L8" s="5">
-        <v>1833.932095128996</v>
-      </c>
-      <c r="M8" s="5">
-        <v>1861.117253346757</v>
-      </c>
-      <c r="N8" s="5">
-        <v>1888.302411564518</v>
-      </c>
-      <c r="O8" s="5">
-        <v>1915.487569782279</v>
-      </c>
-      <c r="P8" s="5">
-        <v>1942.67272800004</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>1969.857886217801</v>
-      </c>
-      <c r="R8" s="5">
-        <v>1997.043044435562</v>
-      </c>
-      <c r="S8" s="5">
-        <v>2024.228202653323</v>
-      </c>
-      <c r="T8" s="5">
-        <v>2051.413360871084</v>
-      </c>
-      <c r="U8" s="5">
-        <v>2078.598519088845</v>
-      </c>
-      <c r="V8" s="5">
-        <v>2105.783677306606</v>
-      </c>
-      <c r="W8" s="5">
-        <v>2132.968835524367</v>
-      </c>
-      <c r="X8" s="5">
-        <v>2160.153993742128</v>
-      </c>
-      <c r="Y8" s="5">
-        <v>2187.339151959889</v>
-      </c>
-      <c r="Z8" s="5">
-        <v>2214.52431017765</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9">
-        <v>1.093E-6</v>
-      </c>
-      <c r="D9" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>148</v>
-      </c>
-      <c r="B10" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10">
-        <v>1.093E-6</v>
-      </c>
-      <c r="D10" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11">
-        <v>1.4243253975000002E-4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12">
-        <v>1.4243253975000002E-4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>0.8</v>
-      </c>
-      <c r="B14" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>330.25</v>
-      </c>
-      <c r="B15" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <f>A15*1.1</f>
-        <v>363.27500000000003</v>
-      </c>
-      <c r="B16" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>1250</v>
-      </c>
-      <c r="B17" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="C18" s="14"/>
-      <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>141</v>
-      </c>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <f>0.17*A16</f>
-        <v>61.756750000000011</v>
-      </c>
-      <c r="B22" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <f>0.19*A16</f>
-        <v>69.022250000000014</v>
-      </c>
-      <c r="B23" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28">
-        <v>1.093</v>
-      </c>
-      <c r="B28" t="s">
-        <v>275</v>
-      </c>
-      <c r="C28" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>283</v>
-      </c>
-      <c r="B30" t="s">
-        <v>282</v>
-      </c>
-      <c r="C30" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31">
-        <v>1000000</v>
-      </c>
-      <c r="B31" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32">
-        <f>A31*A28</f>
-        <v>1093000</v>
-      </c>
-      <c r="B32" t="s">
-        <v>278</v>
-      </c>
-      <c r="C32" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A33">
-        <f>A32*0.5</f>
-        <v>546500</v>
-      </c>
-      <c r="B33" t="s">
-        <v>286</v>
-      </c>
-      <c r="C33" t="s">
-        <v>290</v>
-      </c>
-      <c r="E33" s="38" t="s">
-        <v>291</v>
-      </c>
-      <c r="F33" s="38" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A34" s="57">
-        <f>A33/C34</f>
-        <v>151.81303791469193</v>
-      </c>
-      <c r="B34" t="s">
-        <v>287</v>
-      </c>
-      <c r="C34" s="5">
-        <v>3599.8225679871703</v>
-      </c>
-      <c r="D34" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A35" s="58">
-        <f>A34/8760/C35</f>
-        <v>2.7078524171427643E-2</v>
-      </c>
-      <c r="B35" t="s">
-        <v>285</v>
-      </c>
-      <c r="C35" s="42">
-        <v>0.64</v>
-      </c>
-      <c r="D35" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A37" s="58">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="B37" t="s">
-        <v>289</v>
+      <c r="E8" s="3">
+        <v>6035.0858307307299</v>
+      </c>
+      <c r="F8" s="56">
+        <v>5991.4369513857655</v>
+      </c>
+      <c r="G8" s="56">
+        <v>5947.7880720408011</v>
+      </c>
+      <c r="H8" s="56">
+        <v>5904.1391926958368</v>
+      </c>
+      <c r="I8" s="56">
+        <v>5860.4903133508724</v>
+      </c>
+      <c r="J8" s="56">
+        <v>5816.841434005908</v>
+      </c>
+      <c r="K8" s="56">
+        <v>5773.1925546609436</v>
+      </c>
+      <c r="L8" s="56">
+        <v>5729.5436753159793</v>
+      </c>
+      <c r="M8" s="56">
+        <v>5685.8947959710149</v>
+      </c>
+      <c r="N8" s="56">
+        <v>5642.2459166260505</v>
+      </c>
+      <c r="O8" s="56">
+        <v>5598.5970372810862</v>
+      </c>
+      <c r="P8" s="56">
+        <v>5554.9481579361218</v>
+      </c>
+      <c r="Q8" s="56">
+        <v>5511.2992785911574</v>
+      </c>
+      <c r="R8" s="56">
+        <v>5467.650399246193</v>
+      </c>
+      <c r="S8" s="56">
+        <v>5424.0015199012287</v>
+      </c>
+      <c r="T8" s="56">
+        <v>5380.3526405562643</v>
+      </c>
+      <c r="U8" s="56">
+        <v>5336.7037612112999</v>
+      </c>
+      <c r="V8" s="56">
+        <v>5293.0548818663356</v>
+      </c>
+      <c r="W8" s="56">
+        <v>5249.4060025213712</v>
+      </c>
+      <c r="X8" s="56">
+        <v>5205.7571231764068</v>
+      </c>
+      <c r="Y8" s="56">
+        <v>5162.1082438314425</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F33" r:id="rId1" xr:uid="{B2AA90EC-65DC-42B8-B7B5-135E5DE91F55}"/>
-    <hyperlink ref="E33" r:id="rId2" location=":~:text=A%20simple%20cycle%20natural%20gas,turbine%2C%20which%20generates%20more%20electricity." xr:uid="{CD686FF2-13D5-4E74-BB9A-BF2B38669542}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{78975c20-18d4-40c9-811f-0d8ea387c6ea}" enabled="0" method="" siteId="{78975c20-18d4-40c9-811f-0d8ea387c6ea}" removed="1"/>
+</clbl:labelList>
 </file>
</xml_diff>

<commit_message>
Feb 1st event run
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://randus-my.sharepoint.com/personal/jrojasa_rand_org/Documents/Documents/GitHub/SJV-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="14_{477DE6F6-3490-4777-94BA-8FDDBCE6B90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5B19A90-CC06-4DBA-B934-E76D9E4E1B2C}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="14_{477DE6F6-3490-4777-94BA-8FDDBCE6B90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F71BEFC7-4792-4F77-9792-8D100573CA2A}"/>
   <bookViews>
-    <workbookView xWindow="-14490" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="622" firstSheet="2" activeTab="7" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="-7763" yWindow="-16200" windowWidth="14401" windowHeight="15600" tabRatio="622" activeTab="1" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Land" sheetId="14" r:id="rId1"/>
@@ -5108,10 +5108,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -5154,7 +5155,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -5206,7 +5207,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -5229,7 +5230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -5252,7 +5253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -5275,7 +5276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="36" t="s">
         <v>36</v>
       </c>
@@ -5298,7 +5299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="36" t="s">
         <v>37</v>
       </c>
@@ -5321,7 +5322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="36" t="s">
         <v>38</v>
       </c>
@@ -5461,7 +5462,7 @@
       </c>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="36" t="s">
         <v>44</v>
       </c>
@@ -5485,7 +5486,7 @@
       </c>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
@@ -5511,7 +5512,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>47</v>
       </c>
@@ -5537,7 +5538,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
@@ -5563,7 +5564,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -5592,7 +5593,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -5621,7 +5622,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>11</v>
       </c>
@@ -5673,7 +5674,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -5696,7 +5697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>34</v>
       </c>
@@ -5719,7 +5720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>35</v>
       </c>
@@ -5742,7 +5743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="36" t="s">
         <v>36</v>
       </c>
@@ -5765,7 +5766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="36" t="s">
         <v>37</v>
       </c>
@@ -5785,7 +5786,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="36" t="s">
         <v>38</v>
       </c>
@@ -5897,7 +5898,7 @@
       </c>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="36" t="s">
         <v>44</v>
       </c>
@@ -5924,7 +5925,7 @@
       </c>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -5950,7 +5951,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>47</v>
       </c>
@@ -5976,7 +5977,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>50</v>
       </c>
@@ -6002,7 +6003,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -6022,7 +6023,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -6042,7 +6043,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -6094,7 +6095,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>22</v>
       </c>
@@ -6117,7 +6118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>34</v>
       </c>
@@ -6140,7 +6141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>35</v>
       </c>
@@ -6163,7 +6164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="36" t="s">
         <v>36</v>
       </c>
@@ -6186,7 +6187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="36" t="s">
         <v>37</v>
       </c>
@@ -6206,7 +6207,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="36" t="s">
         <v>38</v>
       </c>
@@ -6318,7 +6319,7 @@
       </c>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="36" t="s">
         <v>44</v>
       </c>
@@ -6345,7 +6346,7 @@
       </c>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>45</v>
       </c>
@@ -6371,7 +6372,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>47</v>
       </c>
@@ -6397,7 +6398,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -6423,7 +6424,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -6443,7 +6444,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>36</v>
       </c>
@@ -6464,7 +6465,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I55" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}"/>
+  <autoFilter ref="A1:I55" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Hydrogen"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8585,9 +8592,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA5616B-DF07-465E-AEEB-CCA6D05FE697}">
   <dimension ref="A1:AK23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G5" sqref="G5"/>
+      <selection pane="topRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Updated CI values for SAF
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A038116-974F-4DC2-8574-8FE49DE2B132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FD76E2-8695-476F-903A-A2F3DADE237F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="622" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="-3600" yWindow="3030" windowWidth="26490" windowHeight="11325" tabRatio="622" activeTab="2" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1904" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="301">
   <si>
     <t>Feedstock</t>
   </si>
@@ -856,9 +856,6 @@
     <t>(Diverted Organic waste vs. Animal Manure to CNG = 15%)</t>
   </si>
   <si>
-    <t>3.6 kg co2/ kg h2</t>
-  </si>
-  <si>
     <t>https://www.iea.org/data-and-statistics/charts/comparison-of-the-emissions-intensity-of-different-hydrogen-production-routes-2021</t>
   </si>
   <si>
@@ -949,9 +946,6 @@
     <t>F2C Conversion Factor</t>
   </si>
   <si>
-    <t>same as nominal</t>
-  </si>
-  <si>
     <t>Input Category</t>
   </si>
   <si>
@@ -968,6 +962,15 @@
   </si>
   <si>
     <t>Fats, Oils, and Greases</t>
+  </si>
+  <si>
+    <t>https://www.icao.int/environmental-protection/CORSIA/Documents/CORSIA_Eligible_Fuels/ICAO%20document%2006%20-%20Default%20Life%20Cycle%20Emissions%20-%20June%202022.pdf</t>
+  </si>
+  <si>
+    <t>Direct emission = 0</t>
+  </si>
+  <si>
+    <t>3.6 kg co2/ kg h2 (mid/upstream)</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1165,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1250,10 +1253,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -1264,6 +1264,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1374,10 +1375,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1682,8 +1683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE3E66E-8E4F-4F0F-BF6D-3E16E49004F7}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+    <sheetView zoomScale="107" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1707,7 +1708,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1734,16 +1735,16 @@
         <v>108</v>
       </c>
       <c r="K1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="L1" t="s">
+        <v>264</v>
+      </c>
+      <c r="M1" t="s">
         <v>265</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>266</v>
-      </c>
-      <c r="N1" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -1751,7 +1752,7 @@
         <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -1776,17 +1777,17 @@
         <v>116</v>
       </c>
       <c r="J2" s="40"/>
-      <c r="K2" s="60">
+      <c r="K2" s="57">
         <v>100</v>
       </c>
-      <c r="L2" s="61" t="s">
+      <c r="L2" s="58" t="s">
+        <v>268</v>
+      </c>
+      <c r="M2" t="s">
         <v>269</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>270</v>
-      </c>
-      <c r="N2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -1794,7 +1795,7 @@
         <v>36</v>
       </c>
       <c r="B3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -1821,17 +1822,17 @@
       <c r="J3" s="40">
         <v>0.25</v>
       </c>
-      <c r="K3" s="60">
+      <c r="K3" s="57">
         <v>100</v>
       </c>
-      <c r="L3" s="61" t="s">
+      <c r="L3" s="58" t="s">
+        <v>268</v>
+      </c>
+      <c r="M3" t="s">
         <v>269</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>270</v>
-      </c>
-      <c r="N3" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -1839,7 +1840,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1850,18 +1851,18 @@
       <c r="F4" s="5"/>
       <c r="H4" s="37"/>
       <c r="J4" s="40"/>
-      <c r="K4" s="60">
+      <c r="K4" s="57">
         <f>K11*K16</f>
         <v>442.1052631578948</v>
       </c>
-      <c r="L4" s="61" t="s">
+      <c r="L4" s="58" t="s">
+        <v>272</v>
+      </c>
+      <c r="M4" t="s">
         <v>273</v>
       </c>
-      <c r="M4" t="s">
-        <v>274</v>
-      </c>
       <c r="N4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1869,7 +1870,7 @@
         <v>44</v>
       </c>
       <c r="B5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -1880,18 +1881,18 @@
       <c r="F5" s="5"/>
       <c r="H5" s="37"/>
       <c r="J5" s="40"/>
-      <c r="K5" s="60">
+      <c r="K5" s="57">
         <f>K12*K16</f>
         <v>420</v>
       </c>
-      <c r="L5" s="61" t="s">
+      <c r="L5" s="58" t="s">
+        <v>272</v>
+      </c>
+      <c r="M5" t="s">
         <v>273</v>
       </c>
-      <c r="M5" t="s">
-        <v>274</v>
-      </c>
       <c r="N5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1926,18 +1927,18 @@
       <c r="J6" s="40">
         <v>0.72</v>
       </c>
-      <c r="K6" s="62">
+      <c r="K6" s="59">
         <f>1/0.167</f>
         <v>5.9880239520958076</v>
       </c>
-      <c r="L6" s="61" t="s">
+      <c r="L6" s="58" t="s">
+        <v>274</v>
+      </c>
+      <c r="M6" t="s">
         <v>275</v>
       </c>
-      <c r="M6" t="s">
-        <v>276</v>
-      </c>
       <c r="N6" s="40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
@@ -1945,7 +1946,7 @@
         <v>37</v>
       </c>
       <c r="B7" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -1972,18 +1973,18 @@
       <c r="J7" s="40">
         <v>0.44</v>
       </c>
-      <c r="K7" s="60">
+      <c r="K7" s="57">
         <f>1/13*10^6</f>
         <v>76923.076923076922</v>
       </c>
-      <c r="L7" s="61" t="s">
+      <c r="L7" s="58" t="s">
+        <v>276</v>
+      </c>
+      <c r="M7" t="s">
         <v>277</v>
       </c>
-      <c r="M7" t="s">
-        <v>278</v>
-      </c>
       <c r="N7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1991,7 +1992,7 @@
         <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -2018,18 +2019,18 @@
       <c r="J8" s="40">
         <v>0.44</v>
       </c>
-      <c r="K8" s="60">
+      <c r="K8" s="57">
         <f>1/13*10^6</f>
         <v>76923.076923076922</v>
       </c>
-      <c r="L8" s="61" t="s">
-        <v>277</v>
+      <c r="L8" s="58" t="s">
+        <v>276</v>
       </c>
       <c r="M8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="N8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -2037,7 +2038,7 @@
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -2062,18 +2063,18 @@
         <v>121</v>
       </c>
       <c r="J9" s="40"/>
-      <c r="K9" s="60">
+      <c r="K9" s="57">
         <f>1/3.29/1.6*10^6</f>
         <v>189969.60486322187</v>
       </c>
-      <c r="L9" s="61" t="s">
+      <c r="L9" s="58" t="s">
+        <v>279</v>
+      </c>
+      <c r="M9" s="53" t="s">
         <v>280</v>
       </c>
-      <c r="M9" s="53" t="s">
-        <v>281</v>
-      </c>
       <c r="N9" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -2081,7 +2082,7 @@
         <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -2106,18 +2107,18 @@
         <v>121</v>
       </c>
       <c r="J10" s="40"/>
-      <c r="K10" s="60">
+      <c r="K10" s="57">
         <f>1/3.29/1.6*10^6</f>
         <v>189969.60486322187</v>
       </c>
-      <c r="L10" s="61" t="s">
-        <v>280</v>
+      <c r="L10" s="58" t="s">
+        <v>279</v>
       </c>
       <c r="M10" s="53" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -2125,7 +2126,7 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
@@ -2149,18 +2150,18 @@
       <c r="I11" t="s">
         <v>134</v>
       </c>
-      <c r="K11" s="60">
+      <c r="K11" s="57">
         <f>56*10^9*0.6/(1.9*10^6)</f>
         <v>17684.21052631579</v>
       </c>
-      <c r="L11" s="61" t="s">
+      <c r="L11" s="58" t="s">
+        <v>282</v>
+      </c>
+      <c r="M11" t="s">
         <v>283</v>
       </c>
-      <c r="M11" t="s">
-        <v>284</v>
-      </c>
       <c r="N11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -2168,7 +2169,7 @@
         <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C12" t="s">
         <v>38</v>
@@ -2196,22 +2197,22 @@
         <f>28000*0.6</f>
         <v>16800</v>
       </c>
-      <c r="L12" s="61" t="s">
-        <v>283</v>
+      <c r="L12" s="58" t="s">
+        <v>282</v>
       </c>
       <c r="M12" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N12" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>48</v>
@@ -2238,14 +2239,14 @@
       <c r="K13" s="2">
         <v>294</v>
       </c>
-      <c r="L13" s="61" t="s">
+      <c r="L13" s="58" t="s">
+        <v>286</v>
+      </c>
+      <c r="M13" t="s">
         <v>287</v>
       </c>
-      <c r="M13" t="s">
-        <v>288</v>
-      </c>
       <c r="N13" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -2253,7 +2254,7 @@
         <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>48</v>
@@ -2277,14 +2278,14 @@
       <c r="I14" t="s">
         <v>139</v>
       </c>
-      <c r="K14" s="63">
+      <c r="K14" s="60">
         <v>56.1</v>
       </c>
-      <c r="L14" s="61" t="s">
+      <c r="L14" s="58" t="s">
+        <v>288</v>
+      </c>
+      <c r="M14" t="s">
         <v>289</v>
-      </c>
-      <c r="M14" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
@@ -2292,7 +2293,7 @@
         <v>36</v>
       </c>
       <c r="B15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>48</v>
@@ -2316,14 +2317,14 @@
       <c r="I15" t="s">
         <v>139</v>
       </c>
-      <c r="K15" s="63">
+      <c r="K15" s="60">
         <v>62.7</v>
       </c>
-      <c r="L15" s="61" t="s">
-        <v>289</v>
+      <c r="L15" s="58" t="s">
+        <v>288</v>
       </c>
       <c r="M15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -2399,13 +2400,13 @@
       <c r="L17" s="40" t="s">
         <v>127</v>
       </c>
-      <c r="N17" s="64"/>
+      <c r="N17" s="61"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="K19" s="65"/>
+      <c r="K19" s="62"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L20" s="66"/>
+      <c r="L20" s="63"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3072,7 +3073,7 @@
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -3155,7 +3156,7 @@
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -3172,7 +3173,7 @@
       <c r="F2" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="68">
+      <c r="G2" s="65">
         <f>AA2/21</f>
         <v>1266.6666666666667</v>
       </c>
@@ -3181,7 +3182,7 @@
         <v>2533.3333333333335</v>
       </c>
       <c r="I2" s="2">
-        <f t="shared" ref="I2:X14" si="0">$AA2/21+H2</f>
+        <f t="shared" ref="I2:X2" si="0">$AA2/21+H2</f>
         <v>3800</v>
       </c>
       <c r="J2" s="2">
@@ -3259,7 +3260,7 @@
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -3276,7 +3277,7 @@
       <c r="F3" t="s">
         <v>114</v>
       </c>
-      <c r="G3" s="68">
+      <c r="G3" s="65">
         <f t="shared" ref="G3:G20" si="2">AA3/21</f>
         <v>26.19047619047619</v>
       </c>
@@ -3363,7 +3364,7 @@
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -3380,7 +3381,7 @@
       <c r="F4" t="s">
         <v>114</v>
       </c>
-      <c r="G4" s="68">
+      <c r="G4" s="65">
         <f t="shared" si="2"/>
         <v>704.76190476190482</v>
       </c>
@@ -3467,7 +3468,7 @@
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
@@ -3484,7 +3485,7 @@
       <c r="F5" t="s">
         <v>114</v>
       </c>
-      <c r="G5" s="68">
+      <c r="G5" s="65">
         <f t="shared" si="2"/>
         <v>47.61904761904762</v>
       </c>
@@ -3588,7 +3589,7 @@
       <c r="F6" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="68">
+      <c r="G6" s="65">
         <f t="shared" si="2"/>
         <v>0.14365994845143032</v>
       </c>
@@ -3692,7 +3693,7 @@
       <c r="F7" t="s">
         <v>114</v>
       </c>
-      <c r="G7" s="68">
+      <c r="G7" s="65">
         <f t="shared" si="2"/>
         <v>1.6326530612244898</v>
       </c>
@@ -3785,7 +3786,7 @@
         <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -3796,7 +3797,7 @@
       <c r="F8" t="s">
         <v>114</v>
       </c>
-      <c r="G8" s="68">
+      <c r="G8" s="65">
         <v>10</v>
       </c>
       <c r="H8" s="2">
@@ -3868,7 +3869,7 @@
         <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -3879,7 +3880,7 @@
       <c r="F9" t="s">
         <v>114</v>
       </c>
-      <c r="G9" s="68">
+      <c r="G9" s="65">
         <v>10</v>
       </c>
       <c r="H9" s="2">
@@ -3945,7 +3946,7 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -3962,7 +3963,7 @@
       <c r="F10" t="s">
         <v>119</v>
       </c>
-      <c r="G10" s="68">
+      <c r="G10" s="65">
         <f t="shared" si="2"/>
         <v>14761.904761904761</v>
       </c>
@@ -4042,7 +4043,7 @@
         <f t="shared" si="1"/>
         <v>295238.09523809515</v>
       </c>
-      <c r="AA10" s="68">
+      <c r="AA10" s="65">
         <f>[1]portfolio_input!C15</f>
         <v>310000</v>
       </c>
@@ -4066,7 +4067,7 @@
       <c r="F11" t="s">
         <v>119</v>
       </c>
-      <c r="G11" s="68">
+      <c r="G11" s="65">
         <f t="shared" si="2"/>
         <v>523.80952380952385</v>
       </c>
@@ -4146,7 +4147,7 @@
         <f t="shared" si="1"/>
         <v>10476.190476190473</v>
       </c>
-      <c r="AA11" s="68">
+      <c r="AA11" s="65">
         <f>[1]portfolio_input!C16</f>
         <v>11000</v>
       </c>
@@ -4170,7 +4171,7 @@
       <c r="F12" t="s">
         <v>119</v>
       </c>
-      <c r="G12" s="68">
+      <c r="G12" s="65">
         <f t="shared" si="2"/>
         <v>5721.7847769028867</v>
       </c>
@@ -4250,7 +4251,7 @@
         <f t="shared" si="1"/>
         <v>114435.69553805776</v>
       </c>
-      <c r="AA12" s="68">
+      <c r="AA12" s="65">
         <f>[1]portfolio_input!C17</f>
         <v>120157.48031496063</v>
       </c>
@@ -4274,7 +4275,7 @@
       <c r="F13" t="s">
         <v>119</v>
       </c>
-      <c r="G13" s="68">
+      <c r="G13" s="65">
         <f t="shared" si="2"/>
         <v>471.35984432151918</v>
       </c>
@@ -4354,7 +4355,7 @@
         <f t="shared" si="1"/>
         <v>9427.196886430389</v>
       </c>
-      <c r="AA13" s="68">
+      <c r="AA13" s="65">
         <f>[1]portfolio_input!C18</f>
         <v>9898.5567307519032</v>
       </c>
@@ -4367,7 +4368,7 @@
         <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D14" t="s">
         <v>19</v>
@@ -4378,7 +4379,7 @@
       <c r="F14" t="s">
         <v>119</v>
       </c>
-      <c r="G14" s="68">
+      <c r="G14" s="65">
         <v>20</v>
       </c>
       <c r="H14" s="2">
@@ -4438,7 +4439,7 @@
       <c r="Z14" s="2">
         <v>20</v>
       </c>
-      <c r="AA14" s="68">
+      <c r="AA14" s="65">
         <v>20</v>
       </c>
     </row>
@@ -4450,7 +4451,7 @@
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D15" t="s">
         <v>19</v>
@@ -4461,7 +4462,7 @@
       <c r="F15" t="s">
         <v>119</v>
       </c>
-      <c r="G15" s="68">
+      <c r="G15" s="65">
         <v>20</v>
       </c>
       <c r="H15" s="2">
@@ -4521,7 +4522,7 @@
       <c r="Z15" s="2">
         <v>20</v>
       </c>
-      <c r="AA15" s="68">
+      <c r="AA15" s="65">
         <v>20</v>
       </c>
     </row>
@@ -4544,7 +4545,7 @@
       <c r="F16" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="68">
+      <c r="G16" s="65">
         <f t="shared" si="2"/>
         <v>274.72527472527474</v>
       </c>
@@ -4624,7 +4625,7 @@
         <f t="shared" si="1"/>
         <v>5494.5054945054953</v>
       </c>
-      <c r="AA16" s="68">
+      <c r="AA16" s="65">
         <f>[1]portfolio_input!C20*1000</f>
         <v>5769.2307692307695</v>
       </c>
@@ -4648,7 +4649,7 @@
       <c r="F17" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="68">
+      <c r="G17" s="65">
         <f t="shared" si="2"/>
         <v>10.989010989010989</v>
       </c>
@@ -4728,7 +4729,7 @@
         <f t="shared" si="1"/>
         <v>219.78021978021971</v>
       </c>
-      <c r="AA17" s="68">
+      <c r="AA17" s="65">
         <f>[1]portfolio_input!C21*1000</f>
         <v>230.76923076923077</v>
       </c>
@@ -4752,7 +4753,7 @@
       <c r="F18" t="s">
         <v>137</v>
       </c>
-      <c r="G18" s="68">
+      <c r="G18" s="65">
         <f t="shared" si="2"/>
         <v>4081.6326530612241</v>
       </c>
@@ -4856,7 +4857,7 @@
       <c r="F19" t="s">
         <v>137</v>
       </c>
-      <c r="G19" s="68">
+      <c r="G19" s="65">
         <f t="shared" si="2"/>
         <v>680.27210884353735</v>
       </c>
@@ -4946,7 +4947,7 @@
         <v>140</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C20" t="s">
         <v>155</v>
@@ -4960,7 +4961,7 @@
       <c r="F20" t="s">
         <v>137</v>
       </c>
-      <c r="G20" s="68">
+      <c r="G20" s="65">
         <f t="shared" si="2"/>
         <v>238.0952380952381</v>
       </c>
@@ -7914,13 +7915,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.875" style="56" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
     <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="5" width="26" customWidth="1"/>
@@ -7930,7 +7931,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -7959,7 +7960,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -7982,19 +7983,19 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="58" t="s">
+      <c r="C3" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="58" t="s">
+      <c r="E3" s="55" t="s">
         <v>15</v>
       </c>
       <c r="F3" t="s">
@@ -8011,7 +8012,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -8034,7 +8035,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="55" t="s">
+      <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -8057,7 +8058,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="55" t="s">
+      <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -8080,7 +8081,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" t="s">
         <v>36</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -8103,7 +8104,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="55" t="s">
         <v>37</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -8126,7 +8127,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -8153,7 +8154,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
@@ -8180,19 +8181,19 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="58" t="s">
+      <c r="A11" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="58" t="s">
+      <c r="B11" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="58" t="s">
+      <c r="D11" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="55" t="s">
         <v>15</v>
       </c>
       <c r="F11" t="s">
@@ -8209,19 +8210,19 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="58" t="s">
+      <c r="E12" s="55" t="s">
         <v>15</v>
       </c>
       <c r="F12" t="s">
@@ -8241,19 +8242,19 @@
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="58" t="s">
+      <c r="A13" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="58" t="s">
+      <c r="D13" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="58" t="s">
+      <c r="E13" s="55" t="s">
         <v>15</v>
       </c>
       <c r="F13" t="s">
@@ -8273,19 +8274,19 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+      <c r="A14" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="58" t="s">
+      <c r="D14" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="58" t="s">
+      <c r="E14" s="55" t="s">
         <v>15</v>
       </c>
       <c r="F14" t="s">
@@ -8300,19 +8301,19 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="58" t="s">
+      <c r="E15" s="55" t="s">
         <v>15</v>
       </c>
       <c r="F15" t="s">
@@ -8326,7 +8327,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="56" t="s">
+      <c r="A16" t="s">
         <v>44</v>
       </c>
       <c r="B16" s="1" t="s">
@@ -8350,7 +8351,7 @@
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="55" t="s">
+      <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -8376,7 +8377,7 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -8402,7 +8403,7 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="55" t="s">
+      <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -8428,7 +8429,7 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
+      <c r="A20" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
@@ -8457,7 +8458,7 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="56" t="s">
+      <c r="A21" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
@@ -8486,7 +8487,7 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="56" t="s">
+      <c r="A22" t="s">
         <v>11</v>
       </c>
       <c r="B22" t="s">
@@ -8509,19 +8510,19 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="58" t="s">
+      <c r="A23" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="58" t="s">
+      <c r="B23" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="58" t="s">
+      <c r="C23" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D23" s="58" t="s">
+      <c r="D23" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E23" s="58" t="s">
+      <c r="E23" s="55" t="s">
         <v>24</v>
       </c>
       <c r="F23" t="s">
@@ -8538,7 +8539,7 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="56" t="s">
+      <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24" t="s">
@@ -8561,7 +8562,7 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="55" t="s">
+      <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B25" s="1" t="s">
@@ -8584,7 +8585,7 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="55" t="s">
+      <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -8607,7 +8608,7 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="56" t="s">
+      <c r="A27" t="s">
         <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
@@ -8630,7 +8631,7 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="56" t="s">
+      <c r="A28" t="s">
         <v>37</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -8653,7 +8654,7 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="57" t="s">
+      <c r="A29" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -8680,7 +8681,7 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="57" t="s">
+      <c r="A30" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B30" s="1" t="s">
@@ -8707,19 +8708,19 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="58" t="s">
+      <c r="A31" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="58" t="s">
+      <c r="C31" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="58" t="s">
+      <c r="D31" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E31" s="58" t="s">
+      <c r="E31" s="55" t="s">
         <v>24</v>
       </c>
       <c r="F31" t="s">
@@ -8736,19 +8737,19 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="58" t="s">
+      <c r="A32" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="58" t="s">
+      <c r="C32" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D32" s="58" t="s">
+      <c r="D32" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E32" s="58" t="s">
+      <c r="E32" s="55" t="s">
         <v>24</v>
       </c>
       <c r="F32" t="s">
@@ -8757,27 +8758,27 @@
       <c r="G32">
         <v>30</v>
       </c>
-      <c r="H32" s="58" t="s">
+      <c r="H32" s="55" t="s">
+        <v>300</v>
+      </c>
+      <c r="I32" s="56" t="s">
         <v>262</v>
       </c>
-      <c r="I32" s="59" t="s">
-        <v>263</v>
-      </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="57" t="s">
+      <c r="A33" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C33" s="58" t="s">
+      <c r="C33" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D33" s="58" t="s">
+      <c r="D33" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="58" t="s">
+      <c r="E33" s="55" t="s">
         <v>24</v>
       </c>
       <c r="F33" t="s">
@@ -8792,19 +8793,19 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="57" t="s">
+      <c r="A34" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C34" s="58" t="s">
+      <c r="C34" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="58" t="s">
+      <c r="D34" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="E34" s="58" t="s">
+      <c r="E34" s="55" t="s">
         <v>24</v>
       </c>
       <c r="F34" t="s">
@@ -8818,19 +8819,19 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="58" t="s">
+      <c r="A35" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="58" t="s">
+      <c r="C35" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D35" s="58" t="s">
+      <c r="D35" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E35" s="58" t="s">
+      <c r="E35" s="55" t="s">
         <v>24</v>
       </c>
       <c r="F35" t="s">
@@ -8839,15 +8840,15 @@
       <c r="G35">
         <v>30</v>
       </c>
-      <c r="H35" s="58" t="s">
+      <c r="H35" s="55" t="s">
+        <v>300</v>
+      </c>
+      <c r="I35" s="56" t="s">
         <v>262</v>
       </c>
-      <c r="I35" s="59" t="s">
-        <v>263</v>
-      </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="56" t="s">
+      <c r="A36" t="s">
         <v>44</v>
       </c>
       <c r="B36" s="1" t="s">
@@ -8874,7 +8875,7 @@
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="56" t="s">
+      <c r="A37" t="s">
         <v>45</v>
       </c>
       <c r="B37" s="1" t="s">
@@ -8900,7 +8901,7 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="56" t="s">
+      <c r="A38" t="s">
         <v>47</v>
       </c>
       <c r="B38" s="1" t="s">
@@ -8926,7 +8927,7 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="56" t="s">
+      <c r="A39" t="s">
         <v>50</v>
       </c>
       <c r="B39" s="1" t="s">
@@ -8952,7 +8953,7 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="56" t="s">
+      <c r="A40" t="s">
         <v>37</v>
       </c>
       <c r="B40" s="1" t="s">
@@ -8970,12 +8971,15 @@
       <c r="F40" t="s">
         <v>32</v>
       </c>
-      <c r="G40" s="12">
-        <v>7.7</v>
+      <c r="G40" s="66">
+        <v>29.3</v>
+      </c>
+      <c r="I40" s="36" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="56" t="s">
+      <c r="A41" t="s">
         <v>36</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -8993,12 +8997,15 @@
       <c r="F41" t="s">
         <v>32</v>
       </c>
-      <c r="G41" s="12">
-        <v>8.3000000000000007</v>
+      <c r="G41" s="66">
+        <v>23.8</v>
+      </c>
+      <c r="I41" s="36" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="56" t="s">
+      <c r="A42" t="s">
         <v>11</v>
       </c>
       <c r="B42" t="s">
@@ -9021,19 +9028,19 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="58" t="s">
+      <c r="A43" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="58" t="s">
+      <c r="B43" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="58" t="s">
+      <c r="D43" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="58" t="s">
+      <c r="E43" s="55" t="s">
         <v>26</v>
       </c>
       <c r="F43" t="s">
@@ -9050,7 +9057,7 @@
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="56" t="s">
+      <c r="A44" t="s">
         <v>22</v>
       </c>
       <c r="B44" t="s">
@@ -9073,7 +9080,7 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="55" t="s">
+      <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B45" s="1" t="s">
@@ -9096,7 +9103,7 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="55" t="s">
+      <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B46" s="1" t="s">
@@ -9119,7 +9126,7 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="56" t="s">
+      <c r="A47" t="s">
         <v>36</v>
       </c>
       <c r="B47" s="1" t="s">
@@ -9142,7 +9149,7 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="56" t="s">
+      <c r="A48" t="s">
         <v>37</v>
       </c>
       <c r="B48" s="1" t="s">
@@ -9165,7 +9172,7 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="57" t="s">
+      <c r="A49" s="13" t="s">
         <v>44</v>
       </c>
       <c r="B49" s="1" t="s">
@@ -9192,7 +9199,7 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="57" t="s">
+      <c r="A50" s="13" t="s">
         <v>45</v>
       </c>
       <c r="B50" s="1" t="s">
@@ -9219,19 +9226,19 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="58" t="s">
+      <c r="A51" s="55" t="s">
         <v>40</v>
       </c>
-      <c r="B51" s="58" t="s">
+      <c r="B51" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C51" s="58" t="s">
+      <c r="C51" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D51" s="58" t="s">
+      <c r="D51" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E51" s="58" t="s">
+      <c r="E51" s="55" t="s">
         <v>26</v>
       </c>
       <c r="F51" t="s">
@@ -9248,47 +9255,48 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="58" t="s">
+      <c r="A52" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B52" s="58" t="s">
+      <c r="B52" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="58" t="s">
+      <c r="C52" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D52" s="58" t="s">
+      <c r="D52" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E52" s="58" t="s">
+      <c r="E52" s="55" t="s">
         <v>26</v>
       </c>
       <c r="F52" t="s">
         <v>32</v>
       </c>
       <c r="G52">
-        <f>G12</f>
-        <v>10.5</v>
-      </c>
-      <c r="H52" s="58" t="s">
-        <v>293</v>
-      </c>
-      <c r="I52" s="59"/>
+        <v>0</v>
+      </c>
+      <c r="H52" s="55" t="s">
+        <v>299</v>
+      </c>
+      <c r="I52" s="56" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="57" t="s">
+      <c r="A53" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C53" s="58" t="s">
+      <c r="C53" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D53" s="58" t="s">
+      <c r="D53" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E53" s="58" t="s">
+      <c r="E53" s="55" t="s">
         <v>26</v>
       </c>
       <c r="F53" t="s">
@@ -9303,19 +9311,19 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="57" t="s">
+      <c r="A54" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B54" s="58" t="s">
+      <c r="B54" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="58" t="s">
+      <c r="C54" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D54" s="58" t="s">
+      <c r="D54" s="55" t="s">
         <v>39</v>
       </c>
-      <c r="E54" s="58" t="s">
+      <c r="E54" s="55" t="s">
         <v>26</v>
       </c>
       <c r="F54" t="s">
@@ -9329,35 +9337,36 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="58" t="s">
+      <c r="A55" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="B55" s="58" t="s">
+      <c r="B55" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C55" s="58" t="s">
+      <c r="C55" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D55" s="58" t="s">
+      <c r="D55" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="E55" s="58" t="s">
+      <c r="E55" s="55" t="s">
         <v>26</v>
       </c>
       <c r="F55" t="s">
         <v>32</v>
       </c>
       <c r="G55">
-        <f>G12</f>
-        <v>10.5</v>
-      </c>
-      <c r="H55" s="58" t="s">
-        <v>293</v>
-      </c>
-      <c r="I55" s="3"/>
+        <v>0</v>
+      </c>
+      <c r="H55" s="55" t="s">
+        <v>299</v>
+      </c>
+      <c r="I55" s="56" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="56" t="s">
+      <c r="A56" t="s">
         <v>44</v>
       </c>
       <c r="B56" s="1" t="s">
@@ -9384,7 +9393,7 @@
       <c r="I56" s="3"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="56" t="s">
+      <c r="A57" t="s">
         <v>45</v>
       </c>
       <c r="B57" s="1" t="s">
@@ -9410,7 +9419,7 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="56" t="s">
+      <c r="A58" t="s">
         <v>47</v>
       </c>
       <c r="B58" s="1" t="s">
@@ -9436,7 +9445,7 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="56" t="s">
+      <c r="A59" t="s">
         <v>50</v>
       </c>
       <c r="B59" s="1" t="s">
@@ -9462,7 +9471,7 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="56" t="s">
+      <c r="A60" t="s">
         <v>37</v>
       </c>
       <c r="B60" s="1" t="s">
@@ -9485,7 +9494,7 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="56" t="s">
+      <c r="A61" t="s">
         <v>36</v>
       </c>
       <c r="B61" s="1" t="s">
@@ -9511,7 +9520,7 @@
       <c r="F67" s="5"/>
     </row>
     <row r="68" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F68" s="67"/>
+      <c r="F68" s="64"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I61" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}"/>
@@ -9519,6 +9528,10 @@
   <hyperlinks>
     <hyperlink ref="I32" r:id="rId1" xr:uid="{43F141C9-7DCE-4726-9197-F655B31D267F}"/>
     <hyperlink ref="I35" r:id="rId2" xr:uid="{C16E4B69-DDEA-45C6-9FA5-AE45F7F38139}"/>
+    <hyperlink ref="I40" r:id="rId3" xr:uid="{3DE9360D-4B28-4580-B9AC-7A8A7FDEC5D9}"/>
+    <hyperlink ref="I41" r:id="rId4" xr:uid="{616833AB-8ACA-41F8-8D0E-642E78789A77}"/>
+    <hyperlink ref="I52" r:id="rId5" xr:uid="{8E40FAC8-BE6F-4972-8F8A-D7FFC804E06E}"/>
+    <hyperlink ref="I55" r:id="rId6" xr:uid="{F8847031-885E-40E1-92C0-8616552E06FA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated functions and output for multiple portfolio analysis
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://randus-my.sharepoint.com/personal/jrojasa_rand_org/Documents/Documents/GitHub/SJV-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6774B8-B659-44BD-9411-CB6AA1998252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:1_{3F6774B8-B659-44BD-9411-CB6AA1998252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5D16CBCC-F905-4BF0-9DD8-FD90F23AB960}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="885" windowWidth="26490" windowHeight="11325" tabRatio="622" firstSheet="5" activeTab="9" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="622" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'F2C CI'!$A$1:$I$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'F2C Jobs'!$A$1:$J$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'F2C Land'!$A$1:$K$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'F2C Water'!$A$1:$L$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'F2C Water'!$A$1:$L$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Unit Conversion'!$A$1:$AK$19</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -1077,7 +1077,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1132,6 +1132,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1162,7 +1168,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1261,6 +1267,8 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1579,27 +1587,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE3E66E-8E4F-4F0F-BF6D-3E16E49004F7}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.375" customWidth="1"/>
-    <col min="2" max="2" width="17.125" customWidth="1"/>
-    <col min="4" max="4" width="27.625" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.08203125" customWidth="1"/>
+    <col min="4" max="4" width="27.58203125" customWidth="1"/>
     <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.625" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.58203125" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="13" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.875" customWidth="1"/>
-    <col min="12" max="12" width="38.375" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" customWidth="1"/>
+    <col min="12" max="12" width="38.33203125" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1643,7 +1651,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1686,7 +1694,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1731,7 +1739,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1761,7 +1769,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1791,7 +1799,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1837,7 +1845,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1883,7 +1891,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1929,7 +1937,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1973,7 +1981,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2017,7 +2025,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2060,7 +2068,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2103,7 +2111,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>285</v>
       </c>
@@ -2145,7 +2153,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2184,7 +2192,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2223,7 +2231,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2260,7 +2268,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2298,10 +2306,10 @@
       </c>
       <c r="N17" s="61"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="K19" s="62"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="L20" s="63"/>
     </row>
   </sheetData>
@@ -2317,20 +2325,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87BF8B-8E54-426F-864A-9E457E959B26}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
-    <col min="2" max="2" width="30.375" customWidth="1"/>
-    <col min="3" max="3" width="8.375" customWidth="1"/>
-    <col min="4" max="4" width="23.875" customWidth="1"/>
+    <col min="1" max="1" width="14.58203125" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="23.83203125" customWidth="1"/>
     <col min="5" max="25" width="8.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2407,7 +2415,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2484,7 +2492,7 @@
         <v>1216.528453322951</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2561,7 +2569,7 @@
         <v>2101.97739666605</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
@@ -2638,7 +2646,7 @@
         <v>1171.0983188067505</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>35</v>
       </c>
@@ -2715,7 +2723,7 @@
         <v>2214.52431017765</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
         <v>36</v>
       </c>
@@ -2792,7 +2800,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>37</v>
       </c>
@@ -2869,7 +2877,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
@@ -2946,7 +2954,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -3032,19 +3040,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4534657-2DF7-8944-A332-1622EE581035}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.125" customWidth="1"/>
-    <col min="2" max="2" width="31.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="21.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.08203125" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>292</v>
       </c>
@@ -3127,7 +3135,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>293</v>
       </c>
@@ -3210,7 +3218,7 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>293</v>
       </c>
@@ -3293,7 +3301,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>294</v>
       </c>
@@ -3376,7 +3384,7 @@
         <v>14800</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>294</v>
       </c>
@@ -3459,7 +3467,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -3542,7 +3550,7 @@
         <v>3.4782608695652177</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -3625,7 +3633,7 @@
         <v>21.118012422360248</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -3708,7 +3716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>140</v>
       </c>
@@ -3791,7 +3799,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>293</v>
       </c>
@@ -3874,7 +3882,7 @@
         <v>4.9689440993788822E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -3957,7 +3965,7 @@
         <v>310000</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -4040,7 +4048,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -4123,7 +4131,7 @@
         <v>83854.869455332082</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>140</v>
       </c>
@@ -4206,7 +4214,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -4289,7 +4297,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -4372,7 +4380,7 @@
         <v>39760971.535051085</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>140</v>
       </c>
@@ -4455,7 +4463,7 @@
         <v>2572768.7463856577</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -4538,7 +4546,7 @@
         <v>5769.2307692307695</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -4621,7 +4629,7 @@
         <v>230.76923076923077</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>140</v>
       </c>
@@ -4717,13 +4725,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.125" customWidth="1"/>
+    <col min="2" max="2" width="21.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -4794,7 +4802,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -4865,7 +4873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -4936,7 +4944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -5007,7 +5015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -5078,7 +5086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -5158,21 +5166,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDDA0F3-A3DE-4AB4-98AB-8BE3425A27E0}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="25.75" customWidth="1"/>
     <col min="2" max="2" width="20.75" customWidth="1"/>
-    <col min="3" max="3" width="20.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.375" customWidth="1"/>
-    <col min="6" max="6" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="32" t="s">
         <v>157</v>
       </c>
@@ -5195,7 +5203,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
@@ -5216,7 +5224,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
@@ -5237,7 +5245,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>34</v>
       </c>
@@ -5258,7 +5266,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>35</v>
       </c>
@@ -5279,7 +5287,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>140</v>
       </c>
@@ -5300,7 +5308,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>140</v>
       </c>
@@ -5321,7 +5329,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>38</v>
       </c>
@@ -5342,7 +5350,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
@@ -5363,7 +5371,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>58</v>
       </c>
@@ -5384,7 +5392,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>140</v>
       </c>
@@ -5405,7 +5413,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>140</v>
       </c>
@@ -5426,7 +5434,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="14" t="s">
         <v>38</v>
       </c>
@@ -5447,7 +5455,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>140</v>
       </c>
@@ -5468,7 +5476,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>140</v>
       </c>
@@ -5489,7 +5497,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="14" t="s">
         <v>160</v>
       </c>
@@ -5510,7 +5518,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>160</v>
       </c>
@@ -5531,7 +5539,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="14" t="s">
         <v>140</v>
       </c>
@@ -5552,7 +5560,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="14" t="s">
         <v>140</v>
       </c>
@@ -5573,7 +5581,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="50" t="s">
         <v>159</v>
       </c>
@@ -5581,7 +5589,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="51" t="s">
         <v>12</v>
       </c>
@@ -5589,7 +5597,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="51" t="s">
         <v>19</v>
       </c>
@@ -5597,7 +5605,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="51" t="s">
         <v>19</v>
       </c>
@@ -5605,7 +5613,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="51" t="s">
         <v>38</v>
       </c>
@@ -5613,7 +5621,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="51" t="s">
         <v>38</v>
       </c>
@@ -5621,7 +5629,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="51" t="s">
         <v>38</v>
       </c>
@@ -5629,7 +5637,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="51" t="s">
         <v>70</v>
       </c>
@@ -5651,17 +5659,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.375" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.625" customWidth="1"/>
+    <col min="4" max="4" width="16.58203125" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -5690,7 +5698,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -5701,7 +5709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -5712,7 +5720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -5729,7 +5737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -5737,7 +5745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -5758,17 +5766,17 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="47.875" customWidth="1"/>
-    <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.83203125" customWidth="1"/>
+    <col min="2" max="2" width="30.08203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="40.875" customWidth="1"/>
-    <col min="5" max="5" width="30.625" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.58203125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -5797,7 +5805,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">
         <v>58</v>
       </c>
@@ -5824,7 +5832,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>154</v>
       </c>
@@ -5851,7 +5859,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
@@ -5878,7 +5886,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
@@ -5905,7 +5913,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
         <v>22</v>
       </c>
@@ -5932,7 +5940,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
@@ -5955,7 +5963,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="14" t="s">
         <v>36</v>
       </c>
@@ -5978,7 +5986,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
         <v>179</v>
       </c>
@@ -6003,7 +6011,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
         <v>179</v>
       </c>
@@ -6028,7 +6036,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>183</v>
       </c>
@@ -6053,7 +6061,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="14" t="s">
         <v>183</v>
       </c>
@@ -6072,7 +6080,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -6087,7 +6095,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -6102,7 +6110,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
         <v>188</v>
       </c>
@@ -6129,7 +6137,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A16" s="20" t="s">
         <v>171</v>
       </c>
@@ -6152,7 +6160,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="62" x14ac:dyDescent="0.35">
       <c r="A17" s="20" t="s">
         <v>176</v>
       </c>
@@ -6175,7 +6183,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="62" x14ac:dyDescent="0.35">
       <c r="A18" s="20" t="s">
         <v>179</v>
       </c>
@@ -6198,7 +6206,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="63" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="62" x14ac:dyDescent="0.35">
       <c r="A19" s="20" t="s">
         <v>183</v>
       </c>
@@ -6212,7 +6220,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A20" s="23" t="s">
         <v>184</v>
       </c>
@@ -6226,7 +6234,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A21" s="23" t="s">
         <v>37</v>
       </c>
@@ -6240,7 +6248,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A22" s="23" t="s">
         <v>36</v>
       </c>
@@ -6254,12 +6262,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" s="26" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" s="32" t="s">
         <v>0</v>
       </c>
@@ -6276,7 +6284,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32" s="14" t="s">
         <v>58</v>
       </c>
@@ -6285,7 +6293,7 @@
       </c>
       <c r="C32" s="14"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="14" t="s">
         <v>154</v>
       </c>
@@ -6294,7 +6302,7 @@
       </c>
       <c r="C33" s="14"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
@@ -6303,7 +6311,7 @@
       </c>
       <c r="C34" s="14"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="14" t="s">
         <v>11</v>
       </c>
@@ -6314,7 +6322,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
         <v>22</v>
       </c>
@@ -6323,7 +6331,7 @@
       </c>
       <c r="C36" s="14"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="14" t="s">
         <v>209</v>
       </c>
@@ -6332,7 +6340,7 @@
       </c>
       <c r="C37" s="14"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="14" t="s">
         <v>35</v>
       </c>
@@ -6341,7 +6349,7 @@
       </c>
       <c r="C38" s="14"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="27" t="s">
         <v>37</v>
       </c>
@@ -6355,7 +6363,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="27" t="s">
         <v>36</v>
       </c>
@@ -6369,7 +6377,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="14" t="s">
         <v>179</v>
       </c>
@@ -6386,7 +6394,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="14" t="s">
         <v>183</v>
       </c>
@@ -6403,12 +6411,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="26" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="32" t="s">
         <v>1</v>
       </c>
@@ -6419,7 +6427,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="14" t="s">
         <v>19</v>
       </c>
@@ -6430,7 +6438,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="30" t="s">
         <v>19</v>
       </c>
@@ -6447,7 +6455,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="30" t="s">
         <v>19</v>
       </c>
@@ -6464,7 +6472,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="30" t="s">
         <v>19</v>
       </c>
@@ -6484,7 +6492,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="27" t="s">
         <v>19</v>
       </c>
@@ -6501,7 +6509,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="27" t="s">
         <v>58</v>
       </c>
@@ -6518,7 +6526,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="14" t="s">
         <v>58</v>
       </c>
@@ -6529,7 +6537,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="27" t="s">
         <v>58</v>
       </c>
@@ -6546,7 +6554,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="27" t="s">
         <v>12</v>
       </c>
@@ -6563,7 +6571,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="14" t="s">
         <v>12</v>
       </c>
@@ -6574,12 +6582,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="26" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="27" t="s">
         <v>233</v>
       </c>
@@ -6590,7 +6598,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="29" t="s">
         <v>235</v>
       </c>
@@ -6598,7 +6606,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="27" t="s">
         <v>236</v>
       </c>
@@ -6606,12 +6614,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="26" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="27" t="s">
         <v>238</v>
       </c>
@@ -6619,7 +6627,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="27" t="s">
         <v>239</v>
       </c>
@@ -6640,13 +6648,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.625" customWidth="1"/>
-    <col min="2" max="5" width="15.625" customWidth="1"/>
+    <col min="1" max="1" width="25.58203125" customWidth="1"/>
+    <col min="2" max="5" width="15.58203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>241</v>
       </c>
@@ -6666,7 +6674,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>242</v>
       </c>
@@ -6677,7 +6685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -6685,7 +6693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -6693,7 +6701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -6707,7 +6715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -6721,7 +6729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>243</v>
       </c>
@@ -6735,7 +6743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>244</v>
       </c>
@@ -6746,7 +6754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>245</v>
       </c>
@@ -6757,7 +6765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>246</v>
       </c>
@@ -6768,7 +6776,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -6776,7 +6784,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -6797,19 +6805,19 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.25" customWidth="1"/>
     <col min="2" max="2" width="12.75" customWidth="1"/>
-    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="11.25" customWidth="1"/>
     <col min="7" max="7" width="8.25" customWidth="1"/>
-    <col min="8" max="9" width="24.125" customWidth="1"/>
+    <col min="8" max="9" width="24.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6844,7 +6852,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -6878,7 +6886,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -6915,7 +6923,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -6944,7 +6952,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -6973,7 +6981,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -7002,7 +7010,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -7031,7 +7039,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -7065,7 +7073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -7102,7 +7110,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
@@ -7131,7 +7139,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -7163,7 +7171,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -7197,7 +7205,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -7226,7 +7234,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -7260,7 +7268,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -7297,7 +7305,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9" t="s">
         <v>22</v>
       </c>
@@ -7327,7 +7335,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
@@ -7359,7 +7367,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
@@ -7392,7 +7400,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9" t="s">
         <v>22</v>
       </c>
@@ -7422,7 +7430,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K19" xr:uid="{E8F51DB9-2485-024A-9940-AED9C0912620}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7431,22 +7438,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}">
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.875" customWidth="1"/>
-    <col min="2" max="2" width="24.375" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="5" width="26" customWidth="1"/>
-    <col min="6" max="7" width="24.125" customWidth="1"/>
+    <col min="6" max="7" width="24.08203125" customWidth="1"/>
     <col min="8" max="8" width="31.5" customWidth="1"/>
-    <col min="9" max="9" width="36.875" customWidth="1"/>
+    <col min="9" max="9" width="36.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7475,7 +7482,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -7498,7 +7505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="55" t="s">
         <v>11</v>
       </c>
@@ -7527,7 +7534,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -7550,7 +7557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -7573,7 +7580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -7596,7 +7603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -7619,7 +7626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="55" t="s">
         <v>37</v>
       </c>
@@ -7642,7 +7649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>44</v>
       </c>
@@ -7669,7 +7676,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>45</v>
       </c>
@@ -7696,7 +7703,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="55" t="s">
         <v>40</v>
       </c>
@@ -7725,7 +7732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="55" t="s">
         <v>37</v>
       </c>
@@ -7757,7 +7764,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="55" t="s">
         <v>36</v>
       </c>
@@ -7789,7 +7796,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>44</v>
       </c>
@@ -7816,7 +7823,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="13" t="s">
         <v>45</v>
       </c>
@@ -7842,7 +7849,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -7866,7 +7873,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -7892,7 +7899,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -7918,9 +7925,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>50</v>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="67" t="s">
+        <v>297</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>48</v>
@@ -7944,7 +7951,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -7973,7 +7980,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -8002,7 +8009,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -8025,7 +8032,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="55" t="s">
         <v>11</v>
       </c>
@@ -8054,7 +8061,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -8077,7 +8084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -8100,7 +8107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -8123,7 +8130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -8146,7 +8153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -8169,7 +8176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="13" t="s">
         <v>44</v>
       </c>
@@ -8196,7 +8203,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="13" t="s">
         <v>45</v>
       </c>
@@ -8223,7 +8230,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="55" t="s">
         <v>40</v>
       </c>
@@ -8252,7 +8259,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="55" t="s">
         <v>37</v>
       </c>
@@ -8281,7 +8288,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="13" t="s">
         <v>44</v>
       </c>
@@ -8308,7 +8315,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="13" t="s">
         <v>45</v>
       </c>
@@ -8334,7 +8341,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="55" t="s">
         <v>36</v>
       </c>
@@ -8363,7 +8370,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -8390,7 +8397,7 @@
       </c>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -8416,7 +8423,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -8442,9 +8449,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>50</v>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="66" t="s">
+        <v>297</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>48</v>
@@ -8468,7 +8475,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -8494,7 +8501,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -8520,7 +8527,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -8543,7 +8550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="55" t="s">
         <v>11</v>
       </c>
@@ -8572,7 +8579,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -8595,7 +8602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
@@ -8618,7 +8625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
@@ -8641,7 +8648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -8664,7 +8671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -8687,7 +8694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="13" t="s">
         <v>44</v>
       </c>
@@ -8714,7 +8721,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="13" t="s">
         <v>45</v>
       </c>
@@ -8741,7 +8748,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="55" t="s">
         <v>40</v>
       </c>
@@ -8770,7 +8777,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="55" t="s">
         <v>37</v>
       </c>
@@ -8799,7 +8806,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="13" t="s">
         <v>44</v>
       </c>
@@ -8826,7 +8833,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="13" t="s">
         <v>45</v>
       </c>
@@ -8852,7 +8859,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="55" t="s">
         <v>36</v>
       </c>
@@ -8881,7 +8888,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -8908,7 +8915,7 @@
       </c>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>45</v>
       </c>
@@ -8934,7 +8941,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -8960,9 +8967,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>50</v>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" s="66" t="s">
+        <v>297</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>48</v>
@@ -8986,7 +8993,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -9009,7 +9016,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -9032,14 +9039,13 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F68" s="64"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I61" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}"/>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I32" r:id="rId1" xr:uid="{43F141C9-7DCE-4726-9197-F655B31D267F}"/>
@@ -9061,17 +9067,17 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="173.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="173.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -9091,7 +9097,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -9108,7 +9114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -9125,7 +9131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -9145,7 +9151,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -9162,7 +9168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -9192,17 +9198,17 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.625" customWidth="1"/>
-    <col min="2" max="2" width="19.125" customWidth="1"/>
+    <col min="1" max="1" width="17.58203125" customWidth="1"/>
+    <col min="2" max="2" width="19.08203125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="25.75" customWidth="1"/>
-    <col min="6" max="6" width="19.125" customWidth="1"/>
+    <col min="6" max="6" width="19.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -9285,7 +9291,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -9368,7 +9374,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -9451,7 +9457,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -9534,7 +9540,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -9617,7 +9623,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -9700,7 +9706,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -9783,7 +9789,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -9866,7 +9872,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -9970,7 +9976,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -10074,7 +10080,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -10157,7 +10163,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -10261,7 +10267,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -10365,7 +10371,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -10448,7 +10454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -10531,7 +10537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -10624,22 +10630,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C58C4D02-922E-2849-99A2-B5A24807FA42}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.875" customWidth="1"/>
-    <col min="2" max="2" width="24.375" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.875" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="8" width="24.125" customWidth="1"/>
+    <col min="7" max="8" width="24.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10677,7 +10683,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -10694,7 +10700,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -10724,7 +10730,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -10742,7 +10748,7 @@
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -10760,7 +10766,7 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -10778,7 +10784,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
         <v>36</v>
       </c>
@@ -10796,7 +10802,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>37</v>
       </c>
@@ -10814,7 +10820,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -10832,7 +10838,7 @@
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -10850,7 +10856,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -10880,7 +10886,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -10910,7 +10916,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -10941,7 +10947,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -10959,7 +10965,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -10977,7 +10983,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -10994,7 +11000,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -11011,7 +11017,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -11028,9 +11034,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>50</v>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" s="67" t="s">
+        <v>297</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>48</v>
@@ -11045,7 +11051,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -11062,7 +11068,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -11079,7 +11085,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -11099,7 +11105,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -11136,7 +11142,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -11157,7 +11163,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -11175,7 +11181,7 @@
       </c>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -11193,7 +11199,7 @@
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>36</v>
       </c>
@@ -11211,7 +11217,7 @@
       </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
         <v>37</v>
       </c>
@@ -11229,7 +11235,7 @@
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -11247,7 +11253,7 @@
       </c>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -11265,7 +11271,7 @@
       </c>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
@@ -11302,7 +11308,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -11339,7 +11345,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -11370,7 +11376,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -11388,7 +11394,7 @@
       </c>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -11406,7 +11412,7 @@
       </c>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -11426,7 +11432,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -11446,7 +11452,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
@@ -11466,9 +11472,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>50</v>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="67" t="s">
+        <v>297</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>48</v>
@@ -11486,7 +11492,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -11503,7 +11509,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -11520,40 +11526,39 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L39" xr:uid="{C58C4D02-922E-2849-99A2-B5A24807FA42}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11566,16 +11571,16 @@
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.875" customWidth="1"/>
-    <col min="2" max="2" width="24.375" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
     <col min="3" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="22.875" customWidth="1"/>
-    <col min="7" max="8" width="24.125" customWidth="1"/>
+    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="7" max="8" width="24.08203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11607,7 +11612,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -11627,7 +11632,7 @@
         <v>3.4599999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="47" t="s">
         <v>11</v>
       </c>
@@ -11651,7 +11656,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -11671,7 +11676,7 @@
         <v>2.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -11691,7 +11696,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -11711,7 +11716,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -11731,7 +11736,7 @@
         <v>4.0899999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -11751,7 +11756,7 @@
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -11771,7 +11776,7 @@
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -11791,7 +11796,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -11811,7 +11816,7 @@
         <v>5.62E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -11831,7 +11836,7 @@
         <v>5.62E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -11865,15 +11870,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5" customWidth="1"/>
     <col min="4" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -11890,7 +11895,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -11907,7 +11912,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -11929,26 +11934,26 @@
       <selection pane="topRight" activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.58203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.75" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="15.25" customWidth="1"/>
-    <col min="6" max="6" width="11.125" customWidth="1"/>
+    <col min="6" max="6" width="11.08203125" customWidth="1"/>
     <col min="7" max="7" width="17.75" customWidth="1"/>
     <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="14.375" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="43.5" customWidth="1"/>
-    <col min="12" max="12" width="14.375" customWidth="1"/>
-    <col min="13" max="13" width="19.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.08203125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="10.5" customWidth="1"/>
     <col min="16" max="16" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12061,7 +12066,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -12154,7 +12159,7 @@
         <v>1216.528453322951</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -12196,7 +12201,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -12289,7 +12294,7 @@
         <v>2101.97739666605</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -12382,7 +12387,7 @@
         <v>1171.0983188067505</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -12475,7 +12480,7 @@
         <v>2214.52431017765</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -12583,7 +12588,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -12680,7 +12685,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -12781,7 +12786,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -12823,7 +12828,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -12859,7 +12864,7 @@
       <c r="L11" s="43"/>
       <c r="O11" s="36"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -12907,7 +12912,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -12955,7 +12960,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -12994,7 +12999,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -13033,7 +13038,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -13069,7 +13074,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -13105,7 +13110,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -13142,7 +13147,7 @@
       </c>
       <c r="O18" s="53"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -13179,7 +13184,7 @@
       </c>
       <c r="O19" s="53"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="L23">
         <v>1000</v>
       </c>

</xml_diff>

<commit_message>
Updated SAF displaced CI values
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6774B8-B659-44BD-9411-CB6AA1998252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FEC040-7AB0-4DB7-A1E3-85104EA59CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3060" yWindow="885" windowWidth="26490" windowHeight="11325" tabRatio="622" firstSheet="5" activeTab="9" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="622" firstSheet="1" activeTab="4" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <sheet name="Feedstock to Commodity Matrix" sheetId="4" r:id="rId16"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'C2U CI'!$A$1:$AA$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'C2U CI'!$A$1:$AA$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'F2C CI'!$A$1:$I$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'F2C Jobs'!$A$1:$J$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'F2C Land'!$A$1:$K$19</definedName>
@@ -2317,8 +2317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87BF8B-8E54-426F-864A-9E457E959B26}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7429,10 +7429,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D72" sqref="D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7475,7 +7476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -7498,7 +7499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>11</v>
       </c>
@@ -7527,7 +7528,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -7550,7 +7551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -7573,7 +7574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -7596,7 +7597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -7619,7 +7620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
         <v>37</v>
       </c>
@@ -7642,7 +7643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>44</v>
       </c>
@@ -7669,7 +7670,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>45</v>
       </c>
@@ -7696,7 +7697,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="55" t="s">
         <v>40</v>
       </c>
@@ -7725,7 +7726,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="55" t="s">
         <v>37</v>
       </c>
@@ -7757,7 +7758,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
         <v>36</v>
       </c>
@@ -7789,7 +7790,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>44</v>
       </c>
@@ -7816,7 +7817,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>45</v>
       </c>
@@ -7842,7 +7843,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -7866,7 +7867,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -8002,7 +8003,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -8025,7 +8026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="55" t="s">
         <v>11</v>
       </c>
@@ -8054,7 +8055,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -8077,7 +8078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -8100,7 +8101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -8123,7 +8124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -8146,7 +8147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -8169,7 +8170,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>44</v>
       </c>
@@ -8196,7 +8197,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>45</v>
       </c>
@@ -8223,7 +8224,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="55" t="s">
         <v>40</v>
       </c>
@@ -8252,7 +8253,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
         <v>37</v>
       </c>
@@ -8281,7 +8282,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>44</v>
       </c>
@@ -8308,7 +8309,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>45</v>
       </c>
@@ -8334,7 +8335,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="55" t="s">
         <v>36</v>
       </c>
@@ -8363,7 +8364,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -8390,7 +8391,7 @@
       </c>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -8520,7 +8521,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -8543,7 +8544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="55" t="s">
         <v>11</v>
       </c>
@@ -8572,7 +8573,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -8595,7 +8596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
@@ -8618,7 +8619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
@@ -8641,7 +8642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -8664,7 +8665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -8687,7 +8688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>44</v>
       </c>
@@ -8714,7 +8715,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>45</v>
       </c>
@@ -8741,7 +8742,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="55" t="s">
         <v>40</v>
       </c>
@@ -8770,7 +8771,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="55" t="s">
         <v>37</v>
       </c>
@@ -8799,7 +8800,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>44</v>
       </c>
@@ -8826,7 +8827,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>45</v>
       </c>
@@ -8852,7 +8853,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="55" t="s">
         <v>36</v>
       </c>
@@ -8881,7 +8882,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -8908,7 +8909,7 @@
       </c>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>45</v>
       </c>
@@ -9039,7 +9040,13 @@
       <c r="F68" s="64"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I61" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}"/>
+  <autoFilter ref="A1:I61" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Sustainable Aviation Fuel"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I32" r:id="rId1" xr:uid="{43F141C9-7DCE-4726-9197-F655B31D267F}"/>
@@ -9058,7 +9065,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9188,8 +9195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FEFDD9-D46C-E64E-8B04-7DDDC1C1B0F3}">
   <dimension ref="A1:AA16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10385,67 +10392,67 @@
         <v>32</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>86.64</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>85.38</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>84.13</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>82.87</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>81.62</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="N14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="O14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="Q14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="R14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="S14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="T14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="U14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="V14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="W14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="Y14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="Z14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
       <c r="AA14">
-        <v>0</v>
+        <v>80.36</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
@@ -10468,67 +10475,88 @@
         <v>32</v>
       </c>
       <c r="G15" s="12">
-        <v>0</v>
+        <f>G14</f>
+        <v>86.64</v>
       </c>
       <c r="H15" s="12">
-        <v>0</v>
+        <f t="shared" ref="H15:AA16" si="22">H14</f>
+        <v>85.38</v>
       </c>
       <c r="I15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>84.13</v>
       </c>
       <c r="J15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>82.87</v>
       </c>
       <c r="K15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>81.62</v>
       </c>
       <c r="L15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="M15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="N15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="O15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="P15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="Q15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="R15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="S15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="T15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="U15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="V15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="W15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="X15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="Y15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="Z15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="AA15" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
@@ -10551,71 +10579,92 @@
         <v>32</v>
       </c>
       <c r="G16" s="12">
-        <v>0</v>
+        <f>G15</f>
+        <v>86.64</v>
       </c>
       <c r="H16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>85.38</v>
       </c>
       <c r="I16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>84.13</v>
       </c>
       <c r="J16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>82.87</v>
       </c>
       <c r="K16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>81.62</v>
       </c>
       <c r="L16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="M16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="N16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="O16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="P16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="Q16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="R16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="S16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="T16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="U16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="V16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="W16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="X16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="Y16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="Z16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
       <c r="AA16" s="12">
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>80.36</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA14" xr:uid="{68FEFDD9-D46C-E64E-8B04-7DDDC1C1B0F3}"/>
+  <autoFilter ref="A1:AA16" xr:uid="{68FEFDD9-D46C-E64E-8B04-7DDDC1C1B0F3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Updates to the feedstock conversion to energy in MJ
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FEC040-7AB0-4DB7-A1E3-85104EA59CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57264FF7-3F4E-4535-B290-568E489A1A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="622" firstSheet="1" activeTab="4" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="622" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1908" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="312">
   <si>
     <t>Feedstock</t>
   </si>
@@ -968,6 +968,39 @@
   </si>
   <si>
     <t>3.6 kg co2/ kg h2 (mid/upstream)</t>
+  </si>
+  <si>
+    <t>Feedstock Energy Conversion (based on LHV)</t>
+  </si>
+  <si>
+    <t>Conversion Unit</t>
+  </si>
+  <si>
+    <t>MJ per million BDT of feedstock</t>
+  </si>
+  <si>
+    <t>assumed that dry ton HHV and LHV are the same. GJ/dry Metric ton biomass (HHV) 19.80 (Net Zero America Study)</t>
+  </si>
+  <si>
+    <t>GJ/dry Metric ton biomass (HHV) 19.80 (Net Zero America Study)</t>
+  </si>
+  <si>
+    <t>MJ per million tons of biogas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45-75% methane variation means that the energy content of biogas can vary; the lower heating value (LHV) is between 16 megajoules per cubic metre (MJ/m3) and 28 MJ/m3 (IEA) 1.15 kg/m3 density </t>
+  </si>
+  <si>
+    <t>MJ per million cubic feet</t>
+  </si>
+  <si>
+    <t>1 cubic foot of natural gas = 1,036 Btu = 1.093 MJ (EIA)</t>
+  </si>
+  <si>
+    <t>MJ per Million Tons of FOG</t>
+  </si>
+  <si>
+    <t>35-39 MJ per kg</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1195,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1261,6 +1294,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1577,10 +1611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE3E66E-8E4F-4F0F-BF6D-3E16E49004F7}">
-  <dimension ref="A1:N20"/>
+  <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1597,9 +1631,10 @@
     <col min="11" max="11" width="18.875" customWidth="1"/>
     <col min="12" max="12" width="38.375" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="38.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1642,8 +1677,17 @@
       <c r="N1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" t="s">
+        <v>301</v>
+      </c>
+      <c r="P1" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1685,8 +1729,18 @@
       <c r="N2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="66">
+        <f>198000*1000000</f>
+        <v>198000000000</v>
+      </c>
+      <c r="P2" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1730,8 +1784,18 @@
       <c r="N3" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="66">
+        <f>198000*1000000</f>
+        <v>198000000000</v>
+      </c>
+      <c r="P3" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1760,8 +1824,18 @@
       <c r="N4" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="66">
+        <f>16/1.15*1000*1000000</f>
+        <v>13913043478.260872</v>
+      </c>
+      <c r="P4" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1790,8 +1864,18 @@
       <c r="N5" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="66">
+        <f>O4</f>
+        <v>13913043478.260872</v>
+      </c>
+      <c r="P5" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -1836,8 +1920,17 @@
       <c r="N6" s="40" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="66">
+        <v>1093000</v>
+      </c>
+      <c r="P6" t="s">
+        <v>308</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1882,8 +1975,15 @@
       <c r="N7" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="66">
+        <f>198000*1000000</f>
+        <v>198000000000</v>
+      </c>
+      <c r="P7" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -1928,8 +2028,15 @@
       <c r="N8" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="66">
+        <f>198000*1000000</f>
+        <v>198000000000</v>
+      </c>
+      <c r="P8" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -1972,8 +2079,18 @@
       <c r="N9" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="66">
+        <f>$O$4</f>
+        <v>13913043478.260872</v>
+      </c>
+      <c r="P9" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2016,8 +2133,18 @@
       <c r="N10" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="66">
+        <f t="shared" ref="O10:O12" si="3">$O$4</f>
+        <v>13913043478.260872</v>
+      </c>
+      <c r="P10" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2059,8 +2186,18 @@
       <c r="N11" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="66">
+        <f t="shared" si="3"/>
+        <v>13913043478.260872</v>
+      </c>
+      <c r="P11" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2102,8 +2239,18 @@
       <c r="N12" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="66">
+        <f t="shared" si="3"/>
+        <v>13913043478.260872</v>
+      </c>
+      <c r="P12" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>285</v>
       </c>
@@ -2144,8 +2291,18 @@
       <c r="N13" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="66">
+        <f>37*1000*1000000</f>
+        <v>37000000000</v>
+      </c>
+      <c r="P13" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2183,8 +2340,18 @@
       <c r="M14" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O14" s="66">
+        <f t="shared" ref="O14:O15" si="4">198000*1000000</f>
+        <v>198000000000</v>
+      </c>
+      <c r="P14" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2222,8 +2389,18 @@
       <c r="M15" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O15" s="66">
+        <f t="shared" si="4"/>
+        <v>198000000000</v>
+      </c>
+      <c r="P15" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -9195,8 +9372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FEFDD9-D46C-E64E-8B04-7DDDC1C1B0F3}">
   <dimension ref="A1:AA16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new architecture file and output
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://randus-my.sharepoint.com/personal/jrojasa_rand_org/Documents/Documents/GitHub/SJV-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{57264FF7-3F4E-4535-B290-568E489A1A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5AF5106E-B93D-4C0E-A2F8-E4AB0F46FD4D}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="13_ncr:1_{57264FF7-3F4E-4535-B290-568E489A1A4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07EE4A24-7C2C-464A-91CB-2022906A8536}"/>
   <bookViews>
-    <workbookView xWindow="-7860" yWindow="-16297" windowWidth="28995" windowHeight="15794" tabRatio="622" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="622" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -19,25 +19,26 @@
     <sheet name="C2U UO Adjustment" sheetId="17" r:id="rId4"/>
     <sheet name="C2U CI" sheetId="10" r:id="rId5"/>
     <sheet name="F2C Water" sheetId="13" r:id="rId6"/>
-    <sheet name="F2C Jobs" sheetId="11" r:id="rId7"/>
-    <sheet name="Infrastructure" sheetId="19" r:id="rId8"/>
-    <sheet name="Unit Conversion" sheetId="18" r:id="rId9"/>
-    <sheet name="Conversion" sheetId="15" r:id="rId10"/>
-    <sheet name="Feedstock to Commodity Buildout" sheetId="7" r:id="rId11"/>
-    <sheet name="Commodity to Use Buildout" sheetId="8" r:id="rId12"/>
-    <sheet name="F2C_ver2" sheetId="20" r:id="rId13"/>
-    <sheet name="Commodity To Use Matrix" sheetId="6" r:id="rId14"/>
-    <sheet name="table from Julia (to be deleted" sheetId="16" r:id="rId15"/>
-    <sheet name="Feedstock to Commodity Matrix" sheetId="4" r:id="rId16"/>
+    <sheet name="F2C Jobs" sheetId="23" r:id="rId7"/>
+    <sheet name="F2C Jobs old" sheetId="11" r:id="rId8"/>
+    <sheet name="Infrastructure" sheetId="19" r:id="rId9"/>
+    <sheet name="Unit Conversion" sheetId="18" r:id="rId10"/>
+    <sheet name="Conversion" sheetId="15" r:id="rId11"/>
+    <sheet name="Feedstock to Commodity Buildout" sheetId="7" r:id="rId12"/>
+    <sheet name="Commodity to Use Buildout" sheetId="8" r:id="rId13"/>
+    <sheet name="F2C_ver2" sheetId="20" r:id="rId14"/>
+    <sheet name="Commodity To Use Matrix" sheetId="6" r:id="rId15"/>
+    <sheet name="table from Julia (to be deleted" sheetId="16" r:id="rId16"/>
+    <sheet name="Feedstock to Commodity Matrix" sheetId="4" r:id="rId17"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'C2U CI'!$A$1:$AA$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'F2C CI'!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'F2C Conversion'!$A$1:$Q$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'F2C Jobs'!$A$1:$J$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'F2C Jobs old'!$A$1:$J$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'F2C Land'!$A$1:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'F2C Water'!$A$19:$L$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Unit Conversion'!$A$1:$AK$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Unit Conversion'!$A$1:$AK$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1937" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2320" uniqueCount="334">
   <si>
     <t>Feedstock</t>
   </si>
@@ -1002,6 +1003,72 @@
   </si>
   <si>
     <t>Animal Fats</t>
+  </si>
+  <si>
+    <t>Mil Ft3/day</t>
+  </si>
+  <si>
+    <t>Bil. BTU</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Type of Energy</t>
+  </si>
+  <si>
+    <t>Electrons</t>
+  </si>
+  <si>
+    <t>Molecules</t>
+  </si>
+  <si>
+    <t>Unit Greg</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>tural Gas + CCS</t>
+  </si>
+  <si>
+    <t>Sustaible Aviation Fuel</t>
+  </si>
+  <si>
+    <t>Technology</t>
+  </si>
+  <si>
+    <t>Utility Solar</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>Indirect</t>
+  </si>
+  <si>
+    <t>Induced</t>
+  </si>
+  <si>
+    <t>Biomass Electric</t>
+  </si>
+  <si>
+    <t>Electrolysis Hydrogen</t>
+  </si>
+  <si>
+    <t>SMR Hydrogen (Blue)</t>
+  </si>
+  <si>
+    <t>Woody Biomass/Cellulosic Biofuel</t>
+  </si>
+  <si>
+    <t>SMR Hydrogen</t>
+  </si>
+  <si>
+    <t>Other Ethanol/Non-Woody Biomass Fuel</t>
   </si>
 </sst>
 </file>
@@ -1196,7 +1263,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1296,6 +1363,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1614,7 +1682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CE3E66E-8E4F-4F0F-BF6D-3E16E49004F7}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+    <sheetView zoomScale="107" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -2494,6 +2562,1291 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA5616B-DF07-465E-AEEB-CCA6D05FE697}">
+  <dimension ref="A1:AK23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.75" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="15.25" customWidth="1"/>
+    <col min="6" max="6" width="11.08203125" customWidth="1"/>
+    <col min="7" max="7" width="17.75" customWidth="1"/>
+    <col min="8" max="8" width="10.5" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="43.5" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.08203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.5" customWidth="1"/>
+    <col min="16" max="16" width="31.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" t="s">
+        <v>105</v>
+      </c>
+      <c r="F1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G1" t="s">
+        <v>107</v>
+      </c>
+      <c r="H1" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" t="s">
+        <v>109</v>
+      </c>
+      <c r="K1" t="s">
+        <v>110</v>
+      </c>
+      <c r="L1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N1" t="s">
+        <v>251</v>
+      </c>
+      <c r="O1" t="s">
+        <v>111</v>
+      </c>
+      <c r="P1" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q1">
+        <v>2025</v>
+      </c>
+      <c r="R1">
+        <v>2026</v>
+      </c>
+      <c r="S1">
+        <v>2027</v>
+      </c>
+      <c r="T1">
+        <v>2028</v>
+      </c>
+      <c r="U1">
+        <v>2029</v>
+      </c>
+      <c r="V1">
+        <v>2030</v>
+      </c>
+      <c r="W1">
+        <v>2031</v>
+      </c>
+      <c r="X1">
+        <v>2032</v>
+      </c>
+      <c r="Y1">
+        <v>2033</v>
+      </c>
+      <c r="Z1">
+        <v>2034</v>
+      </c>
+      <c r="AA1">
+        <v>2035</v>
+      </c>
+      <c r="AB1">
+        <v>2036</v>
+      </c>
+      <c r="AC1">
+        <v>2037</v>
+      </c>
+      <c r="AD1">
+        <v>2038</v>
+      </c>
+      <c r="AE1">
+        <v>2039</v>
+      </c>
+      <c r="AF1">
+        <v>2040</v>
+      </c>
+      <c r="AG1">
+        <v>2041</v>
+      </c>
+      <c r="AH1">
+        <v>2042</v>
+      </c>
+      <c r="AI1">
+        <v>2043</v>
+      </c>
+      <c r="AJ1">
+        <v>2044</v>
+      </c>
+      <c r="AK1">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="5">
+        <f>G2*1000000000000</f>
+        <v>3599.8225679871703</v>
+      </c>
+      <c r="F2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" s="37">
+        <v>3.5998225679871703E-9</v>
+      </c>
+      <c r="H2" t="s">
+        <v>116</v>
+      </c>
+      <c r="P2" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>2294.03577178978</v>
+      </c>
+      <c r="R2" s="5">
+        <v>2240.1604058664384</v>
+      </c>
+      <c r="S2" s="5">
+        <v>2186.2850399430968</v>
+      </c>
+      <c r="T2" s="5">
+        <v>2132.4096740197551</v>
+      </c>
+      <c r="U2" s="5">
+        <v>2078.5343080964135</v>
+      </c>
+      <c r="V2" s="5">
+        <v>2024.6589421730721</v>
+      </c>
+      <c r="W2" s="5">
+        <v>1970.7835762497307</v>
+      </c>
+      <c r="X2" s="5">
+        <v>1916.9082103263893</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>1863.0328444030479</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>1809.1574784797065</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>1755.2821125563651</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>1701.4067466330237</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>1647.5313807096823</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>1593.6560147863408</v>
+      </c>
+      <c r="AE2" s="5">
+        <v>1539.7806488629994</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>1485.905282939658</v>
+      </c>
+      <c r="AG2" s="5">
+        <v>1432.0299170163166</v>
+      </c>
+      <c r="AH2" s="5">
+        <v>1378.1545510929752</v>
+      </c>
+      <c r="AI2" s="5">
+        <v>1324.2791851696338</v>
+      </c>
+      <c r="AJ2" s="5">
+        <v>1270.4038192462924</v>
+      </c>
+      <c r="AK2" s="5">
+        <v>1216.528453322951</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E17" si="0">G3*1000000000000</f>
+        <v>119999.99999999999</v>
+      </c>
+      <c r="F3" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1.1999999999999999E-7</v>
+      </c>
+      <c r="H3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" s="41">
+        <v>0.64900000000000002</v>
+      </c>
+      <c r="J3">
+        <v>51.3</v>
+      </c>
+      <c r="K3" s="41" t="s">
+        <v>122</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="O3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
+        <v>3599.8225679871703</v>
+      </c>
+      <c r="F4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G4" s="37">
+        <v>3.5998225679871703E-9</v>
+      </c>
+      <c r="H4" t="s">
+        <v>116</v>
+      </c>
+      <c r="P4" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>2502.8086901013899</v>
+      </c>
+      <c r="R4" s="5">
+        <v>2482.7671254296229</v>
+      </c>
+      <c r="S4" s="5">
+        <v>2462.7255607578559</v>
+      </c>
+      <c r="T4" s="5">
+        <v>2442.6839960860889</v>
+      </c>
+      <c r="U4" s="5">
+        <v>2422.6424314143219</v>
+      </c>
+      <c r="V4" s="5">
+        <v>2402.6008667425549</v>
+      </c>
+      <c r="W4" s="5">
+        <v>2382.5593020707879</v>
+      </c>
+      <c r="X4" s="5">
+        <v>2362.5177373990209</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>2342.4761727272539</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>2322.4346080554869</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>2302.3930433837199</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>2282.351478711953</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>2262.309914040186</v>
+      </c>
+      <c r="AD4" s="5">
+        <v>2242.268349368419</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>2222.226784696652</v>
+      </c>
+      <c r="AF4" s="5">
+        <v>2202.185220024885</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>2182.143655353118</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>2162.102090681351</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>2142.060526009584</v>
+      </c>
+      <c r="AJ4" s="5">
+        <v>2122.018961337817</v>
+      </c>
+      <c r="AK4" s="5">
+        <v>2101.97739666605</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>3599.8225679871703</v>
+      </c>
+      <c r="F5" t="s">
+        <v>115</v>
+      </c>
+      <c r="G5" s="37">
+        <v>3.5998225679871703E-9</v>
+      </c>
+      <c r="H5" t="s">
+        <v>116</v>
+      </c>
+      <c r="P5" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="R5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="S5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="T5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="U5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="V5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="W5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="X5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="AD5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="AE5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="AF5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="AG5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="AH5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="AI5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="AJ5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+      <c r="AK5" s="5">
+        <v>1171.0983188067505</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>3599.8225679871703</v>
+      </c>
+      <c r="F6" t="s">
+        <v>115</v>
+      </c>
+      <c r="G6" s="37">
+        <v>3.5998225679871703E-9</v>
+      </c>
+      <c r="H6" t="s">
+        <v>116</v>
+      </c>
+      <c r="P6" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>1670.82114582243</v>
+      </c>
+      <c r="R6" s="5">
+        <v>1698.006304040191</v>
+      </c>
+      <c r="S6" s="5">
+        <v>1725.191462257952</v>
+      </c>
+      <c r="T6" s="5">
+        <v>1752.376620475713</v>
+      </c>
+      <c r="U6" s="5">
+        <v>1779.561778693474</v>
+      </c>
+      <c r="V6" s="5">
+        <v>1806.746936911235</v>
+      </c>
+      <c r="W6" s="5">
+        <v>1833.932095128996</v>
+      </c>
+      <c r="X6" s="5">
+        <v>1861.117253346757</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>1888.302411564518</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>1915.487569782279</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>1942.67272800004</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>1969.857886217801</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>1997.043044435562</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>2024.228202653323</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>2051.413360871084</v>
+      </c>
+      <c r="AF6" s="5">
+        <v>2078.598519088845</v>
+      </c>
+      <c r="AG6" s="5">
+        <v>2105.783677306606</v>
+      </c>
+      <c r="AH6" s="5">
+        <v>2132.968835524367</v>
+      </c>
+      <c r="AI6" s="5">
+        <v>2160.153993742128</v>
+      </c>
+      <c r="AJ6" s="5">
+        <v>2187.339151959889</v>
+      </c>
+      <c r="AK6" s="5">
+        <v>2214.52431017765</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="5">
+        <f>G7*1000000000000</f>
+        <v>3599.8225679871703</v>
+      </c>
+      <c r="F7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="37">
+        <v>3.5998225679871703E-9</v>
+      </c>
+      <c r="H7" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="40">
+        <v>0.25</v>
+      </c>
+      <c r="J7" s="12"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7">
+        <v>19800</v>
+      </c>
+      <c r="N7" t="s">
+        <v>125</v>
+      </c>
+      <c r="O7" t="s">
+        <v>126</v>
+      </c>
+      <c r="P7" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>6035.0858307307299</v>
+      </c>
+      <c r="R7" s="5">
+        <v>5991.4369513857655</v>
+      </c>
+      <c r="S7" s="5">
+        <v>5947.7880720408011</v>
+      </c>
+      <c r="T7" s="5">
+        <v>5904.1391926958368</v>
+      </c>
+      <c r="U7" s="5">
+        <v>5860.4903133508724</v>
+      </c>
+      <c r="V7" s="5">
+        <v>5816.841434005908</v>
+      </c>
+      <c r="W7" s="5">
+        <v>5773.1925546609436</v>
+      </c>
+      <c r="X7" s="5">
+        <v>5729.5436753159793</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>5685.8947959710149</v>
+      </c>
+      <c r="Z7" s="5">
+        <v>5642.2459166260505</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>5598.5970372810862</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>5554.9481579361218</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>5511.2992785911574</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>5467.650399246193</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>5424.0015199012287</v>
+      </c>
+      <c r="AF7" s="5">
+        <v>5380.3526405562643</v>
+      </c>
+      <c r="AG7" s="5">
+        <v>5336.7037612112999</v>
+      </c>
+      <c r="AH7" s="5">
+        <v>5293.0548818663356</v>
+      </c>
+      <c r="AI7" s="5">
+        <v>5249.4060025213712</v>
+      </c>
+      <c r="AJ7" s="5">
+        <v>5205.7571231764068</v>
+      </c>
+      <c r="AK7" s="5">
+        <v>5162.1082438314425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" t="s">
+        <v>114</v>
+      </c>
+      <c r="E8" s="5">
+        <f t="shared" ref="E8:E9" si="1">G8*1000000000000</f>
+        <v>3599.8225679871703</v>
+      </c>
+      <c r="F8" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="37">
+        <v>3.5998225679871703E-9</v>
+      </c>
+      <c r="H8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="40"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="40"/>
+      <c r="L8" s="40"/>
+      <c r="P8" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>6035.0858307307299</v>
+      </c>
+      <c r="R8" s="5">
+        <v>5991.4369513857655</v>
+      </c>
+      <c r="S8" s="5">
+        <v>5947.7880720408011</v>
+      </c>
+      <c r="T8" s="5">
+        <v>5904.1391926958368</v>
+      </c>
+      <c r="U8" s="5">
+        <v>5860.4903133508724</v>
+      </c>
+      <c r="V8" s="5">
+        <v>5816.841434005908</v>
+      </c>
+      <c r="W8" s="5">
+        <v>5773.1925546609436</v>
+      </c>
+      <c r="X8" s="5">
+        <v>5729.5436753159793</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>5685.8947959710149</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>5642.2459166260505</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>5598.5970372810862</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>5554.9481579361218</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>5511.2992785911574</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>5467.650399246193</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>5424.0015199012287</v>
+      </c>
+      <c r="AF8" s="5">
+        <v>5380.3526405562643</v>
+      </c>
+      <c r="AG8" s="5">
+        <v>5336.7037612112999</v>
+      </c>
+      <c r="AH8" s="5">
+        <v>5293.0548818663356</v>
+      </c>
+      <c r="AI8" s="5">
+        <v>5249.4060025213712</v>
+      </c>
+      <c r="AJ8" s="5">
+        <v>5205.7571231764068</v>
+      </c>
+      <c r="AK8" s="5">
+        <v>5162.1082438314425</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" si="1"/>
+        <v>3599.8225679871703</v>
+      </c>
+      <c r="F9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" s="37">
+        <v>3.5998225679871703E-9</v>
+      </c>
+      <c r="H9" t="s">
+        <v>116</v>
+      </c>
+      <c r="I9" s="40"/>
+      <c r="J9" s="12">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="K9" s="40" t="s">
+        <v>258</v>
+      </c>
+      <c r="L9" s="40"/>
+      <c r="P9" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>6035.0858307307299</v>
+      </c>
+      <c r="R9" s="5">
+        <v>5991.4369513857655</v>
+      </c>
+      <c r="S9" s="5">
+        <v>5947.7880720408011</v>
+      </c>
+      <c r="T9" s="5">
+        <v>5904.1391926958368</v>
+      </c>
+      <c r="U9" s="5">
+        <v>5860.4903133508724</v>
+      </c>
+      <c r="V9" s="5">
+        <v>5816.841434005908</v>
+      </c>
+      <c r="W9" s="5">
+        <v>5773.1925546609436</v>
+      </c>
+      <c r="X9" s="5">
+        <v>5729.5436753159793</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>5685.8947959710149</v>
+      </c>
+      <c r="Z9" s="5">
+        <v>5642.2459166260505</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>5598.5970372810862</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>5554.9481579361218</v>
+      </c>
+      <c r="AC9" s="5">
+        <v>5511.2992785911574</v>
+      </c>
+      <c r="AD9" s="5">
+        <v>5467.650399246193</v>
+      </c>
+      <c r="AE9" s="5">
+        <v>5424.0015199012287</v>
+      </c>
+      <c r="AF9" s="5">
+        <v>5380.3526405562643</v>
+      </c>
+      <c r="AG9" s="5">
+        <v>5336.7037612112999</v>
+      </c>
+      <c r="AH9" s="5">
+        <v>5293.0548818663356</v>
+      </c>
+      <c r="AI9" s="5">
+        <v>5249.4060025213712</v>
+      </c>
+      <c r="AJ9" s="5">
+        <v>5205.7571231764068</v>
+      </c>
+      <c r="AK9" s="5">
+        <v>5162.1082438314425</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" t="s">
+        <v>119</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>119999.99999999999</v>
+      </c>
+      <c r="F10" t="s">
+        <v>120</v>
+      </c>
+      <c r="G10">
+        <v>1.1999999999999999E-7</v>
+      </c>
+      <c r="H10" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" s="40">
+        <v>0.72</v>
+      </c>
+      <c r="J10">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="K10" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="L10" s="43" t="s">
+        <v>254</v>
+      </c>
+      <c r="O10" s="36" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" t="s">
+        <v>119</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" ref="E11" si="2">G11*1000000000000</f>
+        <v>119999.99999999999</v>
+      </c>
+      <c r="F11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G11">
+        <v>1.1999999999999999E-7</v>
+      </c>
+      <c r="H11" t="s">
+        <v>121</v>
+      </c>
+      <c r="I11" s="40"/>
+      <c r="J11" s="12">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="K11" s="40" t="s">
+        <v>127</v>
+      </c>
+      <c r="L11" s="43"/>
+      <c r="O11" s="36"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>119999.99999999999</v>
+      </c>
+      <c r="F12" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12">
+        <v>1.1999999999999999E-7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>121</v>
+      </c>
+      <c r="I12" s="40">
+        <v>0.44</v>
+      </c>
+      <c r="J12">
+        <v>13</v>
+      </c>
+      <c r="K12" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="L12" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="M12">
+        <v>19800</v>
+      </c>
+      <c r="N12" t="s">
+        <v>125</v>
+      </c>
+      <c r="O12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>119999.99999999999</v>
+      </c>
+      <c r="F13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13">
+        <v>1.1999999999999999E-7</v>
+      </c>
+      <c r="H13" t="s">
+        <v>121</v>
+      </c>
+      <c r="I13" s="40">
+        <v>0.44</v>
+      </c>
+      <c r="J13">
+        <v>13</v>
+      </c>
+      <c r="K13" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="L13" s="43" t="s">
+        <v>128</v>
+      </c>
+      <c r="M13">
+        <v>19800</v>
+      </c>
+      <c r="N13" t="s">
+        <v>125</v>
+      </c>
+      <c r="O13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D14" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
+        <v>1093000</v>
+      </c>
+      <c r="F14" t="s">
+        <v>133</v>
+      </c>
+      <c r="G14">
+        <v>1.093E-6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>134</v>
+      </c>
+      <c r="J14" s="12">
+        <v>50</v>
+      </c>
+      <c r="K14" s="40" t="s">
+        <v>257</v>
+      </c>
+      <c r="M14">
+        <v>19800</v>
+      </c>
+      <c r="N14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" t="s">
+        <v>132</v>
+      </c>
+      <c r="D15" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>1093000</v>
+      </c>
+      <c r="F15" t="s">
+        <v>133</v>
+      </c>
+      <c r="G15">
+        <v>1.093E-6</v>
+      </c>
+      <c r="H15" t="s">
+        <v>134</v>
+      </c>
+      <c r="J15" s="12">
+        <v>20000</v>
+      </c>
+      <c r="K15" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="M15">
+        <v>19800</v>
+      </c>
+      <c r="N15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" t="s">
+        <v>137</v>
+      </c>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>142432539.75000003</v>
+      </c>
+      <c r="F16" t="s">
+        <v>138</v>
+      </c>
+      <c r="G16">
+        <v>1.4243253975000002E-4</v>
+      </c>
+      <c r="H16" t="s">
+        <v>139</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1</v>
+      </c>
+      <c r="K16" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="L16" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>136</v>
+      </c>
+      <c r="D17" t="s">
+        <v>137</v>
+      </c>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>142432539.75000003</v>
+      </c>
+      <c r="F17" t="s">
+        <v>138</v>
+      </c>
+      <c r="G17">
+        <v>1.4243253975000002E-4</v>
+      </c>
+      <c r="H17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J17" s="12">
+        <v>1</v>
+      </c>
+      <c r="K17" s="40" t="s">
+        <v>249</v>
+      </c>
+      <c r="L17" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D18" t="s">
+        <v>137</v>
+      </c>
+      <c r="E18" s="5">
+        <f t="shared" ref="E18:E19" si="3">G18*1000000000000</f>
+        <v>142432539.75000003</v>
+      </c>
+      <c r="F18" t="s">
+        <v>138</v>
+      </c>
+      <c r="G18">
+        <v>1.4243253975000002E-4</v>
+      </c>
+      <c r="H18" t="s">
+        <v>139</v>
+      </c>
+      <c r="J18" s="5">
+        <v>16181.229773462785</v>
+      </c>
+      <c r="K18" s="40" t="s">
+        <v>248</v>
+      </c>
+      <c r="L18" t="s">
+        <v>252</v>
+      </c>
+      <c r="O18" s="53"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" t="s">
+        <v>137</v>
+      </c>
+      <c r="E19" s="5">
+        <f t="shared" si="3"/>
+        <v>142432539.75000003</v>
+      </c>
+      <c r="F19" t="s">
+        <v>138</v>
+      </c>
+      <c r="G19">
+        <v>1.4243253975000002E-4</v>
+      </c>
+      <c r="H19" t="s">
+        <v>139</v>
+      </c>
+      <c r="J19" s="5">
+        <v>14492.753623188406</v>
+      </c>
+      <c r="K19" s="40" t="s">
+        <v>248</v>
+      </c>
+      <c r="L19" t="s">
+        <v>253</v>
+      </c>
+      <c r="O19" s="53"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="L23">
+        <v>1000</v>
+      </c>
+      <c r="M23" t="s">
+        <v>255</v>
+      </c>
+      <c r="N23" t="s">
+        <v>256</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:AK1" xr:uid="{5FA5616B-DF07-465E-AEEB-CCA6D05FE697}"/>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="O10" r:id="rId1" display="https://netl.doe.gov/projects/files/ComparisonofCommercialStateofArtFossilBasedHydrogenProductionTechnologies_041222.pdf" xr:uid="{E7CB3D97-93CD-4126-9FFC-6A55103A1392}"/>
+    <hyperlink ref="L3" r:id="rId2" display="https://www.nrel.gov/docs/fy20osti/77198.pdf" xr:uid="{531AFCC0-D1CD-457F-9290-C08242A339AF}"/>
+    <hyperlink ref="L10" r:id="rId3" display="https://www.nrel.gov/docs/fy20osti/77198.pdf" xr:uid="{979EC4C4-9A4A-47DB-9CBE-1F560C4CD153}"/>
+    <hyperlink ref="L12" r:id="rId4" xr:uid="{C8959CBC-501D-4F10-AA88-D7CD003A447E}"/>
+    <hyperlink ref="L13" r:id="rId5" xr:uid="{A5DBCFA7-F634-44A5-B62E-436D59BDA540}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87BF8B-8E54-426F-864A-9E457E959B26}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
@@ -3208,7 +4561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4534657-2DF7-8944-A332-1622EE581035}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
@@ -4889,7 +6242,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3F942D-1725-B745-A61F-46451943A74C}">
   <dimension ref="A1:W6"/>
   <sheetViews>
@@ -5334,7 +6687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDDA0F3-A3DE-4AB4-98AB-8BE3425A27E0}">
   <dimension ref="A1:G30"/>
   <sheetViews>
@@ -5823,7 +7176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30085204-D4C6-FC4C-98EB-2FC1A2E0E66E}">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -5930,7 +7283,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF7B0DD-C673-4DCD-83AE-47E17C286F51}">
   <dimension ref="A1:K68"/>
   <sheetViews>
@@ -6812,7 +8165,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6977DE39-83AB-8346-8AC1-EC99E6C87D8C}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -6974,7 +8327,7 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -10846,8 +12199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C58C4D02-922E-2849-99A2-B5A24807FA42}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -11781,18 +13134,1567 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16BE7FC-A8FD-4D95-933D-26AA617CB019}">
+  <dimension ref="A1:K49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.9140625" customWidth="1"/>
+    <col min="7" max="7" width="10.25" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="11.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1" t="s">
+        <v>323</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>318</v>
+      </c>
+      <c r="H1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>319</v>
+      </c>
+      <c r="K1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>316</v>
+      </c>
+      <c r="D2" t="s">
+        <v>324</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" t="s">
+        <v>325</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H2" t="s">
+        <v>93</v>
+      </c>
+      <c r="I2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="J2">
+        <v>4.5152412959181799E-2</v>
+      </c>
+      <c r="K2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" t="s">
+        <v>324</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" t="s">
+        <v>326</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" t="s">
+        <v>93</v>
+      </c>
+      <c r="I3">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="J3">
+        <v>4.5152412959181799E-2</v>
+      </c>
+      <c r="K3">
+        <v>9.6900000000000007E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>316</v>
+      </c>
+      <c r="D4" t="s">
+        <v>324</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>327</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="J4">
+        <v>4.5152412959181799E-2</v>
+      </c>
+      <c r="K4">
+        <v>1.6320000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>316</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" t="s">
+        <v>325</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H5" t="s">
+        <v>93</v>
+      </c>
+      <c r="I5">
+        <v>2E-3</v>
+      </c>
+      <c r="J5">
+        <v>8.3034948476273795E-3</v>
+      </c>
+      <c r="K5" s="67">
+        <v>1.84331098696461</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" t="s">
+        <v>326</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" t="s">
+        <v>93</v>
+      </c>
+      <c r="I6">
+        <v>2E-3</v>
+      </c>
+      <c r="J6">
+        <v>8.3034948476273795E-3</v>
+      </c>
+      <c r="K6" s="67">
+        <v>0.44239463687150798</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>316</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" t="s">
+        <v>327</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7">
+        <v>2E-3</v>
+      </c>
+      <c r="J7">
+        <v>8.3034948476273795E-3</v>
+      </c>
+      <c r="K7">
+        <v>0.60829262569832399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" t="s">
+        <v>325</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" t="s">
+        <v>93</v>
+      </c>
+      <c r="I8">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="J8">
+        <v>3.7832039152811102E-2</v>
+      </c>
+      <c r="K8">
+        <v>0.78800000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>316</v>
+      </c>
+      <c r="D9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9" t="s">
+        <v>326</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H9" t="s">
+        <v>93</v>
+      </c>
+      <c r="I9">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="J9">
+        <v>3.7832039152811102E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>316</v>
+      </c>
+      <c r="D10" t="s">
+        <v>145</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10" t="s">
+        <v>327</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H10" t="s">
+        <v>93</v>
+      </c>
+      <c r="I10">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="J10">
+        <v>3.7832039152811102E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>316</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="H11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>316</v>
+      </c>
+      <c r="E12" t="s">
+        <v>91</v>
+      </c>
+      <c r="H12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>316</v>
+      </c>
+      <c r="E13" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>316</v>
+      </c>
+      <c r="D14" t="s">
+        <v>328</v>
+      </c>
+      <c r="E14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" t="s">
+        <v>325</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H14" t="s">
+        <v>93</v>
+      </c>
+      <c r="I14">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J14" s="67">
+        <v>1.1585743964712399E-2</v>
+      </c>
+      <c r="K14" s="67">
+        <v>4.9924583333333299</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>316</v>
+      </c>
+      <c r="D15" t="s">
+        <v>328</v>
+      </c>
+      <c r="E15" t="s">
+        <v>91</v>
+      </c>
+      <c r="F15" t="s">
+        <v>326</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I15">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J15" s="67">
+        <v>1.1585743964712399E-2</v>
+      </c>
+      <c r="K15" s="67">
+        <v>1.29803916666666</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>316</v>
+      </c>
+      <c r="D16" t="s">
+        <v>328</v>
+      </c>
+      <c r="E16" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" t="s">
+        <v>327</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H16" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J16" s="67">
+        <v>1.1585743964712399E-2</v>
+      </c>
+      <c r="K16" s="67">
+        <v>1.7473604166666601</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>316</v>
+      </c>
+      <c r="D17" t="s">
+        <v>328</v>
+      </c>
+      <c r="E17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F17" t="s">
+        <v>325</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" t="s">
+        <v>93</v>
+      </c>
+      <c r="I17">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J17" s="67">
+        <v>1.1585743964712399E-2</v>
+      </c>
+      <c r="K17" s="67">
+        <v>4.9924583333333299</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>316</v>
+      </c>
+      <c r="D18" t="s">
+        <v>328</v>
+      </c>
+      <c r="E18" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" t="s">
+        <v>326</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H18" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J18" s="67">
+        <v>1.1585743964712399E-2</v>
+      </c>
+      <c r="K18" s="67">
+        <v>1.29803916666666</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>316</v>
+      </c>
+      <c r="D19" t="s">
+        <v>328</v>
+      </c>
+      <c r="E19" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" t="s">
+        <v>327</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="H19" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="J19" s="67">
+        <v>1.1585743964712399E-2</v>
+      </c>
+      <c r="K19" s="67">
+        <v>1.7473604166666601</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>317</v>
+      </c>
+      <c r="D20" t="s">
+        <v>329</v>
+      </c>
+      <c r="E20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F20" t="s">
+        <v>325</v>
+      </c>
+      <c r="H20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>317</v>
+      </c>
+      <c r="D21" t="s">
+        <v>329</v>
+      </c>
+      <c r="E21" t="s">
+        <v>91</v>
+      </c>
+      <c r="F21" t="s">
+        <v>326</v>
+      </c>
+      <c r="H21" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>317</v>
+      </c>
+      <c r="D22" t="s">
+        <v>329</v>
+      </c>
+      <c r="E22" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" t="s">
+        <v>327</v>
+      </c>
+      <c r="H22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>321</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>317</v>
+      </c>
+      <c r="D23" t="s">
+        <v>330</v>
+      </c>
+      <c r="E23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F23" t="s">
+        <v>325</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="H23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>321</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>317</v>
+      </c>
+      <c r="D24" t="s">
+        <v>330</v>
+      </c>
+      <c r="E24" t="s">
+        <v>91</v>
+      </c>
+      <c r="F24" t="s">
+        <v>326</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="H24" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>321</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>317</v>
+      </c>
+      <c r="D25" t="s">
+        <v>330</v>
+      </c>
+      <c r="E25" t="s">
+        <v>91</v>
+      </c>
+      <c r="F25" t="s">
+        <v>327</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="H25" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>317</v>
+      </c>
+      <c r="D26" t="s">
+        <v>331</v>
+      </c>
+      <c r="E26" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" t="s">
+        <v>325</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="H26" t="s">
+        <v>93</v>
+      </c>
+      <c r="I26">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J26">
+        <v>2.8358342136926399E-2</v>
+      </c>
+      <c r="K26">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>317</v>
+      </c>
+      <c r="D27" t="s">
+        <v>331</v>
+      </c>
+      <c r="E27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F27" t="s">
+        <v>326</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="H27" t="s">
+        <v>93</v>
+      </c>
+      <c r="I27">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J27">
+        <v>2.8358342136926399E-2</v>
+      </c>
+      <c r="K27" s="67">
+        <v>2.8080000000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>317</v>
+      </c>
+      <c r="D28" t="s">
+        <v>331</v>
+      </c>
+      <c r="E28" t="s">
+        <v>91</v>
+      </c>
+      <c r="F28" t="s">
+        <v>327</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="H28" t="s">
+        <v>93</v>
+      </c>
+      <c r="I28">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J28">
+        <v>2.8358342136926399E-2</v>
+      </c>
+      <c r="K28">
+        <v>5.6160000000000002E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>317</v>
+      </c>
+      <c r="D29" t="s">
+        <v>331</v>
+      </c>
+      <c r="E29" t="s">
+        <v>91</v>
+      </c>
+      <c r="F29" t="s">
+        <v>325</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="H29" t="s">
+        <v>93</v>
+      </c>
+      <c r="I29">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J29">
+        <v>2.8358342136926399E-2</v>
+      </c>
+      <c r="K29">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" t="s">
+        <v>317</v>
+      </c>
+      <c r="D30" t="s">
+        <v>331</v>
+      </c>
+      <c r="E30" t="s">
+        <v>91</v>
+      </c>
+      <c r="F30" t="s">
+        <v>326</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="H30" t="s">
+        <v>93</v>
+      </c>
+      <c r="I30">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J30">
+        <v>2.8358342136926399E-2</v>
+      </c>
+      <c r="K30" s="67">
+        <v>2.8080000000000001E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B31" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" t="s">
+        <v>317</v>
+      </c>
+      <c r="D31" t="s">
+        <v>331</v>
+      </c>
+      <c r="E31" t="s">
+        <v>91</v>
+      </c>
+      <c r="F31" t="s">
+        <v>327</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="H31" t="s">
+        <v>93</v>
+      </c>
+      <c r="I31">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J31">
+        <v>2.8358342136926399E-2</v>
+      </c>
+      <c r="K31">
+        <v>5.6160000000000002E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>317</v>
+      </c>
+      <c r="D32" t="s">
+        <v>332</v>
+      </c>
+      <c r="E32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F32" t="s">
+        <v>325</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="H32" t="s">
+        <v>93</v>
+      </c>
+      <c r="I32">
+        <v>10.436</v>
+      </c>
+      <c r="J32">
+        <v>2.8358342136926399E-2</v>
+      </c>
+      <c r="K32">
+        <v>10.436</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>317</v>
+      </c>
+      <c r="D33" t="s">
+        <v>332</v>
+      </c>
+      <c r="E33" t="s">
+        <v>91</v>
+      </c>
+      <c r="F33" t="s">
+        <v>326</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="H33" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33">
+        <v>10.436</v>
+      </c>
+      <c r="J33">
+        <v>2.8358342136926399E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" t="s">
+        <v>317</v>
+      </c>
+      <c r="D34" t="s">
+        <v>332</v>
+      </c>
+      <c r="E34" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" t="s">
+        <v>327</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="H34" t="s">
+        <v>93</v>
+      </c>
+      <c r="I34">
+        <v>10.436</v>
+      </c>
+      <c r="J34">
+        <v>2.8358342136926399E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>317</v>
+      </c>
+      <c r="D35" t="s">
+        <v>333</v>
+      </c>
+      <c r="E35" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" t="s">
+        <v>325</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="H35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" t="s">
+        <v>317</v>
+      </c>
+      <c r="D36" t="s">
+        <v>333</v>
+      </c>
+      <c r="E36" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" t="s">
+        <v>326</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="H36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>317</v>
+      </c>
+      <c r="D37" t="s">
+        <v>333</v>
+      </c>
+      <c r="E37" t="s">
+        <v>91</v>
+      </c>
+      <c r="F37" t="s">
+        <v>327</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="H37" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" t="s">
+        <v>317</v>
+      </c>
+      <c r="D38" t="s">
+        <v>333</v>
+      </c>
+      <c r="E38" t="s">
+        <v>91</v>
+      </c>
+      <c r="F38" t="s">
+        <v>325</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="H38" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>44</v>
+      </c>
+      <c r="B39" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>317</v>
+      </c>
+      <c r="D39" t="s">
+        <v>333</v>
+      </c>
+      <c r="E39" t="s">
+        <v>91</v>
+      </c>
+      <c r="F39" t="s">
+        <v>326</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="H39" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>317</v>
+      </c>
+      <c r="D40" t="s">
+        <v>333</v>
+      </c>
+      <c r="E40" t="s">
+        <v>91</v>
+      </c>
+      <c r="F40" t="s">
+        <v>327</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="H40" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" t="s">
+        <v>322</v>
+      </c>
+      <c r="C41" t="s">
+        <v>317</v>
+      </c>
+      <c r="D41" t="s">
+        <v>333</v>
+      </c>
+      <c r="E41" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" t="s">
+        <v>325</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="H41" t="s">
+        <v>93</v>
+      </c>
+      <c r="I41">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J41">
+        <v>2.8358342136926399E-2</v>
+      </c>
+      <c r="K41">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" t="s">
+        <v>322</v>
+      </c>
+      <c r="C42" t="s">
+        <v>317</v>
+      </c>
+      <c r="D42" t="s">
+        <v>333</v>
+      </c>
+      <c r="E42" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" t="s">
+        <v>326</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="H42" t="s">
+        <v>93</v>
+      </c>
+      <c r="I42">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J42">
+        <v>2.8358342136926399E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" t="s">
+        <v>322</v>
+      </c>
+      <c r="C43" t="s">
+        <v>317</v>
+      </c>
+      <c r="D43" t="s">
+        <v>333</v>
+      </c>
+      <c r="E43" t="s">
+        <v>91</v>
+      </c>
+      <c r="F43" t="s">
+        <v>327</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>314</v>
+      </c>
+      <c r="H43" t="s">
+        <v>93</v>
+      </c>
+      <c r="I43">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J43">
+        <v>2.8358342136926399E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" t="s">
+        <v>322</v>
+      </c>
+      <c r="C44" t="s">
+        <v>317</v>
+      </c>
+      <c r="D44" t="s">
+        <v>331</v>
+      </c>
+      <c r="E44" t="s">
+        <v>91</v>
+      </c>
+      <c r="F44" t="s">
+        <v>325</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="H44" t="s">
+        <v>93</v>
+      </c>
+      <c r="I44">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J44">
+        <v>2.8358342136926399E-2</v>
+      </c>
+      <c r="K44">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>37</v>
+      </c>
+      <c r="B45" t="s">
+        <v>322</v>
+      </c>
+      <c r="C45" t="s">
+        <v>317</v>
+      </c>
+      <c r="D45" t="s">
+        <v>331</v>
+      </c>
+      <c r="E45" t="s">
+        <v>91</v>
+      </c>
+      <c r="F45" t="s">
+        <v>326</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="H45" t="s">
+        <v>93</v>
+      </c>
+      <c r="I45">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J45">
+        <v>2.8358342136926399E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" t="s">
+        <v>322</v>
+      </c>
+      <c r="C46" t="s">
+        <v>317</v>
+      </c>
+      <c r="D46" t="s">
+        <v>331</v>
+      </c>
+      <c r="E46" t="s">
+        <v>91</v>
+      </c>
+      <c r="F46" t="s">
+        <v>327</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="H46" t="s">
+        <v>93</v>
+      </c>
+      <c r="I46">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J46">
+        <v>2.8358342136926399E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" t="s">
+        <v>322</v>
+      </c>
+      <c r="C47" t="s">
+        <v>317</v>
+      </c>
+      <c r="D47" t="s">
+        <v>331</v>
+      </c>
+      <c r="E47" t="s">
+        <v>91</v>
+      </c>
+      <c r="F47" t="s">
+        <v>325</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="H47" t="s">
+        <v>93</v>
+      </c>
+      <c r="I47">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J47">
+        <v>2.8358342136926399E-2</v>
+      </c>
+      <c r="K47">
+        <v>0.23400000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B48" t="s">
+        <v>322</v>
+      </c>
+      <c r="C48" t="s">
+        <v>317</v>
+      </c>
+      <c r="D48" t="s">
+        <v>331</v>
+      </c>
+      <c r="E48" t="s">
+        <v>91</v>
+      </c>
+      <c r="F48" t="s">
+        <v>326</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="H48" t="s">
+        <v>93</v>
+      </c>
+      <c r="I48">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J48">
+        <v>2.8358342136926399E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>36</v>
+      </c>
+      <c r="B49" t="s">
+        <v>322</v>
+      </c>
+      <c r="C49" t="s">
+        <v>317</v>
+      </c>
+      <c r="D49" t="s">
+        <v>331</v>
+      </c>
+      <c r="E49" t="s">
+        <v>91</v>
+      </c>
+      <c r="F49" t="s">
+        <v>327</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="H49" t="s">
+        <v>93</v>
+      </c>
+      <c r="I49">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="J49">
+        <v>2.8358342136926399E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86CE6374-45B2-3044-B48D-E84DB83BCE11}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
-    <col min="7" max="8" width="24.08203125" customWidth="1"/>
+    <col min="1" max="1" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -12072,12 +14974,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J13" xr:uid="{86CE6374-45B2-3044-B48D-E84DB83BCE11}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBD7D08-7196-4DD6-A58C-02D5A271324B}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -12140,1291 +15041,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA5616B-DF07-465E-AEEB-CCA6D05FE697}">
-  <dimension ref="A1:AK23"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="20.58203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.75" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="15.25" customWidth="1"/>
-    <col min="6" max="6" width="11.08203125" customWidth="1"/>
-    <col min="7" max="7" width="17.75" customWidth="1"/>
-    <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="43.5" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="19.08203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="10.5" customWidth="1"/>
-    <col min="16" max="16" width="31.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" t="s">
-        <v>107</v>
-      </c>
-      <c r="H1" t="s">
-        <v>99</v>
-      </c>
-      <c r="I1" t="s">
-        <v>108</v>
-      </c>
-      <c r="J1" t="s">
-        <v>109</v>
-      </c>
-      <c r="K1" t="s">
-        <v>110</v>
-      </c>
-      <c r="L1" t="s">
-        <v>111</v>
-      </c>
-      <c r="M1" t="s">
-        <v>250</v>
-      </c>
-      <c r="N1" t="s">
-        <v>251</v>
-      </c>
-      <c r="O1" t="s">
-        <v>111</v>
-      </c>
-      <c r="P1" t="s">
-        <v>112</v>
-      </c>
-      <c r="Q1">
-        <v>2025</v>
-      </c>
-      <c r="R1">
-        <v>2026</v>
-      </c>
-      <c r="S1">
-        <v>2027</v>
-      </c>
-      <c r="T1">
-        <v>2028</v>
-      </c>
-      <c r="U1">
-        <v>2029</v>
-      </c>
-      <c r="V1">
-        <v>2030</v>
-      </c>
-      <c r="W1">
-        <v>2031</v>
-      </c>
-      <c r="X1">
-        <v>2032</v>
-      </c>
-      <c r="Y1">
-        <v>2033</v>
-      </c>
-      <c r="Z1">
-        <v>2034</v>
-      </c>
-      <c r="AA1">
-        <v>2035</v>
-      </c>
-      <c r="AB1">
-        <v>2036</v>
-      </c>
-      <c r="AC1">
-        <v>2037</v>
-      </c>
-      <c r="AD1">
-        <v>2038</v>
-      </c>
-      <c r="AE1">
-        <v>2039</v>
-      </c>
-      <c r="AF1">
-        <v>2040</v>
-      </c>
-      <c r="AG1">
-        <v>2041</v>
-      </c>
-      <c r="AH1">
-        <v>2042</v>
-      </c>
-      <c r="AI1">
-        <v>2043</v>
-      </c>
-      <c r="AJ1">
-        <v>2044</v>
-      </c>
-      <c r="AK1">
-        <v>2045</v>
-      </c>
-    </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E2" s="5">
-        <f>G2*1000000000000</f>
-        <v>3599.8225679871703</v>
-      </c>
-      <c r="F2" t="s">
-        <v>115</v>
-      </c>
-      <c r="G2" s="37">
-        <v>3.5998225679871703E-9</v>
-      </c>
-      <c r="H2" t="s">
-        <v>116</v>
-      </c>
-      <c r="P2" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q2" s="5">
-        <v>2294.03577178978</v>
-      </c>
-      <c r="R2" s="5">
-        <v>2240.1604058664384</v>
-      </c>
-      <c r="S2" s="5">
-        <v>2186.2850399430968</v>
-      </c>
-      <c r="T2" s="5">
-        <v>2132.4096740197551</v>
-      </c>
-      <c r="U2" s="5">
-        <v>2078.5343080964135</v>
-      </c>
-      <c r="V2" s="5">
-        <v>2024.6589421730721</v>
-      </c>
-      <c r="W2" s="5">
-        <v>1970.7835762497307</v>
-      </c>
-      <c r="X2" s="5">
-        <v>1916.9082103263893</v>
-      </c>
-      <c r="Y2" s="5">
-        <v>1863.0328444030479</v>
-      </c>
-      <c r="Z2" s="5">
-        <v>1809.1574784797065</v>
-      </c>
-      <c r="AA2" s="5">
-        <v>1755.2821125563651</v>
-      </c>
-      <c r="AB2" s="5">
-        <v>1701.4067466330237</v>
-      </c>
-      <c r="AC2" s="5">
-        <v>1647.5313807096823</v>
-      </c>
-      <c r="AD2" s="5">
-        <v>1593.6560147863408</v>
-      </c>
-      <c r="AE2" s="5">
-        <v>1539.7806488629994</v>
-      </c>
-      <c r="AF2" s="5">
-        <v>1485.905282939658</v>
-      </c>
-      <c r="AG2" s="5">
-        <v>1432.0299170163166</v>
-      </c>
-      <c r="AH2" s="5">
-        <v>1378.1545510929752</v>
-      </c>
-      <c r="AI2" s="5">
-        <v>1324.2791851696338</v>
-      </c>
-      <c r="AJ2" s="5">
-        <v>1270.4038192462924</v>
-      </c>
-      <c r="AK2" s="5">
-        <v>1216.528453322951</v>
-      </c>
-    </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="5">
-        <f t="shared" ref="E3:E17" si="0">G3*1000000000000</f>
-        <v>119999.99999999999</v>
-      </c>
-      <c r="F3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G3" s="7">
-        <v>1.1999999999999999E-7</v>
-      </c>
-      <c r="H3" t="s">
-        <v>121</v>
-      </c>
-      <c r="I3" s="41">
-        <v>0.64900000000000002</v>
-      </c>
-      <c r="J3">
-        <v>51.3</v>
-      </c>
-      <c r="K3" s="41" t="s">
-        <v>122</v>
-      </c>
-      <c r="L3" s="42" t="s">
-        <v>123</v>
-      </c>
-      <c r="O3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E4" s="5">
-        <f t="shared" si="0"/>
-        <v>3599.8225679871703</v>
-      </c>
-      <c r="F4" t="s">
-        <v>115</v>
-      </c>
-      <c r="G4" s="37">
-        <v>3.5998225679871703E-9</v>
-      </c>
-      <c r="H4" t="s">
-        <v>116</v>
-      </c>
-      <c r="P4" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>2502.8086901013899</v>
-      </c>
-      <c r="R4" s="5">
-        <v>2482.7671254296229</v>
-      </c>
-      <c r="S4" s="5">
-        <v>2462.7255607578559</v>
-      </c>
-      <c r="T4" s="5">
-        <v>2442.6839960860889</v>
-      </c>
-      <c r="U4" s="5">
-        <v>2422.6424314143219</v>
-      </c>
-      <c r="V4" s="5">
-        <v>2402.6008667425549</v>
-      </c>
-      <c r="W4" s="5">
-        <v>2382.5593020707879</v>
-      </c>
-      <c r="X4" s="5">
-        <v>2362.5177373990209</v>
-      </c>
-      <c r="Y4" s="5">
-        <v>2342.4761727272539</v>
-      </c>
-      <c r="Z4" s="5">
-        <v>2322.4346080554869</v>
-      </c>
-      <c r="AA4" s="5">
-        <v>2302.3930433837199</v>
-      </c>
-      <c r="AB4" s="5">
-        <v>2282.351478711953</v>
-      </c>
-      <c r="AC4" s="5">
-        <v>2262.309914040186</v>
-      </c>
-      <c r="AD4" s="5">
-        <v>2242.268349368419</v>
-      </c>
-      <c r="AE4" s="5">
-        <v>2222.226784696652</v>
-      </c>
-      <c r="AF4" s="5">
-        <v>2202.185220024885</v>
-      </c>
-      <c r="AG4" s="5">
-        <v>2182.143655353118</v>
-      </c>
-      <c r="AH4" s="5">
-        <v>2162.102090681351</v>
-      </c>
-      <c r="AI4" s="5">
-        <v>2142.060526009584</v>
-      </c>
-      <c r="AJ4" s="5">
-        <v>2122.018961337817</v>
-      </c>
-      <c r="AK4" s="5">
-        <v>2101.97739666605</v>
-      </c>
-    </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D5" t="s">
-        <v>114</v>
-      </c>
-      <c r="E5" s="5">
-        <f t="shared" si="0"/>
-        <v>3599.8225679871703</v>
-      </c>
-      <c r="F5" t="s">
-        <v>115</v>
-      </c>
-      <c r="G5" s="37">
-        <v>3.5998225679871703E-9</v>
-      </c>
-      <c r="H5" t="s">
-        <v>116</v>
-      </c>
-      <c r="P5" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="R5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="S5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="T5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="U5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="V5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="W5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="X5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="Y5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="Z5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="AA5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="AB5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="AC5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="AD5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="AE5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="AF5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="AG5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="AH5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="AI5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="AJ5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-      <c r="AK5" s="5">
-        <v>1171.0983188067505</v>
-      </c>
-    </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" t="s">
-        <v>114</v>
-      </c>
-      <c r="E6" s="5">
-        <f t="shared" si="0"/>
-        <v>3599.8225679871703</v>
-      </c>
-      <c r="F6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G6" s="37">
-        <v>3.5998225679871703E-9</v>
-      </c>
-      <c r="H6" t="s">
-        <v>116</v>
-      </c>
-      <c r="P6" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>1670.82114582243</v>
-      </c>
-      <c r="R6" s="5">
-        <v>1698.006304040191</v>
-      </c>
-      <c r="S6" s="5">
-        <v>1725.191462257952</v>
-      </c>
-      <c r="T6" s="5">
-        <v>1752.376620475713</v>
-      </c>
-      <c r="U6" s="5">
-        <v>1779.561778693474</v>
-      </c>
-      <c r="V6" s="5">
-        <v>1806.746936911235</v>
-      </c>
-      <c r="W6" s="5">
-        <v>1833.932095128996</v>
-      </c>
-      <c r="X6" s="5">
-        <v>1861.117253346757</v>
-      </c>
-      <c r="Y6" s="5">
-        <v>1888.302411564518</v>
-      </c>
-      <c r="Z6" s="5">
-        <v>1915.487569782279</v>
-      </c>
-      <c r="AA6" s="5">
-        <v>1942.67272800004</v>
-      </c>
-      <c r="AB6" s="5">
-        <v>1969.857886217801</v>
-      </c>
-      <c r="AC6" s="5">
-        <v>1997.043044435562</v>
-      </c>
-      <c r="AD6" s="5">
-        <v>2024.228202653323</v>
-      </c>
-      <c r="AE6" s="5">
-        <v>2051.413360871084</v>
-      </c>
-      <c r="AF6" s="5">
-        <v>2078.598519088845</v>
-      </c>
-      <c r="AG6" s="5">
-        <v>2105.783677306606</v>
-      </c>
-      <c r="AH6" s="5">
-        <v>2132.968835524367</v>
-      </c>
-      <c r="AI6" s="5">
-        <v>2160.153993742128</v>
-      </c>
-      <c r="AJ6" s="5">
-        <v>2187.339151959889</v>
-      </c>
-      <c r="AK6" s="5">
-        <v>2214.52431017765</v>
-      </c>
-    </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>113</v>
-      </c>
-      <c r="D7" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="5">
-        <f>G7*1000000000000</f>
-        <v>3599.8225679871703</v>
-      </c>
-      <c r="F7" t="s">
-        <v>115</v>
-      </c>
-      <c r="G7" s="37">
-        <v>3.5998225679871703E-9</v>
-      </c>
-      <c r="H7" t="s">
-        <v>116</v>
-      </c>
-      <c r="I7" s="40">
-        <v>0.25</v>
-      </c>
-      <c r="J7" s="12"/>
-      <c r="K7" s="40"/>
-      <c r="L7" s="40"/>
-      <c r="M7">
-        <v>19800</v>
-      </c>
-      <c r="N7" t="s">
-        <v>125</v>
-      </c>
-      <c r="O7" t="s">
-        <v>126</v>
-      </c>
-      <c r="P7" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>6035.0858307307299</v>
-      </c>
-      <c r="R7" s="5">
-        <v>5991.4369513857655</v>
-      </c>
-      <c r="S7" s="5">
-        <v>5947.7880720408011</v>
-      </c>
-      <c r="T7" s="5">
-        <v>5904.1391926958368</v>
-      </c>
-      <c r="U7" s="5">
-        <v>5860.4903133508724</v>
-      </c>
-      <c r="V7" s="5">
-        <v>5816.841434005908</v>
-      </c>
-      <c r="W7" s="5">
-        <v>5773.1925546609436</v>
-      </c>
-      <c r="X7" s="5">
-        <v>5729.5436753159793</v>
-      </c>
-      <c r="Y7" s="5">
-        <v>5685.8947959710149</v>
-      </c>
-      <c r="Z7" s="5">
-        <v>5642.2459166260505</v>
-      </c>
-      <c r="AA7" s="5">
-        <v>5598.5970372810862</v>
-      </c>
-      <c r="AB7" s="5">
-        <v>5554.9481579361218</v>
-      </c>
-      <c r="AC7" s="5">
-        <v>5511.2992785911574</v>
-      </c>
-      <c r="AD7" s="5">
-        <v>5467.650399246193</v>
-      </c>
-      <c r="AE7" s="5">
-        <v>5424.0015199012287</v>
-      </c>
-      <c r="AF7" s="5">
-        <v>5380.3526405562643</v>
-      </c>
-      <c r="AG7" s="5">
-        <v>5336.7037612112999</v>
-      </c>
-      <c r="AH7" s="5">
-        <v>5293.0548818663356</v>
-      </c>
-      <c r="AI7" s="5">
-        <v>5249.4060025213712</v>
-      </c>
-      <c r="AJ7" s="5">
-        <v>5205.7571231764068</v>
-      </c>
-      <c r="AK7" s="5">
-        <v>5162.1082438314425</v>
-      </c>
-    </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>37</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" t="s">
-        <v>114</v>
-      </c>
-      <c r="E8" s="5">
-        <f t="shared" ref="E8:E9" si="1">G8*1000000000000</f>
-        <v>3599.8225679871703</v>
-      </c>
-      <c r="F8" t="s">
-        <v>115</v>
-      </c>
-      <c r="G8" s="37">
-        <v>3.5998225679871703E-9</v>
-      </c>
-      <c r="H8" t="s">
-        <v>116</v>
-      </c>
-      <c r="I8" s="40"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="40"/>
-      <c r="L8" s="40"/>
-      <c r="P8" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q8" s="5">
-        <v>6035.0858307307299</v>
-      </c>
-      <c r="R8" s="5">
-        <v>5991.4369513857655</v>
-      </c>
-      <c r="S8" s="5">
-        <v>5947.7880720408011</v>
-      </c>
-      <c r="T8" s="5">
-        <v>5904.1391926958368</v>
-      </c>
-      <c r="U8" s="5">
-        <v>5860.4903133508724</v>
-      </c>
-      <c r="V8" s="5">
-        <v>5816.841434005908</v>
-      </c>
-      <c r="W8" s="5">
-        <v>5773.1925546609436</v>
-      </c>
-      <c r="X8" s="5">
-        <v>5729.5436753159793</v>
-      </c>
-      <c r="Y8" s="5">
-        <v>5685.8947959710149</v>
-      </c>
-      <c r="Z8" s="5">
-        <v>5642.2459166260505</v>
-      </c>
-      <c r="AA8" s="5">
-        <v>5598.5970372810862</v>
-      </c>
-      <c r="AB8" s="5">
-        <v>5554.9481579361218</v>
-      </c>
-      <c r="AC8" s="5">
-        <v>5511.2992785911574</v>
-      </c>
-      <c r="AD8" s="5">
-        <v>5467.650399246193</v>
-      </c>
-      <c r="AE8" s="5">
-        <v>5424.0015199012287</v>
-      </c>
-      <c r="AF8" s="5">
-        <v>5380.3526405562643</v>
-      </c>
-      <c r="AG8" s="5">
-        <v>5336.7037612112999</v>
-      </c>
-      <c r="AH8" s="5">
-        <v>5293.0548818663356</v>
-      </c>
-      <c r="AI8" s="5">
-        <v>5249.4060025213712</v>
-      </c>
-      <c r="AJ8" s="5">
-        <v>5205.7571231764068</v>
-      </c>
-      <c r="AK8" s="5">
-        <v>5162.1082438314425</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" t="s">
-        <v>114</v>
-      </c>
-      <c r="E9" s="5">
-        <f t="shared" si="1"/>
-        <v>3599.8225679871703</v>
-      </c>
-      <c r="F9" t="s">
-        <v>115</v>
-      </c>
-      <c r="G9" s="37">
-        <v>3.5998225679871703E-9</v>
-      </c>
-      <c r="H9" t="s">
-        <v>116</v>
-      </c>
-      <c r="I9" s="40"/>
-      <c r="J9" s="12">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="K9" s="40" t="s">
-        <v>258</v>
-      </c>
-      <c r="L9" s="40"/>
-      <c r="P9" s="39" t="s">
-        <v>117</v>
-      </c>
-      <c r="Q9" s="5">
-        <v>6035.0858307307299</v>
-      </c>
-      <c r="R9" s="5">
-        <v>5991.4369513857655</v>
-      </c>
-      <c r="S9" s="5">
-        <v>5947.7880720408011</v>
-      </c>
-      <c r="T9" s="5">
-        <v>5904.1391926958368</v>
-      </c>
-      <c r="U9" s="5">
-        <v>5860.4903133508724</v>
-      </c>
-      <c r="V9" s="5">
-        <v>5816.841434005908</v>
-      </c>
-      <c r="W9" s="5">
-        <v>5773.1925546609436</v>
-      </c>
-      <c r="X9" s="5">
-        <v>5729.5436753159793</v>
-      </c>
-      <c r="Y9" s="5">
-        <v>5685.8947959710149</v>
-      </c>
-      <c r="Z9" s="5">
-        <v>5642.2459166260505</v>
-      </c>
-      <c r="AA9" s="5">
-        <v>5598.5970372810862</v>
-      </c>
-      <c r="AB9" s="5">
-        <v>5554.9481579361218</v>
-      </c>
-      <c r="AC9" s="5">
-        <v>5511.2992785911574</v>
-      </c>
-      <c r="AD9" s="5">
-        <v>5467.650399246193</v>
-      </c>
-      <c r="AE9" s="5">
-        <v>5424.0015199012287</v>
-      </c>
-      <c r="AF9" s="5">
-        <v>5380.3526405562643</v>
-      </c>
-      <c r="AG9" s="5">
-        <v>5336.7037612112999</v>
-      </c>
-      <c r="AH9" s="5">
-        <v>5293.0548818663356</v>
-      </c>
-      <c r="AI9" s="5">
-        <v>5249.4060025213712</v>
-      </c>
-      <c r="AJ9" s="5">
-        <v>5205.7571231764068</v>
-      </c>
-      <c r="AK9" s="5">
-        <v>5162.1082438314425</v>
-      </c>
-    </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>118</v>
-      </c>
-      <c r="D10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E10" s="5">
-        <f t="shared" si="0"/>
-        <v>119999.99999999999</v>
-      </c>
-      <c r="F10" t="s">
-        <v>120</v>
-      </c>
-      <c r="G10">
-        <v>1.1999999999999999E-7</v>
-      </c>
-      <c r="H10" t="s">
-        <v>121</v>
-      </c>
-      <c r="I10" s="40">
-        <v>0.72</v>
-      </c>
-      <c r="J10">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="K10" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="L10" s="43" t="s">
-        <v>254</v>
-      </c>
-      <c r="O10" s="36" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D11" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11" s="5">
-        <f t="shared" ref="E11" si="2">G11*1000000000000</f>
-        <v>119999.99999999999</v>
-      </c>
-      <c r="F11" t="s">
-        <v>120</v>
-      </c>
-      <c r="G11">
-        <v>1.1999999999999999E-7</v>
-      </c>
-      <c r="H11" t="s">
-        <v>121</v>
-      </c>
-      <c r="I11" s="40"/>
-      <c r="J11" s="12">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="K11" s="40" t="s">
-        <v>127</v>
-      </c>
-      <c r="L11" s="43"/>
-      <c r="O11" s="36"/>
-    </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>37</v>
-      </c>
-      <c r="B12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>118</v>
-      </c>
-      <c r="D12" t="s">
-        <v>119</v>
-      </c>
-      <c r="E12" s="5">
-        <f t="shared" si="0"/>
-        <v>119999.99999999999</v>
-      </c>
-      <c r="F12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G12">
-        <v>1.1999999999999999E-7</v>
-      </c>
-      <c r="H12" t="s">
-        <v>121</v>
-      </c>
-      <c r="I12" s="40">
-        <v>0.44</v>
-      </c>
-      <c r="J12">
-        <v>13</v>
-      </c>
-      <c r="K12" s="40" t="s">
-        <v>130</v>
-      </c>
-      <c r="L12" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="M12">
-        <v>19800</v>
-      </c>
-      <c r="N12" t="s">
-        <v>125</v>
-      </c>
-      <c r="O12" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" t="s">
-        <v>119</v>
-      </c>
-      <c r="E13" s="5">
-        <f t="shared" si="0"/>
-        <v>119999.99999999999</v>
-      </c>
-      <c r="F13" t="s">
-        <v>120</v>
-      </c>
-      <c r="G13">
-        <v>1.1999999999999999E-7</v>
-      </c>
-      <c r="H13" t="s">
-        <v>121</v>
-      </c>
-      <c r="I13" s="40">
-        <v>0.44</v>
-      </c>
-      <c r="J13">
-        <v>13</v>
-      </c>
-      <c r="K13" s="40" t="s">
-        <v>130</v>
-      </c>
-      <c r="L13" s="43" t="s">
-        <v>128</v>
-      </c>
-      <c r="M13">
-        <v>19800</v>
-      </c>
-      <c r="N13" t="s">
-        <v>125</v>
-      </c>
-      <c r="O13" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D14" t="s">
-        <v>59</v>
-      </c>
-      <c r="E14" s="5">
-        <f t="shared" si="0"/>
-        <v>1093000</v>
-      </c>
-      <c r="F14" t="s">
-        <v>133</v>
-      </c>
-      <c r="G14">
-        <v>1.093E-6</v>
-      </c>
-      <c r="H14" t="s">
-        <v>134</v>
-      </c>
-      <c r="J14" s="12">
-        <v>50</v>
-      </c>
-      <c r="K14" s="40" t="s">
-        <v>257</v>
-      </c>
-      <c r="M14">
-        <v>19800</v>
-      </c>
-      <c r="N14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>132</v>
-      </c>
-      <c r="D15" t="s">
-        <v>59</v>
-      </c>
-      <c r="E15" s="5">
-        <f t="shared" si="0"/>
-        <v>1093000</v>
-      </c>
-      <c r="F15" t="s">
-        <v>133</v>
-      </c>
-      <c r="G15">
-        <v>1.093E-6</v>
-      </c>
-      <c r="H15" t="s">
-        <v>134</v>
-      </c>
-      <c r="J15" s="12">
-        <v>20000</v>
-      </c>
-      <c r="K15" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="M15">
-        <v>19800</v>
-      </c>
-      <c r="N15" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" t="s">
-        <v>136</v>
-      </c>
-      <c r="D16" t="s">
-        <v>137</v>
-      </c>
-      <c r="E16" s="5">
-        <f t="shared" si="0"/>
-        <v>142432539.75000003</v>
-      </c>
-      <c r="F16" t="s">
-        <v>138</v>
-      </c>
-      <c r="G16">
-        <v>1.4243253975000002E-4</v>
-      </c>
-      <c r="H16" t="s">
-        <v>139</v>
-      </c>
-      <c r="J16" s="12">
-        <v>1</v>
-      </c>
-      <c r="K16" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="L16" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>136</v>
-      </c>
-      <c r="D17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E17" s="5">
-        <f t="shared" si="0"/>
-        <v>142432539.75000003</v>
-      </c>
-      <c r="F17" t="s">
-        <v>138</v>
-      </c>
-      <c r="G17">
-        <v>1.4243253975000002E-4</v>
-      </c>
-      <c r="H17" t="s">
-        <v>139</v>
-      </c>
-      <c r="J17" s="12">
-        <v>1</v>
-      </c>
-      <c r="K17" s="40" t="s">
-        <v>249</v>
-      </c>
-      <c r="L17" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" t="s">
-        <v>136</v>
-      </c>
-      <c r="D18" t="s">
-        <v>137</v>
-      </c>
-      <c r="E18" s="5">
-        <f t="shared" ref="E18:E19" si="3">G18*1000000000000</f>
-        <v>142432539.75000003</v>
-      </c>
-      <c r="F18" t="s">
-        <v>138</v>
-      </c>
-      <c r="G18">
-        <v>1.4243253975000002E-4</v>
-      </c>
-      <c r="H18" t="s">
-        <v>139</v>
-      </c>
-      <c r="J18" s="5">
-        <v>16181.229773462785</v>
-      </c>
-      <c r="K18" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="L18" t="s">
-        <v>252</v>
-      </c>
-      <c r="O18" s="53"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" s="5">
-        <f t="shared" si="3"/>
-        <v>142432539.75000003</v>
-      </c>
-      <c r="F19" t="s">
-        <v>138</v>
-      </c>
-      <c r="G19">
-        <v>1.4243253975000002E-4</v>
-      </c>
-      <c r="H19" t="s">
-        <v>139</v>
-      </c>
-      <c r="J19" s="5">
-        <v>14492.753623188406</v>
-      </c>
-      <c r="K19" s="40" t="s">
-        <v>248</v>
-      </c>
-      <c r="L19" t="s">
-        <v>253</v>
-      </c>
-      <c r="O19" s="53"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="L23">
-        <v>1000</v>
-      </c>
-      <c r="M23" t="s">
-        <v>255</v>
-      </c>
-      <c r="N23" t="s">
-        <v>256</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:AK1" xr:uid="{5FA5616B-DF07-465E-AEEB-CCA6D05FE697}"/>
-  <phoneticPr fontId="10" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="O10" r:id="rId1" display="https://netl.doe.gov/projects/files/ComparisonofCommercialStateofArtFossilBasedHydrogenProductionTechnologies_041222.pdf" xr:uid="{E7CB3D97-93CD-4126-9FFC-6A55103A1392}"/>
-    <hyperlink ref="L3" r:id="rId2" display="https://www.nrel.gov/docs/fy20osti/77198.pdf" xr:uid="{531AFCC0-D1CD-457F-9290-C08242A339AF}"/>
-    <hyperlink ref="L10" r:id="rId3" display="https://www.nrel.gov/docs/fy20osti/77198.pdf" xr:uid="{979EC4C4-9A4A-47DB-9CBE-1F560C4CD153}"/>
-    <hyperlink ref="L12" r:id="rId4" xr:uid="{C8959CBC-501D-4F10-AA88-D7CD003A447E}"/>
-    <hyperlink ref="L13" r:id="rId5" xr:uid="{A5DBCFA7-F634-44A5-B62E-436D59BDA540}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId6"/>
-</worksheet>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{78975c20-18d4-40c9-811f-0d8ea387c6ea}" enabled="0" method="" siteId="{78975c20-18d4-40c9-811f-0d8ea387c6ea}" removed="1"/>

</xml_diff>

<commit_message>
update to job factors
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D2AE2D-D089-40E0-A905-D741A287915D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9F4C85C-4532-4B26-88F7-8B716F27ED0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18930" windowHeight="15600" tabRatio="622" firstSheet="6" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="11400" yWindow="2235" windowWidth="20520" windowHeight="12180" tabRatio="622" firstSheet="6" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -13174,8 +13174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16BE7FC-A8FD-4D95-933D-26AA617CB019}">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K47" sqref="K47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13183,15 +13183,14 @@
     <col min="1" max="1" width="20.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.875" customWidth="1"/>
+    <col min="4" max="4" width="9.75" customWidth="1"/>
+    <col min="5" max="6" width="6.5" customWidth="1"/>
     <col min="7" max="7" width="10.25" style="13" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.75" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11.75" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -14808,6 +14807,9 @@
       <c r="J41">
         <v>2.8358342136926399E-2</v>
       </c>
+      <c r="K41">
+        <v>10.436</v>
+      </c>
       <c r="L41" s="2">
         <f t="shared" si="3"/>
         <v>6.776252054794521E-2</v>
@@ -14931,6 +14933,12 @@
       <c r="I44">
         <v>0.23400000000000001</v>
       </c>
+      <c r="J44">
+        <v>2.8358342136926399E-2</v>
+      </c>
+      <c r="K44">
+        <v>0.23400000000000001</v>
+      </c>
       <c r="L44" s="2">
         <f>I44*0.965</f>
         <v>0.22581000000000001</v>
@@ -14970,6 +14978,9 @@
       <c r="I45">
         <v>0.23400000000000001</v>
       </c>
+      <c r="J45">
+        <v>2.8358342136926399E-2</v>
+      </c>
       <c r="L45" s="2">
         <f t="shared" ref="L45:L49" si="4">I45*0.965</f>
         <v>0.22581000000000001</v>
@@ -15009,6 +15020,9 @@
       <c r="I46">
         <v>0.23400000000000001</v>
       </c>
+      <c r="J46">
+        <v>2.8358342136926399E-2</v>
+      </c>
       <c r="L46" s="2">
         <f t="shared" si="4"/>
         <v>0.22581000000000001</v>
@@ -15048,6 +15062,12 @@
       <c r="I47">
         <v>0.23400000000000001</v>
       </c>
+      <c r="J47">
+        <v>2.8358342136926399E-2</v>
+      </c>
+      <c r="K47">
+        <v>0.23400000000000001</v>
+      </c>
       <c r="L47" s="2">
         <f t="shared" si="4"/>
         <v>0.22581000000000001</v>
@@ -15087,6 +15107,9 @@
       <c r="I48">
         <v>0.23400000000000001</v>
       </c>
+      <c r="J48">
+        <v>2.8358342136926399E-2</v>
+      </c>
       <c r="L48" s="2">
         <f t="shared" si="4"/>
         <v>0.22581000000000001</v>
@@ -15125,6 +15148,9 @@
       </c>
       <c r="I49">
         <v>0.23400000000000001</v>
+      </c>
+      <c r="J49">
+        <v>2.8358342136926399E-2</v>
       </c>
       <c r="L49" s="2">
         <f t="shared" si="4"/>

</xml_diff>

<commit_message>
Assuming no productivity changes in NF - hydrogen pipeline
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://randus-my.sharepoint.com/personal/jrojasa_rand_org/Documents/Documents/GitHub/SJV-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{69B13227-3659-4C7A-9EC5-331DD5EC379F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{247AC68D-77AA-465C-AA9E-57712FFA6D74}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{69B13227-3659-4C7A-9EC5-331DD5EC379F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6312E457-3567-4574-87BD-ADE1DDBA0B3A}"/>
   <bookViews>
     <workbookView xWindow="-14490" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="622" firstSheet="6" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
@@ -13172,8 +13172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16BE7FC-A8FD-4D95-933D-26AA617CB019}">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -14338,6 +14338,9 @@
       <c r="I29" s="2">
         <v>10.436363636363636</v>
       </c>
+      <c r="J29">
+        <v>0</v>
+      </c>
       <c r="K29" s="2">
         <v>10.436</v>
       </c>
@@ -14380,6 +14383,9 @@
       <c r="I30" s="2">
         <v>10.436363636363636</v>
       </c>
+      <c r="J30">
+        <v>0</v>
+      </c>
       <c r="K30" s="2">
         <v>0.16161616161616163</v>
       </c>
@@ -14421,6 +14427,9 @@
       </c>
       <c r="I31" s="2">
         <v>10.436363636363636</v>
+      </c>
+      <c r="J31">
+        <v>0</v>
       </c>
       <c r="K31" s="2">
         <v>8.0808080808080815E-2</v>

</xml_diff>

<commit_message>
productivity adjustment set to zero
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://randus-my.sharepoint.com/personal/jrojasa_rand_org/Documents/Documents/GitHub/SJV-/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{69B13227-3659-4C7A-9EC5-331DD5EC379F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6312E457-3567-4574-87BD-ADE1DDBA0B3A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D4D677-F39F-4AF0-918F-9E8B311ADB2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14490" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="622" firstSheet="6" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="2310" yWindow="3510" windowWidth="26490" windowHeight="12180" tabRatio="622" firstSheet="6" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2511" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2490" uniqueCount="345">
   <si>
     <t>Feedstock</t>
   </si>
@@ -1722,25 +1722,25 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.08203125" customWidth="1"/>
-    <col min="4" max="4" width="27.58203125" customWidth="1"/>
+    <col min="1" max="1" width="30.375" customWidth="1"/>
+    <col min="2" max="2" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="27.625" customWidth="1"/>
     <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.58203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="13" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.83203125" customWidth="1"/>
-    <col min="12" max="12" width="38.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.875" customWidth="1"/>
+    <col min="12" max="12" width="38.375" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="38.25" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1793,7 +1793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1981,7 +1981,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2356,7 +2356,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>311</v>
       </c>
@@ -2408,7 +2408,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2543,7 +2543,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2581,10 +2581,10 @@
       </c>
       <c r="N17" s="61"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K19" s="62"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L20" s="63"/>
     </row>
   </sheetData>
@@ -2605,26 +2605,26 @@
       <selection pane="topRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.75" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="15.25" customWidth="1"/>
-    <col min="6" max="6" width="11.08203125" customWidth="1"/>
+    <col min="6" max="6" width="11.125" customWidth="1"/>
     <col min="7" max="7" width="17.75" customWidth="1"/>
     <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.375" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="43.5" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="19.08203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.375" customWidth="1"/>
+    <col min="13" max="13" width="19.125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="10.5" customWidth="1"/>
     <col min="16" max="16" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>1216.528453322951</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2872,7 +2872,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2965,7 +2965,7 @@
         <v>2101.97739666605</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>1171.0983188067505</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>2214.52431017765</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -3457,7 +3457,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -3535,7 +3535,7 @@
       <c r="L11" s="43"/>
       <c r="O11" s="36"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -3745,7 +3745,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -3781,7 +3781,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -3818,7 +3818,7 @@
       </c>
       <c r="O18" s="53"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -3855,7 +3855,7 @@
       </c>
       <c r="O19" s="53"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L23">
         <v>1000</v>
       </c>
@@ -3889,16 +3889,16 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.58203125" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="30.375" customWidth="1"/>
+    <col min="3" max="3" width="8.375" customWidth="1"/>
+    <col min="4" max="4" width="23.875" customWidth="1"/>
     <col min="5" max="25" width="8.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3975,7 +3975,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4052,7 +4052,7 @@
         <v>1216.528453322951</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>2101.97739666605</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
@@ -4206,7 +4206,7 @@
         <v>1171.0983188067505</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>35</v>
       </c>
@@ -4283,7 +4283,7 @@
         <v>2214.52431017765</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>36</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>37</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -4604,15 +4604,15 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.08203125" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="21.58203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.125" customWidth="1"/>
+    <col min="2" max="2" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>291</v>
       </c>
@@ -4695,7 +4695,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>292</v>
       </c>
@@ -4778,7 +4778,7 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>292</v>
       </c>
@@ -4861,7 +4861,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>293</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>14800</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>293</v>
       </c>
@@ -5027,7 +5027,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -5110,7 +5110,7 @@
         <v>3.4782608695652177</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -5193,7 +5193,7 @@
         <v>21.118012422360248</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>140</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>292</v>
       </c>
@@ -5442,7 +5442,7 @@
         <v>4.9689440993788822E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -5525,7 +5525,7 @@
         <v>310000</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -5608,7 +5608,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -5691,7 +5691,7 @@
         <v>83854.869455332082</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>140</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -5857,7 +5857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -5940,7 +5940,7 @@
         <v>39760971.535051085</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>140</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>2572768.7463856577</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>5769.2307692307695</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>230.76923076923077</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>140</v>
       </c>
@@ -6285,13 +6285,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08203125" customWidth="1"/>
+    <col min="2" max="2" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6362,7 +6362,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6433,7 +6433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -6575,7 +6575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -6646,7 +6646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -6730,17 +6730,17 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.75" customWidth="1"/>
     <col min="2" max="2" width="20.75" customWidth="1"/>
-    <col min="3" max="3" width="20.58203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.375" customWidth="1"/>
+    <col min="6" max="6" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>157</v>
       </c>
@@ -6763,7 +6763,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
@@ -6805,7 +6805,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>34</v>
       </c>
@@ -6826,7 +6826,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>35</v>
       </c>
@@ -6847,7 +6847,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>140</v>
       </c>
@@ -6868,7 +6868,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>140</v>
       </c>
@@ -6889,7 +6889,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>38</v>
       </c>
@@ -6910,7 +6910,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
@@ -6931,7 +6931,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>58</v>
       </c>
@@ -6952,7 +6952,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>140</v>
       </c>
@@ -6973,7 +6973,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>140</v>
       </c>
@@ -6994,7 +6994,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>38</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>140</v>
       </c>
@@ -7036,7 +7036,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>140</v>
       </c>
@@ -7057,7 +7057,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>160</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>160</v>
       </c>
@@ -7099,7 +7099,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>140</v>
       </c>
@@ -7120,7 +7120,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>140</v>
       </c>
@@ -7141,7 +7141,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="50" t="s">
         <v>159</v>
       </c>
@@ -7149,7 +7149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="51" t="s">
         <v>12</v>
       </c>
@@ -7157,7 +7157,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="51" t="s">
         <v>19</v>
       </c>
@@ -7165,7 +7165,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
         <v>19</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="51" t="s">
         <v>38</v>
       </c>
@@ -7181,7 +7181,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="51" t="s">
         <v>38</v>
       </c>
@@ -7189,7 +7189,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="51" t="s">
         <v>38</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="51" t="s">
         <v>70</v>
       </c>
@@ -7219,17 +7219,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.58203125" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -7269,7 +7269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -7280,7 +7280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -7297,7 +7297,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -7305,7 +7305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -7326,17 +7326,17 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.875" customWidth="1"/>
+    <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.58203125" customWidth="1"/>
+    <col min="4" max="4" width="40.875" customWidth="1"/>
+    <col min="5" max="5" width="30.625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -7365,7 +7365,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>58</v>
       </c>
@@ -7392,7 +7392,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>154</v>
       </c>
@@ -7419,7 +7419,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
@@ -7446,7 +7446,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
@@ -7473,7 +7473,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>22</v>
       </c>
@@ -7500,7 +7500,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
@@ -7523,7 +7523,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>36</v>
       </c>
@@ -7546,7 +7546,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>179</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>179</v>
       </c>
@@ -7596,7 +7596,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>183</v>
       </c>
@@ -7621,7 +7621,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>183</v>
       </c>
@@ -7640,7 +7640,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -7655,7 +7655,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -7670,7 +7670,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>188</v>
       </c>
@@ -7697,7 +7697,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>171</v>
       </c>
@@ -7720,7 +7720,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>176</v>
       </c>
@@ -7743,7 +7743,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>179</v>
       </c>
@@ -7766,7 +7766,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>183</v>
       </c>
@@ -7780,7 +7780,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>184</v>
       </c>
@@ -7794,7 +7794,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>37</v>
       </c>
@@ -7808,7 +7808,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>36</v>
       </c>
@@ -7822,12 +7822,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>0</v>
       </c>
@@ -7844,7 +7844,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>58</v>
       </c>
@@ -7853,7 +7853,7 @@
       </c>
       <c r="C32" s="14"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>154</v>
       </c>
@@ -7862,7 +7862,7 @@
       </c>
       <c r="C33" s="14"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
@@ -7871,7 +7871,7 @@
       </c>
       <c r="C34" s="14"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>11</v>
       </c>
@@ -7882,7 +7882,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>22</v>
       </c>
@@ -7891,7 +7891,7 @@
       </c>
       <c r="C36" s="14"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>209</v>
       </c>
@@ -7900,7 +7900,7 @@
       </c>
       <c r="C37" s="14"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>35</v>
       </c>
@@ -7909,7 +7909,7 @@
       </c>
       <c r="C38" s="14"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>37</v>
       </c>
@@ -7923,7 +7923,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>36</v>
       </c>
@@ -7937,7 +7937,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>179</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>183</v>
       </c>
@@ -7971,12 +7971,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
         <v>1</v>
       </c>
@@ -7987,7 +7987,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>19</v>
       </c>
@@ -7998,7 +7998,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="30" t="s">
         <v>19</v>
       </c>
@@ -8015,7 +8015,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
         <v>19</v>
       </c>
@@ -8032,7 +8032,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
         <v>19</v>
       </c>
@@ -8052,7 +8052,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="s">
         <v>19</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>58</v>
       </c>
@@ -8086,7 +8086,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>58</v>
       </c>
@@ -8097,7 +8097,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="s">
         <v>58</v>
       </c>
@@ -8114,7 +8114,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="27" t="s">
         <v>12</v>
       </c>
@@ -8131,7 +8131,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>12</v>
       </c>
@@ -8142,12 +8142,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="26" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
         <v>233</v>
       </c>
@@ -8158,7 +8158,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="29" t="s">
         <v>235</v>
       </c>
@@ -8166,7 +8166,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="27" t="s">
         <v>236</v>
       </c>
@@ -8174,12 +8174,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="26" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="27" t="s">
         <v>238</v>
       </c>
@@ -8187,7 +8187,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="27" t="s">
         <v>239</v>
       </c>
@@ -8208,13 +8208,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.58203125" customWidth="1"/>
-    <col min="2" max="5" width="15.58203125" customWidth="1"/>
+    <col min="1" max="1" width="25.625" customWidth="1"/>
+    <col min="2" max="5" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>241</v>
       </c>
@@ -8234,7 +8234,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>242</v>
       </c>
@@ -8245,7 +8245,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -8253,7 +8253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -8261,7 +8261,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -8275,7 +8275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -8289,7 +8289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>243</v>
       </c>
@@ -8303,7 +8303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>244</v>
       </c>
@@ -8314,7 +8314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>245</v>
       </c>
@@ -8325,7 +8325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>246</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -8344,7 +8344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -8365,19 +8365,19 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.25" customWidth="1"/>
     <col min="2" max="2" width="12.75" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="11.25" customWidth="1"/>
     <col min="7" max="7" width="8.25" customWidth="1"/>
-    <col min="8" max="9" width="24.08203125" customWidth="1"/>
+    <col min="8" max="9" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8412,7 +8412,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -8446,7 +8446,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -8512,7 +8512,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -8541,7 +8541,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -8570,7 +8570,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -8599,7 +8599,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -8633,7 +8633,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -8670,7 +8670,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
@@ -8699,7 +8699,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -8731,7 +8731,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -8765,7 +8765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -8794,7 +8794,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -8828,7 +8828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -8865,7 +8865,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>22</v>
       </c>
@@ -8895,7 +8895,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
@@ -8927,7 +8927,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
@@ -8960,7 +8960,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>22</v>
       </c>
@@ -9003,18 +9003,18 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="5" width="26" customWidth="1"/>
-    <col min="6" max="7" width="24.08203125" customWidth="1"/>
+    <col min="6" max="7" width="24.125" customWidth="1"/>
     <col min="8" max="8" width="31.5" customWidth="1"/>
-    <col min="9" max="9" width="36.83203125" customWidth="1"/>
+    <col min="9" max="9" width="36.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9043,7 +9043,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -9066,7 +9066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>11</v>
       </c>
@@ -9095,7 +9095,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -9118,7 +9118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -9141,7 +9141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -9164,7 +9164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -9187,7 +9187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
         <v>37</v>
       </c>
@@ -9210,7 +9210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>44</v>
       </c>
@@ -9237,7 +9237,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>45</v>
       </c>
@@ -9264,7 +9264,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="55" t="s">
         <v>40</v>
       </c>
@@ -9293,7 +9293,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="55" t="s">
         <v>37</v>
       </c>
@@ -9325,7 +9325,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
         <v>36</v>
       </c>
@@ -9357,7 +9357,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>44</v>
       </c>
@@ -9384,7 +9384,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>45</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -9434,7 +9434,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -9460,7 +9460,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -9486,7 +9486,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -9512,7 +9512,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -9541,7 +9541,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -9570,7 +9570,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -9593,7 +9593,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="55" t="s">
         <v>11</v>
       </c>
@@ -9622,7 +9622,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -9645,7 +9645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -9668,7 +9668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -9691,7 +9691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -9714,7 +9714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -9737,7 +9737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>44</v>
       </c>
@@ -9764,7 +9764,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>45</v>
       </c>
@@ -9791,7 +9791,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="55" t="s">
         <v>40</v>
       </c>
@@ -9820,7 +9820,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
         <v>37</v>
       </c>
@@ -9849,7 +9849,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>44</v>
       </c>
@@ -9876,7 +9876,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>45</v>
       </c>
@@ -9902,7 +9902,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="55" t="s">
         <v>36</v>
       </c>
@@ -9931,7 +9931,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -9958,7 +9958,7 @@
       </c>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -9984,7 +9984,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -10010,7 +10010,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -10036,7 +10036,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -10062,7 +10062,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -10088,7 +10088,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -10111,7 +10111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="55" t="s">
         <v>11</v>
       </c>
@@ -10140,7 +10140,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -10163,7 +10163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
@@ -10186,7 +10186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
@@ -10209,7 +10209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -10232,7 +10232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -10255,7 +10255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>44</v>
       </c>
@@ -10282,7 +10282,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>45</v>
       </c>
@@ -10309,7 +10309,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="55" t="s">
         <v>40</v>
       </c>
@@ -10338,7 +10338,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="55" t="s">
         <v>37</v>
       </c>
@@ -10367,7 +10367,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>44</v>
       </c>
@@ -10394,7 +10394,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>45</v>
       </c>
@@ -10420,7 +10420,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="55" t="s">
         <v>36</v>
       </c>
@@ -10449,7 +10449,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -10476,7 +10476,7 @@
       </c>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>45</v>
       </c>
@@ -10502,7 +10502,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -10528,7 +10528,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>50</v>
       </c>
@@ -10554,7 +10554,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -10577,7 +10577,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -10600,10 +10600,10 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F68" s="64"/>
     </row>
   </sheetData>
@@ -10629,17 +10629,17 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="173.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="173.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -10659,7 +10659,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -10676,7 +10676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -10693,7 +10693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -10713,7 +10713,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -10730,7 +10730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -10760,17 +10760,17 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.58203125" customWidth="1"/>
-    <col min="2" max="2" width="19.08203125" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="25.75" customWidth="1"/>
-    <col min="6" max="6" width="19.08203125" customWidth="1"/>
+    <col min="6" max="6" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -10853,7 +10853,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -10936,7 +10936,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -11019,7 +11019,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -11102,7 +11102,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -11185,7 +11185,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -11268,7 +11268,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -11351,7 +11351,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -11434,7 +11434,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -11538,7 +11538,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -11642,7 +11642,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -11725,7 +11725,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -11829,7 +11829,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -11933,7 +11933,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -12016,7 +12016,7 @@
         <v>80.36</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -12120,7 +12120,7 @@
         <v>80.36</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -12238,18 +12238,18 @@
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.875" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="8" width="24.08203125" customWidth="1"/>
+    <col min="7" max="8" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12287,7 +12287,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -12304,7 +12304,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -12334,7 +12334,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -12352,7 +12352,7 @@
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -12370,7 +12370,7 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -12388,7 +12388,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>36</v>
       </c>
@@ -12406,7 +12406,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>37</v>
       </c>
@@ -12424,7 +12424,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -12442,7 +12442,7 @@
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -12460,7 +12460,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -12490,7 +12490,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -12520,7 +12520,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -12551,7 +12551,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -12569,7 +12569,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -12587,7 +12587,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -12604,7 +12604,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -12621,7 +12621,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -12638,7 +12638,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -12655,7 +12655,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -12672,7 +12672,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -12689,7 +12689,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -12709,7 +12709,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -12746,7 +12746,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -12767,7 +12767,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -12785,7 +12785,7 @@
       </c>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -12803,7 +12803,7 @@
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>36</v>
       </c>
@@ -12821,7 +12821,7 @@
       </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>37</v>
       </c>
@@ -12839,7 +12839,7 @@
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -12857,7 +12857,7 @@
       </c>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -12875,7 +12875,7 @@
       </c>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
@@ -12912,7 +12912,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -12949,7 +12949,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -12980,7 +12980,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -12998,7 +12998,7 @@
       </c>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -13016,7 +13016,7 @@
       </c>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -13036,7 +13036,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -13056,7 +13056,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
@@ -13076,7 +13076,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>50</v>
       </c>
@@ -13096,7 +13096,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -13113,7 +13113,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -13130,35 +13130,35 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
     </row>
@@ -13172,26 +13172,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16BE7FC-A8FD-4D95-933D-26AA617CB019}">
   <dimension ref="A1:N58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.58203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.75" customWidth="1"/>
     <col min="5" max="6" width="6.5" customWidth="1"/>
     <col min="7" max="7" width="10.25" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.08203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6.75" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.08203125" customWidth="1"/>
+    <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13235,7 +13235,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -13264,7 +13264,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="J2">
-        <v>4.5152412959181799E-2</v>
+        <v>0</v>
       </c>
       <c r="K2">
         <v>5.0999999999999997E-2</v>
@@ -13277,7 +13277,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -13306,7 +13306,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="J3">
-        <v>4.5152412959181799E-2</v>
+        <v>0</v>
       </c>
       <c r="K3">
         <v>9.6900000000000007E-3</v>
@@ -13319,7 +13319,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -13348,7 +13348,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="J4">
-        <v>4.5152412959181799E-2</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>1.6320000000000001E-2</v>
@@ -13361,7 +13361,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -13390,7 +13390,7 @@
         <v>2.2229999999999999</v>
       </c>
       <c r="J5">
-        <v>8.3034948476273795E-3</v>
+        <v>0</v>
       </c>
       <c r="K5" s="69">
         <v>2.2265403611043637</v>
@@ -13403,7 +13403,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -13432,7 +13432,7 @@
         <v>2.2229999999999999</v>
       </c>
       <c r="J6">
-        <v>8.3034948476273795E-3</v>
+        <v>0</v>
       </c>
       <c r="K6" s="69">
         <v>0.44530807222087276</v>
@@ -13445,7 +13445,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -13474,7 +13474,7 @@
         <v>2.2229999999999999</v>
       </c>
       <c r="J7">
-        <v>8.3034948476273795E-3</v>
+        <v>0</v>
       </c>
       <c r="K7" s="2">
         <v>0.60723828030119009</v>
@@ -13487,7 +13487,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -13516,7 +13516,7 @@
         <v>0.78800000000000003</v>
       </c>
       <c r="J8">
-        <v>3.7832039152811102E-2</v>
+        <v>0</v>
       </c>
       <c r="K8">
         <v>0.78800000000000003</v>
@@ -13529,7 +13529,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -13557,9 +13557,6 @@
       <c r="I9">
         <v>0.78800000000000003</v>
       </c>
-      <c r="J9">
-        <v>3.7832039152811102E-2</v>
-      </c>
       <c r="L9" t="s">
         <v>344</v>
       </c>
@@ -13567,7 +13564,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -13595,9 +13592,6 @@
       <c r="I10">
         <v>0.78800000000000003</v>
       </c>
-      <c r="J10">
-        <v>3.7832039152811102E-2</v>
-      </c>
       <c r="L10" t="s">
         <v>344</v>
       </c>
@@ -13605,7 +13599,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -13621,23 +13615,8 @@
       <c r="H11" t="s">
         <v>93</v>
       </c>
-      <c r="I11" t="s">
-        <v>344</v>
-      </c>
-      <c r="J11" t="s">
-        <v>344</v>
-      </c>
-      <c r="K11" t="s">
-        <v>344</v>
-      </c>
-      <c r="L11" t="s">
-        <v>344</v>
-      </c>
-      <c r="M11" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -13653,23 +13632,8 @@
       <c r="H12" t="s">
         <v>93</v>
       </c>
-      <c r="I12" t="s">
-        <v>344</v>
-      </c>
-      <c r="J12" t="s">
-        <v>344</v>
-      </c>
-      <c r="K12" t="s">
-        <v>344</v>
-      </c>
-      <c r="L12" t="s">
-        <v>344</v>
-      </c>
-      <c r="M12" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -13685,23 +13649,8 @@
       <c r="H13" t="s">
         <v>93</v>
       </c>
-      <c r="I13" t="s">
-        <v>344</v>
-      </c>
-      <c r="J13" t="s">
-        <v>344</v>
-      </c>
-      <c r="K13" t="s">
-        <v>344</v>
-      </c>
-      <c r="L13" t="s">
-        <v>344</v>
-      </c>
-      <c r="M13" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -13730,7 +13679,7 @@
         <v>4.958333333333333</v>
       </c>
       <c r="J14" s="67">
-        <v>1.1585743964712399E-2</v>
+        <v>0</v>
       </c>
       <c r="K14" s="69">
         <v>4.9157303370786503</v>
@@ -13743,7 +13692,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -13772,7 +13721,7 @@
         <v>4.958333333333333</v>
       </c>
       <c r="J15" s="67">
-        <v>1.1585743964712399E-2</v>
+        <v>0</v>
       </c>
       <c r="K15" s="69">
         <v>1.2780898876404492</v>
@@ -13785,7 +13734,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -13814,7 +13763,7 @@
         <v>4.958333333333333</v>
       </c>
       <c r="J16" s="67">
-        <v>1.1585743964712399E-2</v>
+        <v>0</v>
       </c>
       <c r="K16" s="69">
         <v>1.7205056179775278</v>
@@ -13827,7 +13776,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -13856,7 +13805,7 @@
         <v>4.958333333333333</v>
       </c>
       <c r="J17" s="67">
-        <v>1.1585743964712399E-2</v>
+        <v>0</v>
       </c>
       <c r="K17" s="69">
         <v>4.9157303370786503</v>
@@ -13869,7 +13818,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -13898,7 +13847,7 @@
         <v>4.958333333333333</v>
       </c>
       <c r="J18" s="67">
-        <v>1.1585743964712399E-2</v>
+        <v>0</v>
       </c>
       <c r="K18" s="69">
         <v>1.2780898876404492</v>
@@ -13911,7 +13860,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -13940,7 +13889,7 @@
         <v>4.958333333333333</v>
       </c>
       <c r="J19" s="67">
-        <v>1.1585743964712399E-2</v>
+        <v>0</v>
       </c>
       <c r="K19" s="69">
         <v>1.7205056179775278</v>
@@ -13953,7 +13902,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -13982,7 +13931,7 @@
         <v>4.958333333333333</v>
       </c>
       <c r="J20" s="67">
-        <v>1.1585743964712399E-2</v>
+        <v>0</v>
       </c>
       <c r="K20" s="69">
         <v>4.9157303370786503</v>
@@ -13995,7 +13944,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -14024,7 +13973,7 @@
         <v>4.958333333333333</v>
       </c>
       <c r="J21" s="67">
-        <v>1.1585743964712399E-2</v>
+        <v>0</v>
       </c>
       <c r="K21" s="69">
         <v>1.2780898876404492</v>
@@ -14037,7 +13986,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -14066,7 +14015,7 @@
         <v>4.958333333333333</v>
       </c>
       <c r="J22" s="67">
-        <v>1.1585743964712399E-2</v>
+        <v>0</v>
       </c>
       <c r="K22" s="69">
         <v>1.7205056179775278</v>
@@ -14079,7 +14028,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -14108,7 +14057,7 @@
         <v>4.958333333333333</v>
       </c>
       <c r="J23" s="67">
-        <v>1.1585743964712399E-2</v>
+        <v>0</v>
       </c>
       <c r="K23" s="69">
         <v>4.9157303370786503</v>
@@ -14121,7 +14070,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -14150,7 +14099,7 @@
         <v>4.958333333333333</v>
       </c>
       <c r="J24" s="67">
-        <v>1.1585743964712399E-2</v>
+        <v>0</v>
       </c>
       <c r="K24" s="69">
         <v>1.2780898876404492</v>
@@ -14163,7 +14112,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -14192,7 +14141,7 @@
         <v>4.958333333333333</v>
       </c>
       <c r="J25" s="67">
-        <v>1.1585743964712399E-2</v>
+        <v>0</v>
       </c>
       <c r="K25" s="69">
         <v>1.7205056179775278</v>
@@ -14205,7 +14154,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -14227,12 +14176,6 @@
       <c r="H26" t="s">
         <v>93</v>
       </c>
-      <c r="I26" t="s">
-        <v>344</v>
-      </c>
-      <c r="J26" t="s">
-        <v>344</v>
-      </c>
       <c r="K26" t="s">
         <v>344</v>
       </c>
@@ -14240,7 +14183,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -14262,12 +14205,6 @@
       <c r="H27" t="s">
         <v>93</v>
       </c>
-      <c r="I27" t="s">
-        <v>344</v>
-      </c>
-      <c r="J27" t="s">
-        <v>344</v>
-      </c>
       <c r="K27" t="s">
         <v>344</v>
       </c>
@@ -14275,7 +14212,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -14297,12 +14234,6 @@
       <c r="H28" t="s">
         <v>93</v>
       </c>
-      <c r="I28" t="s">
-        <v>344</v>
-      </c>
-      <c r="J28" t="s">
-        <v>344</v>
-      </c>
       <c r="K28" t="s">
         <v>344</v>
       </c>
@@ -14310,7 +14241,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -14355,7 +14286,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -14400,7 +14331,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -14445,7 +14376,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -14474,7 +14405,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J32">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K32">
         <v>0.23400000000000001</v>
@@ -14490,7 +14421,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -14519,7 +14450,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J33">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K33" s="67">
         <v>2.8080000000000004E-2</v>
@@ -14535,7 +14466,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -14564,7 +14495,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J34">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K34">
         <v>5.6160000000000009E-2</v>
@@ -14580,7 +14511,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -14609,7 +14540,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J35">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K35">
         <v>0.23400000000000001</v>
@@ -14625,7 +14556,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -14654,7 +14585,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J36">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K36" s="67">
         <v>2.8080000000000001E-2</v>
@@ -14670,7 +14601,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -14699,7 +14630,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J37">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K37">
         <v>5.6160000000000002E-2</v>
@@ -14715,7 +14646,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -14744,7 +14675,7 @@
         <v>10.436</v>
       </c>
       <c r="J38">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K38" s="2">
         <v>10.436</v>
@@ -14760,7 +14691,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -14789,7 +14720,7 @@
         <v>10.436</v>
       </c>
       <c r="J39">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K39" s="2">
         <v>0.16161616161616163</v>
@@ -14805,7 +14736,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -14834,7 +14765,7 @@
         <v>10.436</v>
       </c>
       <c r="J40">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K40" s="2">
         <v>8.0808080808080815E-2</v>
@@ -14850,7 +14781,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -14879,7 +14810,7 @@
         <v>10.436</v>
       </c>
       <c r="J41">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K41" s="2">
         <v>10.436</v>
@@ -14895,7 +14826,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -14924,7 +14855,7 @@
         <v>10.436</v>
       </c>
       <c r="J42">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K42" s="2">
         <v>0.16161616161616163</v>
@@ -14940,7 +14871,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -14969,7 +14900,7 @@
         <v>10.436</v>
       </c>
       <c r="J43">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K43" s="2">
         <v>8.0808080808080815E-2</v>
@@ -14985,7 +14916,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -15014,7 +14945,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J44">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K44">
         <v>0.23400000000000001</v>
@@ -15030,7 +14961,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -15059,7 +14990,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J45">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>344</v>
@@ -15071,7 +15002,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -15100,7 +15031,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J46">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>344</v>
@@ -15112,7 +15043,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -15141,7 +15072,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J47">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K47">
         <v>0.23400000000000001</v>
@@ -15157,7 +15088,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -15186,7 +15117,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J48">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="L48" s="2" t="s">
         <v>344</v>
@@ -15198,7 +15129,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>44</v>
       </c>
@@ -15227,7 +15158,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J49">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="L49" s="2" t="s">
         <v>344</v>
@@ -15239,7 +15170,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -15268,7 +15199,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J50">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K50">
         <v>0.23400000000000001</v>
@@ -15284,7 +15215,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -15313,7 +15244,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J51">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>344</v>
@@ -15325,7 +15256,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -15354,7 +15285,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J52">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="L52" s="2" t="s">
         <v>344</v>
@@ -15366,7 +15297,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -15395,7 +15326,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J53">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K53">
         <v>0.23400000000000001</v>
@@ -15411,7 +15342,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -15440,7 +15371,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J54">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K54" s="67">
         <v>2.8080000000000004E-2</v>
@@ -15456,7 +15387,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -15485,7 +15416,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J55">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K55">
         <v>5.6160000000000009E-2</v>
@@ -15501,7 +15432,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -15530,7 +15461,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J56">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K56">
         <v>0.23400000000000001</v>
@@ -15546,7 +15477,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>36</v>
       </c>
@@ -15575,7 +15506,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J57">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K57" s="67">
         <v>2.8080000000000004E-2</v>
@@ -15591,7 +15522,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -15620,7 +15551,7 @@
         <v>0.23400000000000001</v>
       </c>
       <c r="J58">
-        <v>2.8358342136926399E-2</v>
+        <v>0</v>
       </c>
       <c r="K58">
         <v>5.6160000000000009E-2</v>
@@ -15650,21 +15581,21 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="68.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15696,7 +15627,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -15716,7 +15647,7 @@
         <v>3.4599999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>11</v>
       </c>
@@ -15740,7 +15671,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -15760,7 +15691,7 @@
         <v>2.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -15780,7 +15711,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -15800,7 +15731,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -15820,7 +15751,7 @@
         <v>4.0899999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -15840,7 +15771,7 @@
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -15860,7 +15791,7 @@
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -15880,7 +15811,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -15900,7 +15831,7 @@
         <v>5.62E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -15920,7 +15851,7 @@
         <v>5.62E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -15953,15 +15884,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5" customWidth="1"/>
     <col min="4" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -15978,7 +15909,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -15995,7 +15926,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Fixed errors on job factors (conversion)
Billion BTU conversion factors are now correctly applied. All the job factors are in billion BTUs. 1 billion BTU means 7.5 metric ton of Hydrogen vs. 0.007 million gallon of SAF vs. 0.965 million CF.
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://randus-my.sharepoint.com/personal/jrojasa_rand_org/Documents/Documents/GitHub/SJV-/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="13_ncr:1_{69B13227-3659-4C7A-9EC5-331DD5EC379F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB4679C5-A5C4-4607-820A-FAA33E296B69}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B808FC-2D25-4C96-BFDD-413D54CA6FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7860" yWindow="-16297" windowWidth="28995" windowHeight="15794" tabRatio="622" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="26490" windowHeight="12180" tabRatio="622" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -1297,7 +1297,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1398,8 +1398,10 @@
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1722,25 +1724,25 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.08203125" customWidth="1"/>
-    <col min="4" max="4" width="27.58203125" customWidth="1"/>
+    <col min="1" max="1" width="30.375" customWidth="1"/>
+    <col min="2" max="2" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="27.625" customWidth="1"/>
     <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.58203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="13" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.83203125" customWidth="1"/>
-    <col min="12" max="12" width="38.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.875" customWidth="1"/>
+    <col min="12" max="12" width="38.375" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="38.25" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1793,7 +1795,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1846,7 +1848,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -1901,7 +1903,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
@@ -1941,7 +1943,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1981,7 +1983,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -2036,7 +2038,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2089,7 +2091,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -2142,7 +2144,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -2196,7 +2198,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -2250,7 +2252,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -2303,7 +2305,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2356,7 +2358,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>311</v>
       </c>
@@ -2408,7 +2410,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2457,7 +2459,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2506,7 +2508,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2543,7 +2545,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2581,10 +2583,10 @@
       </c>
       <c r="N17" s="61"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K19" s="62"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L20" s="63"/>
     </row>
   </sheetData>
@@ -2605,26 +2607,26 @@
       <selection pane="topRight" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.75" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="15.25" customWidth="1"/>
-    <col min="6" max="6" width="11.08203125" customWidth="1"/>
+    <col min="6" max="6" width="11.125" customWidth="1"/>
     <col min="7" max="7" width="17.75" customWidth="1"/>
     <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.375" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="43.5" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="19.08203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.375" customWidth="1"/>
+    <col min="13" max="13" width="19.125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="10.5" customWidth="1"/>
     <col min="16" max="16" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2737,7 +2739,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2830,7 +2832,7 @@
         <v>1216.528453322951</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -2872,7 +2874,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2965,7 +2967,7 @@
         <v>2101.97739666605</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -3058,7 +3060,7 @@
         <v>1171.0983188067505</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -3151,7 +3153,7 @@
         <v>2214.52431017765</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -3259,7 +3261,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -3356,7 +3358,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -3457,7 +3459,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -3499,7 +3501,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -3535,7 +3537,7 @@
       <c r="L11" s="43"/>
       <c r="O11" s="36"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -3583,7 +3585,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -3631,7 +3633,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -3670,7 +3672,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -3709,7 +3711,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -3745,7 +3747,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -3781,7 +3783,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -3818,7 +3820,7 @@
       </c>
       <c r="O18" s="53"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -3855,7 +3857,7 @@
       </c>
       <c r="O19" s="53"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L23">
         <v>1000</v>
       </c>
@@ -3889,16 +3891,16 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.58203125" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="30.375" customWidth="1"/>
+    <col min="3" max="3" width="8.375" customWidth="1"/>
+    <col min="4" max="4" width="23.875" customWidth="1"/>
     <col min="5" max="25" width="8.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3975,7 +3977,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -4052,7 +4054,7 @@
         <v>1216.528453322951</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -4129,7 +4131,7 @@
         <v>2101.97739666605</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
@@ -4206,7 +4208,7 @@
         <v>1171.0983188067505</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>35</v>
       </c>
@@ -4283,7 +4285,7 @@
         <v>2214.52431017765</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>36</v>
       </c>
@@ -4360,7 +4362,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>37</v>
       </c>
@@ -4437,7 +4439,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>45</v>
       </c>
@@ -4514,7 +4516,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -4604,15 +4606,15 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.08203125" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="21.58203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.125" customWidth="1"/>
+    <col min="2" max="2" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>291</v>
       </c>
@@ -4695,7 +4697,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>292</v>
       </c>
@@ -4778,7 +4780,7 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>292</v>
       </c>
@@ -4861,7 +4863,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>293</v>
       </c>
@@ -4944,7 +4946,7 @@
         <v>14800</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>293</v>
       </c>
@@ -5027,7 +5029,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>140</v>
       </c>
@@ -5110,7 +5112,7 @@
         <v>3.4782608695652177</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>140</v>
       </c>
@@ -5193,7 +5195,7 @@
         <v>21.118012422360248</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>140</v>
       </c>
@@ -5276,7 +5278,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>140</v>
       </c>
@@ -5359,7 +5361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>292</v>
       </c>
@@ -5442,7 +5444,7 @@
         <v>4.9689440993788822E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -5525,7 +5527,7 @@
         <v>310000</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>140</v>
       </c>
@@ -5608,7 +5610,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>140</v>
       </c>
@@ -5691,7 +5693,7 @@
         <v>83854.869455332082</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>140</v>
       </c>
@@ -5774,7 +5776,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>140</v>
       </c>
@@ -5857,7 +5859,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>140</v>
       </c>
@@ -5940,7 +5942,7 @@
         <v>39760971.535051085</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>140</v>
       </c>
@@ -6023,7 +6025,7 @@
         <v>2572768.7463856577</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>140</v>
       </c>
@@ -6106,7 +6108,7 @@
         <v>5769.2307692307695</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>140</v>
       </c>
@@ -6189,7 +6191,7 @@
         <v>230.76923076923077</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>140</v>
       </c>
@@ -6285,13 +6287,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08203125" customWidth="1"/>
+    <col min="2" max="2" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6362,7 +6364,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6433,7 +6435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -6504,7 +6506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -6575,7 +6577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -6646,7 +6648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -6730,17 +6732,17 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.75" customWidth="1"/>
     <col min="2" max="2" width="20.75" customWidth="1"/>
-    <col min="3" max="3" width="20.58203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.375" customWidth="1"/>
+    <col min="6" max="6" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>157</v>
       </c>
@@ -6763,7 +6765,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
@@ -6784,7 +6786,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
@@ -6805,7 +6807,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>34</v>
       </c>
@@ -6826,7 +6828,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>35</v>
       </c>
@@ -6847,7 +6849,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>140</v>
       </c>
@@ -6868,7 +6870,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>140</v>
       </c>
@@ -6889,7 +6891,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>38</v>
       </c>
@@ -6910,7 +6912,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
@@ -6931,7 +6933,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>58</v>
       </c>
@@ -6952,7 +6954,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>140</v>
       </c>
@@ -6973,7 +6975,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>140</v>
       </c>
@@ -6994,7 +6996,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>38</v>
       </c>
@@ -7015,7 +7017,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>140</v>
       </c>
@@ -7036,7 +7038,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>140</v>
       </c>
@@ -7057,7 +7059,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>160</v>
       </c>
@@ -7078,7 +7080,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>160</v>
       </c>
@@ -7099,7 +7101,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>140</v>
       </c>
@@ -7120,7 +7122,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>140</v>
       </c>
@@ -7141,7 +7143,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="50" t="s">
         <v>159</v>
       </c>
@@ -7149,7 +7151,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="51" t="s">
         <v>12</v>
       </c>
@@ -7157,7 +7159,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="51" t="s">
         <v>19</v>
       </c>
@@ -7165,7 +7167,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
         <v>19</v>
       </c>
@@ -7173,7 +7175,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="51" t="s">
         <v>38</v>
       </c>
@@ -7181,7 +7183,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="51" t="s">
         <v>38</v>
       </c>
@@ -7189,7 +7191,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="51" t="s">
         <v>38</v>
       </c>
@@ -7197,7 +7199,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="51" t="s">
         <v>70</v>
       </c>
@@ -7219,17 +7221,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.58203125" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -7258,7 +7260,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>58</v>
       </c>
@@ -7269,7 +7271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -7280,7 +7282,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -7297,7 +7299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -7305,7 +7307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>168</v>
       </c>
@@ -7326,17 +7328,17 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.875" customWidth="1"/>
+    <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.58203125" customWidth="1"/>
+    <col min="4" max="4" width="40.875" customWidth="1"/>
+    <col min="5" max="5" width="30.625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -7365,7 +7367,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>58</v>
       </c>
@@ -7392,7 +7394,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>154</v>
       </c>
@@ -7419,7 +7421,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
@@ -7446,7 +7448,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
@@ -7473,7 +7475,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>22</v>
       </c>
@@ -7500,7 +7502,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
@@ -7523,7 +7525,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>36</v>
       </c>
@@ -7546,7 +7548,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>179</v>
       </c>
@@ -7571,7 +7573,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>179</v>
       </c>
@@ -7596,7 +7598,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>183</v>
       </c>
@@ -7621,7 +7623,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>183</v>
       </c>
@@ -7640,7 +7642,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -7655,7 +7657,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -7670,7 +7672,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>188</v>
       </c>
@@ -7697,7 +7699,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>171</v>
       </c>
@@ -7720,7 +7722,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>176</v>
       </c>
@@ -7743,7 +7745,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>179</v>
       </c>
@@ -7766,7 +7768,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>183</v>
       </c>
@@ -7780,7 +7782,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>184</v>
       </c>
@@ -7794,7 +7796,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>37</v>
       </c>
@@ -7808,7 +7810,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>36</v>
       </c>
@@ -7822,12 +7824,12 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>0</v>
       </c>
@@ -7844,7 +7846,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>58</v>
       </c>
@@ -7853,7 +7855,7 @@
       </c>
       <c r="C32" s="14"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>154</v>
       </c>
@@ -7862,7 +7864,7 @@
       </c>
       <c r="C33" s="14"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>50</v>
       </c>
@@ -7871,7 +7873,7 @@
       </c>
       <c r="C34" s="14"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>11</v>
       </c>
@@ -7882,7 +7884,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>22</v>
       </c>
@@ -7891,7 +7893,7 @@
       </c>
       <c r="C36" s="14"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>209</v>
       </c>
@@ -7900,7 +7902,7 @@
       </c>
       <c r="C37" s="14"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>35</v>
       </c>
@@ -7909,7 +7911,7 @@
       </c>
       <c r="C38" s="14"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>37</v>
       </c>
@@ -7923,7 +7925,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>36</v>
       </c>
@@ -7937,7 +7939,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>179</v>
       </c>
@@ -7954,7 +7956,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>183</v>
       </c>
@@ -7971,12 +7973,12 @@
         <v>213</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
         <v>1</v>
       </c>
@@ -7987,7 +7989,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>19</v>
       </c>
@@ -7998,7 +8000,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="30" t="s">
         <v>19</v>
       </c>
@@ -8015,7 +8017,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
         <v>19</v>
       </c>
@@ -8032,7 +8034,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
         <v>19</v>
       </c>
@@ -8052,7 +8054,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="s">
         <v>19</v>
       </c>
@@ -8069,7 +8071,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>58</v>
       </c>
@@ -8086,7 +8088,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>58</v>
       </c>
@@ -8097,7 +8099,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="s">
         <v>58</v>
       </c>
@@ -8114,7 +8116,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="27" t="s">
         <v>12</v>
       </c>
@@ -8131,7 +8133,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>12</v>
       </c>
@@ -8142,12 +8144,12 @@
         <v>226</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="26" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
         <v>233</v>
       </c>
@@ -8158,7 +8160,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="29" t="s">
         <v>235</v>
       </c>
@@ -8166,7 +8168,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="27" t="s">
         <v>236</v>
       </c>
@@ -8174,12 +8176,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="26" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="27" t="s">
         <v>238</v>
       </c>
@@ -8187,7 +8189,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="27" t="s">
         <v>239</v>
       </c>
@@ -8208,13 +8210,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.58203125" customWidth="1"/>
-    <col min="2" max="5" width="15.58203125" customWidth="1"/>
+    <col min="1" max="1" width="25.625" customWidth="1"/>
+    <col min="2" max="5" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>241</v>
       </c>
@@ -8234,7 +8236,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>242</v>
       </c>
@@ -8245,7 +8247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -8253,7 +8255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -8261,7 +8263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -8275,7 +8277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>141</v>
       </c>
@@ -8289,7 +8291,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>243</v>
       </c>
@@ -8303,7 +8305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>244</v>
       </c>
@@ -8314,7 +8316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>245</v>
       </c>
@@ -8325,7 +8327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>246</v>
       </c>
@@ -8336,7 +8338,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -8344,7 +8346,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -8365,19 +8367,19 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.25" customWidth="1"/>
     <col min="2" max="2" width="12.75" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="11.25" customWidth="1"/>
     <col min="7" max="7" width="8.25" customWidth="1"/>
-    <col min="8" max="9" width="24.08203125" customWidth="1"/>
+    <col min="8" max="9" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8412,7 +8414,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -8446,7 +8448,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -8483,7 +8485,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -8512,7 +8514,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -8541,7 +8543,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -8570,7 +8572,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -8599,7 +8601,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -8633,7 +8635,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -8670,7 +8672,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
@@ -8699,7 +8701,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -8731,7 +8733,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -8765,7 +8767,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -8794,7 +8796,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -8828,7 +8830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -8865,7 +8867,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>22</v>
       </c>
@@ -8895,7 +8897,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
@@ -8927,7 +8929,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
@@ -8960,7 +8962,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>22</v>
       </c>
@@ -9003,18 +9005,18 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="5" width="26" customWidth="1"/>
-    <col min="6" max="7" width="24.08203125" customWidth="1"/>
+    <col min="6" max="7" width="24.125" customWidth="1"/>
     <col min="8" max="8" width="31.5" customWidth="1"/>
-    <col min="9" max="9" width="36.83203125" customWidth="1"/>
+    <col min="9" max="9" width="36.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9043,7 +9045,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -9066,7 +9068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>11</v>
       </c>
@@ -9095,7 +9097,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -9118,7 +9120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -9141,7 +9143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -9164,7 +9166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -9187,7 +9189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
         <v>37</v>
       </c>
@@ -9210,7 +9212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>44</v>
       </c>
@@ -9237,7 +9239,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>45</v>
       </c>
@@ -9264,7 +9266,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="55" t="s">
         <v>40</v>
       </c>
@@ -9293,7 +9295,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="55" t="s">
         <v>37</v>
       </c>
@@ -9325,7 +9327,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
         <v>36</v>
       </c>
@@ -9357,7 +9359,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>44</v>
       </c>
@@ -9384,7 +9386,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>45</v>
       </c>
@@ -9410,7 +9412,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>44</v>
       </c>
@@ -9434,7 +9436,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>45</v>
       </c>
@@ -9460,7 +9462,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -9486,7 +9488,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -9512,7 +9514,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -9541,7 +9543,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -9570,7 +9572,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -9593,7 +9595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="55" t="s">
         <v>11</v>
       </c>
@@ -9622,7 +9624,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -9645,7 +9647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -9668,7 +9670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -9691,7 +9693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -9714,7 +9716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -9737,7 +9739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>44</v>
       </c>
@@ -9764,7 +9766,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>45</v>
       </c>
@@ -9791,7 +9793,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="55" t="s">
         <v>40</v>
       </c>
@@ -9820,7 +9822,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
         <v>37</v>
       </c>
@@ -9849,7 +9851,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>44</v>
       </c>
@@ -9876,7 +9878,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>45</v>
       </c>
@@ -9902,7 +9904,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="55" t="s">
         <v>36</v>
       </c>
@@ -9931,7 +9933,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -9958,7 +9960,7 @@
       </c>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -9984,7 +9986,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>47</v>
       </c>
@@ -10010,7 +10012,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>50</v>
       </c>
@@ -10036,7 +10038,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -10062,7 +10064,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -10088,7 +10090,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -10111,7 +10113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="55" t="s">
         <v>11</v>
       </c>
@@ -10140,7 +10142,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -10163,7 +10165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
@@ -10186,7 +10188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
@@ -10209,7 +10211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -10232,7 +10234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -10255,7 +10257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>44</v>
       </c>
@@ -10282,7 +10284,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>45</v>
       </c>
@@ -10309,7 +10311,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="55" t="s">
         <v>40</v>
       </c>
@@ -10338,7 +10340,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="55" t="s">
         <v>37</v>
       </c>
@@ -10367,7 +10369,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>44</v>
       </c>
@@ -10394,7 +10396,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>45</v>
       </c>
@@ -10420,7 +10422,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="55" t="s">
         <v>36</v>
       </c>
@@ -10449,7 +10451,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>44</v>
       </c>
@@ -10476,7 +10478,7 @@
       </c>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>45</v>
       </c>
@@ -10502,7 +10504,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>47</v>
       </c>
@@ -10528,7 +10530,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>50</v>
       </c>
@@ -10554,7 +10556,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -10577,7 +10579,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -10600,10 +10602,10 @@
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F67" s="5"/>
     </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F68" s="64"/>
     </row>
   </sheetData>
@@ -10629,17 +10631,17 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="173.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="173.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -10659,7 +10661,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -10676,7 +10678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -10693,7 +10695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -10713,7 +10715,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -10730,7 +10732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>48</v>
       </c>
@@ -10760,17 +10762,17 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.58203125" customWidth="1"/>
-    <col min="2" max="2" width="19.08203125" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="25.75" customWidth="1"/>
-    <col min="6" max="6" width="19.08203125" customWidth="1"/>
+    <col min="6" max="6" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -10853,7 +10855,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -10936,7 +10938,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -11019,7 +11021,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -11102,7 +11104,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -11185,7 +11187,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -11268,7 +11270,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -11351,7 +11353,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -11434,7 +11436,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -11538,7 +11540,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -11642,7 +11644,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -11725,7 +11727,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -11829,7 +11831,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -11933,7 +11935,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>48</v>
       </c>
@@ -12016,7 +12018,7 @@
         <v>80.36</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
@@ -12120,7 +12122,7 @@
         <v>80.36</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
@@ -12238,18 +12240,18 @@
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.875" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="8" width="24.08203125" customWidth="1"/>
+    <col min="7" max="8" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12287,7 +12289,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -12304,7 +12306,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -12334,7 +12336,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -12352,7 +12354,7 @@
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -12370,7 +12372,7 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -12388,7 +12390,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>36</v>
       </c>
@@ -12406,7 +12408,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>37</v>
       </c>
@@ -12424,7 +12426,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -12442,7 +12444,7 @@
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -12460,7 +12462,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -12490,7 +12492,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -12520,7 +12522,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -12551,7 +12553,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -12569,7 +12571,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -12587,7 +12589,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -12604,7 +12606,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>44</v>
       </c>
@@ -12621,7 +12623,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>47</v>
       </c>
@@ -12638,7 +12640,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -12655,7 +12657,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -12672,7 +12674,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -12689,7 +12691,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -12709,7 +12711,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -12746,7 +12748,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -12767,7 +12769,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -12785,7 +12787,7 @@
       </c>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -12803,7 +12805,7 @@
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>36</v>
       </c>
@@ -12821,7 +12823,7 @@
       </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>37</v>
       </c>
@@ -12839,7 +12841,7 @@
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>45</v>
       </c>
@@ -12857,7 +12859,7 @@
       </c>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -12875,7 +12877,7 @@
       </c>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
@@ -12912,7 +12914,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -12949,7 +12951,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -12980,7 +12982,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>45</v>
       </c>
@@ -12998,7 +13000,7 @@
       </c>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>44</v>
       </c>
@@ -13016,7 +13018,7 @@
       </c>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>45</v>
       </c>
@@ -13036,7 +13038,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>44</v>
       </c>
@@ -13056,7 +13058,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>47</v>
       </c>
@@ -13076,7 +13078,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>50</v>
       </c>
@@ -13096,7 +13098,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -13113,7 +13115,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -13130,35 +13132,35 @@
         <v>83</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
     </row>
@@ -13172,29 +13174,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16BE7FC-A8FD-4D95-933D-26AA617CB019}">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+    <sheetView tabSelected="1" topLeftCell="D25" workbookViewId="0">
+      <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.9140625" customWidth="1"/>
-    <col min="4" max="4" width="34.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="34.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.4140625" customWidth="1"/>
+    <col min="6" max="6" width="18.375" customWidth="1"/>
     <col min="7" max="7" width="10.25" style="13" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="11.75" customWidth="1"/>
-    <col min="13" max="13" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.75" style="69" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="61.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -13231,7 +13233,7 @@
       <c r="L1" t="s">
         <v>319</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="69" t="s">
         <v>331</v>
       </c>
       <c r="N1" t="s">
@@ -13241,7 +13243,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -13278,7 +13280,7 @@
       <c r="L2">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="69">
         <f>L2</f>
         <v>5.0999999999999997E-2</v>
       </c>
@@ -13286,7 +13288,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -13323,7 +13325,7 @@
       <c r="L3">
         <v>9.6900000000000007E-3</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="69">
         <f t="shared" ref="M3:M8" si="0">L3</f>
         <v>9.6900000000000007E-3</v>
       </c>
@@ -13331,7 +13333,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -13368,7 +13370,7 @@
       <c r="L4">
         <v>1.6320000000000001E-2</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="69">
         <f t="shared" si="0"/>
         <v>1.6320000000000001E-2</v>
       </c>
@@ -13376,7 +13378,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -13410,10 +13412,10 @@
       <c r="K5">
         <v>8.3034948476273795E-3</v>
       </c>
-      <c r="L5" s="69">
+      <c r="L5" s="68">
         <v>2.2265403611043637</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="69">
         <f t="shared" si="0"/>
         <v>2.2265403611043637</v>
       </c>
@@ -13421,7 +13423,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -13455,10 +13457,10 @@
       <c r="K6">
         <v>8.3034948476273795E-3</v>
       </c>
-      <c r="L6" s="69">
+      <c r="L6" s="68">
         <v>0.44530807222087276</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="69">
         <f t="shared" si="0"/>
         <v>0.44530807222087276</v>
       </c>
@@ -13466,7 +13468,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -13503,7 +13505,7 @@
       <c r="L7" s="2">
         <v>0.60723828030119009</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="69">
         <f t="shared" si="0"/>
         <v>0.60723828030119009</v>
       </c>
@@ -13511,7 +13513,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -13548,7 +13550,7 @@
       <c r="L8">
         <v>0.78800000000000003</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="69">
         <f t="shared" si="0"/>
         <v>0.78800000000000003</v>
       </c>
@@ -13556,7 +13558,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -13590,14 +13592,14 @@
       <c r="K9">
         <v>3.7832039152811102E-2</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M9" s="69" t="s">
         <v>343</v>
       </c>
       <c r="N9" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -13631,14 +13633,14 @@
       <c r="K10">
         <v>3.7832039152811102E-2</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M10" s="69" t="s">
         <v>343</v>
       </c>
       <c r="N10" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -13663,14 +13665,14 @@
       <c r="L11" t="s">
         <v>343</v>
       </c>
-      <c r="M11" t="s">
+      <c r="M11" s="69" t="s">
         <v>343</v>
       </c>
       <c r="N11" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -13695,14 +13697,14 @@
       <c r="L12" t="s">
         <v>343</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="69" t="s">
         <v>343</v>
       </c>
       <c r="N12" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -13727,14 +13729,14 @@
       <c r="L13" t="s">
         <v>343</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="69" t="s">
         <v>343</v>
       </c>
       <c r="N13" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -13768,10 +13770,10 @@
       <c r="K14" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L14" s="69">
+      <c r="L14" s="68">
         <v>4.9157303370786503</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="69">
         <f>L14</f>
         <v>4.9157303370786503</v>
       </c>
@@ -13779,7 +13781,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -13813,10 +13815,10 @@
       <c r="K15" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L15" s="69">
+      <c r="L15" s="68">
         <v>1.2780898876404492</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="69">
         <f t="shared" ref="M15:M25" si="1">L15</f>
         <v>1.2780898876404492</v>
       </c>
@@ -13824,7 +13826,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -13858,10 +13860,10 @@
       <c r="K16" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L16" s="69">
+      <c r="L16" s="68">
         <v>1.7205056179775278</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="69">
         <f t="shared" si="1"/>
         <v>1.7205056179775278</v>
       </c>
@@ -13869,7 +13871,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -13903,10 +13905,10 @@
       <c r="K17" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L17" s="69">
+      <c r="L17" s="68">
         <v>4.9157303370786503</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="69">
         <f t="shared" si="1"/>
         <v>4.9157303370786503</v>
       </c>
@@ -13914,7 +13916,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -13948,10 +13950,10 @@
       <c r="K18" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L18" s="69">
+      <c r="L18" s="68">
         <v>1.2780898876404492</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="69">
         <f t="shared" si="1"/>
         <v>1.2780898876404492</v>
       </c>
@@ -13959,7 +13961,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -13993,10 +13995,10 @@
       <c r="K19" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L19" s="69">
+      <c r="L19" s="68">
         <v>1.7205056179775278</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="69">
         <f t="shared" si="1"/>
         <v>1.7205056179775278</v>
       </c>
@@ -14004,7 +14006,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>45</v>
       </c>
@@ -14038,10 +14040,10 @@
       <c r="K20" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L20" s="69">
+      <c r="L20" s="68">
         <v>4.9157303370786503</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="69">
         <f t="shared" si="1"/>
         <v>4.9157303370786503</v>
       </c>
@@ -14049,7 +14051,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>45</v>
       </c>
@@ -14083,10 +14085,10 @@
       <c r="K21" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L21" s="69">
+      <c r="L21" s="68">
         <v>1.2780898876404492</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="69">
         <f t="shared" si="1"/>
         <v>1.2780898876404492</v>
       </c>
@@ -14094,7 +14096,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -14128,10 +14130,10 @@
       <c r="K22" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L22" s="69">
+      <c r="L22" s="68">
         <v>1.7205056179775278</v>
       </c>
-      <c r="M22">
+      <c r="M22" s="69">
         <f t="shared" si="1"/>
         <v>1.7205056179775278</v>
       </c>
@@ -14139,7 +14141,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -14173,10 +14175,10 @@
       <c r="K23" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L23" s="69">
+      <c r="L23" s="68">
         <v>4.9157303370786503</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="69">
         <f t="shared" si="1"/>
         <v>4.9157303370786503</v>
       </c>
@@ -14184,7 +14186,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -14218,10 +14220,10 @@
       <c r="K24" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L24" s="69">
+      <c r="L24" s="68">
         <v>1.2780898876404492</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="69">
         <f t="shared" si="1"/>
         <v>1.2780898876404492</v>
       </c>
@@ -14229,7 +14231,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -14263,10 +14265,10 @@
       <c r="K25" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L25" s="69">
+      <c r="L25" s="68">
         <v>1.7205056179775278</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="69">
         <f t="shared" si="1"/>
         <v>1.7205056179775278</v>
       </c>
@@ -14274,7 +14276,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -14305,11 +14307,11 @@
       <c r="L26" t="s">
         <v>343</v>
       </c>
-      <c r="M26" t="s">
+      <c r="M26" s="69" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -14340,11 +14342,11 @@
       <c r="L27" t="s">
         <v>343</v>
       </c>
-      <c r="M27" t="s">
+      <c r="M27" s="69" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -14375,11 +14377,11 @@
       <c r="L28" t="s">
         <v>343</v>
       </c>
-      <c r="M28" t="s">
+      <c r="M28" s="69" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -14416,9 +14418,9 @@
       <c r="L29" s="2">
         <v>10.436</v>
       </c>
-      <c r="M29" s="2">
-        <f>L29/365*2.37</f>
-        <v>6.776252054794521E-2</v>
+      <c r="M29" s="69">
+        <f>L29/365/2.37</f>
+        <v>1.2064042540893589E-2</v>
       </c>
       <c r="N29" t="s">
         <v>335</v>
@@ -14427,7 +14429,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -14464,9 +14466,9 @@
       <c r="L30" s="2">
         <v>0.16161616161616163</v>
       </c>
-      <c r="M30" s="2">
-        <f t="shared" ref="M30:M31" si="2">L30/365*2.37</f>
-        <v>1.049398090493981E-3</v>
+      <c r="M30" s="69">
+        <f>L30/365/2.37</f>
+        <v>1.8682869385140932E-4</v>
       </c>
       <c r="N30" t="s">
         <v>335</v>
@@ -14475,7 +14477,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -14512,9 +14514,9 @@
       <c r="L31" s="2">
         <v>8.0808080808080815E-2</v>
       </c>
-      <c r="M31" s="2">
-        <f t="shared" si="2"/>
-        <v>5.2469904524699051E-4</v>
+      <c r="M31" s="69">
+        <f>L31/365/2.37</f>
+        <v>9.341434692570466E-5</v>
       </c>
       <c r="N31" t="s">
         <v>335</v>
@@ -14523,7 +14525,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -14560,9 +14562,9 @@
       <c r="L32">
         <v>0.23400000000000001</v>
       </c>
-      <c r="M32" s="48">
-        <f>L32*7.46</f>
-        <v>1.7456400000000001</v>
+      <c r="M32" s="70">
+        <f>L32/7.46</f>
+        <v>3.1367292225201071E-2</v>
       </c>
       <c r="N32" t="s">
         <v>335</v>
@@ -14571,7 +14573,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -14608,9 +14610,9 @@
       <c r="L33" s="67">
         <v>2.8080000000000004E-2</v>
       </c>
-      <c r="M33" s="48">
-        <f t="shared" ref="M33:M37" si="3">L33*7.46</f>
-        <v>0.20947680000000002</v>
+      <c r="M33" s="70">
+        <f>L33/7.46</f>
+        <v>3.7640750670241293E-3</v>
       </c>
       <c r="N33" t="s">
         <v>335</v>
@@ -14619,7 +14621,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -14656,9 +14658,9 @@
       <c r="L34">
         <v>5.6160000000000009E-2</v>
       </c>
-      <c r="M34" s="48">
-        <f t="shared" si="3"/>
-        <v>0.41895360000000004</v>
+      <c r="M34" s="70">
+        <f>L34/7.46</f>
+        <v>7.5281501340482586E-3</v>
       </c>
       <c r="N34" t="s">
         <v>335</v>
@@ -14667,7 +14669,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -14704,9 +14706,9 @@
       <c r="L35">
         <v>0.23400000000000001</v>
       </c>
-      <c r="M35" s="48">
-        <f t="shared" si="3"/>
-        <v>1.7456400000000001</v>
+      <c r="M35" s="70">
+        <f>L35/7.46</f>
+        <v>3.1367292225201071E-2</v>
       </c>
       <c r="N35" t="s">
         <v>335</v>
@@ -14715,7 +14717,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -14752,9 +14754,9 @@
       <c r="L36" s="67">
         <v>2.8080000000000001E-2</v>
       </c>
-      <c r="M36" s="48">
-        <f t="shared" si="3"/>
-        <v>0.20947680000000002</v>
+      <c r="M36" s="70">
+        <f>L36/7.46</f>
+        <v>3.7640750670241288E-3</v>
       </c>
       <c r="N36" t="s">
         <v>335</v>
@@ -14763,7 +14765,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -14800,9 +14802,9 @@
       <c r="L37">
         <v>5.6160000000000002E-2</v>
       </c>
-      <c r="M37" s="48">
-        <f t="shared" si="3"/>
-        <v>0.41895360000000004</v>
+      <c r="M37" s="70">
+        <f>L37/7.46</f>
+        <v>7.5281501340482577E-3</v>
       </c>
       <c r="N37" t="s">
         <v>335</v>
@@ -14811,7 +14813,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -14848,9 +14850,9 @@
       <c r="L38" s="2">
         <v>10.436</v>
       </c>
-      <c r="M38" s="68">
-        <f>L38/365*2.37</f>
-        <v>6.776252054794521E-2</v>
+      <c r="M38" s="71">
+        <f>L38/365/2.37</f>
+        <v>1.2064042540893589E-2</v>
       </c>
       <c r="N38" t="s">
         <v>335</v>
@@ -14859,7 +14861,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>45</v>
       </c>
@@ -14896,9 +14898,9 @@
       <c r="L39" s="2">
         <v>0.16161616161616163</v>
       </c>
-      <c r="M39" s="68">
-        <f t="shared" ref="M39:M43" si="4">L39/365*2.37</f>
-        <v>1.049398090493981E-3</v>
+      <c r="M39" s="71">
+        <f>L39/365/2.37</f>
+        <v>1.8682869385140932E-4</v>
       </c>
       <c r="N39" t="s">
         <v>335</v>
@@ -14907,7 +14909,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>45</v>
       </c>
@@ -14944,9 +14946,9 @@
       <c r="L40" s="2">
         <v>8.0808080808080815E-2</v>
       </c>
-      <c r="M40" s="68">
-        <f t="shared" si="4"/>
-        <v>5.2469904524699051E-4</v>
+      <c r="M40" s="71">
+        <f>L40/365/2.37</f>
+        <v>9.341434692570466E-5</v>
       </c>
       <c r="N40" t="s">
         <v>335</v>
@@ -14955,7 +14957,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>44</v>
       </c>
@@ -14992,9 +14994,9 @@
       <c r="L41" s="2">
         <v>10.436</v>
       </c>
-      <c r="M41" s="68">
-        <f t="shared" si="4"/>
-        <v>6.776252054794521E-2</v>
+      <c r="M41" s="71">
+        <f>L41/365/2.37</f>
+        <v>1.2064042540893589E-2</v>
       </c>
       <c r="N41" t="s">
         <v>335</v>
@@ -15003,7 +15005,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>44</v>
       </c>
@@ -15040,9 +15042,9 @@
       <c r="L42" s="2">
         <v>0.16161616161616163</v>
       </c>
-      <c r="M42" s="68">
-        <f t="shared" si="4"/>
-        <v>1.049398090493981E-3</v>
+      <c r="M42" s="71">
+        <f>L42/365/2.37</f>
+        <v>1.8682869385140932E-4</v>
       </c>
       <c r="N42" t="s">
         <v>335</v>
@@ -15051,7 +15053,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -15088,9 +15090,9 @@
       <c r="L43" s="2">
         <v>8.0808080808080815E-2</v>
       </c>
-      <c r="M43" s="68">
-        <f t="shared" si="4"/>
-        <v>5.2469904524699051E-4</v>
+      <c r="M43" s="71">
+        <f>L43/365/2.37</f>
+        <v>9.341434692570466E-5</v>
       </c>
       <c r="N43" t="s">
         <v>335</v>
@@ -15099,7 +15101,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -15136,9 +15138,9 @@
       <c r="L44">
         <v>0.23400000000000001</v>
       </c>
-      <c r="M44" s="2">
-        <f>L44*0.965</f>
-        <v>0.22581000000000001</v>
+      <c r="M44" s="69">
+        <f>L44/0.965</f>
+        <v>0.24248704663212436</v>
       </c>
       <c r="N44" t="s">
         <v>339</v>
@@ -15147,7 +15149,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -15181,7 +15183,7 @@
       <c r="K45">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="M45" s="2" t="s">
+      <c r="M45" s="69" t="s">
         <v>343</v>
       </c>
       <c r="N45" t="s">
@@ -15191,7 +15193,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -15225,7 +15227,7 @@
       <c r="K46">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="M46" s="2" t="s">
+      <c r="M46" s="69" t="s">
         <v>343</v>
       </c>
       <c r="N46" t="s">
@@ -15235,7 +15237,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -15272,9 +15274,9 @@
       <c r="L47">
         <v>0.23400000000000001</v>
       </c>
-      <c r="M47" s="2">
-        <f>L47*0.965</f>
-        <v>0.22581000000000001</v>
+      <c r="M47" s="69">
+        <f>L47/0.965</f>
+        <v>0.24248704663212436</v>
       </c>
       <c r="N47" t="s">
         <v>339</v>
@@ -15283,7 +15285,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -15317,7 +15319,7 @@
       <c r="K48">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="M48" s="2" t="s">
+      <c r="M48" s="69" t="s">
         <v>343</v>
       </c>
       <c r="N48" t="s">
@@ -15327,7 +15329,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>44</v>
       </c>
@@ -15361,7 +15363,7 @@
       <c r="K49">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="M49" s="2" t="s">
+      <c r="M49" s="69" t="s">
         <v>343</v>
       </c>
       <c r="N49" t="s">
@@ -15371,7 +15373,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -15408,9 +15410,9 @@
       <c r="L50">
         <v>0.23400000000000001</v>
       </c>
-      <c r="M50" s="2">
-        <f>L50*0.007</f>
-        <v>1.6380000000000001E-3</v>
+      <c r="M50" s="69">
+        <f>L50/0.007</f>
+        <v>33.428571428571431</v>
       </c>
       <c r="N50" t="s">
         <v>341</v>
@@ -15419,7 +15421,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -15453,7 +15455,7 @@
       <c r="K51">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="M51" s="2" t="s">
+      <c r="M51" s="69" t="s">
         <v>343</v>
       </c>
       <c r="N51" t="s">
@@ -15463,7 +15465,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -15497,7 +15499,7 @@
       <c r="K52">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="M52" s="2" t="s">
+      <c r="M52" s="69" t="s">
         <v>343</v>
       </c>
       <c r="N52" t="s">
@@ -15507,7 +15509,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -15544,9 +15546,9 @@
       <c r="L53">
         <v>0.23400000000000001</v>
       </c>
-      <c r="M53" s="2">
-        <f>L53*0.007</f>
-        <v>1.6380000000000001E-3</v>
+      <c r="M53" s="69">
+        <f>L53/0.007</f>
+        <v>33.428571428571431</v>
       </c>
       <c r="N53" t="s">
         <v>341</v>
@@ -15555,7 +15557,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -15592,9 +15594,9 @@
       <c r="L54" s="67">
         <v>2.8080000000000004E-2</v>
       </c>
-      <c r="M54" s="2">
-        <f t="shared" ref="M54:M58" si="5">L54*0.007</f>
-        <v>1.9656000000000003E-4</v>
+      <c r="M54" s="69">
+        <f>L54/0.007</f>
+        <v>4.0114285714285716</v>
       </c>
       <c r="N54" t="s">
         <v>341</v>
@@ -15603,7 +15605,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -15640,9 +15642,9 @@
       <c r="L55">
         <v>5.6160000000000009E-2</v>
       </c>
-      <c r="M55" s="2">
-        <f t="shared" si="5"/>
-        <v>3.9312000000000006E-4</v>
+      <c r="M55" s="69">
+        <f t="shared" ref="M55:M58" si="2">L55/0.007</f>
+        <v>8.0228571428571431</v>
       </c>
       <c r="N55" t="s">
         <v>341</v>
@@ -15651,7 +15653,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -15688,9 +15690,9 @@
       <c r="L56">
         <v>0.23400000000000001</v>
       </c>
-      <c r="M56" s="2">
-        <f t="shared" si="5"/>
-        <v>1.6380000000000001E-3</v>
+      <c r="M56" s="69">
+        <f t="shared" si="2"/>
+        <v>33.428571428571431</v>
       </c>
       <c r="N56" t="s">
         <v>341</v>
@@ -15699,7 +15701,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>36</v>
       </c>
@@ -15736,9 +15738,9 @@
       <c r="L57" s="67">
         <v>2.8080000000000004E-2</v>
       </c>
-      <c r="M57" s="2">
-        <f t="shared" si="5"/>
-        <v>1.9656000000000003E-4</v>
+      <c r="M57" s="69">
+        <f t="shared" si="2"/>
+        <v>4.0114285714285716</v>
       </c>
       <c r="N57" t="s">
         <v>341</v>
@@ -15747,7 +15749,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -15784,9 +15786,9 @@
       <c r="L58">
         <v>5.6160000000000009E-2</v>
       </c>
-      <c r="M58" s="2">
-        <f t="shared" si="5"/>
-        <v>3.9312000000000006E-4</v>
+      <c r="M58" s="69">
+        <f t="shared" si="2"/>
+        <v>8.0228571428571431</v>
       </c>
       <c r="N58" t="s">
         <v>341</v>
@@ -15809,21 +15811,21 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="68.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -15855,7 +15857,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -15875,7 +15877,7 @@
         <v>3.4599999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>11</v>
       </c>
@@ -15899,7 +15901,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -15919,7 +15921,7 @@
         <v>2.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -15939,7 +15941,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -15959,7 +15961,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -15979,7 +15981,7 @@
         <v>4.0899999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -15999,7 +16001,7 @@
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -16019,7 +16021,7 @@
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -16039,7 +16041,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -16059,7 +16061,7 @@
         <v>5.62E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -16079,7 +16081,7 @@
         <v>5.62E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -16112,15 +16114,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5" customWidth="1"/>
     <col min="4" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -16137,7 +16139,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -16154,7 +16156,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Adding emission factors and commodity prices
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7DACD4-A74A-4EEC-BE04-6C9C530D5889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB9195A-6F6C-4B42-A630-75D12C1F5676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="622" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="5835" yWindow="1155" windowWidth="26490" windowHeight="12180" tabRatio="622" activeTab="7" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -20,26 +20,28 @@
     <sheet name="C2U CI" sheetId="10" r:id="rId5"/>
     <sheet name="F2C Water" sheetId="13" r:id="rId6"/>
     <sheet name="F2C Jobs" sheetId="23" r:id="rId7"/>
-    <sheet name="F2C Jobs old" sheetId="11" r:id="rId8"/>
-    <sheet name="Infrastructure" sheetId="19" r:id="rId9"/>
-    <sheet name="Unit Conversion" sheetId="18" r:id="rId10"/>
-    <sheet name="Conversion" sheetId="15" r:id="rId11"/>
-    <sheet name="Feedstock to Commodity Buildout" sheetId="7" r:id="rId12"/>
-    <sheet name="Commodity to Use Buildout" sheetId="8" r:id="rId13"/>
-    <sheet name="F2C_ver2" sheetId="20" r:id="rId14"/>
-    <sheet name="Commodity To Use Matrix" sheetId="6" r:id="rId15"/>
-    <sheet name="table from Julia (to be deleted" sheetId="16" r:id="rId16"/>
-    <sheet name="Feedstock to Commodity Matrix" sheetId="4" r:id="rId17"/>
+    <sheet name="Emissions" sheetId="24" r:id="rId8"/>
+    <sheet name="Commodity Prices" sheetId="25" r:id="rId9"/>
+    <sheet name="F2C Jobs old" sheetId="11" r:id="rId10"/>
+    <sheet name="Infrastructure" sheetId="19" r:id="rId11"/>
+    <sheet name="Unit Conversion" sheetId="18" r:id="rId12"/>
+    <sheet name="Conversion" sheetId="15" r:id="rId13"/>
+    <sheet name="Feedstock to Commodity Buildout" sheetId="7" r:id="rId14"/>
+    <sheet name="Commodity to Use Buildout" sheetId="8" r:id="rId15"/>
+    <sheet name="F2C_ver2" sheetId="20" r:id="rId16"/>
+    <sheet name="Commodity To Use Matrix" sheetId="6" r:id="rId17"/>
+    <sheet name="table from Julia (to be deleted" sheetId="16" r:id="rId18"/>
+    <sheet name="Feedstock to Commodity Matrix" sheetId="4" r:id="rId19"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'C2U CI'!$A$1:$AA$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'F2C CI'!$A$1:$J$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'F2C Conversion'!$A$1:$Q$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'F2C Jobs'!$A$1:$O$58</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'F2C Jobs old'!$A$1:$J$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'F2C Jobs old'!$A$1:$J$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'F2C Land'!$A$1:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'F2C Water'!$A$19:$L$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Unit Conversion'!$A$1:$AK$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'Unit Conversion'!$A$1:$AK$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -62,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2509" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2680" uniqueCount="379">
   <si>
     <t>Feedstock</t>
   </si>
@@ -1114,19 +1116,115 @@
   </si>
   <si>
     <t>2.6 kg biomass/ kg H2</t>
+  </si>
+  <si>
+    <t>NOx Emission</t>
+  </si>
+  <si>
+    <t>PM2.5 Emission</t>
+  </si>
+  <si>
+    <t>DRAFT Mobile Emissions Toolkit for Analysis (META)</t>
+  </si>
+  <si>
+    <t>34,752 tons NOx per billion-gallon diesel, 1billion Gallon is 126,832,800,000 MJ</t>
+  </si>
+  <si>
+    <t>gNOx/MJ-diesel</t>
+  </si>
+  <si>
+    <t>343 tons PM2.5 per billion-gallon diesel</t>
+  </si>
+  <si>
+    <t>gPM2.5/MJ-diesel</t>
+  </si>
+  <si>
+    <t>$ per MW</t>
+  </si>
+  <si>
+    <t>$ per MT</t>
+  </si>
+  <si>
+    <t>$ per MCF</t>
+  </si>
+  <si>
+    <t>$ per Mgal</t>
+  </si>
+  <si>
+    <t>reference</t>
+  </si>
+  <si>
+    <t>6.2 cents per kWh, 2,628,000 kWh/MW (30% CF) * 1 $/100 cents</t>
+  </si>
+  <si>
+    <t>$14 per kw-month</t>
+  </si>
+  <si>
+    <t>20 cents per kWh, 6,044,400kWh/MW (69% CF)</t>
+  </si>
+  <si>
+    <t>7.57 $ per kg</t>
+  </si>
+  <si>
+    <t>46 $ per MMBTU, 0.000965 million cf per MMBTU(EIA)</t>
+  </si>
+  <si>
+    <t>$9.4 per gallon</t>
+  </si>
+  <si>
+    <t>3 cents per kWh, 2,628,000 kWh/MW (30% CF) * 1 $/100 cents</t>
+  </si>
+  <si>
+    <t>$9 per kw-month</t>
+  </si>
+  <si>
+    <t>12.8 cents per kWh, 6,044,400kWh/MW (69% CF)</t>
+  </si>
+  <si>
+    <t>$8.3 per gallon</t>
+  </si>
+  <si>
+    <t>45 $ per MMBTU, 0.000965 million cf per MMBTU(EIA)</t>
+  </si>
+  <si>
+    <t>Annual RPS Report to the Legislature – November 2023</t>
+  </si>
+  <si>
+    <t>Annual RPS Report to the Legislature – November 2024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/energy-division/documents/energy-storage/2023-05-31_lumen_energy-storage-procurement-study-report.pdf </t>
+  </si>
+  <si>
+    <t>Platts, part of S&amp;P Global Commodity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://theicct.org/wp-content/uploads/2023/05/case-studies-california-rng-outlook-2030-may23.pdf </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Platts (2022) </t>
+  </si>
+  <si>
+    <t>Global Air</t>
+  </si>
+  <si>
+    <t>Gross Revenue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="6">
+  <numFmts count="9">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0000000000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="174" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="0.0000"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -1303,12 +1401,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1410,11 +1509,16 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -2140,7 +2244,7 @@
       <c r="L8" s="58" t="s">
         <v>274</v>
       </c>
-      <c r="M8" s="70" t="s">
+      <c r="M8" t="s">
         <v>345</v>
       </c>
       <c r="N8" t="s">
@@ -2609,12 +2713,378 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86CE6374-45B2-3044-B48D-E84DB83BCE11}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2">
+        <v>3.4599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3">
+        <v>3.4599999999999999E-2</v>
+      </c>
+      <c r="G3" s="13"/>
+      <c r="I3" s="13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4">
+        <v>2.3599999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5">
+        <v>2.8199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6">
+        <v>2.8199999999999999E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>89</v>
+      </c>
+      <c r="D7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7">
+        <v>4.0899999999999999E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" t="s">
+        <v>94</v>
+      </c>
+      <c r="E8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8">
+        <v>3.3399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D9" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" t="s">
+        <v>91</v>
+      </c>
+      <c r="F9">
+        <v>3.3399999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" t="s">
+        <v>91</v>
+      </c>
+      <c r="F10">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" t="s">
+        <v>91</v>
+      </c>
+      <c r="F11">
+        <v>5.62E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F12">
+        <v>5.62E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13">
+        <v>1.1299999999999999E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBD7D08-7196-4DD6-A58C-02D5A271324B}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>83.81</v>
+      </c>
+      <c r="C2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="https://netzeroamerica.princeton.edu/img/NZA%20Annex%20F%20-%20HV%20Transmission.pdf" xr:uid="{104B4864-4DDD-469C-B108-01D18B28A224}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA5616B-DF07-465E-AEEB-CCA6D05FE697}">
   <dimension ref="A1:AK23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E3" sqref="E3:F3"/>
+      <selection pane="topRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3893,7 +4363,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87BF8B-8E54-426F-864A-9E457E959B26}">
   <dimension ref="A1:Y9"/>
   <sheetViews>
@@ -4608,7 +5078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4534657-2DF7-8944-A332-1622EE581035}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
@@ -6289,7 +6759,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3F942D-1725-B745-A61F-46451943A74C}">
   <dimension ref="A1:W6"/>
   <sheetViews>
@@ -6734,7 +7204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDDA0F3-A3DE-4AB4-98AB-8BE3425A27E0}">
   <dimension ref="A1:G30"/>
   <sheetViews>
@@ -7223,7 +7693,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30085204-D4C6-FC4C-98EB-2FC1A2E0E66E}">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -7330,7 +7800,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF7B0DD-C673-4DCD-83AE-47E17C286F51}">
   <dimension ref="A1:K68"/>
   <sheetViews>
@@ -8212,7 +8682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6977DE39-83AB-8346-8AC1-EC99E6C87D8C}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -9009,10 +9479,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -9078,7 +9549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>11</v>
       </c>
@@ -9276,7 +9747,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="55" t="s">
         <v>40</v>
       </c>
@@ -9303,7 +9774,7 @@
       </c>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="55" t="s">
         <v>37</v>
       </c>
@@ -9328,14 +9799,14 @@
       <c r="H12" t="s">
         <v>347</v>
       </c>
-      <c r="I12" s="69" t="s">
+      <c r="I12" s="3" t="s">
         <v>340</v>
       </c>
       <c r="J12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
         <v>36</v>
       </c>
@@ -9367,7 +9838,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>42</v>
       </c>
@@ -9394,7 +9865,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>43</v>
       </c>
@@ -9420,7 +9891,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -9444,7 +9915,7 @@
       </c>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -9470,7 +9941,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -9496,7 +9967,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
@@ -9522,7 +9993,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -9551,7 +10022,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -9603,7 +10074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="55" t="s">
         <v>11</v>
       </c>
@@ -9801,7 +10272,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="55" t="s">
         <v>40</v>
       </c>
@@ -9828,7 +10299,7 @@
       </c>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
         <v>37</v>
       </c>
@@ -9857,7 +10328,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>42</v>
       </c>
@@ -9884,7 +10355,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>43</v>
       </c>
@@ -9910,7 +10381,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="55" t="s">
         <v>36</v>
       </c>
@@ -9939,7 +10410,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -9966,7 +10437,7 @@
       </c>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -9992,7 +10463,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -10018,7 +10489,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -10044,7 +10515,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -10070,7 +10541,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -10119,7 +10590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="55" t="s">
         <v>11</v>
       </c>
@@ -10317,7 +10788,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="55" t="s">
         <v>40</v>
       </c>
@@ -10344,7 +10815,7 @@
       </c>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="55" t="s">
         <v>37</v>
       </c>
@@ -10373,7 +10844,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>42</v>
       </c>
@@ -10400,7 +10871,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>43</v>
       </c>
@@ -10426,7 +10897,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="55" t="s">
         <v>36</v>
       </c>
@@ -10455,7 +10926,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -10482,7 +10953,7 @@
       </c>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -10508,7 +10979,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>45</v>
       </c>
@@ -10534,7 +11005,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -10560,7 +11031,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -10583,7 +11054,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -10613,7 +11084,13 @@
       <c r="F68" s="64"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J61" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}"/>
+  <autoFilter ref="A1:J61" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Electricity"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="I40" r:id="rId1" xr:uid="{3DE9360D-4B28-4580-B9AC-7A8A7FDEC5D9}"/>
@@ -10766,10 +11243,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FEFDD9-D46C-E64E-8B04-7DDDC1C1B0F3}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F1" sqref="F1:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10865,7 +11343,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -10948,7 +11426,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -11031,7 +11509,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -11114,7 +11592,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -11197,7 +11675,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -11280,7 +11758,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -11654,7 +12132,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -11737,7 +12215,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -11841,7 +12319,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -11945,7 +12423,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -12028,7 +12506,7 @@
         <v>80.36</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -12132,7 +12610,7 @@
         <v>80.36</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -12237,7 +12715,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA16" xr:uid="{68FEFDD9-D46C-E64E-8B04-7DDDC1C1B0F3}"/>
+  <autoFilter ref="A1:AA16" xr:uid="{68FEFDD9-D46C-E64E-8B04-7DDDC1C1B0F3}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Surface Transport Fuel"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13184,7 +13668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16BE7FC-A8FD-4D95-933D-26AA617CB019}">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
@@ -14317,8 +14801,11 @@
       <c r="L26" t="s">
         <v>338</v>
       </c>
-      <c r="M26" t="s">
-        <v>338</v>
+      <c r="M26">
+        <v>1.3599999999999999E-2</v>
+      </c>
+      <c r="N26" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
@@ -14352,8 +14839,11 @@
       <c r="L27" t="s">
         <v>338</v>
       </c>
-      <c r="M27" t="s">
-        <v>338</v>
+      <c r="M27">
+        <v>2.1061515887119567E-4</v>
+      </c>
+      <c r="N27" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
@@ -14387,8 +14877,11 @@
       <c r="L28" t="s">
         <v>338</v>
       </c>
-      <c r="M28" t="s">
-        <v>338</v>
+      <c r="M28">
+        <v>1.0530757943559784E-4</v>
+      </c>
+      <c r="N28" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -15814,366 +16307,731 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86CE6374-45B2-3044-B48D-E84DB83BCE11}">
-  <dimension ref="A1:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8B6CA4-5F91-483F-9DB3-0E00AF0370F3}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="68.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.25" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="55" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>89</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>348</v>
       </c>
       <c r="D2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F2">
-        <v>3.4599999999999999E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="47" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="47" t="s">
+        <v>352</v>
+      </c>
+      <c r="E2" s="72">
+        <f>34752*1000000/126832800000</f>
+        <v>0.27399852404109976</v>
+      </c>
+      <c r="F2" t="s">
+        <v>351</v>
+      </c>
+      <c r="G2" s="69" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
-        <v>89</v>
+      <c r="B3" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>349</v>
       </c>
       <c r="D3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F3">
-        <v>3.4599999999999999E-2</v>
-      </c>
-      <c r="G3" s="13"/>
-      <c r="I3" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4">
-        <v>2.3599999999999999E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>89</v>
-      </c>
-      <c r="D5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" t="s">
-        <v>91</v>
-      </c>
-      <c r="F5">
-        <v>2.8199999999999999E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E6" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6">
-        <v>2.8199999999999999E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" t="s">
-        <v>93</v>
-      </c>
-      <c r="E7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F7">
-        <v>4.0899999999999999E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E8" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8">
-        <v>3.3399999999999999E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>89</v>
-      </c>
-      <c r="D9" t="s">
-        <v>94</v>
-      </c>
-      <c r="E9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F9">
-        <v>3.3399999999999999E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F10">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" t="s">
-        <v>89</v>
-      </c>
-      <c r="D11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" t="s">
-        <v>91</v>
-      </c>
-      <c r="F11">
-        <v>5.62E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D12" t="s">
-        <v>95</v>
-      </c>
-      <c r="E12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F12">
-        <v>5.62E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" t="s">
-        <v>95</v>
-      </c>
-      <c r="E13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F13">
-        <v>1.1299999999999999E-3</v>
+        <v>354</v>
+      </c>
+      <c r="E3" s="72">
+        <f>343*1000000/126832800000</f>
+        <v>2.7043477712389856E-3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>353</v>
+      </c>
+      <c r="G3" s="69" t="s">
+        <v>350</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="https://arb.ca.gov/emfac/meta/on-road-hdv" xr:uid="{F07D1BF2-06AD-4598-AF94-C04C6DE054AA}"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://arb.ca.gov/emfac/meta/on-road-hdv" xr:uid="{61D1EEAB-16A7-441D-9D2C-18104D78ACFE}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBD7D08-7196-4DD6-A58C-02D5A271324B}">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0073DEA3-76EA-4A12-96E2-2D18F90530EF}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5" customWidth="1"/>
-    <col min="4" max="4" width="29.5" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>96</v>
-      </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>97</v>
       </c>
-      <c r="D1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>328</v>
+      </c>
+      <c r="H1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2">
-        <v>83.81</v>
-      </c>
       <c r="C2" t="s">
-        <v>98</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>378</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>355</v>
+      </c>
+      <c r="F2" s="70">
+        <f>6.2*10*8760*0.3</f>
+        <v>162936</v>
+      </c>
+      <c r="G2" t="s">
+        <v>360</v>
+      </c>
+      <c r="H2" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>378</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>355</v>
+      </c>
+      <c r="F3" s="70">
+        <f>6.2*10*8760*0.3</f>
+        <v>162936</v>
+      </c>
+      <c r="G3" t="s">
+        <v>360</v>
+      </c>
+      <c r="H3" s="36" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>378</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F4" s="70">
+        <f>14*12*1000</f>
+        <v>168000</v>
+      </c>
+      <c r="G4" t="s">
+        <v>361</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>378</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>355</v>
+      </c>
+      <c r="F5" s="70"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>378</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>355</v>
+      </c>
+      <c r="F6" s="70">
+        <f>20*10*8760*0.69</f>
+        <v>1208880</v>
+      </c>
+      <c r="G6" t="s">
+        <v>362</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>378</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>355</v>
+      </c>
+      <c r="F7" s="70">
+        <f t="shared" ref="F7:F9" si="0">20*10*8760*0.69</f>
+        <v>1208880</v>
+      </c>
+      <c r="G7" t="s">
+        <v>362</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>378</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" t="s">
+        <v>355</v>
+      </c>
+      <c r="F8" s="70">
+        <f t="shared" si="0"/>
+        <v>1208880</v>
+      </c>
+      <c r="G8" t="s">
+        <v>362</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>378</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>355</v>
+      </c>
+      <c r="F9" s="70">
+        <f t="shared" si="0"/>
+        <v>1208880</v>
+      </c>
+      <c r="G9" t="s">
+        <v>362</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="55" t="s">
         <v>19</v>
       </c>
+      <c r="C10" s="71" t="s">
+        <v>378</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>356</v>
+      </c>
+      <c r="F10" s="70">
+        <f>7.57*1000</f>
+        <v>7570</v>
+      </c>
+      <c r="G10" s="55" t="s">
+        <v>363</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" t="s">
+        <v>378</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>357</v>
+      </c>
+      <c r="F11" s="70">
+        <f>46/0.000965</f>
+        <v>47668.39378238342</v>
+      </c>
+      <c r="G11" t="s">
+        <v>364</v>
+      </c>
+      <c r="H11" s="69" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>378</v>
+      </c>
+      <c r="D12" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" t="s">
+        <v>358</v>
+      </c>
+      <c r="F12" s="70">
+        <f>9.4*1000000</f>
+        <v>9400000</v>
+      </c>
+      <c r="G12" t="s">
+        <v>365</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>378</v>
+      </c>
+      <c r="D13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" t="s">
+        <v>355</v>
+      </c>
+      <c r="F13" s="70">
+        <f>3*10*8760*0.3</f>
+        <v>78840</v>
+      </c>
+      <c r="G13" t="s">
+        <v>366</v>
+      </c>
+      <c r="H13" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>378</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>355</v>
+      </c>
+      <c r="F14" s="70">
+        <f>3*10*8760*0.3</f>
+        <v>78840</v>
+      </c>
+      <c r="G14" t="s">
+        <v>366</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>378</v>
+      </c>
+      <c r="D15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" t="s">
+        <v>355</v>
+      </c>
+      <c r="F15" s="70">
+        <f>9*12*1000</f>
+        <v>108000</v>
+      </c>
+      <c r="G15" t="s">
+        <v>367</v>
+      </c>
+      <c r="H15" s="36" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>378</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" t="s">
+        <v>355</v>
+      </c>
+      <c r="F16" s="70"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>378</v>
+      </c>
+      <c r="D17" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" t="s">
+        <v>355</v>
+      </c>
+      <c r="F17" s="70">
+        <f>12.8*10*8760*0.69</f>
+        <v>773683.19999999995</v>
+      </c>
+      <c r="G17" t="s">
+        <v>368</v>
+      </c>
+      <c r="H17" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" t="s">
+        <v>378</v>
+      </c>
+      <c r="D18" t="s">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>355</v>
+      </c>
+      <c r="F18" s="70">
+        <f t="shared" ref="F18:F20" si="1">12.8*10*8760*0.69</f>
+        <v>773683.19999999995</v>
+      </c>
+      <c r="G18" t="s">
+        <v>368</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" t="s">
+        <v>378</v>
+      </c>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19" t="s">
+        <v>355</v>
+      </c>
+      <c r="F19" s="70">
+        <f t="shared" si="1"/>
+        <v>773683.19999999995</v>
+      </c>
+      <c r="G19" t="s">
+        <v>368</v>
+      </c>
+      <c r="H19" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" t="s">
+        <v>378</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" t="s">
+        <v>355</v>
+      </c>
+      <c r="F20" s="70">
+        <f t="shared" si="1"/>
+        <v>773683.19999999995</v>
+      </c>
+      <c r="G20" t="s">
+        <v>368</v>
+      </c>
+      <c r="H20" s="36" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="71" t="s">
+        <v>378</v>
+      </c>
+      <c r="D21" s="71" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" t="s">
+        <v>356</v>
+      </c>
+      <c r="F21" s="70">
+        <f>7.57*1000</f>
+        <v>7570</v>
+      </c>
+      <c r="G21" s="55" t="s">
+        <v>363</v>
+      </c>
+      <c r="H21" s="36" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" t="s">
+        <v>378</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" t="s">
+        <v>357</v>
+      </c>
+      <c r="F22" s="70">
+        <f>45/0.000965</f>
+        <v>46632.124352331608</v>
+      </c>
+      <c r="G22" t="s">
+        <v>370</v>
+      </c>
+      <c r="H22" s="69" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>378</v>
+      </c>
+      <c r="D23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" t="s">
+        <v>358</v>
+      </c>
+      <c r="F23" s="70">
+        <f>8.3*1000000</f>
+        <v>8300000.0000000009</v>
+      </c>
+      <c r="G23" t="s">
+        <v>369</v>
+      </c>
+      <c r="H23" s="36" t="s">
+        <v>376</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="https://netzeroamerica.princeton.edu/img/NZA%20Annex%20F%20-%20HV%20Transmission.pdf" xr:uid="{104B4864-4DDD-469C-B108-01D18B28A224}"/>
+    <hyperlink ref="H2" r:id="rId1" display="https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/office-of-governmental-affairs-division/reports/2023/2023-rps-annual-report-to-the-legislature.pdf" xr:uid="{0CE41F2F-7EFA-4077-BF74-D0AB32718B5F}"/>
+    <hyperlink ref="H3" r:id="rId2" display="https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/office-of-governmental-affairs-division/reports/2023/2023-rps-annual-report-to-the-legislature.pdf" xr:uid="{F99A5D1D-C6FF-4B64-94B0-018C1B342D4F}"/>
+    <hyperlink ref="H6" r:id="rId3" display="https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/office-of-governmental-affairs-division/reports/2023/2023-rps-annual-report-to-the-legislature.pdf" xr:uid="{44BFF6D9-DDE4-499D-A348-A4A8EDB735FC}"/>
+    <hyperlink ref="H7" r:id="rId4" display="https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/office-of-governmental-affairs-division/reports/2023/2023-rps-annual-report-to-the-legislature.pdf" xr:uid="{D67EF960-8A9E-4BA7-B6BA-28FF325ABE0B}"/>
+    <hyperlink ref="H8" r:id="rId5" display="https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/office-of-governmental-affairs-division/reports/2023/2023-rps-annual-report-to-the-legislature.pdf" xr:uid="{7AA67FA0-4A03-48F4-9880-E4D9AA7D3760}"/>
+    <hyperlink ref="H9" r:id="rId6" display="https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/office-of-governmental-affairs-division/reports/2023/2023-rps-annual-report-to-the-legislature.pdf" xr:uid="{D1497CEC-82A1-45A5-8CD6-BBC565E5A510}"/>
+    <hyperlink ref="H13" r:id="rId7" display="https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/office-of-governmental-affairs-division/reports/2023/2023-rps-annual-report-to-the-legislature.pdf" xr:uid="{D85DA533-F470-431E-8E93-AEA4954E99BC}"/>
+    <hyperlink ref="H14" r:id="rId8" display="https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/office-of-governmental-affairs-division/reports/2023/2023-rps-annual-report-to-the-legislature.pdf" xr:uid="{D47E081D-C74A-4C19-839B-ADC4A72393CE}"/>
+    <hyperlink ref="H17" r:id="rId9" display="https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/office-of-governmental-affairs-division/reports/2023/2023-rps-annual-report-to-the-legislature.pdf" xr:uid="{D1151395-2F3E-45AD-8C1A-9523F5AF18B3}"/>
+    <hyperlink ref="H18" r:id="rId10" display="https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/office-of-governmental-affairs-division/reports/2023/2023-rps-annual-report-to-the-legislature.pdf" xr:uid="{11B2FC45-C117-43E7-A9F3-332DB8A5F5F4}"/>
+    <hyperlink ref="H19" r:id="rId11" display="https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/office-of-governmental-affairs-division/reports/2023/2023-rps-annual-report-to-the-legislature.pdf" xr:uid="{B87028AC-7D3B-445E-AAF0-1D522C62E044}"/>
+    <hyperlink ref="H20" r:id="rId12" display="https://www.cpuc.ca.gov/-/media/cpuc-website/divisions/office-of-governmental-affairs-division/reports/2023/2023-rps-annual-report-to-the-legislature.pdf" xr:uid="{81ECC266-91FC-4512-A0B8-4515E2FEDF4D}"/>
+    <hyperlink ref="H4" r:id="rId13" xr:uid="{68FEC202-E742-4737-B7A2-31A76D9EF0DB}"/>
+    <hyperlink ref="H15" r:id="rId14" xr:uid="{632353F9-78DC-4FBF-A6D8-1C272C63B788}"/>
+    <hyperlink ref="H10" r:id="rId15" display="https://www.spglobal.com/commodityinsights/en/market-insights/latest-news/energy-transition/020223-greener-than-green-hydrogen-project-nears-construction-phase-in-california" xr:uid="{3061FACA-5E37-44B0-BCE6-909E7994D62B}"/>
+    <hyperlink ref="H21" r:id="rId16" display="https://www.spglobal.com/commodityinsights/en/market-insights/latest-news/energy-transition/020223-greener-than-green-hydrogen-project-nears-construction-phase-in-california" xr:uid="{2AC46F89-B0A4-46B7-AE5B-A871E11EFAD3}"/>
+    <hyperlink ref="H11" r:id="rId17" display="https://theicct.org/wp-content/uploads/2023/05/case-studies-california-rng-outlook-2030-may23.pdf" xr:uid="{A9337216-B567-4EF9-84FF-95EB2801414D}"/>
+    <hyperlink ref="H22" r:id="rId18" display="https://theicct.org/wp-content/uploads/2023/05/case-studies-california-rng-outlook-2030-may23.pdf" xr:uid="{E86D63D0-DB42-43D8-A6B4-8A6F272B3354}"/>
+    <hyperlink ref="H23" r:id="rId19" display="https://www.spglobal.com/commodityinsights/en/market-insights/latest-news/agriculture/082422-sustainable-aviation-fuel-a-winner-as-us-renewable-fuel-producers-embrace-inflation-reduction-act" xr:uid="{FC712674-2E7F-4722-BBDE-1F64A7B0DE33}"/>
+    <hyperlink ref="H12" r:id="rId20" location=":~:text=These%20prices%20are%20the%20average,SAF)%20is%20%249.49%20per%20gallon" display="https://www.globalair.com/airport/region.aspx - :~:text=These%20prices%20are%20the%20average,SAF)%20is%20%249.49%20per%20gallon" xr:uid="{1802F9EE-6CF0-4F63-A30F-A15A0BC5E865}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated water use for org waste
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A1BB5E-6F9F-4CAC-9F62-370C2F245BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36AC90A-71A9-4BF3-B2D2-2E7921D21AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="622" firstSheet="5" activeTab="7" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="12255" yWindow="1500" windowWidth="16755" windowHeight="12180" tabRatio="622" firstSheet="2" activeTab="5" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -41,7 +41,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'F2C Jobs'!$A$1:$O$58</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'F2C Jobs old'!$A$1:$J$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'F2C Land'!$A$1:$K$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'F2C Water'!$A$19:$L$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'F2C Water'!$A$1:$L$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Unit Conversion'!$A$1:$AK$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2773" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2775" uniqueCount="399">
   <si>
     <t>Feedstock</t>
   </si>
@@ -1628,7 +1628,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1734,10 +1734,7 @@
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -3940,7 +3937,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E20" sqref="E20"/>
+      <selection pane="topRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5221,10 +5218,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87BF8B-8E54-426F-864A-9E457E959B26}">
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5927,6 +5924,134 @@
       </c>
       <c r="Y9" s="54">
         <v>5162.1082438314425</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E12" s="72">
+        <f>E2/8760</f>
+        <v>0.26187622965636759</v>
+      </c>
+      <c r="F12" s="72">
+        <f t="shared" ref="F12:Y12" si="0">F2/8760</f>
+        <v>0.25572607372904549</v>
+      </c>
+      <c r="G12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.24957591780172336</v>
+      </c>
+      <c r="H12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.24342576187440126</v>
+      </c>
+      <c r="I12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.23727560594707917</v>
+      </c>
+      <c r="J12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.23112545001975709</v>
+      </c>
+      <c r="K12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.224975294092435</v>
+      </c>
+      <c r="L12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.21882513816511293</v>
+      </c>
+      <c r="M12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.21267498223779085</v>
+      </c>
+      <c r="N12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.20652482631046878</v>
+      </c>
+      <c r="O12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.20037467038314669</v>
+      </c>
+      <c r="P12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.19422451445582462</v>
+      </c>
+      <c r="Q12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.18807435852850254</v>
+      </c>
+      <c r="R12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.18192420260118047</v>
+      </c>
+      <c r="S12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.17577404667385838</v>
+      </c>
+      <c r="T12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.1696238907465363</v>
+      </c>
+      <c r="U12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.16347373481921423</v>
+      </c>
+      <c r="V12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.15732357889189214</v>
+      </c>
+      <c r="W12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.15117342296457006</v>
+      </c>
+      <c r="X12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.14502326703724799</v>
+      </c>
+      <c r="Y12" s="72">
+        <f t="shared" si="0"/>
+        <v>0.13887311110992592</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E13" s="72">
+        <f t="shared" ref="E13:E19" si="1">E3/8760</f>
+        <v>0.28570875457778422</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E14" s="72">
+        <f t="shared" si="1"/>
+        <v>0.13368702269483454</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E15" s="72">
+        <f t="shared" si="1"/>
+        <v>0.19073300751397604</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="E16" s="72">
+        <f t="shared" si="1"/>
+        <v>0.68893673866789151</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="72">
+        <f t="shared" si="1"/>
+        <v>0.68893673866789151</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="72">
+        <f t="shared" si="1"/>
+        <v>0.68893673866789151</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="72">
+        <f t="shared" si="1"/>
+        <v>0.68893673866789151</v>
       </c>
     </row>
   </sheetData>
@@ -13586,8 +13711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C58C4D02-922E-2849-99A2-B5A24807FA42}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F11" sqref="A11:F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13919,7 +14044,16 @@
       <c r="E14" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="8">
+        <f t="shared" ref="F14:F15" si="0">H14*1000/325851</f>
+        <v>8.5928844778748563E-3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14">
+        <v>2.8</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -13937,7 +14071,16 @@
       <c r="E15" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="8">
+        <f t="shared" si="0"/>
+        <v>8.5928844778748563E-3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>82</v>
+      </c>
+      <c r="H15">
+        <v>2.8</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -14515,7 +14658,7 @@
       <c r="B52" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A19:L19" xr:uid="{C58C4D02-922E-2849-99A2-B5A24807FA42}"/>
+  <autoFilter ref="A1:L41" xr:uid="{C58C4D02-922E-2849-99A2-B5A24807FA42}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14708,16 +14851,16 @@
       <c r="H4" t="s">
         <v>91</v>
       </c>
-      <c r="I4" s="71">
+      <c r="I4">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="J4" s="71">
+      <c r="J4">
         <v>0</v>
       </c>
-      <c r="K4" s="71">
+      <c r="K4">
         <v>4.5152412959181799E-2</v>
       </c>
-      <c r="L4" s="73">
+      <c r="L4" s="8">
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="M4" s="8">
@@ -14753,16 +14896,16 @@
       <c r="H5" t="s">
         <v>91</v>
       </c>
-      <c r="I5" s="71">
+      <c r="I5">
         <v>2.2229999999999999</v>
       </c>
-      <c r="J5" s="71">
+      <c r="J5">
         <v>26.02</v>
       </c>
-      <c r="K5" s="71">
+      <c r="K5">
         <v>8.3034948476273795E-3</v>
       </c>
-      <c r="L5" s="74">
+      <c r="L5" s="71">
         <v>2.242</v>
       </c>
       <c r="M5" s="8">
@@ -14798,16 +14941,16 @@
       <c r="H6" t="s">
         <v>91</v>
       </c>
-      <c r="I6" s="71">
+      <c r="I6">
         <v>2.2229999999999999</v>
       </c>
-      <c r="J6" s="71">
+      <c r="J6">
         <v>0</v>
       </c>
-      <c r="K6" s="71">
+      <c r="K6">
         <v>8.3034948476273795E-3</v>
       </c>
-      <c r="L6" s="74">
+      <c r="L6" s="71">
         <v>1.044</v>
       </c>
       <c r="M6" s="8">
@@ -14843,16 +14986,16 @@
       <c r="H7" t="s">
         <v>91</v>
       </c>
-      <c r="I7" s="71">
+      <c r="I7">
         <v>2.2229999999999999</v>
       </c>
-      <c r="J7" s="71">
+      <c r="J7">
         <v>0</v>
       </c>
-      <c r="K7" s="71">
+      <c r="K7">
         <v>8.3034948476273795E-3</v>
       </c>
-      <c r="L7" s="73">
+      <c r="L7" s="8">
         <v>1.01</v>
       </c>
       <c r="M7" s="8">
@@ -14888,16 +15031,16 @@
       <c r="H8" t="s">
         <v>91</v>
       </c>
-      <c r="I8" s="71">
+      <c r="I8">
         <v>0.78800000000000003</v>
       </c>
-      <c r="J8" s="71">
+      <c r="J8">
         <v>24.71</v>
       </c>
-      <c r="K8" s="71">
+      <c r="K8">
         <v>3.7832039152811102E-2</v>
       </c>
-      <c r="L8" s="71">
+      <c r="L8">
         <v>0.81899999999999995</v>
       </c>
       <c r="M8">
@@ -14933,16 +15076,16 @@
       <c r="H9" t="s">
         <v>91</v>
       </c>
-      <c r="I9" s="71">
+      <c r="I9">
         <v>0.78800000000000003</v>
       </c>
-      <c r="J9" s="71">
+      <c r="J9">
         <v>0</v>
       </c>
-      <c r="K9" s="71">
+      <c r="K9">
         <v>3.7832039152811102E-2</v>
       </c>
-      <c r="L9" s="71">
+      <c r="L9">
         <v>0.34599999999999997</v>
       </c>
       <c r="M9">
@@ -14978,16 +15121,16 @@
       <c r="H10" t="s">
         <v>91</v>
       </c>
-      <c r="I10" s="71">
+      <c r="I10">
         <v>0.78800000000000003</v>
       </c>
-      <c r="J10" s="71">
+      <c r="J10">
         <v>0</v>
       </c>
-      <c r="K10" s="71">
+      <c r="K10">
         <v>3.7832039152811102E-2</v>
       </c>
-      <c r="L10" s="71">
+      <c r="L10">
         <v>0.33200000000000002</v>
       </c>
       <c r="M10">
@@ -15014,14 +15157,13 @@
       <c r="H11" t="s">
         <v>91</v>
       </c>
-      <c r="I11" s="71" t="s">
+      <c r="I11" t="s">
         <v>335</v>
       </c>
-      <c r="J11" s="71"/>
-      <c r="K11" s="71" t="s">
+      <c r="K11" t="s">
         <v>335</v>
       </c>
-      <c r="L11" s="71" t="s">
+      <c r="L11" t="s">
         <v>335</v>
       </c>
       <c r="M11" t="s">
@@ -15047,14 +15189,13 @@
       <c r="H12" t="s">
         <v>91</v>
       </c>
-      <c r="I12" s="71" t="s">
+      <c r="I12" t="s">
         <v>335</v>
       </c>
-      <c r="J12" s="71"/>
-      <c r="K12" s="71" t="s">
+      <c r="K12" t="s">
         <v>335</v>
       </c>
-      <c r="L12" s="71" t="s">
+      <c r="L12" t="s">
         <v>335</v>
       </c>
       <c r="M12" t="s">
@@ -15080,14 +15221,13 @@
       <c r="H13" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="71" t="s">
+      <c r="I13" t="s">
         <v>335</v>
       </c>
-      <c r="J13" s="71"/>
-      <c r="K13" s="71" t="s">
+      <c r="K13" t="s">
         <v>335</v>
       </c>
-      <c r="L13" s="71" t="s">
+      <c r="L13" t="s">
         <v>335</v>
       </c>
       <c r="M13" t="s">
@@ -15122,16 +15262,16 @@
       <c r="H14" t="s">
         <v>91</v>
       </c>
-      <c r="I14" s="71">
+      <c r="I14">
         <v>4.958333333333333</v>
       </c>
-      <c r="J14" s="71">
+      <c r="J14">
         <v>26.59</v>
       </c>
-      <c r="K14" s="72">
+      <c r="K14" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L14" s="72">
+      <c r="L14" s="67">
         <v>5.016</v>
       </c>
       <c r="M14">
@@ -15167,16 +15307,16 @@
       <c r="H15" t="s">
         <v>91</v>
       </c>
-      <c r="I15" s="71">
+      <c r="I15">
         <v>4.958333333333333</v>
       </c>
-      <c r="J15" s="71">
+      <c r="J15">
         <v>0</v>
       </c>
-      <c r="K15" s="72">
+      <c r="K15" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L15" s="72">
+      <c r="L15" s="67">
         <v>4.2050000000000001</v>
       </c>
       <c r="M15">
@@ -15212,16 +15352,16 @@
       <c r="H16" t="s">
         <v>91</v>
       </c>
-      <c r="I16" s="71">
+      <c r="I16">
         <v>4.958333333333333</v>
       </c>
-      <c r="J16" s="71">
+      <c r="J16">
         <v>0</v>
       </c>
-      <c r="K16" s="72">
+      <c r="K16" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L16" s="72">
+      <c r="L16" s="67">
         <v>4.8159999999999998</v>
       </c>
       <c r="M16">
@@ -15257,16 +15397,16 @@
       <c r="H17" t="s">
         <v>91</v>
       </c>
-      <c r="I17" s="71">
+      <c r="I17">
         <v>4.958333333333333</v>
       </c>
-      <c r="J17" s="71">
+      <c r="J17">
         <v>26.59</v>
       </c>
-      <c r="K17" s="72">
+      <c r="K17" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L17" s="72">
+      <c r="L17" s="67">
         <v>5.016</v>
       </c>
       <c r="M17">
@@ -15302,16 +15442,16 @@
       <c r="H18" t="s">
         <v>91</v>
       </c>
-      <c r="I18" s="71">
+      <c r="I18">
         <v>4.958333333333333</v>
       </c>
-      <c r="J18" s="71">
+      <c r="J18">
         <v>0</v>
       </c>
-      <c r="K18" s="72">
+      <c r="K18" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L18" s="72">
+      <c r="L18" s="67">
         <v>4.2050000000000001</v>
       </c>
       <c r="M18">
@@ -15347,16 +15487,16 @@
       <c r="H19" t="s">
         <v>91</v>
       </c>
-      <c r="I19" s="71">
+      <c r="I19">
         <v>4.958333333333333</v>
       </c>
-      <c r="J19" s="71">
+      <c r="J19">
         <v>0</v>
       </c>
-      <c r="K19" s="72">
+      <c r="K19" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L19" s="72">
+      <c r="L19" s="67">
         <v>4.8159999999999998</v>
       </c>
       <c r="M19">
@@ -15392,16 +15532,16 @@
       <c r="H20" t="s">
         <v>91</v>
       </c>
-      <c r="I20" s="71">
+      <c r="I20">
         <v>4.958333333333333</v>
       </c>
-      <c r="J20" s="71">
+      <c r="J20">
         <v>26.59</v>
       </c>
-      <c r="K20" s="72">
+      <c r="K20" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L20" s="72">
+      <c r="L20" s="67">
         <v>5.016</v>
       </c>
       <c r="M20">
@@ -15437,16 +15577,16 @@
       <c r="H21" t="s">
         <v>91</v>
       </c>
-      <c r="I21" s="71">
+      <c r="I21">
         <v>4.958333333333333</v>
       </c>
-      <c r="J21" s="71">
+      <c r="J21">
         <v>0</v>
       </c>
-      <c r="K21" s="72">
+      <c r="K21" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L21" s="72">
+      <c r="L21" s="67">
         <v>4.2050000000000001</v>
       </c>
       <c r="M21">
@@ -15482,16 +15622,16 @@
       <c r="H22" t="s">
         <v>91</v>
       </c>
-      <c r="I22" s="71">
+      <c r="I22">
         <v>4.958333333333333</v>
       </c>
-      <c r="J22" s="71">
+      <c r="J22">
         <v>0</v>
       </c>
-      <c r="K22" s="72">
+      <c r="K22" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L22" s="72">
+      <c r="L22" s="67">
         <v>4.8159999999999998</v>
       </c>
       <c r="M22">
@@ -15527,16 +15667,16 @@
       <c r="H23" t="s">
         <v>91</v>
       </c>
-      <c r="I23" s="71">
+      <c r="I23">
         <v>4.958333333333333</v>
       </c>
-      <c r="J23" s="71">
+      <c r="J23">
         <v>26.59</v>
       </c>
-      <c r="K23" s="72">
+      <c r="K23" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L23" s="72">
+      <c r="L23" s="67">
         <v>5.016</v>
       </c>
       <c r="M23">
@@ -15572,16 +15712,16 @@
       <c r="H24" t="s">
         <v>91</v>
       </c>
-      <c r="I24" s="71">
+      <c r="I24">
         <v>4.958333333333333</v>
       </c>
-      <c r="J24" s="71">
+      <c r="J24">
         <v>0</v>
       </c>
-      <c r="K24" s="72">
+      <c r="K24" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L24" s="72">
+      <c r="L24" s="67">
         <v>4.2050000000000001</v>
       </c>
       <c r="M24">
@@ -15617,16 +15757,16 @@
       <c r="H25" t="s">
         <v>91</v>
       </c>
-      <c r="I25" s="71">
+      <c r="I25">
         <v>4.958333333333333</v>
       </c>
-      <c r="J25" s="71">
+      <c r="J25">
         <v>0</v>
       </c>
-      <c r="K25" s="72">
+      <c r="K25" s="67">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L25" s="72">
+      <c r="L25" s="67">
         <v>4.8159999999999998</v>
       </c>
       <c r="M25">
@@ -16233,7 +16373,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="M38" s="55">
-        <f>L38</f>
+        <f t="shared" ref="M38:M43" si="4">L38</f>
         <v>1.4E-2</v>
       </c>
       <c r="N38" t="s">
@@ -16281,7 +16421,7 @@
         <v>0.249</v>
       </c>
       <c r="M39" s="55">
-        <f>L39</f>
+        <f t="shared" si="4"/>
         <v>0.249</v>
       </c>
       <c r="N39" t="s">
@@ -16329,7 +16469,7 @@
         <v>0.187</v>
       </c>
       <c r="M40" s="55">
-        <f>L40</f>
+        <f t="shared" si="4"/>
         <v>0.187</v>
       </c>
       <c r="N40" t="s">
@@ -16377,7 +16517,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="M41" s="55">
-        <f>L41</f>
+        <f t="shared" si="4"/>
         <v>1.4E-2</v>
       </c>
       <c r="N41" t="s">
@@ -16425,7 +16565,7 @@
         <v>0.249</v>
       </c>
       <c r="M42" s="55">
-        <f>L42</f>
+        <f t="shared" si="4"/>
         <v>0.249</v>
       </c>
       <c r="N42" t="s">
@@ -16473,7 +16613,7 @@
         <v>0.187</v>
       </c>
       <c r="M43" s="55">
-        <f>L43</f>
+        <f t="shared" si="4"/>
         <v>0.187</v>
       </c>
       <c r="N43" t="s">
@@ -16566,7 +16706,7 @@
         <v>2.8358342136926399E-2</v>
       </c>
       <c r="M45">
-        <f t="shared" ref="M45:M49" si="4">I45/0.965</f>
+        <f t="shared" ref="M45:M49" si="5">I45/0.965</f>
         <v>0.1751295336787565</v>
       </c>
       <c r="N45" t="s">
@@ -16611,7 +16751,7 @@
         <v>2.8358342136926399E-2</v>
       </c>
       <c r="M46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.19274611398963731</v>
       </c>
       <c r="N46" t="s">
@@ -16704,7 +16844,7 @@
         <v>2.8358342136926399E-2</v>
       </c>
       <c r="M48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.1751295336787565</v>
       </c>
       <c r="N48" t="s">
@@ -16749,7 +16889,7 @@
         <v>2.8358342136926399E-2</v>
       </c>
       <c r="M49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.19274611398963731</v>
       </c>
       <c r="N49" t="s">
@@ -17037,7 +17177,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="M55" s="70">
-        <f t="shared" ref="M55:M58" si="5">L55/0.007</f>
+        <f t="shared" ref="M55:M58" si="6">L55/0.007</f>
         <v>12.285714285714285</v>
       </c>
       <c r="N55" t="s">
@@ -17085,7 +17225,7 @@
         <v>0.24099999999999999</v>
       </c>
       <c r="M56" s="70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>34.428571428571423</v>
       </c>
       <c r="N56" t="s">
@@ -17133,7 +17273,7 @@
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="M57" s="70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.142857142857144</v>
       </c>
       <c r="N57" t="s">
@@ -17181,7 +17321,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="M58" s="70">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12.285714285714285</v>
       </c>
       <c r="N58" t="s">
@@ -17205,8 +17345,8 @@
   </sheetPr>
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M14:M15"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -17288,25 +17428,25 @@
       <c r="D2" t="s">
         <v>315</v>
       </c>
-      <c r="E2" s="75">
+      <c r="E2" s="72">
         <v>0</v>
       </c>
-      <c r="F2" s="75">
+      <c r="F2" s="72">
         <v>2.564102564102564E-2</v>
       </c>
-      <c r="G2" s="75">
+      <c r="G2" s="72">
         <v>0.51282051282051277</v>
       </c>
-      <c r="H2" s="75">
+      <c r="H2" s="72">
         <v>0.12820512820512819</v>
       </c>
-      <c r="I2" s="75">
+      <c r="I2" s="72">
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="J2" s="75">
+      <c r="J2" s="72">
         <v>0.15384615384615385</v>
       </c>
-      <c r="K2" s="75">
+      <c r="K2" s="72">
         <v>0.10256410256410256</v>
       </c>
       <c r="M2" s="13" t="s">
@@ -17351,25 +17491,25 @@
       <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="75">
+      <c r="E3" s="72">
         <v>0</v>
       </c>
-      <c r="F3" s="75">
+      <c r="F3" s="72">
         <v>6.7226890756302518E-2</v>
       </c>
-      <c r="G3" s="75">
+      <c r="G3" s="72">
         <v>0.36134453781512604</v>
       </c>
-      <c r="H3" s="75">
+      <c r="H3" s="72">
         <v>0.18487394957983194</v>
       </c>
-      <c r="I3" s="75">
+      <c r="I3" s="72">
         <v>0.10084033613445378</v>
       </c>
-      <c r="J3" s="75">
+      <c r="J3" s="72">
         <v>0.26050420168067229</v>
       </c>
-      <c r="K3" s="75">
+      <c r="K3" s="72">
         <v>2.5210084033613446E-2</v>
       </c>
       <c r="M3" s="13" t="s">
@@ -17414,25 +17554,25 @@
       <c r="D4" t="s">
         <v>143</v>
       </c>
-      <c r="E4" s="75">
+      <c r="E4" s="72">
         <v>0</v>
       </c>
-      <c r="F4" s="75">
+      <c r="F4" s="72">
         <v>0</v>
       </c>
-      <c r="G4" s="75">
+      <c r="G4" s="72">
         <v>0.51249999999999996</v>
       </c>
-      <c r="H4" s="75">
+      <c r="H4" s="72">
         <v>0.1875</v>
       </c>
-      <c r="I4" s="75">
+      <c r="I4" s="72">
         <v>0.1125</v>
       </c>
-      <c r="J4" s="75">
+      <c r="J4" s="72">
         <v>0.17499999999999999</v>
       </c>
-      <c r="K4" s="75">
+      <c r="K4" s="72">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="M4" s="13" t="s">
@@ -17477,25 +17617,25 @@
       <c r="D5" t="s">
         <v>319</v>
       </c>
-      <c r="E5" s="75">
+      <c r="E5" s="72">
         <v>0</v>
       </c>
-      <c r="F5" s="75">
+      <c r="F5" s="72">
         <v>0.1702127659574468</v>
       </c>
-      <c r="G5" s="75">
+      <c r="G5" s="72">
         <v>0.42553191489361702</v>
       </c>
-      <c r="H5" s="75">
+      <c r="H5" s="72">
         <v>8.5106382978723402E-2</v>
       </c>
-      <c r="I5" s="75">
+      <c r="I5" s="72">
         <v>4.2553191489361701E-2</v>
       </c>
-      <c r="J5" s="75">
+      <c r="J5" s="72">
         <v>0.25531914893617019</v>
       </c>
-      <c r="K5" s="75">
+      <c r="K5" s="72">
         <v>2.1276595744680851E-2</v>
       </c>
       <c r="M5" s="13" t="s">
@@ -17540,25 +17680,25 @@
       <c r="D6" t="s">
         <v>319</v>
       </c>
-      <c r="E6" s="75">
+      <c r="E6" s="72">
         <v>0</v>
       </c>
-      <c r="F6" s="75">
+      <c r="F6" s="72">
         <v>0.1702127659574468</v>
       </c>
-      <c r="G6" s="75">
+      <c r="G6" s="72">
         <v>0.42553191489361702</v>
       </c>
-      <c r="H6" s="75">
+      <c r="H6" s="72">
         <v>8.5106382978723402E-2</v>
       </c>
-      <c r="I6" s="75">
+      <c r="I6" s="72">
         <v>4.2553191489361701E-2</v>
       </c>
-      <c r="J6" s="75">
+      <c r="J6" s="72">
         <v>0.25531914893617019</v>
       </c>
-      <c r="K6" s="75">
+      <c r="K6" s="72">
         <v>2.1276595744680851E-2</v>
       </c>
       <c r="M6" s="13" t="s">
@@ -17603,25 +17743,25 @@
       <c r="D7" t="s">
         <v>319</v>
       </c>
-      <c r="E7" s="75">
+      <c r="E7" s="72">
         <v>0</v>
       </c>
-      <c r="F7" s="75">
+      <c r="F7" s="72">
         <v>0.1702127659574468</v>
       </c>
-      <c r="G7" s="75">
+      <c r="G7" s="72">
         <v>0.42553191489361702</v>
       </c>
-      <c r="H7" s="75">
+      <c r="H7" s="72">
         <v>8.5106382978723402E-2</v>
       </c>
-      <c r="I7" s="75">
+      <c r="I7" s="72">
         <v>4.2553191489361701E-2</v>
       </c>
-      <c r="J7" s="75">
+      <c r="J7" s="72">
         <v>0.25531914893617019</v>
       </c>
-      <c r="K7" s="75">
+      <c r="K7" s="72">
         <v>2.1276595744680851E-2</v>
       </c>
       <c r="M7" s="13" t="s">
@@ -17666,25 +17806,25 @@
       <c r="D8" t="s">
         <v>319</v>
       </c>
-      <c r="E8" s="75">
+      <c r="E8" s="72">
         <v>0</v>
       </c>
-      <c r="F8" s="75">
+      <c r="F8" s="72">
         <v>0.1702127659574468</v>
       </c>
-      <c r="G8" s="75">
+      <c r="G8" s="72">
         <v>0.42553191489361702</v>
       </c>
-      <c r="H8" s="75">
+      <c r="H8" s="72">
         <v>8.5106382978723402E-2</v>
       </c>
-      <c r="I8" s="75">
+      <c r="I8" s="72">
         <v>4.2553191489361701E-2</v>
       </c>
-      <c r="J8" s="75">
+      <c r="J8" s="72">
         <v>0.25531914893617019</v>
       </c>
-      <c r="K8" s="75">
+      <c r="K8" s="72">
         <v>2.1276595744680851E-2</v>
       </c>
       <c r="M8" s="13" t="s">
@@ -17729,25 +17869,25 @@
       <c r="D9" t="s">
         <v>321</v>
       </c>
-      <c r="E9" s="75">
+      <c r="E9" s="72">
         <v>0</v>
       </c>
-      <c r="F9" s="75">
+      <c r="F9" s="72">
         <v>0</v>
       </c>
-      <c r="G9" s="75">
+      <c r="G9" s="72">
         <v>0</v>
       </c>
-      <c r="H9" s="75">
+      <c r="H9" s="72">
         <v>0.40625</v>
       </c>
-      <c r="I9" s="75">
+      <c r="I9" s="72">
         <v>0.328125</v>
       </c>
-      <c r="J9" s="75">
+      <c r="J9" s="72">
         <v>0.265625</v>
       </c>
-      <c r="K9" s="75">
+      <c r="K9" s="72">
         <v>0</v>
       </c>
       <c r="M9" s="13" t="s">
@@ -17876,7 +18016,7 @@
       <c r="K11" s="40">
         <v>0</v>
       </c>
-      <c r="M11" s="76" t="s">
+      <c r="M11" s="73" t="s">
         <v>398</v>
       </c>
     </row>
@@ -17998,25 +18138,25 @@
       <c r="D15" t="s">
         <v>377</v>
       </c>
-      <c r="E15" s="75">
+      <c r="E15" s="72">
         <v>0</v>
       </c>
-      <c r="F15" s="75">
+      <c r="F15" s="72">
         <v>0</v>
       </c>
-      <c r="G15" s="75">
+      <c r="G15" s="72">
         <v>0</v>
       </c>
-      <c r="H15" s="75">
+      <c r="H15" s="72">
         <v>4.7619047619047616E-2</v>
       </c>
-      <c r="I15" s="75">
+      <c r="I15" s="72">
         <v>0</v>
       </c>
-      <c r="J15" s="75">
+      <c r="J15" s="72">
         <v>0.95238095238095233</v>
       </c>
-      <c r="K15" s="75">
+      <c r="K15" s="72">
         <v>0</v>
       </c>
     </row>
@@ -18068,25 +18208,25 @@
       <c r="D17" t="s">
         <v>322</v>
       </c>
-      <c r="E17" s="75">
+      <c r="E17" s="72">
         <v>0.12209302325581395</v>
       </c>
-      <c r="F17" s="75">
+      <c r="F17" s="72">
         <v>0</v>
       </c>
-      <c r="G17" s="75">
+      <c r="G17" s="72">
         <v>0</v>
       </c>
-      <c r="H17" s="75">
+      <c r="H17" s="72">
         <v>0.12790697674418605</v>
       </c>
-      <c r="I17" s="75">
+      <c r="I17" s="72">
         <v>0.27325581395348836</v>
       </c>
-      <c r="J17" s="75">
+      <c r="J17" s="72">
         <v>0.47093023255813954</v>
       </c>
-      <c r="K17" s="75">
+      <c r="K17" s="72">
         <v>5.8139534883720929E-3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed GHG emission factors
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36AC90A-71A9-4BF3-B2D2-2E7921D21AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA80DF48-F7D0-4FE0-B811-D16DB36D19A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12255" yWindow="1500" windowWidth="16755" windowHeight="12180" tabRatio="622" firstSheet="2" activeTab="5" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="3975" yWindow="945" windowWidth="16755" windowHeight="12180" tabRatio="622" firstSheet="6" activeTab="8" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -36,7 +36,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'C2U CI'!$A$1:$AA$16</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'F2C CI'!$A$1:$J$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'F2C CI'!$A$1:$I$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'F2C Conversion'!$A$1:$Q$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'F2C Jobs'!$A$1:$O$58</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'F2C Jobs old'!$A$1:$J$13</definedName>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2775" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2714" uniqueCount="399">
   <si>
     <t>Feedstock</t>
   </si>
@@ -1628,7 +1628,7 @@
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1725,7 +1725,6 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -2174,7 +2173,7 @@
       <c r="N2" t="s">
         <v>268</v>
       </c>
-      <c r="O2" s="66">
+      <c r="O2" s="65">
         <f>198000*1000000</f>
         <v>198000000000</v>
       </c>
@@ -2229,7 +2228,7 @@
       <c r="N3" t="s">
         <v>268</v>
       </c>
-      <c r="O3" s="66">
+      <c r="O3" s="65">
         <f>198000*1000000</f>
         <v>198000000000</v>
       </c>
@@ -2269,7 +2268,7 @@
       <c r="N4" t="s">
         <v>268</v>
       </c>
-      <c r="O4" s="66">
+      <c r="O4" s="65">
         <f>16/1.15*1000*1000000</f>
         <v>13913043478.260872</v>
       </c>
@@ -2309,7 +2308,7 @@
       <c r="N5" t="s">
         <v>268</v>
       </c>
-      <c r="O5" s="66">
+      <c r="O5" s="65">
         <f>O4</f>
         <v>13913043478.260872</v>
       </c>
@@ -2365,7 +2364,7 @@
       <c r="N6" s="40" t="s">
         <v>268</v>
       </c>
-      <c r="O6" s="66">
+      <c r="O6" s="65">
         <v>1093000</v>
       </c>
       <c r="P6" t="s">
@@ -2420,7 +2419,7 @@
       <c r="N7" t="s">
         <v>268</v>
       </c>
-      <c r="O7" s="66">
+      <c r="O7" s="65">
         <f>198000*1000000</f>
         <v>198000000000</v>
       </c>
@@ -2473,7 +2472,7 @@
       <c r="N8" t="s">
         <v>268</v>
       </c>
-      <c r="O8" s="66">
+      <c r="O8" s="65">
         <f>198000*1000000</f>
         <v>198000000000</v>
       </c>
@@ -2524,7 +2523,7 @@
       <c r="N9" t="s">
         <v>268</v>
       </c>
-      <c r="O9" s="66">
+      <c r="O9" s="65">
         <f>$O$4</f>
         <v>13913043478.260872</v>
       </c>
@@ -2578,7 +2577,7 @@
       <c r="N10" t="s">
         <v>268</v>
       </c>
-      <c r="O10" s="66">
+      <c r="O10" s="65">
         <f t="shared" ref="O10:O12" si="3">$O$4</f>
         <v>13913043478.260872</v>
       </c>
@@ -2631,7 +2630,7 @@
       <c r="N11" t="s">
         <v>268</v>
       </c>
-      <c r="O11" s="66">
+      <c r="O11" s="65">
         <f t="shared" si="3"/>
         <v>13913043478.260872</v>
       </c>
@@ -2684,7 +2683,7 @@
       <c r="N12" t="s">
         <v>268</v>
       </c>
-      <c r="O12" s="66">
+      <c r="O12" s="65">
         <f t="shared" si="3"/>
         <v>13913043478.260872</v>
       </c>
@@ -2736,7 +2735,7 @@
       <c r="N13" t="s">
         <v>268</v>
       </c>
-      <c r="O13" s="66">
+      <c r="O13" s="65">
         <f>37*1000*1000000</f>
         <v>37000000000</v>
       </c>
@@ -2785,7 +2784,7 @@
       <c r="M14" t="s">
         <v>285</v>
       </c>
-      <c r="O14" s="66">
+      <c r="O14" s="65">
         <f t="shared" ref="O14:O15" si="4">198000*1000000</f>
         <v>198000000000</v>
       </c>
@@ -2834,7 +2833,7 @@
       <c r="M15" t="s">
         <v>286</v>
       </c>
-      <c r="O15" s="66">
+      <c r="O15" s="65">
         <f t="shared" si="4"/>
         <v>198000000000</v>
       </c>
@@ -2995,7 +2994,7 @@
       <c r="E2" t="s">
         <v>352</v>
       </c>
-      <c r="F2" s="69">
+      <c r="F2" s="68">
         <f>6.2*10*8760*0.3</f>
         <v>162936</v>
       </c>
@@ -3022,7 +3021,7 @@
       <c r="E3" t="s">
         <v>352</v>
       </c>
-      <c r="F3" s="69">
+      <c r="F3" s="68">
         <f>6.2*10*8760*0.3</f>
         <v>162936</v>
       </c>
@@ -3049,7 +3048,7 @@
       <c r="E4" t="s">
         <v>352</v>
       </c>
-      <c r="F4" s="69">
+      <c r="F4" s="68">
         <f>14*12*1000</f>
         <v>168000</v>
       </c>
@@ -3076,7 +3075,7 @@
       <c r="E5" t="s">
         <v>352</v>
       </c>
-      <c r="F5" s="69"/>
+      <c r="F5" s="68"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3094,7 +3093,7 @@
       <c r="E6" t="s">
         <v>352</v>
       </c>
-      <c r="F6" s="69">
+      <c r="F6" s="68">
         <f>20*10*8760*0.69</f>
         <v>1208880</v>
       </c>
@@ -3121,7 +3120,7 @@
       <c r="E7" t="s">
         <v>352</v>
       </c>
-      <c r="F7" s="69">
+      <c r="F7" s="68">
         <f t="shared" ref="F7:F9" si="0">20*10*8760*0.69</f>
         <v>1208880</v>
       </c>
@@ -3148,7 +3147,7 @@
       <c r="E8" t="s">
         <v>352</v>
       </c>
-      <c r="F8" s="69">
+      <c r="F8" s="68">
         <f t="shared" si="0"/>
         <v>1208880</v>
       </c>
@@ -3175,7 +3174,7 @@
       <c r="E9" t="s">
         <v>352</v>
       </c>
-      <c r="F9" s="69">
+      <c r="F9" s="68">
         <f t="shared" si="0"/>
         <v>1208880</v>
       </c>
@@ -3199,7 +3198,7 @@
       <c r="E10" t="s">
         <v>353</v>
       </c>
-      <c r="F10" s="69">
+      <c r="F10" s="68">
         <f>7.57*1000</f>
         <v>7570</v>
       </c>
@@ -3223,14 +3222,14 @@
       <c r="E11" t="s">
         <v>354</v>
       </c>
-      <c r="F11" s="69">
+      <c r="F11" s="68">
         <f>46/0.000965</f>
         <v>47668.39378238342</v>
       </c>
       <c r="G11" t="s">
         <v>361</v>
       </c>
-      <c r="H11" s="68" t="s">
+      <c r="H11" s="67" t="s">
         <v>372</v>
       </c>
     </row>
@@ -3247,7 +3246,7 @@
       <c r="E12" t="s">
         <v>355</v>
       </c>
-      <c r="F12" s="69">
+      <c r="F12" s="68">
         <f>9.4*1000000</f>
         <v>9400000</v>
       </c>
@@ -3274,7 +3273,7 @@
       <c r="E13" t="s">
         <v>352</v>
       </c>
-      <c r="F13" s="69">
+      <c r="F13" s="68">
         <f>3*10*8760*0.3</f>
         <v>78840</v>
       </c>
@@ -3301,7 +3300,7 @@
       <c r="E14" t="s">
         <v>352</v>
       </c>
-      <c r="F14" s="69">
+      <c r="F14" s="68">
         <f>3*10*8760*0.3</f>
         <v>78840</v>
       </c>
@@ -3328,7 +3327,7 @@
       <c r="E15" t="s">
         <v>352</v>
       </c>
-      <c r="F15" s="69">
+      <c r="F15" s="68">
         <f>9*12*1000</f>
         <v>108000</v>
       </c>
@@ -3355,7 +3354,7 @@
       <c r="E16" t="s">
         <v>352</v>
       </c>
-      <c r="F16" s="69"/>
+      <c r="F16" s="68"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -3373,7 +3372,7 @@
       <c r="E17" t="s">
         <v>352</v>
       </c>
-      <c r="F17" s="69">
+      <c r="F17" s="68">
         <f>12.8*10*8760*0.69</f>
         <v>773683.19999999995</v>
       </c>
@@ -3400,7 +3399,7 @@
       <c r="E18" t="s">
         <v>352</v>
       </c>
-      <c r="F18" s="69">
+      <c r="F18" s="68">
         <f t="shared" ref="F18:F20" si="1">12.8*10*8760*0.69</f>
         <v>773683.19999999995</v>
       </c>
@@ -3427,7 +3426,7 @@
       <c r="E19" t="s">
         <v>352</v>
       </c>
-      <c r="F19" s="69">
+      <c r="F19" s="68">
         <f t="shared" si="1"/>
         <v>773683.19999999995</v>
       </c>
@@ -3454,7 +3453,7 @@
       <c r="E20" t="s">
         <v>352</v>
       </c>
-      <c r="F20" s="69">
+      <c r="F20" s="68">
         <f t="shared" si="1"/>
         <v>773683.19999999995</v>
       </c>
@@ -3478,7 +3477,7 @@
       <c r="E21" t="s">
         <v>353</v>
       </c>
-      <c r="F21" s="69">
+      <c r="F21" s="68">
         <f>7.57*1000</f>
         <v>7570</v>
       </c>
@@ -3502,14 +3501,14 @@
       <c r="E22" t="s">
         <v>354</v>
       </c>
-      <c r="F22" s="69">
+      <c r="F22" s="68">
         <f>45/0.000965</f>
         <v>46632.124352331608</v>
       </c>
       <c r="G22" t="s">
         <v>367</v>
       </c>
-      <c r="H22" s="68" t="s">
+      <c r="H22" s="67" t="s">
         <v>372</v>
       </c>
     </row>
@@ -3526,7 +3525,7 @@
       <c r="E23" t="s">
         <v>355</v>
       </c>
-      <c r="F23" s="69">
+      <c r="F23" s="68">
         <f>8.3*1000000</f>
         <v>8300000.0000000009</v>
       </c>
@@ -5927,129 +5926,129 @@
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E12" s="72">
+      <c r="E12" s="71">
         <f>E2/8760</f>
         <v>0.26187622965636759</v>
       </c>
-      <c r="F12" s="72">
+      <c r="F12" s="71">
         <f t="shared" ref="F12:Y12" si="0">F2/8760</f>
         <v>0.25572607372904549</v>
       </c>
-      <c r="G12" s="72">
+      <c r="G12" s="71">
         <f t="shared" si="0"/>
         <v>0.24957591780172336</v>
       </c>
-      <c r="H12" s="72">
+      <c r="H12" s="71">
         <f t="shared" si="0"/>
         <v>0.24342576187440126</v>
       </c>
-      <c r="I12" s="72">
+      <c r="I12" s="71">
         <f t="shared" si="0"/>
         <v>0.23727560594707917</v>
       </c>
-      <c r="J12" s="72">
+      <c r="J12" s="71">
         <f t="shared" si="0"/>
         <v>0.23112545001975709</v>
       </c>
-      <c r="K12" s="72">
+      <c r="K12" s="71">
         <f t="shared" si="0"/>
         <v>0.224975294092435</v>
       </c>
-      <c r="L12" s="72">
+      <c r="L12" s="71">
         <f t="shared" si="0"/>
         <v>0.21882513816511293</v>
       </c>
-      <c r="M12" s="72">
+      <c r="M12" s="71">
         <f t="shared" si="0"/>
         <v>0.21267498223779085</v>
       </c>
-      <c r="N12" s="72">
+      <c r="N12" s="71">
         <f t="shared" si="0"/>
         <v>0.20652482631046878</v>
       </c>
-      <c r="O12" s="72">
+      <c r="O12" s="71">
         <f t="shared" si="0"/>
         <v>0.20037467038314669</v>
       </c>
-      <c r="P12" s="72">
+      <c r="P12" s="71">
         <f t="shared" si="0"/>
         <v>0.19422451445582462</v>
       </c>
-      <c r="Q12" s="72">
+      <c r="Q12" s="71">
         <f t="shared" si="0"/>
         <v>0.18807435852850254</v>
       </c>
-      <c r="R12" s="72">
+      <c r="R12" s="71">
         <f t="shared" si="0"/>
         <v>0.18192420260118047</v>
       </c>
-      <c r="S12" s="72">
+      <c r="S12" s="71">
         <f t="shared" si="0"/>
         <v>0.17577404667385838</v>
       </c>
-      <c r="T12" s="72">
+      <c r="T12" s="71">
         <f t="shared" si="0"/>
         <v>0.1696238907465363</v>
       </c>
-      <c r="U12" s="72">
+      <c r="U12" s="71">
         <f t="shared" si="0"/>
         <v>0.16347373481921423</v>
       </c>
-      <c r="V12" s="72">
+      <c r="V12" s="71">
         <f t="shared" si="0"/>
         <v>0.15732357889189214</v>
       </c>
-      <c r="W12" s="72">
+      <c r="W12" s="71">
         <f t="shared" si="0"/>
         <v>0.15117342296457006</v>
       </c>
-      <c r="X12" s="72">
+      <c r="X12" s="71">
         <f t="shared" si="0"/>
         <v>0.14502326703724799</v>
       </c>
-      <c r="Y12" s="72">
+      <c r="Y12" s="71">
         <f t="shared" si="0"/>
         <v>0.13887311110992592</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E13" s="72">
+      <c r="E13" s="71">
         <f t="shared" ref="E13:E19" si="1">E3/8760</f>
         <v>0.28570875457778422</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E14" s="72">
+      <c r="E14" s="71">
         <f t="shared" si="1"/>
         <v>0.13368702269483454</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E15" s="72">
+      <c r="E15" s="71">
         <f t="shared" si="1"/>
         <v>0.19073300751397604</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="E16" s="72">
+      <c r="E16" s="71">
         <f t="shared" si="1"/>
         <v>0.68893673866789151</v>
       </c>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E17" s="72">
+      <c r="E17" s="71">
         <f t="shared" si="1"/>
         <v>0.68893673866789151</v>
       </c>
     </row>
     <row r="18" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E18" s="72">
+      <c r="E18" s="71">
         <f t="shared" si="1"/>
         <v>0.68893673866789151</v>
       </c>
     </row>
     <row r="19" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E19" s="72">
+      <c r="E19" s="71">
         <f t="shared" si="1"/>
         <v>0.68893673866789151</v>
       </c>
@@ -6177,7 +6176,7 @@
       <c r="F2" t="s">
         <v>112</v>
       </c>
-      <c r="G2" s="65">
+      <c r="G2" s="64">
         <v>1266.6666666666667</v>
       </c>
       <c r="H2" s="2">
@@ -6260,7 +6259,7 @@
       <c r="F3" t="s">
         <v>112</v>
       </c>
-      <c r="G3" s="65">
+      <c r="G3" s="64">
         <v>26.19047619047619</v>
       </c>
       <c r="H3" s="2">
@@ -6343,7 +6342,7 @@
       <c r="F4" t="s">
         <v>112</v>
       </c>
-      <c r="G4" s="65">
+      <c r="G4" s="64">
         <v>704.76190476190482</v>
       </c>
       <c r="H4" s="2">
@@ -6426,7 +6425,7 @@
       <c r="F5" t="s">
         <v>112</v>
       </c>
-      <c r="G5" s="65">
+      <c r="G5" s="64">
         <v>47.61904761904762</v>
       </c>
       <c r="H5" s="2">
@@ -6509,7 +6508,7 @@
       <c r="F6" t="s">
         <v>112</v>
       </c>
-      <c r="G6" s="65">
+      <c r="G6" s="64">
         <v>0.16563146997929609</v>
       </c>
       <c r="H6" s="2">
@@ -6592,7 +6591,7 @@
       <c r="F7" t="s">
         <v>112</v>
       </c>
-      <c r="G7" s="65">
+      <c r="G7" s="64">
         <v>1.0056196391600118</v>
       </c>
       <c r="H7" s="2">
@@ -6675,7 +6674,7 @@
       <c r="F8" t="s">
         <v>112</v>
       </c>
-      <c r="G8" s="65">
+      <c r="G8" s="64">
         <v>10</v>
       </c>
       <c r="H8" s="2">
@@ -6758,7 +6757,7 @@
       <c r="F9" t="s">
         <v>112</v>
       </c>
-      <c r="G9" s="65">
+      <c r="G9" s="64">
         <v>10</v>
       </c>
       <c r="H9" s="2">
@@ -6841,7 +6840,7 @@
       <c r="F10" t="s">
         <v>117</v>
       </c>
-      <c r="G10" s="65">
+      <c r="G10" s="64">
         <v>2.3661638568470866E-5</v>
       </c>
       <c r="H10" s="2">
@@ -6901,7 +6900,7 @@
       <c r="Z10" s="2">
         <v>4.7323277136941721E-4</v>
       </c>
-      <c r="AA10" s="65">
+      <c r="AA10" s="64">
         <v>4.9689440993788822E-4</v>
       </c>
     </row>
@@ -6924,7 +6923,7 @@
       <c r="F11" t="s">
         <v>117</v>
       </c>
-      <c r="G11" s="65">
+      <c r="G11" s="64">
         <v>14761.904761904761</v>
       </c>
       <c r="H11" s="2">
@@ -6984,7 +6983,7 @@
       <c r="Z11" s="2">
         <v>295238.09523809515</v>
       </c>
-      <c r="AA11" s="65">
+      <c r="AA11" s="64">
         <v>310000</v>
       </c>
     </row>
@@ -7007,7 +7006,7 @@
       <c r="F12" t="s">
         <v>117</v>
       </c>
-      <c r="G12" s="65">
+      <c r="G12" s="64">
         <v>523.80952380952385</v>
       </c>
       <c r="H12" s="2">
@@ -7067,7 +7066,7 @@
       <c r="Z12" s="2">
         <v>10476.190476190473</v>
       </c>
-      <c r="AA12" s="65">
+      <c r="AA12" s="64">
         <v>11000</v>
       </c>
     </row>
@@ -7090,7 +7089,7 @@
       <c r="F13" t="s">
         <v>117</v>
       </c>
-      <c r="G13" s="65">
+      <c r="G13" s="64">
         <v>3993.0890216824801</v>
       </c>
       <c r="H13" s="2">
@@ -7150,7 +7149,7 @@
       <c r="Z13" s="2">
         <v>79861.780433649576</v>
       </c>
-      <c r="AA13" s="65">
+      <c r="AA13" s="64">
         <v>83854.869455332082</v>
       </c>
     </row>
@@ -7173,7 +7172,7 @@
       <c r="F14" t="s">
         <v>117</v>
       </c>
-      <c r="G14" s="65">
+      <c r="G14" s="64">
         <v>20</v>
       </c>
       <c r="H14" s="2">
@@ -7233,7 +7232,7 @@
       <c r="Z14" s="2">
         <v>20</v>
       </c>
-      <c r="AA14" s="65">
+      <c r="AA14" s="64">
         <v>20</v>
       </c>
     </row>
@@ -7256,7 +7255,7 @@
       <c r="F15" t="s">
         <v>117</v>
       </c>
-      <c r="G15" s="65">
+      <c r="G15" s="64">
         <v>20</v>
       </c>
       <c r="H15" s="2">
@@ -7316,7 +7315,7 @@
       <c r="Z15" s="2">
         <v>20</v>
       </c>
-      <c r="AA15" s="65">
+      <c r="AA15" s="64">
         <v>20</v>
       </c>
     </row>
@@ -7339,7 +7338,7 @@
       <c r="F16" t="s">
         <v>57</v>
       </c>
-      <c r="G16" s="65">
+      <c r="G16" s="64">
         <v>1893379.5969071945</v>
       </c>
       <c r="H16" s="2">
@@ -7399,7 +7398,7 @@
       <c r="Z16" s="2">
         <v>37867591.938143879</v>
       </c>
-      <c r="AA16" s="65">
+      <c r="AA16" s="64">
         <v>39760971.535051085</v>
       </c>
     </row>
@@ -7422,7 +7421,7 @@
       <c r="F17" t="s">
         <v>57</v>
       </c>
-      <c r="G17" s="65">
+      <c r="G17" s="64">
         <v>122512.79744693608</v>
       </c>
       <c r="H17" s="2">
@@ -7482,7 +7481,7 @@
       <c r="Z17" s="2">
         <v>2450255.9489387218</v>
       </c>
-      <c r="AA17" s="65">
+      <c r="AA17" s="64">
         <v>2572768.7463856577</v>
       </c>
     </row>
@@ -7505,7 +7504,7 @@
       <c r="F18" t="s">
         <v>135</v>
       </c>
-      <c r="G18" s="65">
+      <c r="G18" s="64">
         <v>274.72527472527474</v>
       </c>
       <c r="H18" s="2">
@@ -7588,7 +7587,7 @@
       <c r="F19" t="s">
         <v>135</v>
       </c>
-      <c r="G19" s="65">
+      <c r="G19" s="64">
         <v>10.989010989010989</v>
       </c>
       <c r="H19" s="2">
@@ -7671,7 +7670,7 @@
       <c r="F20" t="s">
         <v>135</v>
       </c>
-      <c r="G20" s="65">
+      <c r="G20" s="64">
         <v>4081.6326530612241</v>
       </c>
       <c r="H20" s="2">
@@ -9667,8 +9666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8F51DB9-2485-024A-9940-AED9C0912620}">
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10461,24 +10460,25 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J68"/>
+  <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.875" customWidth="1"/>
     <col min="2" max="2" width="24.375" customWidth="1"/>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="5" width="26" customWidth="1"/>
-    <col min="6" max="7" width="24.125" customWidth="1"/>
-    <col min="8" max="8" width="31.5" customWidth="1"/>
-    <col min="9" max="9" width="36.875" customWidth="1"/>
+    <col min="3" max="3" width="21" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="26" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="24.125" customWidth="1"/>
+    <col min="7" max="7" width="31.5" customWidth="1"/>
+    <col min="8" max="8" width="36.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10495,19 +10495,16 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -10523,14 +10520,11 @@
       <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2">
+      <c r="F2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>11</v>
       </c>
@@ -10546,20 +10540,17 @@
       <c r="E3" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="38">
+      <c r="F3" s="38">
         <v>18</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="H3" s="36" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -10575,14 +10566,11 @@
       <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4">
+      <c r="F4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -10598,14 +10586,11 @@
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5">
+      <c r="F5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -10621,14 +10606,11 @@
       <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6">
+      <c r="F6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -10644,14 +10626,11 @@
       <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="F7" t="s">
-        <v>32</v>
-      </c>
-      <c r="G7">
+      <c r="F7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
         <v>37</v>
       </c>
@@ -10667,14 +10646,11 @@
       <c r="E8" t="s">
         <v>15</v>
       </c>
-      <c r="F8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G8">
+      <c r="F8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>42</v>
       </c>
@@ -10690,18 +10666,15 @@
       <c r="E9" t="s">
         <v>15</v>
       </c>
-      <c r="F9" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="48">
-        <f>G10*15%</f>
+      <c r="F9" s="48">
+        <f>F10*15%</f>
         <v>-8.1</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>43</v>
       </c>
@@ -10717,18 +10690,15 @@
       <c r="E10" t="s">
         <v>15</v>
       </c>
-      <c r="F10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="48">
+      <c r="F10" s="48">
         <f>-94+'C2U CI'!G5</f>
         <v>-54</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="55" t="s">
         <v>40</v>
       </c>
@@ -10744,18 +10714,15 @@
       <c r="E11" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="F11" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11">
-        <v>25</v>
-      </c>
-      <c r="H11" s="36" t="s">
+      <c r="F11" s="2">
+        <v>47</v>
+      </c>
+      <c r="G11" s="36" t="s">
         <v>340</v>
       </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="55" t="s">
         <v>37</v>
       </c>
@@ -10771,23 +10738,20 @@
       <c r="E12" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="F12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12">
+      <c r="F12">
         <v>22</v>
       </c>
-      <c r="H12" t="s">
+      <c r="G12" t="s">
         <v>344</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="J12" t="s">
+      <c r="I12" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
         <v>36</v>
       </c>
@@ -10803,23 +10767,20 @@
       <c r="E13" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="F13" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13">
+      <c r="F13">
         <v>22</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G13" t="s">
         <v>344</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J13" t="s">
+      <c r="I13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>42</v>
       </c>
@@ -10835,18 +10796,15 @@
       <c r="E14" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="F14" t="s">
-        <v>32</v>
-      </c>
-      <c r="G14">
-        <f>G15*15%</f>
+      <c r="F14">
+        <f>F15*15%</f>
         <v>-30</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>43</v>
       </c>
@@ -10862,17 +10820,14 @@
       <c r="E15" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="F15" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15">
+      <c r="F15">
         <v>-200</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -10888,15 +10843,12 @@
       <c r="E16" t="s">
         <v>15</v>
       </c>
-      <c r="F16" t="s">
-        <v>32</v>
-      </c>
-      <c r="G16">
+      <c r="F16">
         <v>45</v>
       </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -10912,17 +10864,14 @@
       <c r="E17" t="s">
         <v>15</v>
       </c>
-      <c r="F17" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17">
+      <c r="F17">
         <v>-150</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="G17" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -10938,17 +10887,14 @@
       <c r="E18" t="s">
         <v>15</v>
       </c>
-      <c r="F18" t="s">
-        <v>32</v>
-      </c>
-      <c r="G18">
+      <c r="F18">
         <v>70</v>
       </c>
-      <c r="H18" t="s">
+      <c r="G18" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
@@ -10964,17 +10910,14 @@
       <c r="E19" t="s">
         <v>15</v>
       </c>
-      <c r="F19" t="s">
-        <v>32</v>
-      </c>
-      <c r="G19">
+      <c r="F19">
         <v>50</v>
       </c>
-      <c r="H19" t="s">
+      <c r="G19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -10990,20 +10933,17 @@
       <c r="E20" t="s">
         <v>15</v>
       </c>
-      <c r="F20" t="s">
-        <v>32</v>
-      </c>
-      <c r="G20">
+      <c r="F20">
         <v>7.7</v>
       </c>
-      <c r="H20" t="s">
+      <c r="G20" t="s">
         <v>47</v>
       </c>
-      <c r="I20" t="s">
+      <c r="H20" s="36" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -11019,20 +10959,17 @@
       <c r="E21" t="s">
         <v>15</v>
       </c>
-      <c r="F21" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21">
+      <c r="F21">
         <v>8.3000000000000007</v>
       </c>
+      <c r="G21" t="s">
+        <v>47</v>
+      </c>
       <c r="H21" t="s">
-        <v>47</v>
-      </c>
-      <c r="I21" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -11048,14 +10985,11 @@
       <c r="E22" t="s">
         <v>24</v>
       </c>
-      <c r="F22" t="s">
-        <v>32</v>
-      </c>
-      <c r="G22">
+      <c r="F22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="55" t="s">
         <v>11</v>
       </c>
@@ -11071,20 +11005,17 @@
       <c r="E23" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="F23" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23">
-        <v>11</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="F23" s="2">
+        <v>21</v>
+      </c>
+      <c r="G23" t="s">
         <v>33</v>
       </c>
-      <c r="I23" s="36" t="s">
+      <c r="H23" s="36" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -11100,14 +11031,11 @@
       <c r="E24" t="s">
         <v>24</v>
       </c>
-      <c r="F24" t="s">
-        <v>32</v>
-      </c>
-      <c r="G24">
+      <c r="F24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -11123,14 +11051,11 @@
       <c r="E25" t="s">
         <v>24</v>
       </c>
-      <c r="F25" t="s">
-        <v>32</v>
-      </c>
-      <c r="G25">
+      <c r="F25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -11146,14 +11071,11 @@
       <c r="E26" t="s">
         <v>24</v>
       </c>
-      <c r="F26" t="s">
-        <v>32</v>
-      </c>
-      <c r="G26">
+      <c r="F26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -11169,14 +11091,11 @@
       <c r="E27" t="s">
         <v>24</v>
       </c>
-      <c r="F27" t="s">
-        <v>32</v>
-      </c>
-      <c r="G27">
+      <c r="F27">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -11192,14 +11111,11 @@
       <c r="E28" t="s">
         <v>24</v>
       </c>
-      <c r="F28" t="s">
-        <v>32</v>
-      </c>
-      <c r="G28">
+      <c r="F28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>42</v>
       </c>
@@ -11215,18 +11131,15 @@
       <c r="E29" t="s">
         <v>24</v>
       </c>
-      <c r="F29" t="s">
-        <v>32</v>
-      </c>
-      <c r="G29" s="48">
-        <f>G30*15%</f>
-        <v>-73.5</v>
-      </c>
-      <c r="I29" s="3" t="s">
+      <c r="F29" s="48">
+        <f>F30*15%</f>
+        <v>-8.1</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>43</v>
       </c>
@@ -11242,534 +11155,471 @@
       <c r="E30" t="s">
         <v>24</v>
       </c>
-      <c r="F30" t="s">
-        <v>32</v>
-      </c>
-      <c r="G30">
+      <c r="F30">
+        <f>F10</f>
+        <v>-54</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="55" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="2">
+        <v>76</v>
+      </c>
+      <c r="G31" s="36" t="s">
+        <v>340</v>
+      </c>
+      <c r="H31" s="3"/>
+    </row>
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="F32">
+        <v>71.7</v>
+      </c>
+      <c r="G32" s="55" t="s">
+        <v>339</v>
+      </c>
+      <c r="H32" s="56" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33">
+        <f>F34*15%</f>
+        <v>-13.5</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D34" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34">
+        <v>-90</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="55" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D35" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="E35" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35">
+        <v>71.7</v>
+      </c>
+      <c r="G35" s="55" t="s">
+        <v>339</v>
+      </c>
+      <c r="H35" s="36" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" t="s">
+        <v>31</v>
+      </c>
+      <c r="E36" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36">
+        <v>45</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H36" s="3"/>
+    </row>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37">
+        <v>-132.5</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>30</v>
+      </c>
+      <c r="D38" t="s">
+        <v>31</v>
+      </c>
+      <c r="E38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38">
+        <v>70</v>
+      </c>
+      <c r="G38" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" t="s">
+        <v>30</v>
+      </c>
+      <c r="D39" t="s">
+        <v>31</v>
+      </c>
+      <c r="E39" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39">
+        <v>50</v>
+      </c>
+      <c r="G39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D40" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" t="s">
+        <v>24</v>
+      </c>
+      <c r="F40">
+        <v>29.3</v>
+      </c>
+      <c r="H40" s="36" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" t="s">
+        <v>31</v>
+      </c>
+      <c r="E41" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41">
+        <v>23.8</v>
+      </c>
+      <c r="H41" s="36" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>11</v>
+      </c>
+      <c r="B42" t="s">
+        <v>12</v>
+      </c>
+      <c r="C42" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" t="s">
+        <v>31</v>
+      </c>
+      <c r="E42" t="s">
+        <v>26</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="55" t="s">
+        <v>11</v>
+      </c>
+      <c r="B43" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="D43" s="55" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43" s="55" t="s">
+        <v>26</v>
+      </c>
+      <c r="F43">
+        <v>11</v>
+      </c>
+      <c r="G43" t="s">
+        <v>33</v>
+      </c>
+      <c r="H43" s="36" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" t="s">
+        <v>31</v>
+      </c>
+      <c r="E44" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" t="s">
+        <v>31</v>
+      </c>
+      <c r="E45" t="s">
+        <v>26</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C46" t="s">
+        <v>30</v>
+      </c>
+      <c r="D46" t="s">
+        <v>31</v>
+      </c>
+      <c r="E46" t="s">
+        <v>26</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>36</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" t="s">
+        <v>26</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>37</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C48" t="s">
+        <v>30</v>
+      </c>
+      <c r="D48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E48" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" t="s">
+        <v>31</v>
+      </c>
+      <c r="E49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F49" s="48">
+        <f>F50*15%</f>
+        <v>-73.5</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" t="s">
+        <v>30</v>
+      </c>
+      <c r="D50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" t="s">
+        <v>26</v>
+      </c>
+      <c r="F50">
         <f>-530+'C2U CI'!G5</f>
         <v>-490</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="H50" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="55" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="E31" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G31">
-        <v>47</v>
-      </c>
-      <c r="H31" s="36" t="s">
-        <v>340</v>
-      </c>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="55" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="E32" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="F32" t="s">
-        <v>32</v>
-      </c>
-      <c r="G32">
-        <v>71.7</v>
-      </c>
-      <c r="H32" s="55" t="s">
-        <v>339</v>
-      </c>
-      <c r="I32" s="56" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C33" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="E33" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="F33" t="s">
-        <v>32</v>
-      </c>
-      <c r="G33">
-        <f>G34*15%</f>
-        <v>-13.5</v>
-      </c>
-      <c r="I33" s="3" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B34" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D34" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="E34" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="F34" t="s">
-        <v>32</v>
-      </c>
-      <c r="G34">
-        <v>-90</v>
-      </c>
-      <c r="I34" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C35" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D35" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="E35" s="55" t="s">
-        <v>24</v>
-      </c>
-      <c r="F35" t="s">
-        <v>32</v>
-      </c>
-      <c r="G35">
-        <v>71.7</v>
-      </c>
-      <c r="H35" s="55" t="s">
-        <v>339</v>
-      </c>
-      <c r="I35" s="36" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>42</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C36" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36" t="s">
-        <v>31</v>
-      </c>
-      <c r="E36" t="s">
-        <v>24</v>
-      </c>
-      <c r="F36" t="s">
-        <v>32</v>
-      </c>
-      <c r="G36">
-        <v>45</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>43</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" t="s">
-        <v>30</v>
-      </c>
-      <c r="D37" t="s">
-        <v>31</v>
-      </c>
-      <c r="E37" t="s">
-        <v>24</v>
-      </c>
-      <c r="F37" t="s">
-        <v>32</v>
-      </c>
-      <c r="G37">
-        <v>-132.5</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C38" t="s">
-        <v>30</v>
-      </c>
-      <c r="D38" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" t="s">
-        <v>24</v>
-      </c>
-      <c r="F38" t="s">
-        <v>32</v>
-      </c>
-      <c r="G38">
-        <v>70</v>
-      </c>
-      <c r="H38" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>48</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D39" t="s">
-        <v>31</v>
-      </c>
-      <c r="E39" t="s">
-        <v>24</v>
-      </c>
-      <c r="F39" t="s">
-        <v>32</v>
-      </c>
-      <c r="G39">
-        <v>50</v>
-      </c>
-      <c r="H39" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" t="s">
-        <v>30</v>
-      </c>
-      <c r="D40" t="s">
-        <v>31</v>
-      </c>
-      <c r="E40" t="s">
-        <v>24</v>
-      </c>
-      <c r="F40" t="s">
-        <v>32</v>
-      </c>
-      <c r="G40">
-        <v>29.3</v>
-      </c>
-      <c r="I40" s="36" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>36</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" t="s">
-        <v>30</v>
-      </c>
-      <c r="D41" t="s">
-        <v>31</v>
-      </c>
-      <c r="E41" t="s">
-        <v>24</v>
-      </c>
-      <c r="F41" t="s">
-        <v>32</v>
-      </c>
-      <c r="G41">
-        <v>23.8</v>
-      </c>
-      <c r="I41" s="36" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>11</v>
-      </c>
-      <c r="B42" t="s">
-        <v>12</v>
-      </c>
-      <c r="C42" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" t="s">
-        <v>31</v>
-      </c>
-      <c r="E42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F42" t="s">
-        <v>32</v>
-      </c>
-      <c r="G42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="55" t="s">
-        <v>11</v>
-      </c>
-      <c r="B43" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="C43" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" s="55" t="s">
-        <v>31</v>
-      </c>
-      <c r="E43" s="55" t="s">
-        <v>26</v>
-      </c>
-      <c r="F43" t="s">
-        <v>32</v>
-      </c>
-      <c r="G43">
-        <v>21</v>
-      </c>
-      <c r="H43" t="s">
-        <v>33</v>
-      </c>
-      <c r="I43" s="36" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>22</v>
-      </c>
-      <c r="B44" t="s">
-        <v>12</v>
-      </c>
-      <c r="C44" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" t="s">
-        <v>31</v>
-      </c>
-      <c r="E44" t="s">
-        <v>26</v>
-      </c>
-      <c r="F44" t="s">
-        <v>32</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C45" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" t="s">
-        <v>31</v>
-      </c>
-      <c r="E45" t="s">
-        <v>26</v>
-      </c>
-      <c r="F45" t="s">
-        <v>32</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C46" t="s">
-        <v>30</v>
-      </c>
-      <c r="D46" t="s">
-        <v>31</v>
-      </c>
-      <c r="E46" t="s">
-        <v>26</v>
-      </c>
-      <c r="F46" t="s">
-        <v>32</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>36</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C47" t="s">
-        <v>30</v>
-      </c>
-      <c r="D47" t="s">
-        <v>31</v>
-      </c>
-      <c r="E47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" t="s">
-        <v>32</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>37</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C48" t="s">
-        <v>30</v>
-      </c>
-      <c r="D48" t="s">
-        <v>31</v>
-      </c>
-      <c r="E48" t="s">
-        <v>26</v>
-      </c>
-      <c r="F48" t="s">
-        <v>32</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" t="s">
-        <v>30</v>
-      </c>
-      <c r="D49" t="s">
-        <v>31</v>
-      </c>
-      <c r="E49" t="s">
-        <v>26</v>
-      </c>
-      <c r="F49" t="s">
-        <v>32</v>
-      </c>
-      <c r="G49" s="48">
-        <f>G50*15%</f>
-        <v>-108.3</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" t="s">
-        <v>30</v>
-      </c>
-      <c r="D50" t="s">
-        <v>31</v>
-      </c>
-      <c r="E50" t="s">
-        <v>26</v>
-      </c>
-      <c r="F50" t="s">
-        <v>32</v>
-      </c>
-      <c r="G50">
-        <f>-762+'C2U CI'!G5</f>
-        <v>-722</v>
-      </c>
-      <c r="I50" s="3" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="55" t="s">
         <v>40</v>
       </c>
@@ -11785,18 +11635,15 @@
       <c r="E51" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="F51" t="s">
-        <v>32</v>
-      </c>
-      <c r="G51">
-        <v>76</v>
-      </c>
-      <c r="H51" s="36" t="s">
+      <c r="F51" s="2">
+        <v>25</v>
+      </c>
+      <c r="G51" s="36" t="s">
         <v>340</v>
       </c>
-      <c r="I51" s="3"/>
-    </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="55" t="s">
         <v>37</v>
       </c>
@@ -11812,20 +11659,17 @@
       <c r="E52" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="F52" t="s">
-        <v>32</v>
-      </c>
-      <c r="G52">
+      <c r="F52">
         <v>3</v>
       </c>
-      <c r="H52" s="55" t="s">
+      <c r="G52" s="55" t="s">
         <v>343</v>
       </c>
-      <c r="I52" s="56" t="s">
+      <c r="H52" s="56" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>42</v>
       </c>
@@ -11841,18 +11685,15 @@
       <c r="E53" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="F53" t="s">
-        <v>32</v>
-      </c>
-      <c r="G53">
-        <f>G54*15%</f>
+      <c r="F53">
+        <f>F54*15%</f>
         <v>-46.35</v>
       </c>
-      <c r="I53" s="3" t="s">
+      <c r="H53" s="3" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>43</v>
       </c>
@@ -11868,17 +11709,14 @@
       <c r="E54" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="F54" t="s">
-        <v>32</v>
-      </c>
-      <c r="G54">
+      <c r="F54">
         <v>-309</v>
       </c>
-      <c r="I54" s="3" t="s">
+      <c r="H54" s="3" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="55" t="s">
         <v>36</v>
       </c>
@@ -11894,20 +11732,17 @@
       <c r="E55" s="55" t="s">
         <v>26</v>
       </c>
-      <c r="F55" t="s">
-        <v>32</v>
-      </c>
-      <c r="G55">
+      <c r="F55">
         <v>3</v>
       </c>
-      <c r="H55" s="55" t="s">
+      <c r="G55" s="55" t="s">
         <v>343</v>
       </c>
-      <c r="I55" s="56" t="s">
+      <c r="H55" s="56" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -11923,18 +11758,15 @@
       <c r="E56" t="s">
         <v>26</v>
       </c>
-      <c r="F56" t="s">
-        <v>32</v>
-      </c>
-      <c r="G56">
+      <c r="F56">
         <v>45</v>
       </c>
-      <c r="H56" s="6" t="s">
+      <c r="G56" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="I56" s="3"/>
-    </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -11950,17 +11782,14 @@
       <c r="E57" t="s">
         <v>26</v>
       </c>
-      <c r="F57" t="s">
-        <v>32</v>
-      </c>
-      <c r="G57">
+      <c r="F57">
         <v>-328.8</v>
       </c>
-      <c r="H57" s="6" t="s">
+      <c r="G57" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>45</v>
       </c>
@@ -11976,17 +11805,14 @@
       <c r="E58" t="s">
         <v>26</v>
       </c>
-      <c r="F58" t="s">
-        <v>32</v>
-      </c>
-      <c r="G58">
+      <c r="F58">
         <v>47.5</v>
       </c>
-      <c r="H58" t="s">
+      <c r="G58" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -12002,17 +11828,14 @@
       <c r="E59" t="s">
         <v>26</v>
       </c>
-      <c r="F59" t="s">
-        <v>32</v>
-      </c>
-      <c r="G59">
+      <c r="F59">
         <v>32.799999999999997</v>
       </c>
-      <c r="H59" t="s">
+      <c r="G59" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -12028,14 +11851,11 @@
       <c r="E60" t="s">
         <v>26</v>
       </c>
-      <c r="F60" t="s">
-        <v>32</v>
-      </c>
-      <c r="G60" s="12">
+      <c r="F60" s="12">
         <v>7.7</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -12051,41 +11871,40 @@
       <c r="E61" t="s">
         <v>26</v>
       </c>
-      <c r="F61" t="s">
-        <v>32</v>
-      </c>
-      <c r="G61" s="12">
+      <c r="F61" s="12">
         <v>8.3000000000000007</v>
       </c>
     </row>
-    <row r="67" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F67" s="5"/>
-    </row>
-    <row r="68" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F68" s="64"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J61" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}">
+  <autoFilter ref="A1:I61" xr:uid="{732D9AEE-59CF-9744-8E33-A83B08C738C6}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Agricultural waste"/>
+        <filter val="Animal Fat"/>
+        <filter val="Forest waste"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="1">
       <filters>
-        <filter val="Electricity"/>
+        <filter val="Sustainable Aviation Fuel"/>
       </filters>
     </filterColumn>
   </autoFilter>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I40" r:id="rId1" xr:uid="{3DE9360D-4B28-4580-B9AC-7A8A7FDEC5D9}"/>
-    <hyperlink ref="I41" r:id="rId2" xr:uid="{616833AB-8ACA-41F8-8D0E-642E78789A77}"/>
-    <hyperlink ref="I52" r:id="rId3" xr:uid="{8E40FAC8-BE6F-4972-8F8A-D7FFC804E06E}"/>
-    <hyperlink ref="I55" r:id="rId4" xr:uid="{F8847031-885E-40E1-92C0-8616552E06FA}"/>
-    <hyperlink ref="I32" r:id="rId5" xr:uid="{5E2BC77F-A5F7-4E28-8FD6-6908622A66F4}"/>
-    <hyperlink ref="I35" r:id="rId6" display="https://bof.fire.ca.gov/media/10190/introduction-to-the-hydrogen-market-in-california-draft-for-comment_ada.pdf" xr:uid="{D1B92899-5F56-4BC1-9B1A-753C033ABE12}"/>
-    <hyperlink ref="H11" r:id="rId7" xr:uid="{ABF6638B-67E6-4462-9698-7878ED08063F}"/>
-    <hyperlink ref="H31" r:id="rId8" xr:uid="{6CC27E2D-896B-4F52-9EBF-B1D4967B49EA}"/>
-    <hyperlink ref="H51" r:id="rId9" xr:uid="{3FA6F57B-1576-49E0-BC0A-B6213F870ACC}"/>
-    <hyperlink ref="I3" r:id="rId10" display="https://bof.fire.ca.gov/media/10190/introduction-to-the-hydrogen-market-in-california-draft-for-comment_ada.pdf" xr:uid="{40CAFF63-7148-4667-98FE-FFF89E0DA688}"/>
-    <hyperlink ref="I23" r:id="rId11" display="https://bof.fire.ca.gov/media/10190/introduction-to-the-hydrogen-market-in-california-draft-for-comment_ada.pdf" xr:uid="{42190A8E-57A6-46F3-8FA3-71EA01DCB935}"/>
-    <hyperlink ref="I43" r:id="rId12" display="https://bof.fire.ca.gov/media/10190/introduction-to-the-hydrogen-market-in-california-draft-for-comment_ada.pdf" xr:uid="{4D26B25D-D196-4051-BCD5-66F3EB235350}"/>
+    <hyperlink ref="H40" r:id="rId1" xr:uid="{3DE9360D-4B28-4580-B9AC-7A8A7FDEC5D9}"/>
+    <hyperlink ref="H41" r:id="rId2" xr:uid="{616833AB-8ACA-41F8-8D0E-642E78789A77}"/>
+    <hyperlink ref="H52" r:id="rId3" xr:uid="{8E40FAC8-BE6F-4972-8F8A-D7FFC804E06E}"/>
+    <hyperlink ref="H55" r:id="rId4" xr:uid="{F8847031-885E-40E1-92C0-8616552E06FA}"/>
+    <hyperlink ref="H32" r:id="rId5" xr:uid="{5E2BC77F-A5F7-4E28-8FD6-6908622A66F4}"/>
+    <hyperlink ref="H35" r:id="rId6" display="https://bof.fire.ca.gov/media/10190/introduction-to-the-hydrogen-market-in-california-draft-for-comment_ada.pdf" xr:uid="{D1B92899-5F56-4BC1-9B1A-753C033ABE12}"/>
+    <hyperlink ref="G11" r:id="rId7" xr:uid="{ABF6638B-67E6-4462-9698-7878ED08063F}"/>
+    <hyperlink ref="G31" r:id="rId8" xr:uid="{6CC27E2D-896B-4F52-9EBF-B1D4967B49EA}"/>
+    <hyperlink ref="G51" r:id="rId9" xr:uid="{3FA6F57B-1576-49E0-BC0A-B6213F870ACC}"/>
+    <hyperlink ref="H3" r:id="rId10" display="https://bof.fire.ca.gov/media/10190/introduction-to-the-hydrogen-market-in-california-draft-for-comment_ada.pdf" xr:uid="{40CAFF63-7148-4667-98FE-FFF89E0DA688}"/>
+    <hyperlink ref="H23" r:id="rId11" display="https://bof.fire.ca.gov/media/10190/introduction-to-the-hydrogen-market-in-california-draft-for-comment_ada.pdf" xr:uid="{42190A8E-57A6-46F3-8FA3-71EA01DCB935}"/>
+    <hyperlink ref="H43" r:id="rId12" display="https://bof.fire.ca.gov/media/10190/introduction-to-the-hydrogen-market-in-california-draft-for-comment_ada.pdf" xr:uid="{4D26B25D-D196-4051-BCD5-66F3EB235350}"/>
+    <hyperlink ref="H20" r:id="rId13" xr:uid="{88B8FD66-4AC8-4CA2-B7D0-7617FFEA76D1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12224,11 +12043,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FEFDD9-D46C-E64E-8B04-7DDDC1C1B0F3}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F10"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12324,7 +12142,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -12407,7 +12225,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -12490,7 +12308,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -12573,7 +12391,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -12656,7 +12474,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -12739,7 +12557,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -13113,7 +12931,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -13196,7 +13014,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -13300,7 +13118,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -13404,7 +13222,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -13487,7 +13305,7 @@
         <v>80.36</v>
       </c>
     </row>
-    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -13591,7 +13409,7 @@
         <v>80.36</v>
       </c>
     </row>
-    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -13696,13 +13514,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA16" xr:uid="{68FEFDD9-D46C-E64E-8B04-7DDDC1C1B0F3}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Surface Transport Fuel"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AA16" xr:uid="{68FEFDD9-D46C-E64E-8B04-7DDDC1C1B0F3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13711,8 +13523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C58C4D02-922E-2849-99A2-B5A24807FA42}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F11" sqref="A11:F11"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -14905,7 +14717,7 @@
       <c r="K5">
         <v>8.3034948476273795E-3</v>
       </c>
-      <c r="L5" s="71">
+      <c r="L5" s="70">
         <v>2.242</v>
       </c>
       <c r="M5" s="8">
@@ -14950,7 +14762,7 @@
       <c r="K6">
         <v>8.3034948476273795E-3</v>
       </c>
-      <c r="L6" s="71">
+      <c r="L6" s="70">
         <v>1.044</v>
       </c>
       <c r="M6" s="8">
@@ -15268,10 +15080,10 @@
       <c r="J14">
         <v>26.59</v>
       </c>
-      <c r="K14" s="67">
+      <c r="K14" s="66">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L14" s="67">
+      <c r="L14" s="66">
         <v>5.016</v>
       </c>
       <c r="M14">
@@ -15313,10 +15125,10 @@
       <c r="J15">
         <v>0</v>
       </c>
-      <c r="K15" s="67">
+      <c r="K15" s="66">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L15" s="67">
+      <c r="L15" s="66">
         <v>4.2050000000000001</v>
       </c>
       <c r="M15">
@@ -15358,10 +15170,10 @@
       <c r="J16">
         <v>0</v>
       </c>
-      <c r="K16" s="67">
+      <c r="K16" s="66">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L16" s="67">
+      <c r="L16" s="66">
         <v>4.8159999999999998</v>
       </c>
       <c r="M16">
@@ -15403,10 +15215,10 @@
       <c r="J17">
         <v>26.59</v>
       </c>
-      <c r="K17" s="67">
+      <c r="K17" s="66">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L17" s="67">
+      <c r="L17" s="66">
         <v>5.016</v>
       </c>
       <c r="M17">
@@ -15448,10 +15260,10 @@
       <c r="J18">
         <v>0</v>
       </c>
-      <c r="K18" s="67">
+      <c r="K18" s="66">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L18" s="67">
+      <c r="L18" s="66">
         <v>4.2050000000000001</v>
       </c>
       <c r="M18">
@@ -15493,10 +15305,10 @@
       <c r="J19">
         <v>0</v>
       </c>
-      <c r="K19" s="67">
+      <c r="K19" s="66">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L19" s="67">
+      <c r="L19" s="66">
         <v>4.8159999999999998</v>
       </c>
       <c r="M19">
@@ -15538,10 +15350,10 @@
       <c r="J20">
         <v>26.59</v>
       </c>
-      <c r="K20" s="67">
+      <c r="K20" s="66">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L20" s="67">
+      <c r="L20" s="66">
         <v>5.016</v>
       </c>
       <c r="M20">
@@ -15583,10 +15395,10 @@
       <c r="J21">
         <v>0</v>
       </c>
-      <c r="K21" s="67">
+      <c r="K21" s="66">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L21" s="67">
+      <c r="L21" s="66">
         <v>4.2050000000000001</v>
       </c>
       <c r="M21">
@@ -15628,10 +15440,10 @@
       <c r="J22">
         <v>0</v>
       </c>
-      <c r="K22" s="67">
+      <c r="K22" s="66">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L22" s="67">
+      <c r="L22" s="66">
         <v>4.8159999999999998</v>
       </c>
       <c r="M22">
@@ -15673,10 +15485,10 @@
       <c r="J23">
         <v>26.59</v>
       </c>
-      <c r="K23" s="67">
+      <c r="K23" s="66">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L23" s="67">
+      <c r="L23" s="66">
         <v>5.016</v>
       </c>
       <c r="M23">
@@ -15718,10 +15530,10 @@
       <c r="J24">
         <v>0</v>
       </c>
-      <c r="K24" s="67">
+      <c r="K24" s="66">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L24" s="67">
+      <c r="L24" s="66">
         <v>4.2050000000000001</v>
       </c>
       <c r="M24">
@@ -15763,10 +15575,10 @@
       <c r="J25">
         <v>0</v>
       </c>
-      <c r="K25" s="67">
+      <c r="K25" s="66">
         <v>1.1585743964712399E-2</v>
       </c>
-      <c r="L25" s="67">
+      <c r="L25" s="66">
         <v>4.8159999999999998</v>
       </c>
       <c r="M25">
@@ -16129,7 +15941,7 @@
       <c r="K33">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="L33" s="67">
+      <c r="L33" s="66">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="M33" s="13">
@@ -16273,7 +16085,7 @@
       <c r="K36">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="L36" s="67">
+      <c r="L36" s="66">
         <v>8.5000000000000006E-2</v>
       </c>
       <c r="M36" s="13">
@@ -16936,7 +16748,7 @@
       <c r="L50">
         <v>1.7509999999999999</v>
       </c>
-      <c r="M50" s="70">
+      <c r="M50" s="69">
         <f>L50/0.007</f>
         <v>250.14285714285711</v>
       </c>
@@ -16984,7 +16796,7 @@
       <c r="L51">
         <v>0.78400000000000003</v>
       </c>
-      <c r="M51" s="70">
+      <c r="M51" s="69">
         <f>L51/0.007</f>
         <v>112</v>
       </c>
@@ -17032,7 +16844,7 @@
       <c r="L52">
         <v>0.70299999999999996</v>
       </c>
-      <c r="M52" s="70">
+      <c r="M52" s="69">
         <f>L52/0.007</f>
         <v>100.42857142857142</v>
       </c>
@@ -17080,7 +16892,7 @@
       <c r="L53">
         <v>0.24099999999999999</v>
       </c>
-      <c r="M53" s="70">
+      <c r="M53" s="69">
         <f>L53/0.007</f>
         <v>34.428571428571423</v>
       </c>
@@ -17125,10 +16937,10 @@
       <c r="K54">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="L54" s="67">
+      <c r="L54" s="66">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="M54" s="70">
+      <c r="M54" s="69">
         <f>L54/0.007</f>
         <v>12.142857142857144</v>
       </c>
@@ -17176,7 +16988,7 @@
       <c r="L55">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="M55" s="70">
+      <c r="M55" s="69">
         <f t="shared" ref="M55:M58" si="6">L55/0.007</f>
         <v>12.285714285714285</v>
       </c>
@@ -17224,7 +17036,7 @@
       <c r="L56">
         <v>0.24099999999999999</v>
       </c>
-      <c r="M56" s="70">
+      <c r="M56" s="69">
         <f t="shared" si="6"/>
         <v>34.428571428571423</v>
       </c>
@@ -17269,10 +17081,10 @@
       <c r="K57">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="L57" s="67">
+      <c r="L57" s="66">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="M57" s="70">
+      <c r="M57" s="69">
         <f t="shared" si="6"/>
         <v>12.142857142857144</v>
       </c>
@@ -17320,7 +17132,7 @@
       <c r="L58">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="M58" s="70">
+      <c r="M58" s="69">
         <f t="shared" si="6"/>
         <v>12.285714285714285</v>
       </c>
@@ -17428,25 +17240,25 @@
       <c r="D2" t="s">
         <v>315</v>
       </c>
-      <c r="E2" s="72">
+      <c r="E2" s="71">
         <v>0</v>
       </c>
-      <c r="F2" s="72">
+      <c r="F2" s="71">
         <v>2.564102564102564E-2</v>
       </c>
-      <c r="G2" s="72">
+      <c r="G2" s="71">
         <v>0.51282051282051277</v>
       </c>
-      <c r="H2" s="72">
+      <c r="H2" s="71">
         <v>0.12820512820512819</v>
       </c>
-      <c r="I2" s="72">
+      <c r="I2" s="71">
         <v>7.6923076923076927E-2</v>
       </c>
-      <c r="J2" s="72">
+      <c r="J2" s="71">
         <v>0.15384615384615385</v>
       </c>
-      <c r="K2" s="72">
+      <c r="K2" s="71">
         <v>0.10256410256410256</v>
       </c>
       <c r="M2" s="13" t="s">
@@ -17491,25 +17303,25 @@
       <c r="D3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="72">
+      <c r="E3" s="71">
         <v>0</v>
       </c>
-      <c r="F3" s="72">
+      <c r="F3" s="71">
         <v>6.7226890756302518E-2</v>
       </c>
-      <c r="G3" s="72">
+      <c r="G3" s="71">
         <v>0.36134453781512604</v>
       </c>
-      <c r="H3" s="72">
+      <c r="H3" s="71">
         <v>0.18487394957983194</v>
       </c>
-      <c r="I3" s="72">
+      <c r="I3" s="71">
         <v>0.10084033613445378</v>
       </c>
-      <c r="J3" s="72">
+      <c r="J3" s="71">
         <v>0.26050420168067229</v>
       </c>
-      <c r="K3" s="72">
+      <c r="K3" s="71">
         <v>2.5210084033613446E-2</v>
       </c>
       <c r="M3" s="13" t="s">
@@ -17554,25 +17366,25 @@
       <c r="D4" t="s">
         <v>143</v>
       </c>
-      <c r="E4" s="72">
+      <c r="E4" s="71">
         <v>0</v>
       </c>
-      <c r="F4" s="72">
+      <c r="F4" s="71">
         <v>0</v>
       </c>
-      <c r="G4" s="72">
+      <c r="G4" s="71">
         <v>0.51249999999999996</v>
       </c>
-      <c r="H4" s="72">
+      <c r="H4" s="71">
         <v>0.1875</v>
       </c>
-      <c r="I4" s="72">
+      <c r="I4" s="71">
         <v>0.1125</v>
       </c>
-      <c r="J4" s="72">
+      <c r="J4" s="71">
         <v>0.17499999999999999</v>
       </c>
-      <c r="K4" s="72">
+      <c r="K4" s="71">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="M4" s="13" t="s">
@@ -17617,25 +17429,25 @@
       <c r="D5" t="s">
         <v>319</v>
       </c>
-      <c r="E5" s="72">
+      <c r="E5" s="71">
         <v>0</v>
       </c>
-      <c r="F5" s="72">
+      <c r="F5" s="71">
         <v>0.1702127659574468</v>
       </c>
-      <c r="G5" s="72">
+      <c r="G5" s="71">
         <v>0.42553191489361702</v>
       </c>
-      <c r="H5" s="72">
+      <c r="H5" s="71">
         <v>8.5106382978723402E-2</v>
       </c>
-      <c r="I5" s="72">
+      <c r="I5" s="71">
         <v>4.2553191489361701E-2</v>
       </c>
-      <c r="J5" s="72">
+      <c r="J5" s="71">
         <v>0.25531914893617019</v>
       </c>
-      <c r="K5" s="72">
+      <c r="K5" s="71">
         <v>2.1276595744680851E-2</v>
       </c>
       <c r="M5" s="13" t="s">
@@ -17680,25 +17492,25 @@
       <c r="D6" t="s">
         <v>319</v>
       </c>
-      <c r="E6" s="72">
+      <c r="E6" s="71">
         <v>0</v>
       </c>
-      <c r="F6" s="72">
+      <c r="F6" s="71">
         <v>0.1702127659574468</v>
       </c>
-      <c r="G6" s="72">
+      <c r="G6" s="71">
         <v>0.42553191489361702</v>
       </c>
-      <c r="H6" s="72">
+      <c r="H6" s="71">
         <v>8.5106382978723402E-2</v>
       </c>
-      <c r="I6" s="72">
+      <c r="I6" s="71">
         <v>4.2553191489361701E-2</v>
       </c>
-      <c r="J6" s="72">
+      <c r="J6" s="71">
         <v>0.25531914893617019</v>
       </c>
-      <c r="K6" s="72">
+      <c r="K6" s="71">
         <v>2.1276595744680851E-2</v>
       </c>
       <c r="M6" s="13" t="s">
@@ -17743,25 +17555,25 @@
       <c r="D7" t="s">
         <v>319</v>
       </c>
-      <c r="E7" s="72">
+      <c r="E7" s="71">
         <v>0</v>
       </c>
-      <c r="F7" s="72">
+      <c r="F7" s="71">
         <v>0.1702127659574468</v>
       </c>
-      <c r="G7" s="72">
+      <c r="G7" s="71">
         <v>0.42553191489361702</v>
       </c>
-      <c r="H7" s="72">
+      <c r="H7" s="71">
         <v>8.5106382978723402E-2</v>
       </c>
-      <c r="I7" s="72">
+      <c r="I7" s="71">
         <v>4.2553191489361701E-2</v>
       </c>
-      <c r="J7" s="72">
+      <c r="J7" s="71">
         <v>0.25531914893617019</v>
       </c>
-      <c r="K7" s="72">
+      <c r="K7" s="71">
         <v>2.1276595744680851E-2</v>
       </c>
       <c r="M7" s="13" t="s">
@@ -17806,25 +17618,25 @@
       <c r="D8" t="s">
         <v>319</v>
       </c>
-      <c r="E8" s="72">
+      <c r="E8" s="71">
         <v>0</v>
       </c>
-      <c r="F8" s="72">
+      <c r="F8" s="71">
         <v>0.1702127659574468</v>
       </c>
-      <c r="G8" s="72">
+      <c r="G8" s="71">
         <v>0.42553191489361702</v>
       </c>
-      <c r="H8" s="72">
+      <c r="H8" s="71">
         <v>8.5106382978723402E-2</v>
       </c>
-      <c r="I8" s="72">
+      <c r="I8" s="71">
         <v>4.2553191489361701E-2</v>
       </c>
-      <c r="J8" s="72">
+      <c r="J8" s="71">
         <v>0.25531914893617019</v>
       </c>
-      <c r="K8" s="72">
+      <c r="K8" s="71">
         <v>2.1276595744680851E-2</v>
       </c>
       <c r="M8" s="13" t="s">
@@ -17869,25 +17681,25 @@
       <c r="D9" t="s">
         <v>321</v>
       </c>
-      <c r="E9" s="72">
+      <c r="E9" s="71">
         <v>0</v>
       </c>
-      <c r="F9" s="72">
+      <c r="F9" s="71">
         <v>0</v>
       </c>
-      <c r="G9" s="72">
+      <c r="G9" s="71">
         <v>0</v>
       </c>
-      <c r="H9" s="72">
+      <c r="H9" s="71">
         <v>0.40625</v>
       </c>
-      <c r="I9" s="72">
+      <c r="I9" s="71">
         <v>0.328125</v>
       </c>
-      <c r="J9" s="72">
+      <c r="J9" s="71">
         <v>0.265625</v>
       </c>
-      <c r="K9" s="72">
+      <c r="K9" s="71">
         <v>0</v>
       </c>
       <c r="M9" s="13" t="s">
@@ -18016,7 +17828,7 @@
       <c r="K11" s="40">
         <v>0</v>
       </c>
-      <c r="M11" s="73" t="s">
+      <c r="M11" s="72" t="s">
         <v>398</v>
       </c>
     </row>
@@ -18138,25 +17950,25 @@
       <c r="D15" t="s">
         <v>377</v>
       </c>
-      <c r="E15" s="72">
+      <c r="E15" s="71">
         <v>0</v>
       </c>
-      <c r="F15" s="72">
+      <c r="F15" s="71">
         <v>0</v>
       </c>
-      <c r="G15" s="72">
+      <c r="G15" s="71">
         <v>0</v>
       </c>
-      <c r="H15" s="72">
+      <c r="H15" s="71">
         <v>4.7619047619047616E-2</v>
       </c>
-      <c r="I15" s="72">
+      <c r="I15" s="71">
         <v>0</v>
       </c>
-      <c r="J15" s="72">
+      <c r="J15" s="71">
         <v>0.95238095238095233</v>
       </c>
-      <c r="K15" s="72">
+      <c r="K15" s="71">
         <v>0</v>
       </c>
     </row>
@@ -18208,25 +18020,25 @@
       <c r="D17" t="s">
         <v>322</v>
       </c>
-      <c r="E17" s="72">
+      <c r="E17" s="71">
         <v>0.12209302325581395</v>
       </c>
-      <c r="F17" s="72">
+      <c r="F17" s="71">
         <v>0</v>
       </c>
-      <c r="G17" s="72">
+      <c r="G17" s="71">
         <v>0</v>
       </c>
-      <c r="H17" s="72">
+      <c r="H17" s="71">
         <v>0.12790697674418605</v>
       </c>
-      <c r="I17" s="72">
+      <c r="I17" s="71">
         <v>0.27325581395348836</v>
       </c>
-      <c r="J17" s="72">
+      <c r="J17" s="71">
         <v>0.47093023255813954</v>
       </c>
-      <c r="K17" s="72">
+      <c r="K17" s="71">
         <v>5.8139534883720929E-3</v>
       </c>
     </row>
@@ -18312,8 +18124,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18362,14 +18174,14 @@
       <c r="D2" t="s">
         <v>349</v>
       </c>
-      <c r="E2" s="70">
+      <c r="E2" s="69">
         <f>34752*1000000/126832800000</f>
         <v>0.27399852404109976</v>
       </c>
       <c r="F2" t="s">
         <v>348</v>
       </c>
-      <c r="G2" s="68" t="s">
+      <c r="G2" s="67" t="s">
         <v>347</v>
       </c>
     </row>
@@ -18386,14 +18198,14 @@
       <c r="D3" t="s">
         <v>351</v>
       </c>
-      <c r="E3" s="70">
+      <c r="E3" s="69">
         <f>343*1000000/126832800000</f>
         <v>2.7043477712389856E-3</v>
       </c>
       <c r="F3" t="s">
         <v>350</v>
       </c>
-      <c r="G3" s="68" t="s">
+      <c r="G3" s="67" t="s">
         <v>347</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updating Job Multipliers for SMR Hydrogen
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrojasa\OneDrive - RAND Corporation\Documents\GitHub\SJV-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05370C29-50C6-4343-B00D-152E67594486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B7718E-72A0-4571-9780-BE0D086D6EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7860" yWindow="-16297" windowWidth="28995" windowHeight="15794" tabRatio="622" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="8625" yWindow="1335" windowWidth="17400" windowHeight="10815" tabRatio="622" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -1883,25 +1883,25 @@
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.08203125" customWidth="1"/>
-    <col min="4" max="4" width="27.58203125" customWidth="1"/>
+    <col min="1" max="1" width="30.375" customWidth="1"/>
+    <col min="2" max="2" width="17.125" customWidth="1"/>
+    <col min="4" max="4" width="27.625" customWidth="1"/>
     <col min="5" max="5" width="0" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="12.58203125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="0" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="13" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="0" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="11" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.83203125" customWidth="1"/>
-    <col min="12" max="12" width="38.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.875" customWidth="1"/>
+    <col min="12" max="12" width="38.375" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="38.25" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -2102,7 +2102,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2250,7 +2250,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
@@ -2303,7 +2303,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -2517,7 +2517,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>306</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>38</v>
       </c>
@@ -2704,7 +2704,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2742,10 +2742,10 @@
       </c>
       <c r="N17" s="61"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K19" s="62"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L20" s="63"/>
     </row>
   </sheetData>
@@ -2768,15 +2768,15 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2802,7 +2802,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2829,7 +2829,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -2883,7 +2883,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -2901,7 +2901,7 @@
       </c>
       <c r="F5" s="68"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -2928,7 +2928,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -2955,7 +2955,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -2982,7 +2982,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -3009,7 +3009,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="55" t="s">
         <v>19</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
@@ -3057,7 +3057,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>46</v>
       </c>
@@ -3081,7 +3081,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -3135,7 +3135,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -3180,7 +3180,7 @@
       </c>
       <c r="F16" s="68"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -3261,7 +3261,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -3288,7 +3288,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="55" t="s">
         <v>19</v>
       </c>
@@ -3312,7 +3312,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>38</v>
       </c>
@@ -3336,7 +3336,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>46</v>
       </c>
@@ -3396,21 +3396,21 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.08203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="68.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="68.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3442,7 +3442,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>3.4599999999999999E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
         <v>11</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -3506,7 +3506,7 @@
         <v>2.3599999999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>2.8199999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>4.0899999999999999E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>3.3399999999999999E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -3626,7 +3626,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -3646,7 +3646,7 @@
         <v>5.62E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -3666,7 +3666,7 @@
         <v>5.62E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -3699,15 +3699,15 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5" customWidth="1"/>
     <col min="4" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3724,7 +3724,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -3741,7 +3741,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -3763,26 +3763,26 @@
       <selection pane="topRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.75" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="15.25" customWidth="1"/>
-    <col min="6" max="6" width="11.08203125" customWidth="1"/>
+    <col min="6" max="6" width="11.125" customWidth="1"/>
     <col min="7" max="7" width="17.75" customWidth="1"/>
     <col min="8" max="8" width="10.5" customWidth="1"/>
-    <col min="9" max="9" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="14.375" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="43.5" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="19.08203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.375" customWidth="1"/>
+    <col min="13" max="13" width="19.125" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="10.5" customWidth="1"/>
     <col min="16" max="16" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3895,7 +3895,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>1216.528453322951</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -4030,7 +4030,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>2101.97739666605</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>1171.0983188067505</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -4309,7 +4309,7 @@
         <v>2214.52431017765</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -4417,7 +4417,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -4514,7 +4514,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -4657,7 +4657,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>38</v>
       </c>
@@ -4693,7 +4693,7 @@
       <c r="L11" s="43"/>
       <c r="O11" s="36"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -4789,7 +4789,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -4828,7 +4828,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -4939,7 +4939,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -4976,7 +4976,7 @@
       </c>
       <c r="O18" s="53"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -5013,7 +5013,7 @@
       </c>
       <c r="O19" s="53"/>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L23">
         <v>1000</v>
       </c>
@@ -5047,16 +5047,16 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.58203125" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="14.625" customWidth="1"/>
+    <col min="2" max="2" width="30.375" customWidth="1"/>
+    <col min="3" max="3" width="8.375" customWidth="1"/>
+    <col min="4" max="4" width="23.875" customWidth="1"/>
     <col min="5" max="25" width="8.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -5210,7 +5210,7 @@
         <v>1216.528453322951</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>2101.97739666605</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>34</v>
       </c>
@@ -5364,7 +5364,7 @@
         <v>1171.0983188067505</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>35</v>
       </c>
@@ -5441,7 +5441,7 @@
         <v>2214.52431017765</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>36</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>37</v>
       </c>
@@ -5595,7 +5595,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>43</v>
       </c>
@@ -5672,7 +5672,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -5749,7 +5749,7 @@
         <v>5162.1082438314425</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E12" s="71">
         <f>E2/8760</f>
         <v>0.26187622965636759</v>
@@ -5835,43 +5835,43 @@
         <v>0.13887311110992592</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E13" s="71">
         <f t="shared" ref="E13:E19" si="1">E3/8760</f>
         <v>0.28570875457778422</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E14" s="71">
         <f t="shared" si="1"/>
         <v>0.13368702269483454</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E15" s="71">
         <f t="shared" si="1"/>
         <v>0.19073300751397604</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="E16" s="71">
         <f t="shared" si="1"/>
         <v>0.68893673866789151</v>
       </c>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E17" s="71">
         <f t="shared" si="1"/>
         <v>0.68893673866789151</v>
       </c>
     </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E18" s="71">
         <f t="shared" si="1"/>
         <v>0.68893673866789151</v>
       </c>
     </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E19" s="71">
         <f t="shared" si="1"/>
         <v>0.68893673866789151</v>
@@ -5890,15 +5890,15 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.08203125" customWidth="1"/>
-    <col min="2" max="2" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="21.58203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.125" customWidth="1"/>
+    <col min="2" max="2" width="31.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>288</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>289</v>
       </c>
@@ -6064,7 +6064,7 @@
         <v>26600</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>289</v>
       </c>
@@ -6147,7 +6147,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>290</v>
       </c>
@@ -6230,7 +6230,7 @@
         <v>14800</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>290</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -6396,7 +6396,7 @@
         <v>3.4782608695652177</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>138</v>
       </c>
@@ -6479,7 +6479,7 @@
         <v>21.118012422360248</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>138</v>
       </c>
@@ -6562,7 +6562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>138</v>
       </c>
@@ -6645,7 +6645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>289</v>
       </c>
@@ -6728,7 +6728,7 @@
         <v>4.9689440993788822E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>56</v>
       </c>
@@ -6811,7 +6811,7 @@
         <v>310000</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>138</v>
       </c>
@@ -6894,7 +6894,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>138</v>
       </c>
@@ -6977,7 +6977,7 @@
         <v>83854.869455332082</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -7060,7 +7060,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -7143,7 +7143,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>138</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>39760971.535051085</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>138</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>2572768.7463856577</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>138</v>
       </c>
@@ -7392,7 +7392,7 @@
         <v>5769.2307692307695</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>138</v>
       </c>
@@ -7475,7 +7475,7 @@
         <v>230.76923076923077</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>138</v>
       </c>
@@ -7571,13 +7571,13 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.08203125" customWidth="1"/>
+    <col min="2" max="2" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -7648,7 +7648,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -7719,7 +7719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -7861,7 +7861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -7932,7 +7932,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
@@ -8016,17 +8016,17 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.75" customWidth="1"/>
     <col min="2" max="2" width="20.75" customWidth="1"/>
-    <col min="3" max="3" width="20.58203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.375" customWidth="1"/>
+    <col min="6" max="6" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="32" t="s">
         <v>155</v>
       </c>
@@ -8049,7 +8049,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>11</v>
       </c>
@@ -8070,7 +8070,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>22</v>
       </c>
@@ -8091,7 +8091,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>34</v>
       </c>
@@ -8112,7 +8112,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>35</v>
       </c>
@@ -8133,7 +8133,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>138</v>
       </c>
@@ -8154,7 +8154,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>138</v>
       </c>
@@ -8175,7 +8175,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>38</v>
       </c>
@@ -8196,7 +8196,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>56</v>
       </c>
@@ -8238,7 +8238,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>138</v>
       </c>
@@ -8259,7 +8259,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>138</v>
       </c>
@@ -8280,7 +8280,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>38</v>
       </c>
@@ -8301,7 +8301,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>138</v>
       </c>
@@ -8322,7 +8322,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>138</v>
       </c>
@@ -8343,7 +8343,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>158</v>
       </c>
@@ -8364,7 +8364,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
         <v>158</v>
       </c>
@@ -8385,7 +8385,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="14" t="s">
         <v>138</v>
       </c>
@@ -8406,7 +8406,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="14" t="s">
         <v>138</v>
       </c>
@@ -8427,7 +8427,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="50" t="s">
         <v>157</v>
       </c>
@@ -8435,7 +8435,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="51" t="s">
         <v>12</v>
       </c>
@@ -8443,7 +8443,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="51" t="s">
         <v>19</v>
       </c>
@@ -8451,7 +8451,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="51" t="s">
         <v>19</v>
       </c>
@@ -8459,7 +8459,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="51" t="s">
         <v>38</v>
       </c>
@@ -8467,7 +8467,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="51" t="s">
         <v>38</v>
       </c>
@@ -8475,7 +8475,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="51" t="s">
         <v>38</v>
       </c>
@@ -8483,7 +8483,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="51" t="s">
         <v>68</v>
       </c>
@@ -8505,17 +8505,17 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" customWidth="1"/>
+    <col min="1" max="1" width="23.375" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="16.58203125" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
     <col min="7" max="7" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -8544,7 +8544,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -8555,7 +8555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -8566,7 +8566,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -8583,7 +8583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -8591,7 +8591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>166</v>
       </c>
@@ -8612,17 +8612,17 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.875" customWidth="1"/>
+    <col min="2" max="2" width="30.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.58203125" customWidth="1"/>
+    <col min="4" max="4" width="40.875" customWidth="1"/>
+    <col min="5" max="5" width="30.625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -8651,7 +8651,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>56</v>
       </c>
@@ -8678,7 +8678,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>152</v>
       </c>
@@ -8705,7 +8705,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
@@ -8732,7 +8732,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
@@ -8759,7 +8759,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>22</v>
       </c>
@@ -8786,7 +8786,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
@@ -8809,7 +8809,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>36</v>
       </c>
@@ -8832,7 +8832,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>177</v>
       </c>
@@ -8857,7 +8857,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>177</v>
       </c>
@@ -8882,7 +8882,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>181</v>
       </c>
@@ -8907,7 +8907,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>181</v>
       </c>
@@ -8926,7 +8926,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -8941,7 +8941,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -8956,7 +8956,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>186</v>
       </c>
@@ -8983,7 +8983,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" s="20" t="s">
         <v>169</v>
       </c>
@@ -9006,7 +9006,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
         <v>174</v>
       </c>
@@ -9029,7 +9029,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
         <v>177</v>
       </c>
@@ -9052,7 +9052,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="63" x14ac:dyDescent="0.25">
       <c r="A19" s="20" t="s">
         <v>181</v>
       </c>
@@ -9066,7 +9066,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>182</v>
       </c>
@@ -9080,7 +9080,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>37</v>
       </c>
@@ -9094,7 +9094,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>36</v>
       </c>
@@ -9108,12 +9108,12 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="26" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="32" t="s">
         <v>0</v>
       </c>
@@ -9130,7 +9130,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="14" t="s">
         <v>56</v>
       </c>
@@ -9139,7 +9139,7 @@
       </c>
       <c r="C32" s="14"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="14" t="s">
         <v>152</v>
       </c>
@@ -9148,7 +9148,7 @@
       </c>
       <c r="C33" s="14"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="14" t="s">
         <v>48</v>
       </c>
@@ -9157,7 +9157,7 @@
       </c>
       <c r="C34" s="14"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="14" t="s">
         <v>11</v>
       </c>
@@ -9168,7 +9168,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="14" t="s">
         <v>22</v>
       </c>
@@ -9177,7 +9177,7 @@
       </c>
       <c r="C36" s="14"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="14" t="s">
         <v>207</v>
       </c>
@@ -9186,7 +9186,7 @@
       </c>
       <c r="C37" s="14"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="14" t="s">
         <v>35</v>
       </c>
@@ -9195,7 +9195,7 @@
       </c>
       <c r="C38" s="14"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="27" t="s">
         <v>37</v>
       </c>
@@ -9209,7 +9209,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="27" t="s">
         <v>36</v>
       </c>
@@ -9223,7 +9223,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="14" t="s">
         <v>177</v>
       </c>
@@ -9240,7 +9240,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="14" t="s">
         <v>181</v>
       </c>
@@ -9257,12 +9257,12 @@
         <v>211</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
         <v>1</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>19</v>
       </c>
@@ -9284,7 +9284,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="30" t="s">
         <v>19</v>
       </c>
@@ -9301,7 +9301,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="30" t="s">
         <v>19</v>
       </c>
@@ -9318,7 +9318,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="30" t="s">
         <v>19</v>
       </c>
@@ -9338,7 +9338,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="27" t="s">
         <v>19</v>
       </c>
@@ -9355,7 +9355,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="27" t="s">
         <v>56</v>
       </c>
@@ -9372,7 +9372,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="14" t="s">
         <v>56</v>
       </c>
@@ -9383,7 +9383,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="27" t="s">
         <v>56</v>
       </c>
@@ -9400,7 +9400,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="27" t="s">
         <v>12</v>
       </c>
@@ -9417,7 +9417,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
         <v>12</v>
       </c>
@@ -9428,12 +9428,12 @@
         <v>224</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="26" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="27" t="s">
         <v>231</v>
       </c>
@@ -9444,7 +9444,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="29" t="s">
         <v>233</v>
       </c>
@@ -9452,7 +9452,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="27" t="s">
         <v>234</v>
       </c>
@@ -9460,12 +9460,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="26" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="27" t="s">
         <v>236</v>
       </c>
@@ -9473,7 +9473,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="27" t="s">
         <v>237</v>
       </c>
@@ -9494,19 +9494,19 @@
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.25" customWidth="1"/>
     <col min="2" max="2" width="12.75" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
     <col min="6" max="6" width="11.25" customWidth="1"/>
     <col min="7" max="7" width="8.25" customWidth="1"/>
-    <col min="8" max="9" width="24.08203125" customWidth="1"/>
+    <col min="8" max="9" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9541,7 +9541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -9575,7 +9575,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -9612,7 +9612,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -9641,7 +9641,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>11</v>
       </c>
@@ -9670,7 +9670,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -9699,7 +9699,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -9728,7 +9728,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>11</v>
       </c>
@@ -9762,7 +9762,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>11</v>
       </c>
@@ -9799,7 +9799,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>22</v>
       </c>
@@ -9828,7 +9828,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>11</v>
       </c>
@@ -9860,7 +9860,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
@@ -9894,7 +9894,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
@@ -9923,7 +9923,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>11</v>
       </c>
@@ -9957,7 +9957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -9994,7 +9994,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>22</v>
       </c>
@@ -10024,7 +10024,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>11</v>
       </c>
@@ -10056,7 +10056,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>11</v>
       </c>
@@ -10089,7 +10089,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>22</v>
       </c>
@@ -10132,13 +10132,13 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.58203125" customWidth="1"/>
-    <col min="2" max="5" width="15.58203125" customWidth="1"/>
+    <col min="1" max="1" width="25.625" customWidth="1"/>
+    <col min="2" max="5" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>239</v>
       </c>
@@ -10158,7 +10158,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>240</v>
       </c>
@@ -10169,7 +10169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -10177,7 +10177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>56</v>
       </c>
@@ -10185,7 +10185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -10199,7 +10199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -10213,7 +10213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>241</v>
       </c>
@@ -10227,7 +10227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>242</v>
       </c>
@@ -10238,7 +10238,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>243</v>
       </c>
@@ -10249,7 +10249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>244</v>
       </c>
@@ -10260,7 +10260,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -10268,7 +10268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -10290,18 +10290,18 @@
       <selection activeCell="F1" sqref="F1:F61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="5" width="26" customWidth="1"/>
-    <col min="6" max="6" width="24.08203125" customWidth="1"/>
+    <col min="6" max="6" width="24.125" customWidth="1"/>
     <col min="7" max="7" width="31.5" customWidth="1"/>
-    <col min="8" max="8" width="36.83203125" customWidth="1"/>
+    <col min="8" max="8" width="36.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10327,7 +10327,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -10347,7 +10347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>11</v>
       </c>
@@ -10373,7 +10373,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -10393,7 +10393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -10413,7 +10413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -10433,7 +10433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -10453,7 +10453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="55" t="s">
         <v>37</v>
       </c>
@@ -10473,7 +10473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>42</v>
       </c>
@@ -10497,7 +10497,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>43</v>
       </c>
@@ -10521,7 +10521,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="55" t="s">
         <v>40</v>
       </c>
@@ -10545,7 +10545,7 @@
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="55" t="s">
         <v>37</v>
       </c>
@@ -10574,7 +10574,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
         <v>36</v>
       </c>
@@ -10603,7 +10603,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>42</v>
       </c>
@@ -10627,7 +10627,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>43</v>
       </c>
@@ -10650,7 +10650,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -10671,7 +10671,7 @@
       </c>
       <c r="H16" s="3"/>
     </row>
-    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -10694,7 +10694,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -10717,7 +10717,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
@@ -10740,7 +10740,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -10766,7 +10766,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -10792,7 +10792,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -10812,7 +10812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="55" t="s">
         <v>11</v>
       </c>
@@ -10838,7 +10838,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -10858,7 +10858,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -10878,7 +10878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -10898,7 +10898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -10918,7 +10918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -10938,7 +10938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13" t="s">
         <v>42</v>
       </c>
@@ -10962,7 +10962,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>43</v>
       </c>
@@ -10986,7 +10986,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="55" t="s">
         <v>40</v>
       </c>
@@ -11010,7 +11010,7 @@
       </c>
       <c r="H31" s="3"/>
     </row>
-    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
         <v>37</v>
       </c>
@@ -11036,7 +11036,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>42</v>
       </c>
@@ -11060,7 +11060,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>43</v>
       </c>
@@ -11083,7 +11083,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="55" t="s">
         <v>36</v>
       </c>
@@ -11109,7 +11109,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>42</v>
       </c>
@@ -11133,7 +11133,7 @@
       </c>
       <c r="H36" s="3"/>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>43</v>
       </c>
@@ -11156,7 +11156,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>45</v>
       </c>
@@ -11179,7 +11179,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -11202,7 +11202,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -11225,7 +11225,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -11248,7 +11248,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>11</v>
       </c>
@@ -11268,7 +11268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="55" t="s">
         <v>11</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -11314,7 +11314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>34</v>
       </c>
@@ -11334,7 +11334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>35</v>
       </c>
@@ -11354,7 +11354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>36</v>
       </c>
@@ -11374,7 +11374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -11394,7 +11394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="13" t="s">
         <v>42</v>
       </c>
@@ -11418,7 +11418,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="13" t="s">
         <v>43</v>
       </c>
@@ -11442,7 +11442,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="55" t="s">
         <v>40</v>
       </c>
@@ -11466,7 +11466,7 @@
       </c>
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="55" t="s">
         <v>37</v>
       </c>
@@ -11492,7 +11492,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="13" t="s">
         <v>42</v>
       </c>
@@ -11516,7 +11516,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13" t="s">
         <v>43</v>
       </c>
@@ -11539,7 +11539,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="55" t="s">
         <v>36</v>
       </c>
@@ -11565,7 +11565,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>42</v>
       </c>
@@ -11589,7 +11589,7 @@
       </c>
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>43</v>
       </c>
@@ -11612,7 +11612,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>45</v>
       </c>
@@ -11635,7 +11635,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>48</v>
       </c>
@@ -11658,7 +11658,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -11678,7 +11678,7 @@
         <v>7.7</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>36</v>
       </c>
@@ -11741,17 +11741,17 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="173.08203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="173.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -11771,7 +11771,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -11788,7 +11788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -11805,7 +11805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -11825,7 +11825,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -11842,7 +11842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>46</v>
       </c>
@@ -11872,17 +11872,17 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.58203125" customWidth="1"/>
-    <col min="2" max="2" width="19.08203125" customWidth="1"/>
+    <col min="1" max="1" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="19.125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
     <col min="5" max="5" width="25.75" customWidth="1"/>
-    <col min="6" max="6" width="19.08203125" customWidth="1"/>
+    <col min="6" max="6" width="19.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -11965,7 +11965,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -12048,7 +12048,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -12131,7 +12131,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -12214,7 +12214,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -12297,7 +12297,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -12380,7 +12380,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -12463,7 +12463,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -12546,7 +12546,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -12650,7 +12650,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -12754,7 +12754,7 @@
         <v>80.360000000000014</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -12837,7 +12837,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -12941,7 +12941,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -13045,7 +13045,7 @@
         <v>117.7</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
@@ -13128,7 +13128,7 @@
         <v>80.36</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>46</v>
       </c>
@@ -13232,7 +13232,7 @@
         <v>80.36</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>46</v>
       </c>
@@ -13350,18 +13350,18 @@
       <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.83203125" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.875" customWidth="1"/>
+    <col min="2" max="2" width="24.375" customWidth="1"/>
     <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
+    <col min="5" max="5" width="22.875" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
-    <col min="7" max="8" width="24.08203125" customWidth="1"/>
+    <col min="7" max="8" width="24.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13399,7 +13399,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -13416,7 +13416,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -13446,7 +13446,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -13464,7 +13464,7 @@
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -13482,7 +13482,7 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -13500,7 +13500,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>36</v>
       </c>
@@ -13518,7 +13518,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>37</v>
       </c>
@@ -13536,7 +13536,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>43</v>
       </c>
@@ -13554,7 +13554,7 @@
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -13572,7 +13572,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>40</v>
       </c>
@@ -13602,7 +13602,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -13632,7 +13632,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -13663,7 +13663,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -13690,7 +13690,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -13717,7 +13717,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>43</v>
       </c>
@@ -13734,7 +13734,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -13751,7 +13751,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -13768,7 +13768,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>48</v>
       </c>
@@ -13785,7 +13785,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -13802,7 +13802,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>36</v>
       </c>
@@ -13819,7 +13819,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>11</v>
       </c>
@@ -13839,7 +13839,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
@@ -13876,7 +13876,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -13897,7 +13897,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>34</v>
       </c>
@@ -13915,7 +13915,7 @@
       </c>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>35</v>
       </c>
@@ -13933,7 +13933,7 @@
       </c>
       <c r="F26" s="8"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
         <v>36</v>
       </c>
@@ -13951,7 +13951,7 @@
       </c>
       <c r="F27" s="8"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
         <v>37</v>
       </c>
@@ -13969,7 +13969,7 @@
       </c>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -13987,7 +13987,7 @@
       </c>
       <c r="F29" s="8"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -14005,7 +14005,7 @@
       </c>
       <c r="F30" s="8"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>40</v>
       </c>
@@ -14042,7 +14042,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -14079,7 +14079,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -14110,7 +14110,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -14128,7 +14128,7 @@
       </c>
       <c r="F34" s="8"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>42</v>
       </c>
@@ -14146,7 +14146,7 @@
       </c>
       <c r="F35" s="8"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>43</v>
       </c>
@@ -14166,7 +14166,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>42</v>
       </c>
@@ -14186,7 +14186,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
@@ -14206,7 +14206,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>48</v>
       </c>
@@ -14226,7 +14226,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -14243,7 +14243,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -14260,35 +14260,35 @@
         <v>81</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
     </row>
@@ -14303,28 +14303,28 @@
   <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L16" sqref="K16:L16"/>
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" customWidth="1"/>
-    <col min="4" max="4" width="34.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.375" customWidth="1"/>
+    <col min="3" max="3" width="12.875" customWidth="1"/>
+    <col min="4" max="4" width="34.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.375" customWidth="1"/>
     <col min="7" max="7" width="10.25" style="13" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
     <col min="9" max="9" width="11.75" customWidth="1"/>
-    <col min="10" max="10" width="10.9140625" customWidth="1"/>
+    <col min="10" max="10" width="10.875" customWidth="1"/>
     <col min="11" max="12" width="11.75" customWidth="1"/>
     <col min="13" max="13" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.58203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="61.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="61.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -14371,7 +14371,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -14416,7 +14416,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -14461,7 +14461,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -14506,7 +14506,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -14551,7 +14551,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -14596,7 +14596,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -14641,7 +14641,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -14686,7 +14686,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>34</v>
       </c>
@@ -14731,7 +14731,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -14776,7 +14776,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -14808,7 +14808,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -14840,7 +14840,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -14872,7 +14872,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -14917,7 +14917,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -14962,7 +14962,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -15007,7 +15007,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -15052,7 +15052,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -15097,7 +15097,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -15142,7 +15142,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>43</v>
       </c>
@@ -15187,7 +15187,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -15232,7 +15232,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>43</v>
       </c>
@@ -15277,7 +15277,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -15322,7 +15322,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>42</v>
       </c>
@@ -15367,7 +15367,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -15412,7 +15412,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -15440,12 +15440,12 @@
       <c r="K26" s="73" t="s">
         <v>335</v>
       </c>
-      <c r="L26">
-        <v>1.4E-2</v>
+      <c r="L26" s="48">
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="M26" s="8">
         <f>L26+M2/123</f>
-        <v>1.443089430894309E-2</v>
+        <v>7.6430894308943093E-2</v>
       </c>
       <c r="N26" t="s">
         <v>327</v>
@@ -15454,7 +15454,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>11</v>
       </c>
@@ -15482,12 +15482,12 @@
       <c r="K27" s="73" t="s">
         <v>335</v>
       </c>
-      <c r="L27">
-        <v>0.249</v>
+      <c r="L27" s="48">
+        <v>1.9E-2</v>
       </c>
       <c r="M27" s="8">
         <f>L27+M3/123</f>
-        <v>0.24915447154471546</v>
+        <v>1.9154471544715446E-2</v>
       </c>
       <c r="N27" t="s">
         <v>327</v>
@@ -15496,7 +15496,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -15524,12 +15524,12 @@
       <c r="K28" s="73" t="s">
         <v>335</v>
       </c>
-      <c r="L28">
-        <v>0.187</v>
+      <c r="L28" s="48">
+        <v>1.4E-2</v>
       </c>
       <c r="M28" s="8">
         <f>L28+M4/123</f>
-        <v>0.18717073170731707</v>
+        <v>1.4170731707317074E-2</v>
       </c>
       <c r="N28" t="s">
         <v>327</v>
@@ -15538,7 +15538,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>40</v>
       </c>
@@ -15572,12 +15572,12 @@
       <c r="K29">
         <v>0</v>
       </c>
-      <c r="L29">
-        <v>1.4E-2</v>
+      <c r="L29" s="48">
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="M29">
         <f>L29</f>
-        <v>1.4E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="N29" t="s">
         <v>327</v>
@@ -15586,7 +15586,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -15620,12 +15620,12 @@
       <c r="K30">
         <v>0</v>
       </c>
-      <c r="L30">
-        <v>0.249</v>
+      <c r="L30" s="48">
+        <v>1.9E-2</v>
       </c>
       <c r="M30">
         <f t="shared" ref="M30:M31" si="2">L30</f>
-        <v>0.249</v>
+        <v>1.9E-2</v>
       </c>
       <c r="N30" t="s">
         <v>327</v>
@@ -15634,7 +15634,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>40</v>
       </c>
@@ -15668,12 +15668,12 @@
       <c r="K31">
         <v>0</v>
       </c>
-      <c r="L31">
-        <v>0.187</v>
+      <c r="L31" s="48">
+        <v>1.4E-2</v>
       </c>
       <c r="M31">
         <f t="shared" si="2"/>
-        <v>0.187</v>
+        <v>1.4E-2</v>
       </c>
       <c r="N31" t="s">
         <v>327</v>
@@ -15682,7 +15682,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -15730,7 +15730,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -15778,7 +15778,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -15826,7 +15826,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -15874,7 +15874,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -15922,7 +15922,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -15970,7 +15970,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>43</v>
       </c>
@@ -16004,12 +16004,12 @@
       <c r="K38">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="L38">
-        <v>1.4E-2</v>
+      <c r="L38" s="48">
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="M38" s="55">
         <f t="shared" ref="M38:M43" si="4">L38</f>
-        <v>1.4E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="N38" t="s">
         <v>327</v>
@@ -16018,7 +16018,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -16052,12 +16052,12 @@
       <c r="K39">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="L39">
-        <v>0.249</v>
+      <c r="L39" s="48">
+        <v>1.9E-2</v>
       </c>
       <c r="M39" s="55">
         <f t="shared" si="4"/>
-        <v>0.249</v>
+        <v>1.9E-2</v>
       </c>
       <c r="N39" t="s">
         <v>327</v>
@@ -16066,7 +16066,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
@@ -16100,12 +16100,12 @@
       <c r="K40">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="L40">
-        <v>0.187</v>
+      <c r="L40" s="48">
+        <v>1.4E-2</v>
       </c>
       <c r="M40" s="55">
         <f t="shared" si="4"/>
-        <v>0.187</v>
+        <v>1.4E-2</v>
       </c>
       <c r="N40" t="s">
         <v>327</v>
@@ -16114,7 +16114,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -16148,12 +16148,12 @@
       <c r="K41">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="L41">
-        <v>1.4E-2</v>
+      <c r="L41" s="48">
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="M41" s="55">
         <f t="shared" si="4"/>
-        <v>1.4E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="N41" t="s">
         <v>327</v>
@@ -16162,7 +16162,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -16196,12 +16196,12 @@
       <c r="K42">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="L42">
-        <v>0.249</v>
+      <c r="L42" s="48">
+        <v>1.9E-2</v>
       </c>
       <c r="M42" s="55">
         <f t="shared" si="4"/>
-        <v>0.249</v>
+        <v>1.9E-2</v>
       </c>
       <c r="N42" t="s">
         <v>327</v>
@@ -16210,7 +16210,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -16244,12 +16244,12 @@
       <c r="K43">
         <v>2.8358342136926399E-2</v>
       </c>
-      <c r="L43">
-        <v>0.187</v>
+      <c r="L43" s="48">
+        <v>1.4E-2</v>
       </c>
       <c r="M43" s="55">
         <f t="shared" si="4"/>
-        <v>0.187</v>
+        <v>1.4E-2</v>
       </c>
       <c r="N43" t="s">
         <v>327</v>
@@ -16258,7 +16258,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -16306,7 +16306,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -16351,7 +16351,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -16396,7 +16396,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>42</v>
       </c>
@@ -16444,7 +16444,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>42</v>
       </c>
@@ -16489,7 +16489,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>42</v>
       </c>
@@ -16534,7 +16534,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -16582,7 +16582,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -16630,7 +16630,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -16678,7 +16678,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -16726,7 +16726,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -16774,7 +16774,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -16822,7 +16822,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>36</v>
       </c>
@@ -16870,7 +16870,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>36</v>
       </c>
@@ -16918,7 +16918,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -16983,31 +16983,31 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.58203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="49.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14.75" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.25" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="56.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.25" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.08203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="14.75" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="18.25" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="5.5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17051,7 +17051,7 @@
       <c r="T1" s="13"/>
       <c r="U1" s="13"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -17095,7 +17095,7 @@
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -17139,7 +17139,7 @@
       <c r="T3" s="13"/>
       <c r="U3" s="13"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -17183,7 +17183,7 @@
       <c r="T4" s="13"/>
       <c r="U4" s="13"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>36</v>
       </c>
@@ -17227,7 +17227,7 @@
       <c r="T5" s="13"/>
       <c r="U5" s="13"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>37</v>
       </c>
@@ -17271,7 +17271,7 @@
       <c r="T6" s="13"/>
       <c r="U6" s="13"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -17315,7 +17315,7 @@
       <c r="T7" s="13"/>
       <c r="U7" s="13"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>42</v>
       </c>
@@ -17359,7 +17359,7 @@
       <c r="T8" s="13"/>
       <c r="U8" s="13"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -17403,7 +17403,7 @@
       <c r="T9" s="13"/>
       <c r="U9" s="13"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -17447,7 +17447,7 @@
       <c r="T10" s="13"/>
       <c r="U10" s="13"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -17483,7 +17483,7 @@
       </c>
       <c r="M11" s="72"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -17518,7 +17518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -17553,7 +17553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -17588,7 +17588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>43</v>
       </c>
@@ -17623,7 +17623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -17658,7 +17658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -17693,7 +17693,7 @@
         <v>5.8139534883720929E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -17728,7 +17728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -17779,7 +17779,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.25" bestFit="1" customWidth="1"/>
@@ -17789,7 +17789,7 @@
     <col min="6" max="6" width="34.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="55" t="s">
         <v>1</v>
       </c>
@@ -17812,7 +17812,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="55" t="s">
         <v>19</v>
       </c>
@@ -17836,7 +17836,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="55" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
Re-update to multipliers for indirect/induced jobs (including Toby's update)
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmpark\PATH\Git\SJV\SJV-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B7718E-72A0-4571-9780-BE0D086D6EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{345803EE-97B0-4B57-9975-032704E24264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8625" yWindow="1335" windowWidth="17400" windowHeight="10815" tabRatio="622" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="3435" yWindow="2355" windowWidth="17400" windowHeight="10815" tabRatio="622" activeTab="6" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -14302,8 +14302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16BE7FC-A8FD-4D95-933D-26AA617CB019}">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M53" sqref="M53"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15483,11 +15483,11 @@
         <v>335</v>
       </c>
       <c r="L27" s="48">
-        <v>1.9E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="M27" s="8">
         <f>L27+M3/123</f>
-        <v>1.9154471544715446E-2</v>
+        <v>5.1154471544715446E-2</v>
       </c>
       <c r="N27" t="s">
         <v>327</v>
@@ -15525,11 +15525,11 @@
         <v>335</v>
       </c>
       <c r="L28" s="48">
-        <v>1.4E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="M28" s="8">
         <f>L28+M4/123</f>
-        <v>1.4170731707317074E-2</v>
+        <v>3.7170731707317071E-2</v>
       </c>
       <c r="N28" t="s">
         <v>327</v>
@@ -15621,11 +15621,11 @@
         <v>0</v>
       </c>
       <c r="L30" s="48">
-        <v>1.9E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="M30">
         <f t="shared" ref="M30:M31" si="2">L30</f>
-        <v>1.9E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="N30" t="s">
         <v>327</v>
@@ -15669,11 +15669,11 @@
         <v>0</v>
       </c>
       <c r="L31" s="48">
-        <v>1.4E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="M31">
         <f t="shared" si="2"/>
-        <v>1.4E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="N31" t="s">
         <v>327</v>
@@ -16053,11 +16053,11 @@
         <v>2.8358342136926399E-2</v>
       </c>
       <c r="L39" s="48">
-        <v>1.9E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="M39" s="55">
         <f t="shared" si="4"/>
-        <v>1.9E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="N39" t="s">
         <v>327</v>
@@ -16101,11 +16101,11 @@
         <v>2.8358342136926399E-2</v>
       </c>
       <c r="L40" s="48">
-        <v>1.4E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="M40" s="55">
         <f t="shared" si="4"/>
-        <v>1.4E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="N40" t="s">
         <v>327</v>
@@ -16197,11 +16197,11 @@
         <v>2.8358342136926399E-2</v>
       </c>
       <c r="L42" s="48">
-        <v>1.9E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="M42" s="55">
         <f t="shared" si="4"/>
-        <v>1.9E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="N42" t="s">
         <v>327</v>
@@ -16245,11 +16245,11 @@
         <v>2.8358342136926399E-2</v>
       </c>
       <c r="L43" s="48">
-        <v>1.4E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="M43" s="55">
         <f t="shared" si="4"/>
-        <v>1.4E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="N43" t="s">
         <v>327</v>
@@ -16967,6 +16967,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:O58" xr:uid="{B16BE7FC-A8FD-4D95-933D-26AA617CB019}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
MIT living wages data
</commit_message>
<xml_diff>
--- a/SJV Variable Architecture.xlsx
+++ b/SJV Variable Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://randus-my.sharepoint.com/personal/jrojasa_rand_org/Documents/Documents/GitHub/SJV-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{345803EE-97B0-4B57-9975-032704E24264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A53D210E-78E5-4DB2-9736-61596282E4D2}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:1_{345803EE-97B0-4B57-9975-032704E24264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65E7BD45-290A-41A6-91F6-DA289FBB551E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="622" activeTab="5" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
+    <workbookView xWindow="-7860" yWindow="-16297" windowWidth="28995" windowHeight="15794" tabRatio="622" activeTab="7" xr2:uid="{4DD06761-560B-AB45-B502-623564D836E8}"/>
   </bookViews>
   <sheets>
     <sheet name="F2C Conversion" sheetId="22" r:id="rId1"/>
@@ -20,29 +20,30 @@
     <sheet name="C2U CI" sheetId="10" r:id="rId5"/>
     <sheet name="F2C Water" sheetId="13" r:id="rId6"/>
     <sheet name="F2C Jobs" sheetId="23" r:id="rId7"/>
-    <sheet name="Job_IndustryWeights" sheetId="26" r:id="rId8"/>
-    <sheet name="Emissions" sheetId="24" r:id="rId9"/>
-    <sheet name="Commodity Prices" sheetId="25" r:id="rId10"/>
-    <sheet name="F2C Jobs old" sheetId="11" r:id="rId11"/>
-    <sheet name="Infrastructure" sheetId="19" r:id="rId12"/>
-    <sheet name="Unit Conversion" sheetId="18" r:id="rId13"/>
-    <sheet name="Conversion" sheetId="15" r:id="rId14"/>
-    <sheet name="Feedstock to Commodity Buildout" sheetId="7" r:id="rId15"/>
-    <sheet name="Commodity to Use Buildout" sheetId="8" r:id="rId16"/>
-    <sheet name="F2C_ver2" sheetId="20" r:id="rId17"/>
-    <sheet name="Commodity To Use Matrix" sheetId="6" r:id="rId18"/>
-    <sheet name="table from Julia (to be deleted" sheetId="16" r:id="rId19"/>
-    <sheet name="Feedstock to Commodity Matrix" sheetId="4" r:id="rId20"/>
+    <sheet name="Wage Distribution" sheetId="27" r:id="rId8"/>
+    <sheet name="Job_IndustryWeights" sheetId="26" r:id="rId9"/>
+    <sheet name="Emissions" sheetId="24" r:id="rId10"/>
+    <sheet name="Commodity Prices" sheetId="25" r:id="rId11"/>
+    <sheet name="F2C Jobs old" sheetId="11" r:id="rId12"/>
+    <sheet name="Infrastructure" sheetId="19" r:id="rId13"/>
+    <sheet name="Unit Conversion" sheetId="18" r:id="rId14"/>
+    <sheet name="Conversion" sheetId="15" r:id="rId15"/>
+    <sheet name="Feedstock to Commodity Buildout" sheetId="7" r:id="rId16"/>
+    <sheet name="Commodity to Use Buildout" sheetId="8" r:id="rId17"/>
+    <sheet name="F2C_ver2" sheetId="20" r:id="rId18"/>
+    <sheet name="Commodity To Use Matrix" sheetId="6" r:id="rId19"/>
+    <sheet name="table from Julia (to be deleted" sheetId="16" r:id="rId20"/>
+    <sheet name="Feedstock to Commodity Matrix" sheetId="4" r:id="rId21"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'C2U CI'!$A$1:$AA$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'F2C CI'!$A$1:$I$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'F2C Conversion'!$A$1:$Q$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'F2C Jobs'!$A$1:$O$58</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'F2C Jobs old'!$A$1:$J$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'F2C Jobs old'!$A$1:$J$13</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'F2C Land'!$A$1:$K$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'F2C Water'!$A$1:$L$41</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'Unit Conversion'!$A$1:$AK$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'Unit Conversion'!$A$1:$AK$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -65,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2696" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2929" uniqueCount="389">
   <si>
     <t>Feedstock</t>
   </si>
@@ -1234,6 +1235,12 @@
   </si>
   <si>
     <t>Productivity</t>
+  </si>
+  <si>
+    <t>Share of Postings Over Living Wage</t>
+  </si>
+  <si>
+    <t>Share of Postings Under Living Wage</t>
   </si>
 </sst>
 </file>
@@ -1251,7 +1258,7 @@
     <numFmt numFmtId="169" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1353,6 +1360,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -1440,12 +1453,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1557,11 +1571,12 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="5" xr:uid="{0F11785E-7C0D-45F6-B74A-E0DEC65AA1F0}"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2757,6 +2772,107 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8B6CA4-5F91-483F-9DB3-0E00AF0370F3}">
+  <sheetPr>
+    <tabColor theme="5" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.25" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="55" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="55" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>343</v>
+      </c>
+      <c r="D2" t="s">
+        <v>347</v>
+      </c>
+      <c r="E2" s="69">
+        <f>34752*1000000/126832800000</f>
+        <v>0.27399852404109976</v>
+      </c>
+      <c r="F2" t="s">
+        <v>346</v>
+      </c>
+      <c r="G2" s="67" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" s="55" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="55" t="s">
+        <v>344</v>
+      </c>
+      <c r="D3" t="s">
+        <v>349</v>
+      </c>
+      <c r="E3" s="69">
+        <f>343*1000000/126832800000</f>
+        <v>2.7043477712389856E-3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>348</v>
+      </c>
+      <c r="G3" s="67" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" display="https://arb.ca.gov/emfac/meta/on-road-hdv" xr:uid="{F07D1BF2-06AD-4598-AF94-C04C6DE054AA}"/>
+    <hyperlink ref="G3" r:id="rId2" display="https://arb.ca.gov/emfac/meta/on-road-hdv" xr:uid="{61D1EEAB-16A7-441D-9D2C-18104D78ACFE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0073DEA3-76EA-4A12-96E2-2D18F90530EF}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -3387,7 +3503,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86CE6374-45B2-3044-B48D-E84DB83BCE11}">
   <dimension ref="A1:J13"/>
   <sheetViews>
@@ -3690,7 +3806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EBD7D08-7196-4DD6-A58C-02D5A271324B}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -3753,7 +3869,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FA5616B-DF07-465E-AEEB-CCA6D05FE697}">
   <dimension ref="A1:AK23"/>
   <sheetViews>
@@ -5038,7 +5154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB87BF8B-8E54-426F-864A-9E457E959B26}">
   <dimension ref="A1:Y19"/>
   <sheetViews>
@@ -5881,7 +5997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4534657-2DF7-8944-A332-1622EE581035}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
@@ -7562,7 +7678,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3F942D-1725-B745-A61F-46451943A74C}">
   <dimension ref="A1:W6"/>
   <sheetViews>
@@ -8007,7 +8123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DDDA0F3-A3DE-4AB4-98AB-8BE3425A27E0}">
   <dimension ref="A1:G30"/>
   <sheetViews>
@@ -8496,7 +8612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30085204-D4C6-FC4C-98EB-2FC1A2E0E66E}">
   <dimension ref="A1:I6"/>
   <sheetViews>
@@ -8596,888 +8712,6 @@
       </c>
       <c r="G6">
         <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF7B0DD-C673-4DCD-83AE-47E17C286F51}">
-  <dimension ref="A1:K68"/>
-  <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="47.83203125" customWidth="1"/>
-    <col min="2" max="2" width="30.08203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" customWidth="1"/>
-    <col min="5" max="5" width="30.58203125" customWidth="1"/>
-    <col min="6" max="6" width="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>159</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" t="s">
-        <v>159</v>
-      </c>
-      <c r="K1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="F2" s="14" t="s">
-        <v>169</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="15"/>
-      <c r="F3" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="D4" s="15"/>
-      <c r="F4" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="I4" t="s">
-        <v>56</v>
-      </c>
-      <c r="J4" t="s">
-        <v>178</v>
-      </c>
-      <c r="K4" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="F5" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="I5" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="F6" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15"/>
-      <c r="F7" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" t="s">
-        <v>56</v>
-      </c>
-      <c r="J7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15"/>
-      <c r="F8" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="I8" t="s">
-        <v>183</v>
-      </c>
-      <c r="J8" t="s">
-        <v>171</v>
-      </c>
-      <c r="K8" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="F9" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" t="s">
-        <v>183</v>
-      </c>
-      <c r="J9" t="s">
-        <v>175</v>
-      </c>
-      <c r="K9" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="F10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>183</v>
-      </c>
-      <c r="I10" t="s">
-        <v>183</v>
-      </c>
-      <c r="J10" t="s">
-        <v>178</v>
-      </c>
-      <c r="K10" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="F11" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="I11" t="s">
-        <v>183</v>
-      </c>
-      <c r="J11" t="s">
-        <v>71</v>
-      </c>
-      <c r="K11" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>185</v>
-      </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="I12" t="s">
-        <v>183</v>
-      </c>
-      <c r="J12" t="s">
-        <v>184</v>
-      </c>
-      <c r="K12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="I13" t="s">
-        <v>183</v>
-      </c>
-      <c r="J13" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="15"/>
-      <c r="I14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" t="s">
-        <v>178</v>
-      </c>
-      <c r="K15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="B16" s="20" t="s">
-        <v>190</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16" s="21" t="s">
-        <v>191</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="62" x14ac:dyDescent="0.35">
-      <c r="A17" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="D17" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="62" x14ac:dyDescent="0.35">
-      <c r="A18" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>195</v>
-      </c>
-      <c r="I18" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="62" x14ac:dyDescent="0.35">
-      <c r="A19" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="B19" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C19" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="23" t="s">
-        <v>182</v>
-      </c>
-      <c r="B20" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="C20" s="24" t="s">
-        <v>199</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="C21" s="24" t="s">
-        <v>199</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="C22" s="24" t="s">
-        <v>199</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="26" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A31" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31" s="32" t="s">
-        <v>202</v>
-      </c>
-      <c r="C31" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="D31" t="s">
-        <v>204</v>
-      </c>
-      <c r="E31" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B32" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="14"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B33" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="14"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" s="14"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="14" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C36" s="14"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="14" t="s">
-        <v>207</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="C37" s="14"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="B38" s="14" t="s">
-        <v>208</v>
-      </c>
-      <c r="C38" s="14"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="B41" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>209</v>
-      </c>
-      <c r="D41" t="s">
-        <v>210</v>
-      </c>
-      <c r="E41" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="B42" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="C42" s="27" t="s">
-        <v>209</v>
-      </c>
-      <c r="D42" t="s">
-        <v>210</v>
-      </c>
-      <c r="E42" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="26" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="B46" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="C46" s="32" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B47" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="C47" s="34" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B48" s="31" t="s">
-        <v>215</v>
-      </c>
-      <c r="C48" s="28" t="s">
-        <v>216</v>
-      </c>
-      <c r="D48" t="s">
-        <v>24</v>
-      </c>
-      <c r="E48" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A49" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B49" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="C49" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="D49" t="s">
-        <v>218</v>
-      </c>
-      <c r="E49" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A50" s="30" t="s">
-        <v>19</v>
-      </c>
-      <c r="B50" s="31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="D50" t="s">
-        <v>221</v>
-      </c>
-      <c r="E50" t="s">
-        <v>222</v>
-      </c>
-      <c r="F50" s="35" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A51" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="B51" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="C51" s="27" t="s">
-        <v>224</v>
-      </c>
-      <c r="D51" t="s">
-        <v>24</v>
-      </c>
-      <c r="E51" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A52" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B52" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="C52" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="D52" t="s">
-        <v>26</v>
-      </c>
-      <c r="E52" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A53" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C53" s="34" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A54" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="B54" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="C54" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="D54" t="s">
-        <v>26</v>
-      </c>
-      <c r="E54" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A55" s="27" t="s">
-        <v>12</v>
-      </c>
-      <c r="B55" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="C55" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="D55" t="s">
-        <v>24</v>
-      </c>
-      <c r="E55" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A56" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B56" s="15" t="s">
-        <v>229</v>
-      </c>
-      <c r="C56" s="34" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A60" s="26" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A61" s="27" t="s">
-        <v>231</v>
-      </c>
-      <c r="D61" t="s">
-        <v>24</v>
-      </c>
-      <c r="E61" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A62" s="29" t="s">
-        <v>233</v>
-      </c>
-      <c r="D62" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A63" s="27" t="s">
-        <v>234</v>
-      </c>
-      <c r="D63" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A66" s="26" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A67" s="27" t="s">
-        <v>236</v>
-      </c>
-      <c r="D67" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A68" s="27" t="s">
-        <v>237</v>
-      </c>
-      <c r="D68" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>
@@ -10123,6 +9357,888 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF7B0DD-C673-4DCD-83AE-47E17C286F51}">
+  <dimension ref="A1:K68"/>
+  <sheetViews>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="47.83203125" customWidth="1"/>
+    <col min="2" max="2" width="30.08203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
+    <col min="5" max="5" width="30.58203125" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" t="s">
+        <v>159</v>
+      </c>
+      <c r="K1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="F2" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="15"/>
+      <c r="F3" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="F4" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="I4" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" t="s">
+        <v>178</v>
+      </c>
+      <c r="K4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="F5" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="F6" s="16" t="s">
+        <v>182</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="F7" s="14" t="s">
+        <v>182</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="15"/>
+      <c r="F8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="I8" t="s">
+        <v>183</v>
+      </c>
+      <c r="J8" t="s">
+        <v>171</v>
+      </c>
+      <c r="K8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="F9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" t="s">
+        <v>183</v>
+      </c>
+      <c r="J9" t="s">
+        <v>175</v>
+      </c>
+      <c r="K9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="F10" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="16" t="s">
+        <v>183</v>
+      </c>
+      <c r="I10" t="s">
+        <v>183</v>
+      </c>
+      <c r="J10" t="s">
+        <v>178</v>
+      </c>
+      <c r="K10" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="F11" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" t="s">
+        <v>183</v>
+      </c>
+      <c r="J11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="I12" t="s">
+        <v>183</v>
+      </c>
+      <c r="J12" t="s">
+        <v>184</v>
+      </c>
+      <c r="K12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="15"/>
+      <c r="I13" t="s">
+        <v>183</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="15"/>
+      <c r="I14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" t="s">
+        <v>178</v>
+      </c>
+      <c r="K15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="46.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+      <c r="A17" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+      <c r="A18" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="I18" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="62" x14ac:dyDescent="0.35">
+      <c r="A19" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="D19" s="21" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="23" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="77.5" x14ac:dyDescent="0.35">
+      <c r="A22" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30" s="26" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="32" t="s">
+        <v>202</v>
+      </c>
+      <c r="C31" s="32" t="s">
+        <v>203</v>
+      </c>
+      <c r="D31" t="s">
+        <v>204</v>
+      </c>
+      <c r="E31" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="14"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="14"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C35" s="14" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="14"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C37" s="14"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="C38" s="14"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C39" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D41" t="s">
+        <v>210</v>
+      </c>
+      <c r="E41" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="14" t="s">
+        <v>181</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D42" t="s">
+        <v>210</v>
+      </c>
+      <c r="E42" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="B46" s="33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C47" s="34" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A48" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B48" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="D48" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B49" s="31" t="s">
+        <v>163</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" t="s">
+        <v>218</v>
+      </c>
+      <c r="E49" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A50" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B50" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C50" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="D50" t="s">
+        <v>221</v>
+      </c>
+      <c r="E50" t="s">
+        <v>222</v>
+      </c>
+      <c r="F50" s="35" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A51" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B51" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C51" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="D51" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A52" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="C52" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="D52" t="s">
+        <v>26</v>
+      </c>
+      <c r="E52" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A53" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A54" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C54" s="27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D54" t="s">
+        <v>26</v>
+      </c>
+      <c r="E54" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A55" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="C55" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="D55" t="s">
+        <v>24</v>
+      </c>
+      <c r="E55" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A56" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B56" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C56" s="34" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A60" s="26" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A61" s="27" t="s">
+        <v>231</v>
+      </c>
+      <c r="D61" t="s">
+        <v>24</v>
+      </c>
+      <c r="E61" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A62" s="29" t="s">
+        <v>233</v>
+      </c>
+      <c r="D62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A63" s="27" t="s">
+        <v>234</v>
+      </c>
+      <c r="D63" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="26" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67" s="27" t="s">
+        <v>236</v>
+      </c>
+      <c r="D67" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="27" t="s">
+        <v>237</v>
+      </c>
+      <c r="D68" t="s">
+        <v>238</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6977DE39-83AB-8346-8AC1-EC99E6C87D8C}">
   <dimension ref="A1:F12"/>
   <sheetViews>
@@ -13345,7 +13461,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -14308,8 +14424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B16BE7FC-A8FD-4D95-933D-26AA617CB019}">
   <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N24" sqref="N24"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -16980,6 +17096,897 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A38D628-CFB3-4EEB-8A14-4144429F721F}">
+  <dimension ref="A1:G39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
+    <col min="4" max="4" width="48.58203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D2" t="s">
+        <v>314</v>
+      </c>
+      <c r="E2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F2" t="s">
+        <v>388</v>
+      </c>
+      <c r="G2">
+        <v>0.51100000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>309</v>
+      </c>
+      <c r="D3" t="s">
+        <v>314</v>
+      </c>
+      <c r="E3" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" t="s">
+        <v>387</v>
+      </c>
+      <c r="G3">
+        <v>0.48899999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>309</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F4" t="s">
+        <v>388</v>
+      </c>
+      <c r="G4">
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" t="s">
+        <v>387</v>
+      </c>
+      <c r="G5">
+        <v>0.66300000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D6" t="s">
+        <v>143</v>
+      </c>
+      <c r="E6" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" t="s">
+        <v>388</v>
+      </c>
+      <c r="G6">
+        <v>0.23899999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>309</v>
+      </c>
+      <c r="D7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F7" t="s">
+        <v>387</v>
+      </c>
+      <c r="G7">
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>309</v>
+      </c>
+      <c r="E8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" t="s">
+        <v>388</v>
+      </c>
+      <c r="G8">
+        <v>0.23899999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>309</v>
+      </c>
+      <c r="E9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" t="s">
+        <v>387</v>
+      </c>
+      <c r="G9">
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" t="s">
+        <v>309</v>
+      </c>
+      <c r="D10" t="s">
+        <v>318</v>
+      </c>
+      <c r="E10" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>309</v>
+      </c>
+      <c r="D11" t="s">
+        <v>318</v>
+      </c>
+      <c r="E11" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>309</v>
+      </c>
+      <c r="D12" t="s">
+        <v>318</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>309</v>
+      </c>
+      <c r="D13" t="s">
+        <v>318</v>
+      </c>
+      <c r="E13" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>309</v>
+      </c>
+      <c r="D14" t="s">
+        <v>318</v>
+      </c>
+      <c r="E14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F14" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>309</v>
+      </c>
+      <c r="D15" t="s">
+        <v>318</v>
+      </c>
+      <c r="E15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F15" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" t="s">
+        <v>309</v>
+      </c>
+      <c r="D16" t="s">
+        <v>318</v>
+      </c>
+      <c r="E16" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>309</v>
+      </c>
+      <c r="D17" t="s">
+        <v>318</v>
+      </c>
+      <c r="E17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>310</v>
+      </c>
+      <c r="D18" t="s">
+        <v>320</v>
+      </c>
+      <c r="E18" t="s">
+        <v>89</v>
+      </c>
+      <c r="F18" t="s">
+        <v>388</v>
+      </c>
+      <c r="G18">
+        <v>0.376</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>310</v>
+      </c>
+      <c r="D19" t="s">
+        <v>320</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" t="s">
+        <v>387</v>
+      </c>
+      <c r="G19">
+        <v>0.624</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>310</v>
+      </c>
+      <c r="D20" t="s">
+        <v>320</v>
+      </c>
+      <c r="E20" t="s">
+        <v>89</v>
+      </c>
+      <c r="F20" t="s">
+        <v>388</v>
+      </c>
+      <c r="G20">
+        <v>0.376</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>310</v>
+      </c>
+      <c r="D21" t="s">
+        <v>320</v>
+      </c>
+      <c r="E21" t="s">
+        <v>89</v>
+      </c>
+      <c r="F21" t="s">
+        <v>387</v>
+      </c>
+      <c r="G21">
+        <v>0.624</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>310</v>
+      </c>
+      <c r="D22" t="s">
+        <v>319</v>
+      </c>
+      <c r="E22" t="s">
+        <v>89</v>
+      </c>
+      <c r="F22" t="s">
+        <v>388</v>
+      </c>
+      <c r="G22">
+        <v>0.376</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>310</v>
+      </c>
+      <c r="D23" t="s">
+        <v>319</v>
+      </c>
+      <c r="E23" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" t="s">
+        <v>387</v>
+      </c>
+      <c r="G23">
+        <v>0.624</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>310</v>
+      </c>
+      <c r="D24" t="s">
+        <v>319</v>
+      </c>
+      <c r="E24" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24" t="s">
+        <v>388</v>
+      </c>
+      <c r="G24">
+        <v>0.376</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" t="s">
+        <v>310</v>
+      </c>
+      <c r="D25" t="s">
+        <v>319</v>
+      </c>
+      <c r="E25" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25" t="s">
+        <v>387</v>
+      </c>
+      <c r="G25">
+        <v>0.624</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" t="s">
+        <v>310</v>
+      </c>
+      <c r="D26" t="s">
+        <v>320</v>
+      </c>
+      <c r="E26" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26" t="s">
+        <v>388</v>
+      </c>
+      <c r="G26">
+        <v>0.376</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" t="s">
+        <v>310</v>
+      </c>
+      <c r="D27" t="s">
+        <v>320</v>
+      </c>
+      <c r="E27" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27" t="s">
+        <v>387</v>
+      </c>
+      <c r="G27">
+        <v>0.624</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>310</v>
+      </c>
+      <c r="D28" t="s">
+        <v>320</v>
+      </c>
+      <c r="E28" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28" t="s">
+        <v>388</v>
+      </c>
+      <c r="G28">
+        <v>0.376</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>310</v>
+      </c>
+      <c r="D29" t="s">
+        <v>320</v>
+      </c>
+      <c r="E29" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29" t="s">
+        <v>387</v>
+      </c>
+      <c r="G29">
+        <v>0.624</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>310</v>
+      </c>
+      <c r="D30" t="s">
+        <v>375</v>
+      </c>
+      <c r="E30" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30" t="s">
+        <v>388</v>
+      </c>
+      <c r="G30">
+        <v>0.58199999999999996</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" t="s">
+        <v>310</v>
+      </c>
+      <c r="D31" t="s">
+        <v>375</v>
+      </c>
+      <c r="E31" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" t="s">
+        <v>387</v>
+      </c>
+      <c r="G31">
+        <v>0.41799999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>310</v>
+      </c>
+      <c r="D32" t="s">
+        <v>375</v>
+      </c>
+      <c r="E32" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32" t="s">
+        <v>388</v>
+      </c>
+      <c r="G32">
+        <v>0.58199999999999996</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>310</v>
+      </c>
+      <c r="D33" t="s">
+        <v>375</v>
+      </c>
+      <c r="E33" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" t="s">
+        <v>387</v>
+      </c>
+      <c r="G33">
+        <v>0.41799999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C34" t="s">
+        <v>310</v>
+      </c>
+      <c r="D34" t="s">
+        <v>321</v>
+      </c>
+      <c r="E34" t="s">
+        <v>89</v>
+      </c>
+      <c r="F34" t="s">
+        <v>388</v>
+      </c>
+      <c r="G34">
+        <v>0.40300000000000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" t="s">
+        <v>310</v>
+      </c>
+      <c r="D35" t="s">
+        <v>321</v>
+      </c>
+      <c r="E35" t="s">
+        <v>89</v>
+      </c>
+      <c r="F35" t="s">
+        <v>387</v>
+      </c>
+      <c r="G35">
+        <v>0.59699999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" t="s">
+        <v>46</v>
+      </c>
+      <c r="C36" t="s">
+        <v>310</v>
+      </c>
+      <c r="D36" t="s">
+        <v>319</v>
+      </c>
+      <c r="E36" t="s">
+        <v>89</v>
+      </c>
+      <c r="F36" t="s">
+        <v>388</v>
+      </c>
+      <c r="G36">
+        <v>0.40300000000000002</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" t="s">
+        <v>310</v>
+      </c>
+      <c r="D37" t="s">
+        <v>319</v>
+      </c>
+      <c r="E37" t="s">
+        <v>89</v>
+      </c>
+      <c r="F37" t="s">
+        <v>387</v>
+      </c>
+      <c r="G37">
+        <v>0.59699999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>36</v>
+      </c>
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38" t="s">
+        <v>310</v>
+      </c>
+      <c r="D38" t="s">
+        <v>319</v>
+      </c>
+      <c r="E38" t="s">
+        <v>89</v>
+      </c>
+      <c r="F38" t="s">
+        <v>388</v>
+      </c>
+      <c r="G38">
+        <v>0.40300000000000002</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" t="s">
+        <v>310</v>
+      </c>
+      <c r="D39" t="s">
+        <v>319</v>
+      </c>
+      <c r="E39" t="s">
+        <v>89</v>
+      </c>
+      <c r="F39" t="s">
+        <v>387</v>
+      </c>
+      <c r="G39">
+        <v>0.59699999999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D290F1B-2D07-493A-830D-4D26C0F8027E}">
   <sheetPr>
     <tabColor theme="5" tint="0.79998168889431442"/>
@@ -17775,107 +18782,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8B6CA4-5F91-483F-9DB3-0E00AF0370F3}">
-  <sheetPr>
-    <tabColor theme="5" tint="0.79998168889431442"/>
-  </sheetPr>
-  <dimension ref="A1:G3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.25" customWidth="1"/>
-    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.75" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="55" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="55" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="55" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C2" s="55" t="s">
-        <v>343</v>
-      </c>
-      <c r="D2" t="s">
-        <v>347</v>
-      </c>
-      <c r="E2" s="69">
-        <f>34752*1000000/126832800000</f>
-        <v>0.27399852404109976</v>
-      </c>
-      <c r="F2" t="s">
-        <v>346</v>
-      </c>
-      <c r="G2" s="67" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="55" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="C3" s="55" t="s">
-        <v>344</v>
-      </c>
-      <c r="D3" t="s">
-        <v>349</v>
-      </c>
-      <c r="E3" s="69">
-        <f>343*1000000/126832800000</f>
-        <v>2.7043477712389856E-3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>348</v>
-      </c>
-      <c r="G3" s="67" t="s">
-        <v>345</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" display="https://arb.ca.gov/emfac/meta/on-road-hdv" xr:uid="{F07D1BF2-06AD-4598-AF94-C04C6DE054AA}"/>
-    <hyperlink ref="G3" r:id="rId2" display="https://arb.ca.gov/emfac/meta/on-road-hdv" xr:uid="{61D1EEAB-16A7-441D-9D2C-18104D78ACFE}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{78975c20-18d4-40c9-811f-0d8ea387c6ea}" enabled="0" method="" siteId="{78975c20-18d4-40c9-811f-0d8ea387c6ea}" removed="1"/>

</xml_diff>